<commit_message>
Q3 2021 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\0. IAD activities\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2021\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\0. IAD activities\6. MAS_Series\2018-base\NAP\NAP detailed series as of November 2021\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10788"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="EOS" sheetId="5" r:id="rId1"/>
@@ -42,9 +42,9 @@
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt" localSheetId="0">EOS!$A$37:$A$48</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EOS!$A$1:$CI$174</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EOS!$A$1:$CJ$174</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="56">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -215,13 +215,13 @@
     <t>2021 - 2021</t>
   </si>
   <si>
-    <t>As of August 2021</t>
+    <t>As of November 2021</t>
   </si>
   <si>
-    <t>Q1 2000 to Q2 2021</t>
+    <t>Q1 2000 to Q3 2021</t>
   </si>
   <si>
-    <t>Q1 2001 to Q2 2021</t>
+    <t>Q1 2001 to Q3 2021</t>
   </si>
 </sst>
 </file>
@@ -339,9 +339,6 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -354,6 +351,9 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -697,12 +697,12 @@
   </sheetPr>
   <dimension ref="A1:EU174"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="87" zoomScaleNormal="95" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CA3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="95" zoomScaleNormal="95" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="CA50" activePane="bottomRight" state="frozen"/>
       <selection activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="topRight" activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="bottomLeft" activeCell="P1" sqref="P1:AF1048576"/>
-      <selection pane="bottomRight" activeCell="BY28" sqref="BY28"/>
+      <selection pane="bottomRight" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -711,8 +711,8 @@
     <col min="2" max="73" width="8.81640625" style="1" customWidth="1"/>
     <col min="74" max="80" width="10" style="1" customWidth="1"/>
     <col min="81" max="81" width="10.26953125" style="1" customWidth="1"/>
-    <col min="82" max="87" width="10.26953125" style="18" customWidth="1"/>
-    <col min="88" max="16384" width="7.81640625" style="1"/>
+    <col min="82" max="88" width="11.36328125" style="18" customWidth="1"/>
+    <col min="89" max="16384" width="7.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:151" x14ac:dyDescent="0.25">
@@ -877,6 +877,7 @@
         <v>2021</v>
       </c>
       <c r="CI9" s="28"/>
+      <c r="CJ9" s="28"/>
     </row>
     <row r="10" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1120,23 +1121,26 @@
       <c r="CC10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CD10" s="20" t="s">
+      <c r="CD10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CE10" s="20" t="s">
+      <c r="CE10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="CF10" s="20" t="s">
+      <c r="CF10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="CG10" s="20" t="s">
+      <c r="CG10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="CH10" s="20" t="s">
+      <c r="CH10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CI10" s="20" t="s">
+      <c r="CI10" s="19" t="s">
         <v>8</v>
+      </c>
+      <c r="CJ10" s="19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1386,25 +1390,27 @@
       <c r="CC12" s="7">
         <v>45790.436819050155</v>
       </c>
-      <c r="CD12" s="21">
+      <c r="CD12" s="20">
         <v>32010.978337237957</v>
       </c>
-      <c r="CE12" s="21">
+      <c r="CE12" s="20">
         <v>13299.247113344074</v>
       </c>
-      <c r="CF12" s="21">
+      <c r="CF12" s="20">
         <v>21183.699192354972</v>
       </c>
-      <c r="CG12" s="21">
+      <c r="CG12" s="20">
         <v>23901.456567192312</v>
       </c>
-      <c r="CH12" s="21">
+      <c r="CH12" s="20">
         <v>20322.731784015399</v>
       </c>
-      <c r="CI12" s="21">
-        <v>17066.282796217383</v>
-      </c>
-      <c r="CJ12" s="8"/>
+      <c r="CI12" s="20">
+        <v>16391.545194812847</v>
+      </c>
+      <c r="CJ12" s="20">
+        <v>25716.285814568222</v>
+      </c>
       <c r="CK12" s="8"/>
       <c r="CL12" s="8"/>
       <c r="CM12" s="8"/>
@@ -1713,25 +1719,27 @@
       <c r="CC13" s="7">
         <v>811.98755828997855</v>
       </c>
-      <c r="CD13" s="21">
+      <c r="CD13" s="20">
         <v>455.76866341495628</v>
       </c>
-      <c r="CE13" s="21">
+      <c r="CE13" s="20">
         <v>271.15791756005291</v>
       </c>
-      <c r="CF13" s="21">
+      <c r="CF13" s="20">
         <v>700.97163490021353</v>
       </c>
-      <c r="CG13" s="21">
+      <c r="CG13" s="20">
         <v>785.29196317838819</v>
       </c>
-      <c r="CH13" s="21">
+      <c r="CH13" s="20">
         <v>493.50282696812621</v>
       </c>
-      <c r="CI13" s="21">
-        <v>369.48270512812536</v>
-      </c>
-      <c r="CJ13" s="8"/>
+      <c r="CI13" s="20">
+        <v>387.57697975435258</v>
+      </c>
+      <c r="CJ13" s="20">
+        <v>812.3587129134221</v>
+      </c>
       <c r="CK13" s="8"/>
       <c r="CL13" s="8"/>
       <c r="CM13" s="8"/>
@@ -2040,25 +2048,27 @@
       <c r="CC14" s="7">
         <v>102672.183663597</v>
       </c>
-      <c r="CD14" s="21">
+      <c r="CD14" s="20">
         <v>113062.26479711011</v>
       </c>
-      <c r="CE14" s="21">
+      <c r="CE14" s="20">
         <v>5409.6907766346912</v>
       </c>
-      <c r="CF14" s="21">
+      <c r="CF14" s="20">
         <v>14472.992673047263</v>
       </c>
-      <c r="CG14" s="21">
+      <c r="CG14" s="20">
         <v>8252.2359478950566</v>
       </c>
-      <c r="CH14" s="21">
+      <c r="CH14" s="20">
         <v>2347.5074399000005</v>
       </c>
-      <c r="CI14" s="21">
-        <v>17497.304546236614</v>
-      </c>
-      <c r="CJ14" s="8"/>
+      <c r="CI14" s="20">
+        <v>29673.480158083239</v>
+      </c>
+      <c r="CJ14" s="20">
+        <v>23247.77711361623</v>
+      </c>
       <c r="CK14" s="8"/>
       <c r="CL14" s="8"/>
       <c r="CM14" s="8"/>
@@ -2367,25 +2377,27 @@
       <c r="CC15" s="7">
         <v>2687.5370860009766</v>
       </c>
-      <c r="CD15" s="21">
+      <c r="CD15" s="20">
         <v>2525.5740580868278</v>
       </c>
-      <c r="CE15" s="21">
+      <c r="CE15" s="20">
         <v>2718.4891110303574</v>
       </c>
-      <c r="CF15" s="21">
+      <c r="CF15" s="20">
         <v>2967.0275841402954</v>
       </c>
-      <c r="CG15" s="21">
+      <c r="CG15" s="20">
         <v>2953.3815928242416</v>
       </c>
-      <c r="CH15" s="21">
+      <c r="CH15" s="20">
         <v>3085.9450636350798</v>
       </c>
-      <c r="CI15" s="21">
-        <v>3360.4202604514762</v>
-      </c>
-      <c r="CJ15" s="8"/>
+      <c r="CI15" s="20">
+        <v>3438.8113492011848</v>
+      </c>
+      <c r="CJ15" s="20">
+        <v>3776.4891554276164</v>
+      </c>
       <c r="CK15" s="8"/>
       <c r="CL15" s="8"/>
       <c r="CM15" s="8"/>
@@ -2694,25 +2706,27 @@
       <c r="CC16" s="7">
         <v>64546.344676669141</v>
       </c>
-      <c r="CD16" s="21">
+      <c r="CD16" s="20">
         <v>106388.76006203156</v>
       </c>
-      <c r="CE16" s="21">
+      <c r="CE16" s="20">
         <v>86074.346190977856</v>
       </c>
-      <c r="CF16" s="21">
+      <c r="CF16" s="20">
         <v>58108.39956313611</v>
       </c>
-      <c r="CG16" s="21">
+      <c r="CG16" s="20">
         <v>60540.715796021614</v>
       </c>
-      <c r="CH16" s="21">
+      <c r="CH16" s="20">
         <v>104028.14005270365</v>
       </c>
-      <c r="CI16" s="21">
-        <v>104314.74675903127</v>
-      </c>
-      <c r="CJ16" s="8"/>
+      <c r="CI16" s="20">
+        <v>101878.54866967555</v>
+      </c>
+      <c r="CJ16" s="20">
+        <v>70922.376110319237</v>
+      </c>
       <c r="CK16" s="8"/>
       <c r="CL16" s="8"/>
       <c r="CM16" s="8"/>
@@ -3021,25 +3035,27 @@
       <c r="CC17" s="7">
         <v>269156.31011836824</v>
       </c>
-      <c r="CD17" s="21">
+      <c r="CD17" s="20">
         <v>346096.80980260269</v>
       </c>
-      <c r="CE17" s="21">
+      <c r="CE17" s="20">
         <v>299196.14261641022</v>
       </c>
-      <c r="CF17" s="21">
+      <c r="CF17" s="20">
         <v>251241.18618202559</v>
       </c>
-      <c r="CG17" s="21">
+      <c r="CG17" s="20">
         <v>270907.40938500199</v>
       </c>
-      <c r="CH17" s="21">
+      <c r="CH17" s="20">
         <v>342299.43622982444</v>
       </c>
-      <c r="CI17" s="21">
-        <v>352260.9583559772</v>
-      </c>
-      <c r="CJ17" s="8"/>
+      <c r="CI17" s="20">
+        <v>346990.80493395386</v>
+      </c>
+      <c r="CJ17" s="20">
+        <v>259288.63493118281</v>
+      </c>
       <c r="CK17" s="8"/>
       <c r="CL17" s="8"/>
       <c r="CM17" s="8"/>
@@ -3348,25 +3364,27 @@
       <c r="CC18" s="7">
         <v>46459.03507256334</v>
       </c>
-      <c r="CD18" s="21">
+      <c r="CD18" s="20">
         <v>71805.642590515621</v>
       </c>
-      <c r="CE18" s="21">
+      <c r="CE18" s="20">
         <v>59520.593464625519</v>
       </c>
-      <c r="CF18" s="21">
+      <c r="CF18" s="20">
         <v>45589.088109905439</v>
       </c>
-      <c r="CG18" s="21">
+      <c r="CG18" s="20">
         <v>42373.462819087537</v>
       </c>
-      <c r="CH18" s="21">
+      <c r="CH18" s="20">
         <v>70739.801760135873</v>
       </c>
-      <c r="CI18" s="21">
-        <v>71574.124143462002</v>
-      </c>
-      <c r="CJ18" s="8"/>
+      <c r="CI18" s="20">
+        <v>73530.605226210522</v>
+      </c>
+      <c r="CJ18" s="20">
+        <v>60443.261262100285</v>
+      </c>
       <c r="CK18" s="8"/>
       <c r="CL18" s="8"/>
       <c r="CM18" s="8"/>
@@ -3675,25 +3693,27 @@
       <c r="CC19" s="7">
         <v>7878.07073289245</v>
       </c>
-      <c r="CD19" s="21">
+      <c r="CD19" s="20">
         <v>6248.762207795804</v>
       </c>
-      <c r="CE19" s="21">
+      <c r="CE19" s="20">
         <v>6149.9095023102891</v>
       </c>
-      <c r="CF19" s="21">
+      <c r="CF19" s="20">
         <v>5608.2856491674693</v>
       </c>
-      <c r="CG19" s="21">
+      <c r="CG19" s="20">
         <v>5681.5271120043963</v>
       </c>
-      <c r="CH19" s="21">
+      <c r="CH19" s="20">
         <v>5334.4905963892161</v>
       </c>
-      <c r="CI19" s="21">
-        <v>6675.029720399265</v>
-      </c>
-      <c r="CJ19" s="8"/>
+      <c r="CI19" s="20">
+        <v>6709.2897414248655</v>
+      </c>
+      <c r="CJ19" s="20">
+        <v>6887.3941455703925</v>
+      </c>
       <c r="CK19" s="8"/>
       <c r="CL19" s="8"/>
       <c r="CM19" s="8"/>
@@ -3839,13 +3859,13 @@
       <c r="CA20" s="8"/>
       <c r="CB20" s="8"/>
       <c r="CC20" s="8"/>
-      <c r="CD20" s="22"/>
-      <c r="CE20" s="22"/>
-      <c r="CF20" s="22"/>
-      <c r="CG20" s="22"/>
-      <c r="CH20" s="22"/>
-      <c r="CI20" s="22"/>
-      <c r="CJ20" s="8"/>
+      <c r="CD20" s="21"/>
+      <c r="CE20" s="21"/>
+      <c r="CF20" s="21"/>
+      <c r="CG20" s="21"/>
+      <c r="CH20" s="21"/>
+      <c r="CI20" s="21"/>
+      <c r="CJ20" s="21"/>
       <c r="CK20" s="8"/>
       <c r="CL20" s="8"/>
       <c r="CM20" s="8"/>
@@ -4154,25 +4174,27 @@
       <c r="CC21" s="10">
         <v>540001.90572743129</v>
       </c>
-      <c r="CD21" s="23">
+      <c r="CD21" s="22">
         <v>678594.56051879551</v>
       </c>
-      <c r="CE21" s="23">
+      <c r="CE21" s="22">
         <v>472639.57669289305</v>
       </c>
-      <c r="CF21" s="23">
+      <c r="CF21" s="22">
         <v>399871.65058867732</v>
       </c>
-      <c r="CG21" s="23">
+      <c r="CG21" s="22">
         <v>415395.48118320556</v>
       </c>
-      <c r="CH21" s="23">
+      <c r="CH21" s="22">
         <v>548651.5557535718</v>
       </c>
-      <c r="CI21" s="23">
-        <v>573118.34928690339</v>
-      </c>
-      <c r="CJ21" s="8"/>
+      <c r="CI21" s="22">
+        <v>579000.66225311637</v>
+      </c>
+      <c r="CJ21" s="22">
+        <v>451094.57724569825</v>
+      </c>
       <c r="CK21" s="8"/>
       <c r="CL21" s="8"/>
       <c r="CM21" s="8"/>
@@ -4319,12 +4341,13 @@
       <c r="CA22" s="11"/>
       <c r="CB22" s="11"/>
       <c r="CC22" s="11"/>
-      <c r="CD22" s="24"/>
-      <c r="CE22" s="24"/>
-      <c r="CF22" s="24"/>
-      <c r="CG22" s="24"/>
-      <c r="CH22" s="24"/>
-      <c r="CI22" s="24"/>
+      <c r="CD22" s="23"/>
+      <c r="CE22" s="23"/>
+      <c r="CF22" s="23"/>
+      <c r="CG22" s="23"/>
+      <c r="CH22" s="23"/>
+      <c r="CI22" s="23"/>
+      <c r="CJ22" s="23"/>
     </row>
     <row r="23" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
@@ -4412,13 +4435,13 @@
       <c r="CA24" s="8"/>
       <c r="CB24" s="8"/>
       <c r="CC24" s="8"/>
-      <c r="CD24" s="22"/>
-      <c r="CE24" s="22"/>
-      <c r="CF24" s="22"/>
-      <c r="CG24" s="22"/>
-      <c r="CH24" s="22"/>
-      <c r="CI24" s="22"/>
-      <c r="CJ24" s="8"/>
+      <c r="CD24" s="21"/>
+      <c r="CE24" s="21"/>
+      <c r="CF24" s="21"/>
+      <c r="CG24" s="21"/>
+      <c r="CH24" s="21"/>
+      <c r="CI24" s="21"/>
+      <c r="CJ24" s="21"/>
       <c r="CK24" s="8"/>
       <c r="CL24" s="8"/>
       <c r="CM24" s="8"/>
@@ -4564,13 +4587,13 @@
       <c r="CA25" s="8"/>
       <c r="CB25" s="8"/>
       <c r="CC25" s="8"/>
-      <c r="CD25" s="22"/>
-      <c r="CE25" s="22"/>
-      <c r="CF25" s="22"/>
-      <c r="CG25" s="22"/>
-      <c r="CH25" s="22"/>
-      <c r="CI25" s="22"/>
-      <c r="CJ25" s="8"/>
+      <c r="CD25" s="21"/>
+      <c r="CE25" s="21"/>
+      <c r="CF25" s="21"/>
+      <c r="CG25" s="21"/>
+      <c r="CH25" s="21"/>
+      <c r="CI25" s="21"/>
+      <c r="CJ25" s="21"/>
       <c r="CK25" s="8"/>
       <c r="CL25" s="8"/>
       <c r="CM25" s="8"/>
@@ -4799,6 +4822,7 @@
       <c r="CI34" s="28">
         <v>0</v>
       </c>
+      <c r="CJ34" s="28"/>
     </row>
     <row r="35" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
@@ -5042,23 +5066,26 @@
       <c r="CC35" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CD35" s="25" t="s">
+      <c r="CD35" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CE35" s="25" t="s">
+      <c r="CE35" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="CF35" s="25" t="s">
+      <c r="CF35" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="CG35" s="25" t="s">
+      <c r="CG35" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="CH35" s="25" t="s">
+      <c r="CH35" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CI35" s="25" t="s">
+      <c r="CI35" s="24" t="s">
         <v>8</v>
+      </c>
+      <c r="CJ35" s="24" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5308,25 +5335,27 @@
       <c r="CC37" s="7">
         <v>44725.990643891746</v>
       </c>
-      <c r="CD37" s="21">
+      <c r="CD37" s="20">
         <v>30626.489402743518</v>
       </c>
-      <c r="CE37" s="21">
+      <c r="CE37" s="20">
         <v>13543.604832631756</v>
       </c>
-      <c r="CF37" s="21">
+      <c r="CF37" s="20">
         <v>20313.003574479371</v>
       </c>
-      <c r="CG37" s="21">
+      <c r="CG37" s="20">
         <v>21626.707123416036</v>
       </c>
-      <c r="CH37" s="21">
+      <c r="CH37" s="20">
         <v>17520.856490481521</v>
       </c>
-      <c r="CI37" s="21">
-        <v>15734.679460408563</v>
-      </c>
-      <c r="CJ37" s="8"/>
+      <c r="CI37" s="20">
+        <v>15112.588522108954</v>
+      </c>
+      <c r="CJ37" s="20">
+        <v>23160.921553686745</v>
+      </c>
       <c r="CK37" s="8"/>
       <c r="CL37" s="8"/>
       <c r="CM37" s="8"/>
@@ -5635,25 +5664,27 @@
       <c r="CC38" s="7">
         <v>802.96901766546466</v>
       </c>
-      <c r="CD38" s="21">
+      <c r="CD38" s="20">
         <v>436.66876559975907</v>
       </c>
-      <c r="CE38" s="21">
+      <c r="CE38" s="20">
         <v>261.39181244364426</v>
       </c>
-      <c r="CF38" s="21">
+      <c r="CF38" s="20">
         <v>662.7779598139482</v>
       </c>
-      <c r="CG38" s="21">
+      <c r="CG38" s="20">
         <v>759.35743635758683</v>
       </c>
-      <c r="CH38" s="21">
+      <c r="CH38" s="20">
         <v>460.05588510441675</v>
       </c>
-      <c r="CI38" s="21">
-        <v>343.34089511218372</v>
-      </c>
-      <c r="CJ38" s="8"/>
+      <c r="CI38" s="20">
+        <v>360.15495531134843</v>
+      </c>
+      <c r="CJ38" s="20">
+        <v>743.48303901949737</v>
+      </c>
       <c r="CK38" s="8"/>
       <c r="CL38" s="8"/>
       <c r="CM38" s="8"/>
@@ -5962,25 +5993,27 @@
       <c r="CC39" s="7">
         <v>101660.9649982664</v>
       </c>
-      <c r="CD39" s="21">
+      <c r="CD39" s="20">
         <v>107615.99078256269</v>
       </c>
-      <c r="CE39" s="21">
+      <c r="CE39" s="20">
         <v>5149.6507164927534</v>
       </c>
-      <c r="CF39" s="21">
+      <c r="CF39" s="20">
         <v>13657.848098351255</v>
       </c>
-      <c r="CG39" s="21">
+      <c r="CG39" s="20">
         <v>7924.9178789822236</v>
       </c>
-      <c r="CH39" s="21">
+      <c r="CH39" s="20">
         <v>2138.9207396531883</v>
       </c>
-      <c r="CI39" s="21">
-        <v>15956.901007324566</v>
-      </c>
-      <c r="CJ39" s="8"/>
+      <c r="CI39" s="20">
+        <v>27061.127282441081</v>
+      </c>
+      <c r="CJ39" s="20">
+        <v>20980.58990697519</v>
+      </c>
       <c r="CK39" s="8"/>
       <c r="CL39" s="8"/>
       <c r="CM39" s="8"/>
@@ -6289,25 +6322,27 @@
       <c r="CC40" s="7">
         <v>2593.7949415158037</v>
       </c>
-      <c r="CD40" s="21">
+      <c r="CD40" s="20">
         <v>2466.8598585310178</v>
       </c>
-      <c r="CE40" s="21">
+      <c r="CE40" s="20">
         <v>2657.164078613212</v>
       </c>
-      <c r="CF40" s="21">
+      <c r="CF40" s="20">
         <v>2831.4912304316867</v>
       </c>
-      <c r="CG40" s="21">
+      <c r="CG40" s="20">
         <v>2794.4417354123757</v>
       </c>
-      <c r="CH40" s="21">
+      <c r="CH40" s="20">
         <v>2945.8113808788394</v>
       </c>
-      <c r="CI40" s="21">
-        <v>3205.4940922249707</v>
-      </c>
-      <c r="CJ40" s="8"/>
+      <c r="CI40" s="20">
+        <v>3280.2710999783149</v>
+      </c>
+      <c r="CJ40" s="20">
+        <v>3529.4697269102971</v>
+      </c>
       <c r="CK40" s="8"/>
       <c r="CL40" s="8"/>
       <c r="CM40" s="8"/>
@@ -6616,25 +6651,27 @@
       <c r="CC41" s="7">
         <v>65415.838723488094</v>
       </c>
-      <c r="CD41" s="21">
+      <c r="CD41" s="20">
         <v>105383.42652976808</v>
       </c>
-      <c r="CE41" s="21">
+      <c r="CE41" s="20">
         <v>85303.114535815388</v>
       </c>
-      <c r="CF41" s="21">
+      <c r="CF41" s="20">
         <v>57311.639636476502</v>
       </c>
-      <c r="CG41" s="21">
+      <c r="CG41" s="20">
         <v>61175.574457265568</v>
       </c>
-      <c r="CH41" s="21">
+      <c r="CH41" s="20">
         <v>102809.30125245436</v>
       </c>
-      <c r="CI41" s="21">
-        <v>103109.78309572217</v>
-      </c>
-      <c r="CJ41" s="8"/>
+      <c r="CI41" s="20">
+        <v>100701.72609154858</v>
+      </c>
+      <c r="CJ41" s="20">
+        <v>69767.204458864173</v>
+      </c>
       <c r="CK41" s="8"/>
       <c r="CL41" s="8"/>
       <c r="CM41" s="8"/>
@@ -6943,25 +6980,27 @@
       <c r="CC42" s="7">
         <v>261437.80028709813</v>
       </c>
-      <c r="CD42" s="21">
+      <c r="CD42" s="20">
         <v>325938.64012443181</v>
       </c>
-      <c r="CE42" s="21">
+      <c r="CE42" s="20">
         <v>297685.5064581047</v>
       </c>
-      <c r="CF42" s="21">
+      <c r="CF42" s="20">
         <v>237666.84089454132</v>
       </c>
-      <c r="CG42" s="21">
+      <c r="CG42" s="20">
         <v>257306.27757503474</v>
       </c>
-      <c r="CH42" s="21">
+      <c r="CH42" s="20">
         <v>313658.9729647651</v>
       </c>
-      <c r="CI42" s="21">
-        <v>337853.12707987509</v>
-      </c>
-      <c r="CJ42" s="8"/>
+      <c r="CI42" s="20">
+        <v>332798.52829001442</v>
+      </c>
+      <c r="CJ42" s="20">
+        <v>237419.75301103739</v>
+      </c>
       <c r="CK42" s="8"/>
       <c r="CL42" s="8"/>
       <c r="CM42" s="8"/>
@@ -7270,25 +7309,27 @@
       <c r="CC43" s="7">
         <v>46048.282508936878</v>
       </c>
-      <c r="CD43" s="21">
+      <c r="CD43" s="20">
         <v>68758.770421120236</v>
       </c>
-      <c r="CE43" s="21">
+      <c r="CE43" s="20">
         <v>57421.867763688169</v>
       </c>
-      <c r="CF43" s="21">
+      <c r="CF43" s="20">
         <v>43178.869113891196</v>
       </c>
-      <c r="CG43" s="21">
+      <c r="CG43" s="20">
         <v>41067.937424928037</v>
       </c>
-      <c r="CH43" s="21">
+      <c r="CH43" s="20">
         <v>65909.291972822029</v>
       </c>
-      <c r="CI43" s="21">
-        <v>66562.225553229669</v>
-      </c>
-      <c r="CJ43" s="8"/>
+      <c r="CI43" s="20">
+        <v>68381.706220006774</v>
+      </c>
+      <c r="CJ43" s="20">
+        <v>55413.279870243554</v>
+      </c>
       <c r="CK43" s="8"/>
       <c r="CL43" s="8"/>
       <c r="CM43" s="8"/>
@@ -7597,25 +7638,27 @@
       <c r="CC44" s="7">
         <v>7800.6818332445764</v>
       </c>
-      <c r="CD44" s="21">
+      <c r="CD44" s="20">
         <v>5980.2912905260628</v>
       </c>
-      <c r="CE44" s="21">
+      <c r="CE44" s="20">
         <v>5915.9463217096045</v>
       </c>
-      <c r="CF44" s="21">
+      <c r="CF44" s="20">
         <v>5306.3257063791525</v>
       </c>
-      <c r="CG44" s="21">
+      <c r="CG44" s="20">
         <v>5501.0229420066535</v>
       </c>
-      <c r="CH44" s="21">
+      <c r="CH44" s="20">
         <v>4967.4622236797732</v>
       </c>
-      <c r="CI44" s="21">
-        <v>6189.7118785046732</v>
-      </c>
-      <c r="CJ44" s="8"/>
+      <c r="CI44" s="20">
+        <v>6221.4809743713067</v>
+      </c>
+      <c r="CJ44" s="20">
+        <v>6307.7478536294502</v>
+      </c>
       <c r="CK44" s="8"/>
       <c r="CL44" s="8"/>
       <c r="CM44" s="8"/>
@@ -7761,13 +7804,13 @@
       <c r="CA45" s="8"/>
       <c r="CB45" s="8"/>
       <c r="CC45" s="8"/>
-      <c r="CD45" s="22"/>
-      <c r="CE45" s="22"/>
-      <c r="CF45" s="22"/>
-      <c r="CG45" s="22"/>
-      <c r="CH45" s="22"/>
-      <c r="CI45" s="22"/>
-      <c r="CJ45" s="8"/>
+      <c r="CD45" s="21"/>
+      <c r="CE45" s="21"/>
+      <c r="CF45" s="21"/>
+      <c r="CG45" s="21"/>
+      <c r="CH45" s="21"/>
+      <c r="CI45" s="21"/>
+      <c r="CJ45" s="21"/>
       <c r="CK45" s="8"/>
       <c r="CL45" s="8"/>
       <c r="CM45" s="8"/>
@@ -8076,25 +8119,27 @@
       <c r="CC46" s="10">
         <v>530486.32295410708</v>
       </c>
-      <c r="CD46" s="23">
+      <c r="CD46" s="22">
         <v>647207.13717528316</v>
       </c>
-      <c r="CE46" s="23">
+      <c r="CE46" s="22">
         <v>467938.24651949923</v>
       </c>
-      <c r="CF46" s="23">
+      <c r="CF46" s="22">
         <v>380928.79621436441</v>
       </c>
-      <c r="CG46" s="23">
+      <c r="CG46" s="22">
         <v>398156.23657340318</v>
       </c>
-      <c r="CH46" s="23">
+      <c r="CH46" s="22">
         <v>510410.6729098392</v>
       </c>
-      <c r="CI46" s="23">
-        <v>548955.26306240191</v>
-      </c>
-      <c r="CJ46" s="8"/>
+      <c r="CI46" s="22">
+        <v>553917.58343578083</v>
+      </c>
+      <c r="CJ46" s="22">
+        <v>417322.44942036632</v>
+      </c>
       <c r="CK46" s="8"/>
       <c r="CL46" s="8"/>
       <c r="CM46" s="8"/>
@@ -8241,12 +8286,13 @@
       <c r="CA47" s="11"/>
       <c r="CB47" s="11"/>
       <c r="CC47" s="11"/>
-      <c r="CD47" s="24"/>
-      <c r="CE47" s="24"/>
-      <c r="CF47" s="24"/>
-      <c r="CG47" s="24"/>
-      <c r="CH47" s="24"/>
-      <c r="CI47" s="24"/>
+      <c r="CD47" s="23"/>
+      <c r="CE47" s="23"/>
+      <c r="CF47" s="23"/>
+      <c r="CG47" s="23"/>
+      <c r="CH47" s="23"/>
+      <c r="CI47" s="23"/>
+      <c r="CJ47" s="23"/>
     </row>
     <row r="48" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
@@ -8334,13 +8380,13 @@
       <c r="CA49" s="8"/>
       <c r="CB49" s="8"/>
       <c r="CC49" s="8"/>
-      <c r="CD49" s="22"/>
-      <c r="CE49" s="22"/>
-      <c r="CF49" s="22"/>
-      <c r="CG49" s="22"/>
-      <c r="CH49" s="22"/>
-      <c r="CI49" s="22"/>
-      <c r="CJ49" s="8"/>
+      <c r="CD49" s="21"/>
+      <c r="CE49" s="21"/>
+      <c r="CF49" s="21"/>
+      <c r="CG49" s="21"/>
+      <c r="CH49" s="21"/>
+      <c r="CI49" s="21"/>
+      <c r="CJ49" s="21"/>
       <c r="CK49" s="8"/>
       <c r="CL49" s="8"/>
       <c r="CM49" s="8"/>
@@ -8486,13 +8532,13 @@
       <c r="CA50" s="8"/>
       <c r="CB50" s="8"/>
       <c r="CC50" s="8"/>
-      <c r="CD50" s="22"/>
-      <c r="CE50" s="22"/>
-      <c r="CF50" s="22"/>
-      <c r="CG50" s="22"/>
-      <c r="CH50" s="22"/>
-      <c r="CI50" s="22"/>
-      <c r="CJ50" s="8"/>
+      <c r="CD50" s="21"/>
+      <c r="CE50" s="21"/>
+      <c r="CF50" s="21"/>
+      <c r="CG50" s="21"/>
+      <c r="CH50" s="21"/>
+      <c r="CI50" s="21"/>
+      <c r="CJ50" s="21"/>
       <c r="CK50" s="8"/>
       <c r="CL50" s="8"/>
       <c r="CM50" s="8"/>
@@ -8715,10 +8761,11 @@
       <c r="CE59" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="CF59" s="19"/>
-      <c r="CG59" s="19"/>
-      <c r="CH59" s="19"/>
-      <c r="CI59" s="19"/>
+      <c r="CF59" s="27"/>
+      <c r="CG59" s="27"/>
+      <c r="CH59" s="27"/>
+      <c r="CI59" s="27"/>
+      <c r="CJ59" s="27"/>
     </row>
     <row r="60" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
@@ -8962,16 +9009,19 @@
       <c r="CC60" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CD60" s="20" t="s">
+      <c r="CD60" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CE60" s="20" t="s">
+      <c r="CE60" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="CF60" s="20"/>
-      <c r="CG60" s="20"/>
-      <c r="CH60" s="20"/>
-      <c r="CI60" s="20"/>
+      <c r="CF60" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG60" s="19"/>
+      <c r="CH60" s="19"/>
+      <c r="CI60" s="19"/>
+      <c r="CJ60" s="19"/>
     </row>
     <row r="61" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
@@ -9220,17 +9270,19 @@
       <c r="CC62" s="14">
         <v>-47.802514613163481</v>
       </c>
-      <c r="CD62" s="26">
+      <c r="CD62" s="25">
         <v>-36.513243769328263</v>
       </c>
-      <c r="CE62" s="26">
-        <v>28.325179995291421</v>
-      </c>
-      <c r="CF62" s="22"/>
-      <c r="CG62" s="22"/>
-      <c r="CH62" s="22"/>
-      <c r="CI62" s="22"/>
-      <c r="CJ62" s="8"/>
+      <c r="CE62" s="25">
+        <v>23.251677746224075</v>
+      </c>
+      <c r="CF62" s="25">
+        <v>21.396577533771932</v>
+      </c>
+      <c r="CG62" s="21"/>
+      <c r="CH62" s="21"/>
+      <c r="CI62" s="21"/>
+      <c r="CJ62" s="21"/>
       <c r="CK62" s="8"/>
       <c r="CL62" s="8"/>
       <c r="CM62" s="8"/>
@@ -9535,17 +9587,19 @@
       <c r="CC63" s="14">
         <v>-3.2876852408687824</v>
       </c>
-      <c r="CD63" s="26">
+      <c r="CD63" s="25">
         <v>8.2792360647258221</v>
       </c>
-      <c r="CE63" s="26">
-        <v>36.261079319690765</v>
-      </c>
-      <c r="CF63" s="22"/>
-      <c r="CG63" s="22"/>
-      <c r="CH63" s="22"/>
-      <c r="CI63" s="22"/>
-      <c r="CJ63" s="8"/>
+      <c r="CE63" s="25">
+        <v>42.934044943945452</v>
+      </c>
+      <c r="CF63" s="25">
+        <v>15.890383072214462</v>
+      </c>
+      <c r="CG63" s="21"/>
+      <c r="CH63" s="21"/>
+      <c r="CI63" s="21"/>
+      <c r="CJ63" s="21"/>
       <c r="CK63" s="8"/>
       <c r="CL63" s="8"/>
       <c r="CM63" s="8"/>
@@ -9850,17 +9904,19 @@
       <c r="CC64" s="14">
         <v>-91.962539751824778</v>
       </c>
-      <c r="CD64" s="26">
+      <c r="CD64" s="25">
         <v>-97.923703859892953</v>
       </c>
-      <c r="CE64" s="26">
-        <v>223.44370997710689</v>
-      </c>
-      <c r="CF64" s="22"/>
-      <c r="CG64" s="22"/>
-      <c r="CH64" s="22"/>
-      <c r="CI64" s="22"/>
-      <c r="CJ64" s="8"/>
+      <c r="CE64" s="25">
+        <v>448.5245161562226</v>
+      </c>
+      <c r="CF64" s="25">
+        <v>60.628680182434238</v>
+      </c>
+      <c r="CG64" s="21"/>
+      <c r="CH64" s="21"/>
+      <c r="CI64" s="21"/>
+      <c r="CJ64" s="21"/>
       <c r="CK64" s="8"/>
       <c r="CL64" s="8"/>
       <c r="CM64" s="8"/>
@@ -10165,17 +10221,19 @@
       <c r="CC65" s="14">
         <v>9.8917521253200107</v>
       </c>
-      <c r="CD65" s="26">
+      <c r="CD65" s="25">
         <v>22.187866705153908</v>
       </c>
-      <c r="CE65" s="26">
-        <v>23.613526602569877</v>
-      </c>
-      <c r="CF65" s="22"/>
-      <c r="CG65" s="22"/>
-      <c r="CH65" s="22"/>
-      <c r="CI65" s="22"/>
-      <c r="CJ65" s="8"/>
+      <c r="CE65" s="25">
+        <v>26.497153703801743</v>
+      </c>
+      <c r="CF65" s="25">
+        <v>27.281902453962687</v>
+      </c>
+      <c r="CG65" s="21"/>
+      <c r="CH65" s="21"/>
+      <c r="CI65" s="21"/>
+      <c r="CJ65" s="21"/>
       <c r="CK65" s="8"/>
       <c r="CL65" s="8"/>
       <c r="CM65" s="8"/>
@@ -10480,17 +10538,19 @@
       <c r="CC66" s="14">
         <v>-6.2058183166108734</v>
       </c>
-      <c r="CD66" s="26">
+      <c r="CD66" s="25">
         <v>-2.2188622256256423</v>
       </c>
-      <c r="CE66" s="26">
-        <v>21.191448294689863</v>
-      </c>
-      <c r="CF66" s="22"/>
-      <c r="CG66" s="22"/>
-      <c r="CH66" s="22"/>
-      <c r="CI66" s="22"/>
-      <c r="CJ66" s="8"/>
+      <c r="CE66" s="25">
+        <v>18.361106622444794</v>
+      </c>
+      <c r="CF66" s="25">
+        <v>22.051849033048043</v>
+      </c>
+      <c r="CG66" s="21"/>
+      <c r="CH66" s="21"/>
+      <c r="CI66" s="21"/>
+      <c r="CJ66" s="21"/>
       <c r="CK66" s="8"/>
       <c r="CL66" s="8"/>
       <c r="CM66" s="8"/>
@@ -10795,17 +10855,19 @@
       <c r="CC67" s="14">
         <v>0.65058822728832411</v>
       </c>
-      <c r="CD67" s="26">
+      <c r="CD67" s="25">
         <v>-1.097199819595005</v>
       </c>
-      <c r="CE67" s="26">
-        <v>17.735795413512292</v>
-      </c>
-      <c r="CF67" s="22"/>
-      <c r="CG67" s="22"/>
-      <c r="CH67" s="22"/>
-      <c r="CI67" s="22"/>
-      <c r="CJ67" s="8"/>
+      <c r="CE67" s="25">
+        <v>15.974357790708439</v>
+      </c>
+      <c r="CF67" s="25">
+        <v>3.2030770398157529</v>
+      </c>
+      <c r="CG67" s="21"/>
+      <c r="CH67" s="21"/>
+      <c r="CI67" s="21"/>
+      <c r="CJ67" s="21"/>
       <c r="CK67" s="8"/>
       <c r="CL67" s="8"/>
       <c r="CM67" s="8"/>
@@ -11110,17 +11172,19 @@
       <c r="CC68" s="14">
         <v>-8.7939240388756161</v>
       </c>
-      <c r="CD68" s="26">
+      <c r="CD68" s="25">
         <v>-1.4843413301903041</v>
       </c>
-      <c r="CE68" s="26">
-        <v>20.25102569919801</v>
-      </c>
-      <c r="CF68" s="22"/>
-      <c r="CG68" s="22"/>
-      <c r="CH68" s="22"/>
-      <c r="CI68" s="22"/>
-      <c r="CJ68" s="8"/>
+      <c r="CE68" s="25">
+        <v>23.53809151770551</v>
+      </c>
+      <c r="CF68" s="25">
+        <v>32.582738036752659</v>
+      </c>
+      <c r="CG68" s="21"/>
+      <c r="CH68" s="21"/>
+      <c r="CI68" s="21"/>
+      <c r="CJ68" s="21"/>
       <c r="CK68" s="8"/>
       <c r="CL68" s="8"/>
       <c r="CM68" s="8"/>
@@ -11425,17 +11489,19 @@
       <c r="CC69" s="14">
         <v>-27.881745358252047</v>
       </c>
-      <c r="CD69" s="26">
+      <c r="CD69" s="25">
         <v>-14.631243452758767</v>
       </c>
-      <c r="CE69" s="26">
-        <v>8.5386657786054911</v>
-      </c>
-      <c r="CF69" s="22"/>
-      <c r="CG69" s="22"/>
-      <c r="CH69" s="22"/>
-      <c r="CI69" s="22"/>
-      <c r="CJ69" s="8"/>
+      <c r="CE69" s="25">
+        <v>9.0957474887140677</v>
+      </c>
+      <c r="CF69" s="25">
+        <v>22.807477657504876</v>
+      </c>
+      <c r="CG69" s="21"/>
+      <c r="CH69" s="21"/>
+      <c r="CI69" s="21"/>
+      <c r="CJ69" s="21"/>
       <c r="CK69" s="8"/>
       <c r="CL69" s="8"/>
       <c r="CM69" s="8"/>
@@ -11577,13 +11643,13 @@
       <c r="CA70" s="8"/>
       <c r="CB70" s="8"/>
       <c r="CC70" s="8"/>
-      <c r="CD70" s="22"/>
-      <c r="CE70" s="22"/>
-      <c r="CF70" s="22"/>
-      <c r="CG70" s="22"/>
-      <c r="CH70" s="22"/>
-      <c r="CI70" s="22"/>
-      <c r="CJ70" s="8"/>
+      <c r="CD70" s="21"/>
+      <c r="CE70" s="21"/>
+      <c r="CF70" s="21"/>
+      <c r="CG70" s="21"/>
+      <c r="CH70" s="21"/>
+      <c r="CI70" s="21"/>
+      <c r="CJ70" s="21"/>
       <c r="CK70" s="8"/>
       <c r="CL70" s="8"/>
       <c r="CM70" s="8"/>
@@ -11888,17 +11954,19 @@
       <c r="CC71" s="14">
         <v>-23.07518236928621</v>
       </c>
-      <c r="CD71" s="26">
+      <c r="CD71" s="25">
         <v>-19.148842670633897</v>
       </c>
-      <c r="CE71" s="26">
-        <v>21.25906875955468</v>
-      </c>
-      <c r="CF71" s="22"/>
-      <c r="CG71" s="22"/>
-      <c r="CH71" s="22"/>
-      <c r="CI71" s="22"/>
-      <c r="CJ71" s="8"/>
+      <c r="CE71" s="25">
+        <v>22.503635075260235</v>
+      </c>
+      <c r="CF71" s="25">
+        <v>12.809842003455941</v>
+      </c>
+      <c r="CG71" s="21"/>
+      <c r="CH71" s="21"/>
+      <c r="CI71" s="21"/>
+      <c r="CJ71" s="21"/>
       <c r="CK71" s="8"/>
       <c r="CL71" s="8"/>
       <c r="CM71" s="8"/>
@@ -12041,12 +12109,13 @@
       <c r="CA72" s="11"/>
       <c r="CB72" s="11"/>
       <c r="CC72" s="11"/>
-      <c r="CD72" s="24"/>
-      <c r="CE72" s="24"/>
-      <c r="CF72" s="24"/>
-      <c r="CG72" s="24"/>
-      <c r="CH72" s="24"/>
-      <c r="CI72" s="24"/>
+      <c r="CD72" s="23"/>
+      <c r="CE72" s="23"/>
+      <c r="CF72" s="23"/>
+      <c r="CG72" s="23"/>
+      <c r="CH72" s="23"/>
+      <c r="CI72" s="23"/>
+      <c r="CJ72" s="23"/>
     </row>
     <row r="73" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
@@ -12134,13 +12203,13 @@
       <c r="CA74" s="8"/>
       <c r="CB74" s="8"/>
       <c r="CC74" s="8"/>
-      <c r="CD74" s="22"/>
-      <c r="CE74" s="22"/>
-      <c r="CF74" s="22"/>
-      <c r="CG74" s="22"/>
-      <c r="CH74" s="22"/>
-      <c r="CI74" s="22"/>
-      <c r="CJ74" s="8"/>
+      <c r="CD74" s="21"/>
+      <c r="CE74" s="21"/>
+      <c r="CF74" s="21"/>
+      <c r="CG74" s="21"/>
+      <c r="CH74" s="21"/>
+      <c r="CI74" s="21"/>
+      <c r="CJ74" s="21"/>
       <c r="CK74" s="8"/>
       <c r="CL74" s="8"/>
       <c r="CM74" s="8"/>
@@ -12282,13 +12351,13 @@
       <c r="CA75" s="8"/>
       <c r="CB75" s="8"/>
       <c r="CC75" s="8"/>
-      <c r="CD75" s="22"/>
-      <c r="CE75" s="22"/>
-      <c r="CF75" s="22"/>
-      <c r="CG75" s="22"/>
-      <c r="CH75" s="22"/>
-      <c r="CI75" s="22"/>
-      <c r="CJ75" s="8"/>
+      <c r="CD75" s="21"/>
+      <c r="CE75" s="21"/>
+      <c r="CF75" s="21"/>
+      <c r="CG75" s="21"/>
+      <c r="CH75" s="21"/>
+      <c r="CI75" s="21"/>
+      <c r="CJ75" s="21"/>
       <c r="CK75" s="8"/>
       <c r="CL75" s="8"/>
       <c r="CM75" s="8"/>
@@ -12507,10 +12576,11 @@
       <c r="CE84" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="CF84" s="19"/>
-      <c r="CG84" s="19"/>
-      <c r="CH84" s="19"/>
-      <c r="CI84" s="19"/>
+      <c r="CF84" s="28"/>
+      <c r="CG84" s="27"/>
+      <c r="CH84" s="27"/>
+      <c r="CI84" s="27"/>
+      <c r="CJ84" s="27"/>
     </row>
     <row r="85" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
@@ -12754,16 +12824,19 @@
       <c r="CC85" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CD85" s="20" t="s">
+      <c r="CD85" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CE85" s="20" t="s">
+      <c r="CE85" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="CF85" s="20"/>
-      <c r="CG85" s="20"/>
-      <c r="CH85" s="20"/>
-      <c r="CI85" s="20"/>
+      <c r="CF85" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="CG85" s="19"/>
+      <c r="CH85" s="19"/>
+      <c r="CI85" s="19"/>
+      <c r="CJ85" s="19"/>
     </row>
     <row r="86" spans="1:147" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
@@ -13012,17 +13085,19 @@
       <c r="CC87" s="14">
         <v>-51.646219989607751</v>
       </c>
-      <c r="CD87" s="26">
+      <c r="CD87" s="25">
         <v>-42.79182226836614</v>
       </c>
-      <c r="CE87" s="26">
-        <v>16.177927921358616</v>
-      </c>
-      <c r="CF87" s="22"/>
-      <c r="CG87" s="22"/>
-      <c r="CH87" s="22"/>
-      <c r="CI87" s="22"/>
-      <c r="CJ87" s="8"/>
+      <c r="CE87" s="25">
+        <v>11.58468302099979</v>
+      </c>
+      <c r="CF87" s="25">
+        <v>14.020171703141955</v>
+      </c>
+      <c r="CG87" s="21"/>
+      <c r="CH87" s="21"/>
+      <c r="CI87" s="21"/>
+      <c r="CJ87" s="21"/>
       <c r="CK87" s="8"/>
       <c r="CL87" s="8"/>
       <c r="CM87" s="8"/>
@@ -13327,17 +13402,19 @@
       <c r="CC88" s="14">
         <v>-5.43129066606744</v>
       </c>
-      <c r="CD88" s="26">
+      <c r="CD88" s="25">
         <v>5.3558031503663273</v>
       </c>
-      <c r="CE88" s="26">
-        <v>31.35105185676295</v>
-      </c>
-      <c r="CF88" s="22"/>
-      <c r="CG88" s="22"/>
-      <c r="CH88" s="22"/>
-      <c r="CI88" s="22"/>
-      <c r="CJ88" s="8"/>
+      <c r="CE88" s="25">
+        <v>37.783564046787944</v>
+      </c>
+      <c r="CF88" s="25">
+        <v>12.176789829915947</v>
+      </c>
+      <c r="CG88" s="21"/>
+      <c r="CH88" s="21"/>
+      <c r="CI88" s="21"/>
+      <c r="CJ88" s="21"/>
       <c r="CK88" s="8"/>
       <c r="CL88" s="8"/>
       <c r="CM88" s="8"/>
@@ -13642,17 +13719,19 @@
       <c r="CC89" s="14">
         <v>-92.20456162390613</v>
       </c>
-      <c r="CD89" s="26">
+      <c r="CD89" s="25">
         <v>-98.012450822503823</v>
       </c>
-      <c r="CE89" s="26">
-        <v>209.86375359826837</v>
-      </c>
-      <c r="CF89" s="22"/>
-      <c r="CG89" s="22"/>
-      <c r="CH89" s="22"/>
-      <c r="CI89" s="22"/>
-      <c r="CJ89" s="8"/>
+      <c r="CE89" s="25">
+        <v>425.49442228717726</v>
+      </c>
+      <c r="CF89" s="25">
+        <v>53.615633706659253</v>
+      </c>
+      <c r="CG89" s="21"/>
+      <c r="CH89" s="21"/>
+      <c r="CI89" s="21"/>
+      <c r="CJ89" s="21"/>
       <c r="CK89" s="8"/>
       <c r="CL89" s="8"/>
       <c r="CM89" s="8"/>
@@ -13957,17 +14036,19 @@
       <c r="CC90" s="14">
         <v>7.735645971277691</v>
       </c>
-      <c r="CD90" s="26">
+      <c r="CD90" s="25">
         <v>19.415432972063144</v>
       </c>
-      <c r="CE90" s="26">
-        <v>20.635910970839817</v>
-      </c>
-      <c r="CF90" s="22"/>
-      <c r="CG90" s="22"/>
-      <c r="CH90" s="22"/>
-      <c r="CI90" s="22"/>
-      <c r="CJ90" s="8"/>
+      <c r="CE90" s="25">
+        <v>23.450076959127998</v>
+      </c>
+      <c r="CF90" s="25">
+        <v>24.650561830353851</v>
+      </c>
+      <c r="CG90" s="21"/>
+      <c r="CH90" s="21"/>
+      <c r="CI90" s="21"/>
+      <c r="CJ90" s="21"/>
       <c r="CK90" s="8"/>
       <c r="CL90" s="8"/>
       <c r="CM90" s="8"/>
@@ -14272,17 +14353,19 @@
       <c r="CC91" s="14">
         <v>-6.4820146755987764</v>
       </c>
-      <c r="CD91" s="26">
+      <c r="CD91" s="25">
         <v>-2.4426281836514363</v>
       </c>
-      <c r="CE91" s="26">
-        <v>20.874581961987417</v>
-      </c>
-      <c r="CF91" s="22"/>
-      <c r="CG91" s="22"/>
-      <c r="CH91" s="22"/>
-      <c r="CI91" s="22"/>
-      <c r="CJ91" s="8"/>
+      <c r="CE91" s="25">
+        <v>18.05164048174106</v>
+      </c>
+      <c r="CF91" s="25">
+        <v>21.733045680410484</v>
+      </c>
+      <c r="CG91" s="21"/>
+      <c r="CH91" s="21"/>
+      <c r="CI91" s="21"/>
+      <c r="CJ91" s="21"/>
       <c r="CK91" s="8"/>
       <c r="CL91" s="8"/>
       <c r="CM91" s="8"/>
@@ -14587,17 +14670,19 @@
       <c r="CC92" s="14">
         <v>-1.5803080914567005</v>
       </c>
-      <c r="CD92" s="26">
+      <c r="CD92" s="25">
         <v>-3.7674781839240552</v>
       </c>
-      <c r="CE92" s="26">
-        <v>13.493307450432908</v>
-      </c>
-      <c r="CF92" s="22"/>
-      <c r="CG92" s="22"/>
-      <c r="CH92" s="22"/>
-      <c r="CI92" s="22"/>
-      <c r="CJ92" s="8"/>
+      <c r="CE92" s="25">
+        <v>11.795341415740495</v>
+      </c>
+      <c r="CF92" s="25">
+        <v>-0.10396397014153536</v>
+      </c>
+      <c r="CG92" s="21"/>
+      <c r="CH92" s="21"/>
+      <c r="CI92" s="21"/>
+      <c r="CJ92" s="21"/>
       <c r="CK92" s="8"/>
       <c r="CL92" s="8"/>
       <c r="CM92" s="8"/>
@@ -14902,17 +14987,19 @@
       <c r="CC93" s="14">
         <v>-10.815484992393081</v>
       </c>
-      <c r="CD93" s="26">
+      <c r="CD93" s="25">
         <v>-4.1441672543680994</v>
       </c>
-      <c r="CE93" s="26">
-        <v>15.917904006810417</v>
-      </c>
-      <c r="CF93" s="22"/>
-      <c r="CG93" s="22"/>
-      <c r="CH93" s="22"/>
-      <c r="CI93" s="22"/>
-      <c r="CJ93" s="8"/>
+      <c r="CE93" s="25">
+        <v>19.086523798602855</v>
+      </c>
+      <c r="CF93" s="25">
+        <v>28.334254711678852</v>
+      </c>
+      <c r="CG93" s="21"/>
+      <c r="CH93" s="21"/>
+      <c r="CI93" s="21"/>
+      <c r="CJ93" s="21"/>
       <c r="CK93" s="8"/>
       <c r="CL93" s="8"/>
       <c r="CM93" s="8"/>
@@ -15217,17 +15304,19 @@
       <c r="CC94" s="14">
         <v>-29.480229297871702</v>
       </c>
-      <c r="CD94" s="26">
+      <c r="CD94" s="25">
         <v>-16.936115945569526</v>
       </c>
-      <c r="CE94" s="26">
-        <v>4.6275868966294951</v>
-      </c>
-      <c r="CF94" s="22"/>
-      <c r="CG94" s="22"/>
-      <c r="CH94" s="22"/>
-      <c r="CI94" s="22"/>
-      <c r="CJ94" s="8"/>
+      <c r="CE94" s="25">
+        <v>5.1645947418503368</v>
+      </c>
+      <c r="CF94" s="25">
+        <v>18.872232928453855</v>
+      </c>
+      <c r="CG94" s="21"/>
+      <c r="CH94" s="21"/>
+      <c r="CI94" s="21"/>
+      <c r="CJ94" s="21"/>
       <c r="CK94" s="8"/>
       <c r="CL94" s="8"/>
       <c r="CM94" s="8"/>
@@ -15369,13 +15458,13 @@
       <c r="CA95" s="8"/>
       <c r="CB95" s="8"/>
       <c r="CC95" s="8"/>
-      <c r="CD95" s="22"/>
-      <c r="CE95" s="22"/>
-      <c r="CF95" s="22"/>
-      <c r="CG95" s="22"/>
-      <c r="CH95" s="22"/>
-      <c r="CI95" s="22"/>
-      <c r="CJ95" s="8"/>
+      <c r="CD95" s="21"/>
+      <c r="CE95" s="21"/>
+      <c r="CF95" s="21"/>
+      <c r="CG95" s="21"/>
+      <c r="CH95" s="21"/>
+      <c r="CI95" s="21"/>
+      <c r="CJ95" s="21"/>
       <c r="CK95" s="8"/>
       <c r="CL95" s="8"/>
       <c r="CM95" s="8"/>
@@ -15680,17 +15769,19 @@
       <c r="CC96" s="14">
         <v>-24.945051484796139</v>
       </c>
-      <c r="CD96" s="26">
+      <c r="CD96" s="25">
         <v>-21.136427027441044</v>
       </c>
-      <c r="CE96" s="26">
-        <v>17.313612884927252</v>
-      </c>
-      <c r="CF96" s="22"/>
-      <c r="CG96" s="22"/>
-      <c r="CH96" s="22"/>
-      <c r="CI96" s="22"/>
-      <c r="CJ96" s="8"/>
+      <c r="CE96" s="25">
+        <v>18.374077681358926</v>
+      </c>
+      <c r="CF96" s="25">
+        <v>9.55392544950098</v>
+      </c>
+      <c r="CG96" s="21"/>
+      <c r="CH96" s="21"/>
+      <c r="CI96" s="21"/>
+      <c r="CJ96" s="21"/>
       <c r="CK96" s="8"/>
       <c r="CL96" s="8"/>
       <c r="CM96" s="8"/>
@@ -15833,12 +15924,13 @@
       <c r="CA97" s="11"/>
       <c r="CB97" s="11"/>
       <c r="CC97" s="11"/>
-      <c r="CD97" s="24"/>
-      <c r="CE97" s="24"/>
-      <c r="CF97" s="24"/>
-      <c r="CG97" s="24"/>
-      <c r="CH97" s="24"/>
-      <c r="CI97" s="24"/>
+      <c r="CD97" s="23"/>
+      <c r="CE97" s="23"/>
+      <c r="CF97" s="23"/>
+      <c r="CG97" s="23"/>
+      <c r="CH97" s="23"/>
+      <c r="CI97" s="23"/>
+      <c r="CJ97" s="23"/>
     </row>
     <row r="98" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
@@ -15926,13 +16018,13 @@
       <c r="CA99" s="8"/>
       <c r="CB99" s="8"/>
       <c r="CC99" s="8"/>
-      <c r="CD99" s="22"/>
-      <c r="CE99" s="22"/>
-      <c r="CF99" s="22"/>
-      <c r="CG99" s="22"/>
-      <c r="CH99" s="22"/>
-      <c r="CI99" s="22"/>
-      <c r="CJ99" s="8"/>
+      <c r="CD99" s="21"/>
+      <c r="CE99" s="21"/>
+      <c r="CF99" s="21"/>
+      <c r="CG99" s="21"/>
+      <c r="CH99" s="21"/>
+      <c r="CI99" s="21"/>
+      <c r="CJ99" s="21"/>
       <c r="CK99" s="8"/>
       <c r="CL99" s="8"/>
       <c r="CM99" s="8"/>
@@ -16074,13 +16166,13 @@
       <c r="CA100" s="8"/>
       <c r="CB100" s="8"/>
       <c r="CC100" s="8"/>
-      <c r="CD100" s="22"/>
-      <c r="CE100" s="22"/>
-      <c r="CF100" s="22"/>
-      <c r="CG100" s="22"/>
-      <c r="CH100" s="22"/>
-      <c r="CI100" s="22"/>
-      <c r="CJ100" s="8"/>
+      <c r="CD100" s="21"/>
+      <c r="CE100" s="21"/>
+      <c r="CF100" s="21"/>
+      <c r="CG100" s="21"/>
+      <c r="CH100" s="21"/>
+      <c r="CI100" s="21"/>
+      <c r="CJ100" s="21"/>
       <c r="CK100" s="8"/>
       <c r="CL100" s="8"/>
       <c r="CM100" s="8"/>
@@ -16300,6 +16392,7 @@
       <c r="CI108" s="28">
         <v>0</v>
       </c>
+      <c r="CJ108" s="28"/>
     </row>
     <row r="109" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
@@ -16543,23 +16636,26 @@
       <c r="CC109" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CD109" s="25" t="s">
+      <c r="CD109" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CE109" s="25" t="s">
+      <c r="CE109" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="CF109" s="25" t="s">
+      <c r="CF109" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="CG109" s="25" t="s">
+      <c r="CG109" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="CH109" s="25" t="s">
+      <c r="CH109" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CI109" s="25" t="s">
+      <c r="CI109" s="24" t="s">
         <v>8</v>
+      </c>
+      <c r="CJ109" s="24" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -16809,25 +16905,27 @@
       <c r="CC111" s="14">
         <v>102.37992755405583</v>
       </c>
-      <c r="CD111" s="26">
+      <c r="CD111" s="25">
         <v>104.52056034332951</v>
       </c>
-      <c r="CE111" s="26">
+      <c r="CE111" s="25">
         <v>98.195770459140022</v>
       </c>
-      <c r="CF111" s="26">
+      <c r="CF111" s="25">
         <v>104.28639523782448</v>
       </c>
-      <c r="CG111" s="26">
+      <c r="CG111" s="25">
         <v>110.51824224000019</v>
       </c>
-      <c r="CH111" s="26">
+      <c r="CH111" s="25">
         <v>115.99165711479939</v>
       </c>
-      <c r="CI111" s="26">
-        <v>108.46285645131435</v>
-      </c>
-      <c r="CJ111" s="8"/>
+      <c r="CI111" s="25">
+        <v>108.46285645131437</v>
+      </c>
+      <c r="CJ111" s="25">
+        <v>111.03308542778909</v>
+      </c>
       <c r="CK111" s="8"/>
       <c r="CL111" s="8"/>
       <c r="CM111" s="8"/>
@@ -17136,25 +17234,27 @@
       <c r="CC112" s="14">
         <v>101.12314926555126</v>
       </c>
-      <c r="CD112" s="26">
+      <c r="CD112" s="25">
         <v>104.37400137584005</v>
       </c>
-      <c r="CE112" s="26">
+      <c r="CE112" s="25">
         <v>103.73619396304321</v>
       </c>
-      <c r="CF112" s="26">
+      <c r="CF112" s="25">
         <v>105.76266523663323</v>
       </c>
-      <c r="CG112" s="26">
+      <c r="CG112" s="25">
         <v>103.41532532363173</v>
       </c>
-      <c r="CH112" s="26">
+      <c r="CH112" s="25">
         <v>107.27019106735656</v>
       </c>
-      <c r="CI112" s="26">
+      <c r="CI112" s="25">
         <v>107.61395172788841</v>
       </c>
-      <c r="CJ112" s="8"/>
+      <c r="CJ112" s="25">
+        <v>109.26391999268171</v>
+      </c>
       <c r="CK112" s="8"/>
       <c r="CL112" s="8"/>
       <c r="CM112" s="8"/>
@@ -17463,25 +17563,27 @@
       <c r="CC113" s="14">
         <v>100.99469709474806</v>
       </c>
-      <c r="CD113" s="26">
+      <c r="CD113" s="25">
         <v>105.06084084246513</v>
       </c>
-      <c r="CE113" s="26">
+      <c r="CE113" s="25">
         <v>105.04966403467151</v>
       </c>
-      <c r="CF113" s="26">
+      <c r="CF113" s="25">
         <v>105.9683236248206</v>
       </c>
-      <c r="CG113" s="26">
+      <c r="CG113" s="25">
         <v>104.13023925182767</v>
       </c>
-      <c r="CH113" s="26">
+      <c r="CH113" s="25">
         <v>109.75196024704653</v>
       </c>
-      <c r="CI113" s="26">
+      <c r="CI113" s="25">
         <v>109.65352569527735</v>
       </c>
-      <c r="CJ113" s="8"/>
+      <c r="CJ113" s="25">
+        <v>110.8061175433742</v>
+      </c>
       <c r="CK113" s="8"/>
       <c r="CL113" s="8"/>
       <c r="CM113" s="8"/>
@@ -17790,25 +17892,27 @@
       <c r="CC114" s="14">
         <v>103.61409234726899</v>
       </c>
-      <c r="CD114" s="26">
+      <c r="CD114" s="25">
         <v>102.38011897403744</v>
       </c>
-      <c r="CE114" s="26">
+      <c r="CE114" s="25">
         <v>102.30791289520786</v>
       </c>
-      <c r="CF114" s="26">
+      <c r="CF114" s="25">
         <v>104.7867481365268</v>
       </c>
-      <c r="CG114" s="26">
+      <c r="CG114" s="25">
         <v>105.68771412900513</v>
       </c>
-      <c r="CH114" s="26">
+      <c r="CH114" s="25">
         <v>104.75704872572098</v>
       </c>
-      <c r="CI114" s="26">
+      <c r="CI114" s="25">
         <v>104.8331447124574</v>
       </c>
-      <c r="CJ114" s="8"/>
+      <c r="CJ114" s="25">
+        <v>106.99876886983701</v>
+      </c>
       <c r="CK114" s="8"/>
       <c r="CL114" s="8"/>
       <c r="CM114" s="8"/>
@@ -18117,25 +18221,27 @@
       <c r="CC115" s="14">
         <v>98.670820303177194</v>
       </c>
-      <c r="CD115" s="26">
+      <c r="CD115" s="25">
         <v>100.95397688741834</v>
       </c>
-      <c r="CE115" s="26">
+      <c r="CE115" s="25">
         <v>100.90410726426484</v>
       </c>
-      <c r="CF115" s="26">
+      <c r="CF115" s="25">
         <v>101.3902235771187</v>
       </c>
-      <c r="CG115" s="26">
+      <c r="CG115" s="25">
         <v>98.962235063787702</v>
       </c>
-      <c r="CH115" s="26">
+      <c r="CH115" s="25">
         <v>101.18553359025013</v>
       </c>
-      <c r="CI115" s="26">
-        <v>101.1686220522746</v>
-      </c>
-      <c r="CJ115" s="8"/>
+      <c r="CI115" s="25">
+        <v>101.16862205227457</v>
+      </c>
+      <c r="CJ115" s="25">
+        <v>101.65575166787164</v>
+      </c>
       <c r="CK115" s="8"/>
       <c r="CL115" s="8"/>
       <c r="CM115" s="8"/>
@@ -18444,25 +18550,27 @@
       <c r="CC116" s="14">
         <v>102.95233123243617</v>
       </c>
-      <c r="CD116" s="26">
+      <c r="CD116" s="25">
         <v>106.18465170943685</v>
       </c>
-      <c r="CE116" s="26">
+      <c r="CE116" s="25">
         <v>100.50746043241381</v>
       </c>
-      <c r="CF116" s="26">
+      <c r="CF116" s="25">
         <v>105.71150154409111</v>
       </c>
-      <c r="CG116" s="26">
+      <c r="CG116" s="25">
         <v>105.2859696771296</v>
       </c>
-      <c r="CH116" s="26">
+      <c r="CH116" s="25">
         <v>109.13108367165275</v>
       </c>
-      <c r="CI116" s="26">
+      <c r="CI116" s="25">
         <v>104.26452506171293</v>
       </c>
-      <c r="CJ116" s="8"/>
+      <c r="CJ116" s="25">
+        <v>109.21106253493944</v>
+      </c>
       <c r="CK116" s="8"/>
       <c r="CL116" s="8"/>
       <c r="CM116" s="8"/>
@@ -18771,25 +18879,27 @@
       <c r="CC117" s="14">
         <v>100.89200409059067</v>
       </c>
-      <c r="CD117" s="26">
+      <c r="CD117" s="25">
         <v>104.43124877122511</v>
       </c>
-      <c r="CE117" s="26">
+      <c r="CE117" s="25">
         <v>103.65492413025359</v>
       </c>
-      <c r="CF117" s="26">
+      <c r="CF117" s="25">
         <v>105.58194099446399</v>
       </c>
-      <c r="CG117" s="26">
+      <c r="CG117" s="25">
         <v>103.17894074068363</v>
       </c>
-      <c r="CH117" s="26">
+      <c r="CH117" s="25">
         <v>107.32902697438431</v>
       </c>
-      <c r="CI117" s="26">
+      <c r="CI117" s="25">
         <v>107.52964395131941</v>
       </c>
-      <c r="CJ117" s="8"/>
+      <c r="CJ117" s="25">
+        <v>109.07721290570601</v>
+      </c>
       <c r="CK117" s="8"/>
       <c r="CL117" s="8"/>
       <c r="CM117" s="8"/>
@@ -19098,25 +19208,27 @@
       <c r="CC118" s="14">
         <v>100.99207865802271</v>
       </c>
-      <c r="CD118" s="26">
+      <c r="CD118" s="25">
         <v>104.48926154642419</v>
       </c>
-      <c r="CE118" s="26">
+      <c r="CE118" s="25">
         <v>103.95478876713462</v>
       </c>
-      <c r="CF118" s="26">
+      <c r="CF118" s="25">
         <v>105.69056555320957</v>
       </c>
-      <c r="CG118" s="26">
+      <c r="CG118" s="25">
         <v>103.28128371578649</v>
       </c>
-      <c r="CH118" s="26">
+      <c r="CH118" s="25">
         <v>107.38864949913112</v>
       </c>
-      <c r="CI118" s="26">
-        <v>107.84071781402264</v>
-      </c>
-      <c r="CJ118" s="8"/>
+      <c r="CI118" s="25">
+        <v>107.84071781402263</v>
+      </c>
+      <c r="CJ118" s="25">
+        <v>109.18943346169769</v>
+      </c>
       <c r="CK118" s="8"/>
       <c r="CL118" s="8"/>
       <c r="CM118" s="8"/>
@@ -19262,13 +19374,13 @@
       <c r="CA119" s="8"/>
       <c r="CB119" s="8"/>
       <c r="CC119" s="8"/>
-      <c r="CD119" s="22"/>
-      <c r="CE119" s="22"/>
-      <c r="CF119" s="22"/>
-      <c r="CG119" s="22"/>
-      <c r="CH119" s="22"/>
-      <c r="CI119" s="22"/>
-      <c r="CJ119" s="8"/>
+      <c r="CD119" s="21"/>
+      <c r="CE119" s="21"/>
+      <c r="CF119" s="21"/>
+      <c r="CG119" s="21"/>
+      <c r="CH119" s="21"/>
+      <c r="CI119" s="21"/>
+      <c r="CJ119" s="21"/>
       <c r="CK119" s="8"/>
       <c r="CL119" s="8"/>
       <c r="CM119" s="8"/>
@@ -19577,25 +19689,27 @@
       <c r="CC120" s="14">
         <v>101.79374705088249</v>
       </c>
-      <c r="CD120" s="26">
+      <c r="CD120" s="25">
         <v>104.8496720046231</v>
       </c>
-      <c r="CE120" s="26">
+      <c r="CE120" s="25">
         <v>101.00469030013299</v>
       </c>
-      <c r="CF120" s="26">
+      <c r="CF120" s="25">
         <v>104.9728071394353</v>
       </c>
-      <c r="CG120" s="26">
+      <c r="CG120" s="25">
         <v>104.32976882596793</v>
       </c>
-      <c r="CH120" s="26">
+      <c r="CH120" s="25">
         <v>107.49217931234124</v>
       </c>
-      <c r="CI120" s="26">
-        <v>104.40164943308956</v>
-      </c>
-      <c r="CJ120" s="8"/>
+      <c r="CI120" s="25">
+        <v>104.5283052149659</v>
+      </c>
+      <c r="CJ120" s="25">
+        <v>108.09257394905048</v>
+      </c>
       <c r="CK120" s="8"/>
       <c r="CL120" s="8"/>
       <c r="CM120" s="8"/>
@@ -19742,12 +19856,13 @@
       <c r="CA121" s="11"/>
       <c r="CB121" s="11"/>
       <c r="CC121" s="11"/>
-      <c r="CD121" s="24"/>
-      <c r="CE121" s="24"/>
-      <c r="CF121" s="24"/>
-      <c r="CG121" s="24"/>
-      <c r="CH121" s="24"/>
-      <c r="CI121" s="24"/>
+      <c r="CD121" s="23"/>
+      <c r="CE121" s="23"/>
+      <c r="CF121" s="23"/>
+      <c r="CG121" s="23"/>
+      <c r="CH121" s="23"/>
+      <c r="CI121" s="23"/>
+      <c r="CJ121" s="23"/>
     </row>
     <row r="122" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
@@ -19918,6 +20033,7 @@
       <c r="CI133" s="28">
         <v>0</v>
       </c>
+      <c r="CJ133" s="28"/>
     </row>
     <row r="134" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
@@ -20161,23 +20277,26 @@
       <c r="CC134" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CD134" s="25" t="s">
+      <c r="CD134" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CE134" s="25" t="s">
+      <c r="CE134" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="CF134" s="25" t="s">
+      <c r="CF134" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="CG134" s="25" t="s">
+      <c r="CG134" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="CH134" s="25" t="s">
+      <c r="CH134" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CI134" s="25" t="s">
+      <c r="CI134" s="24" t="s">
         <v>8</v>
+      </c>
+      <c r="CJ134" s="24" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -20427,25 +20546,27 @@
       <c r="CC136" s="15">
         <v>8.4796805961946209</v>
       </c>
-      <c r="CD136" s="27">
+      <c r="CD136" s="26">
         <v>4.7172465268164094</v>
       </c>
-      <c r="CE136" s="27">
+      <c r="CE136" s="26">
         <v>2.8138242688858712</v>
       </c>
-      <c r="CF136" s="27">
+      <c r="CF136" s="26">
         <v>5.2976246656068406</v>
       </c>
-      <c r="CG136" s="27">
+      <c r="CG136" s="26">
         <v>5.7539038458270664</v>
       </c>
-      <c r="CH136" s="27">
+      <c r="CH136" s="26">
         <v>3.7041236046623744</v>
       </c>
-      <c r="CI136" s="27">
-        <v>2.9777938217214523</v>
-      </c>
-      <c r="CJ136" s="8"/>
+      <c r="CI136" s="26">
+        <v>2.8310062947125103</v>
+      </c>
+      <c r="CJ136" s="26">
+        <v>5.7008634356873014</v>
+      </c>
       <c r="CK136" s="8"/>
       <c r="CL136" s="8"/>
       <c r="CM136" s="8"/>
@@ -20754,25 +20875,27 @@
       <c r="CC137" s="15">
         <v>0.15036753568418579</v>
       </c>
-      <c r="CD137" s="27">
+      <c r="CD137" s="26">
         <v>6.7163618739666059E-2</v>
       </c>
-      <c r="CE137" s="27">
+      <c r="CE137" s="26">
         <v>5.7370971651881611E-2</v>
       </c>
-      <c r="CF137" s="27">
+      <c r="CF137" s="26">
         <v>0.17529915758425663</v>
       </c>
-      <c r="CG137" s="27">
+      <c r="CG137" s="26">
         <v>0.18904682375012258</v>
       </c>
-      <c r="CH137" s="27">
+      <c r="CH137" s="26">
         <v>8.994831451636022E-2</v>
       </c>
-      <c r="CI137" s="27">
-        <v>6.4468831889233774E-2</v>
-      </c>
-      <c r="CJ137" s="8"/>
+      <c r="CI137" s="26">
+        <v>6.693895275458582E-2</v>
+      </c>
+      <c r="CJ137" s="26">
+        <v>0.1800861180538984</v>
+      </c>
       <c r="CK137" s="8"/>
       <c r="CL137" s="8"/>
       <c r="CM137" s="8"/>
@@ -21081,25 +21204,27 @@
       <c r="CC138" s="15">
         <v>19.013300244799748</v>
       </c>
-      <c r="CD138" s="27">
+      <c r="CD138" s="26">
         <v>16.661239475699947</v>
       </c>
-      <c r="CE138" s="27">
+      <c r="CE138" s="26">
         <v>1.1445699944314536</v>
       </c>
-      <c r="CF138" s="27">
+      <c r="CF138" s="26">
         <v>3.6194095409716147</v>
       </c>
-      <c r="CG138" s="27">
+      <c r="CG138" s="26">
         <v>1.9865974286454744</v>
       </c>
-      <c r="CH138" s="27">
+      <c r="CH138" s="26">
         <v>0.42786854703723631</v>
       </c>
-      <c r="CI138" s="27">
-        <v>3.0530002342461127</v>
-      </c>
-      <c r="CJ138" s="8"/>
+      <c r="CI138" s="26">
+        <v>5.1249475333261634</v>
+      </c>
+      <c r="CJ138" s="26">
+        <v>5.153637016778819</v>
+      </c>
       <c r="CK138" s="8"/>
       <c r="CL138" s="8"/>
       <c r="CM138" s="8"/>
@@ -21408,25 +21533,27 @@
       <c r="CC139" s="15">
         <v>0.4976902965519393</v>
       </c>
-      <c r="CD139" s="27">
+      <c r="CD139" s="26">
         <v>0.37217717397498579</v>
       </c>
-      <c r="CE139" s="27">
+      <c r="CE139" s="26">
         <v>0.57517170484365721</v>
       </c>
-      <c r="CF139" s="27">
+      <c r="CF139" s="26">
         <v>0.74199498258312124</v>
       </c>
-      <c r="CG139" s="27">
+      <c r="CG139" s="26">
         <v>0.71098067422685463</v>
       </c>
-      <c r="CH139" s="27">
+      <c r="CH139" s="26">
         <v>0.56245991308573628</v>
       </c>
-      <c r="CI139" s="27">
-        <v>0.58633967393168351</v>
-      </c>
-      <c r="CJ139" s="8"/>
+      <c r="CI139" s="26">
+        <v>0.59392183349487626</v>
+      </c>
+      <c r="CJ139" s="26">
+        <v>0.83718345241172598</v>
+      </c>
       <c r="CK139" s="8"/>
       <c r="CL139" s="8"/>
       <c r="CM139" s="8"/>
@@ -21735,25 +21862,27 @@
       <c r="CC140" s="15">
         <v>11.952984608400481</v>
       </c>
-      <c r="CD140" s="27">
+      <c r="CD140" s="26">
         <v>15.677809144343243</v>
       </c>
-      <c r="CE140" s="27">
+      <c r="CE140" s="26">
         <v>18.21141318576171</v>
       </c>
-      <c r="CF140" s="27">
+      <c r="CF140" s="26">
         <v>14.531762748769742</v>
       </c>
-      <c r="CG140" s="27">
+      <c r="CG140" s="26">
         <v>14.574235526967808</v>
       </c>
-      <c r="CH140" s="27">
+      <c r="CH140" s="26">
         <v>18.960693533406864</v>
       </c>
-      <c r="CI140" s="27">
-        <v>18.20125753935881</v>
-      </c>
-      <c r="CJ140" s="8"/>
+      <c r="CI140" s="26">
+        <v>17.595584135124572</v>
+      </c>
+      <c r="CJ140" s="26">
+        <v>15.722285234142785</v>
+      </c>
       <c r="CK140" s="8"/>
       <c r="CL140" s="8"/>
       <c r="CM140" s="8"/>
@@ -22062,25 +22191,27 @@
       <c r="CC141" s="15">
         <v>49.84358522879478</v>
       </c>
-      <c r="CD141" s="27">
+      <c r="CD141" s="26">
         <v>51.002001775258357</v>
       </c>
-      <c r="CE141" s="27">
+      <c r="CE141" s="26">
         <v>63.303235143767665</v>
       </c>
-      <c r="CF141" s="27">
+      <c r="CF141" s="26">
         <v>62.830457175985579</v>
       </c>
-      <c r="CG141" s="27">
+      <c r="CG141" s="26">
         <v>65.216744441550929</v>
       </c>
-      <c r="CH141" s="27">
+      <c r="CH141" s="26">
         <v>62.389221836740596</v>
       </c>
-      <c r="CI141" s="27">
-        <v>61.463912086268792</v>
-      </c>
-      <c r="CJ141" s="8"/>
+      <c r="CI141" s="26">
+        <v>59.929258730668444</v>
+      </c>
+      <c r="CJ141" s="26">
+        <v>57.479882935936011</v>
+      </c>
       <c r="CK141" s="8"/>
       <c r="CL141" s="8"/>
       <c r="CM141" s="8"/>
@@ -22389,25 +22520,27 @@
       <c r="CC142" s="15">
         <v>8.603494650630692</v>
       </c>
-      <c r="CD142" s="27">
+      <c r="CD142" s="26">
         <v>10.581523455716939</v>
       </c>
-      <c r="CE142" s="27">
+      <c r="CE142" s="26">
         <v>12.593230952240001</v>
       </c>
-      <c r="CF142" s="27">
+      <c r="CF142" s="26">
         <v>11.40093028420263</v>
       </c>
-      <c r="CG142" s="27">
+      <c r="CG142" s="26">
         <v>10.200751991425538</v>
       </c>
-      <c r="CH142" s="27">
+      <c r="CH142" s="26">
         <v>12.89339308679712</v>
       </c>
-      <c r="CI142" s="27">
-        <v>12.488541717869856</v>
-      </c>
-      <c r="CJ142" s="8"/>
+      <c r="CI142" s="26">
+        <v>12.699571869240078</v>
+      </c>
+      <c r="CJ142" s="26">
+        <v>13.399243597907093</v>
+      </c>
       <c r="CK142" s="8"/>
       <c r="CL142" s="8"/>
       <c r="CM142" s="8"/>
@@ -22716,25 +22849,27 @@
       <c r="CC143" s="15">
         <v>1.4588968389435548</v>
       </c>
-      <c r="CD143" s="27">
+      <c r="CD143" s="26">
         <v>0.92083882945046491</v>
       </c>
-      <c r="CE143" s="27">
+      <c r="CE143" s="26">
         <v>1.3011837784177593</v>
       </c>
-      <c r="CF143" s="27">
+      <c r="CF143" s="26">
         <v>1.4025214442962244</v>
       </c>
-      <c r="CG143" s="27">
+      <c r="CG143" s="26">
         <v>1.3677392676061928</v>
       </c>
-      <c r="CH143" s="27">
+      <c r="CH143" s="26">
         <v>0.97229116375370606</v>
       </c>
-      <c r="CI143" s="27">
-        <v>1.1646860947140503</v>
-      </c>
-      <c r="CJ143" s="8"/>
+      <c r="CI143" s="26">
+        <v>1.1587706506787772</v>
+      </c>
+      <c r="CJ143" s="26">
+        <v>1.5268182090823554</v>
+      </c>
       <c r="CK143" s="8"/>
       <c r="CL143" s="8"/>
       <c r="CM143" s="8"/>
@@ -22880,13 +23015,13 @@
       <c r="CA144" s="8"/>
       <c r="CB144" s="8"/>
       <c r="CC144" s="8"/>
-      <c r="CD144" s="22"/>
-      <c r="CE144" s="22"/>
-      <c r="CF144" s="22"/>
-      <c r="CG144" s="22"/>
-      <c r="CH144" s="22"/>
-      <c r="CI144" s="22"/>
-      <c r="CJ144" s="8"/>
+      <c r="CD144" s="21"/>
+      <c r="CE144" s="21"/>
+      <c r="CF144" s="21"/>
+      <c r="CG144" s="21"/>
+      <c r="CH144" s="21"/>
+      <c r="CI144" s="21"/>
+      <c r="CJ144" s="21"/>
       <c r="CK144" s="8"/>
       <c r="CL144" s="8"/>
       <c r="CM144" s="8"/>
@@ -23195,25 +23330,27 @@
       <c r="CC145" s="14">
         <v>100</v>
       </c>
-      <c r="CD145" s="26">
+      <c r="CD145" s="25">
         <v>100</v>
       </c>
-      <c r="CE145" s="26">
+      <c r="CE145" s="25">
         <v>100</v>
       </c>
-      <c r="CF145" s="26">
+      <c r="CF145" s="25">
         <v>100</v>
       </c>
-      <c r="CG145" s="26">
+      <c r="CG145" s="25">
         <v>100</v>
       </c>
-      <c r="CH145" s="26">
+      <c r="CH145" s="25">
         <v>100</v>
       </c>
-      <c r="CI145" s="26">
+      <c r="CI145" s="25">
         <v>100</v>
       </c>
-      <c r="CJ145" s="8"/>
+      <c r="CJ145" s="25">
+        <v>100</v>
+      </c>
       <c r="CK145" s="8"/>
       <c r="CL145" s="8"/>
       <c r="CM145" s="8"/>
@@ -23360,12 +23497,13 @@
       <c r="CA146" s="11"/>
       <c r="CB146" s="11"/>
       <c r="CC146" s="11"/>
-      <c r="CD146" s="24"/>
-      <c r="CE146" s="24"/>
-      <c r="CF146" s="24"/>
-      <c r="CG146" s="24"/>
-      <c r="CH146" s="24"/>
-      <c r="CI146" s="24"/>
+      <c r="CD146" s="23"/>
+      <c r="CE146" s="23"/>
+      <c r="CF146" s="23"/>
+      <c r="CG146" s="23"/>
+      <c r="CH146" s="23"/>
+      <c r="CI146" s="23"/>
+      <c r="CJ146" s="23"/>
     </row>
     <row r="147" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
@@ -23453,13 +23591,13 @@
       <c r="CA148" s="8"/>
       <c r="CB148" s="8"/>
       <c r="CC148" s="8"/>
-      <c r="CD148" s="22"/>
-      <c r="CE148" s="22"/>
-      <c r="CF148" s="22"/>
-      <c r="CG148" s="22"/>
-      <c r="CH148" s="22"/>
-      <c r="CI148" s="22"/>
-      <c r="CJ148" s="8"/>
+      <c r="CD148" s="21"/>
+      <c r="CE148" s="21"/>
+      <c r="CF148" s="21"/>
+      <c r="CG148" s="21"/>
+      <c r="CH148" s="21"/>
+      <c r="CI148" s="21"/>
+      <c r="CJ148" s="21"/>
       <c r="CK148" s="8"/>
       <c r="CL148" s="8"/>
       <c r="CM148" s="8"/>
@@ -23605,13 +23743,13 @@
       <c r="CA149" s="8"/>
       <c r="CB149" s="8"/>
       <c r="CC149" s="8"/>
-      <c r="CD149" s="22"/>
-      <c r="CE149" s="22"/>
-      <c r="CF149" s="22"/>
-      <c r="CG149" s="22"/>
-      <c r="CH149" s="22"/>
-      <c r="CI149" s="22"/>
-      <c r="CJ149" s="8"/>
+      <c r="CD149" s="21"/>
+      <c r="CE149" s="21"/>
+      <c r="CF149" s="21"/>
+      <c r="CG149" s="21"/>
+      <c r="CH149" s="21"/>
+      <c r="CI149" s="21"/>
+      <c r="CJ149" s="21"/>
       <c r="CK149" s="8"/>
       <c r="CL149" s="8"/>
       <c r="CM149" s="8"/>
@@ -23840,6 +23978,7 @@
       <c r="CI158" s="28">
         <v>0</v>
       </c>
+      <c r="CJ158" s="28"/>
     </row>
     <row r="159" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
@@ -24083,23 +24222,26 @@
       <c r="CC159" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CD159" s="25" t="s">
+      <c r="CD159" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CE159" s="25" t="s">
+      <c r="CE159" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="CF159" s="25" t="s">
+      <c r="CF159" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="CG159" s="25" t="s">
+      <c r="CG159" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="CH159" s="25" t="s">
+      <c r="CH159" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CI159" s="25" t="s">
+      <c r="CI159" s="24" t="s">
         <v>8</v>
+      </c>
+      <c r="CJ159" s="24" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -24349,25 +24491,27 @@
       <c r="CC161" s="15">
         <v>8.4311298347575008</v>
       </c>
-      <c r="CD161" s="27">
+      <c r="CD161" s="26">
         <v>4.7321000717655783</v>
       </c>
-      <c r="CE161" s="27">
+      <c r="CE161" s="26">
         <v>2.8943145667977341</v>
       </c>
-      <c r="CF161" s="27">
+      <c r="CF161" s="26">
         <v>5.3324935726435347</v>
       </c>
-      <c r="CG161" s="27">
+      <c r="CG161" s="26">
         <v>5.4317137688307904</v>
       </c>
-      <c r="CH161" s="27">
+      <c r="CH161" s="26">
         <v>3.4326979078622184</v>
       </c>
-      <c r="CI161" s="27">
-        <v>2.8662954013103139</v>
-      </c>
-      <c r="CJ161" s="8"/>
+      <c r="CI161" s="26">
+        <v>2.7283099461060982</v>
+      </c>
+      <c r="CJ161" s="26">
+        <v>5.549886325515379</v>
+      </c>
       <c r="CK161" s="8"/>
       <c r="CL161" s="8"/>
       <c r="CM161" s="8"/>
@@ -24676,25 +24820,27 @@
       <c r="CC162" s="15">
         <v>0.15136469743347755</v>
       </c>
-      <c r="CD162" s="27">
+      <c r="CD162" s="26">
         <v>6.7469707998831299E-2</v>
       </c>
-      <c r="CE162" s="27">
+      <c r="CE162" s="26">
         <v>5.5860322251464416E-2</v>
       </c>
-      <c r="CF162" s="27">
+      <c r="CF162" s="26">
         <v>0.17398998616029426</v>
       </c>
-      <c r="CG162" s="27">
+      <c r="CG162" s="26">
         <v>0.19071845838526591</v>
       </c>
-      <c r="CH162" s="27">
+      <c r="CH162" s="26">
         <v>9.013445633525824E-2</v>
       </c>
-      <c r="CI162" s="27">
-        <v>6.254442177980446E-2</v>
-      </c>
-      <c r="CJ162" s="8"/>
+      <c r="CI162" s="26">
+        <v>6.5019592459480649E-2</v>
+      </c>
+      <c r="CJ162" s="26">
+        <v>0.17815553418037944</v>
+      </c>
       <c r="CK162" s="8"/>
       <c r="CL162" s="8"/>
       <c r="CM162" s="8"/>
@@ -25003,25 +25149,27 @@
       <c r="CC163" s="15">
         <v>19.163729694697746</v>
       </c>
-      <c r="CD163" s="27">
+      <c r="CD163" s="26">
         <v>16.627750931834523</v>
       </c>
-      <c r="CE163" s="27">
+      <c r="CE163" s="26">
         <v>1.100497929971656</v>
       </c>
-      <c r="CF163" s="27">
+      <c r="CF163" s="26">
         <v>3.5854070981458221</v>
       </c>
-      <c r="CG163" s="27">
+      <c r="CG163" s="26">
         <v>1.9904040552485993</v>
       </c>
-      <c r="CH163" s="27">
+      <c r="CH163" s="26">
         <v>0.41905878015035458</v>
       </c>
-      <c r="CI163" s="27">
-        <v>2.9067762131120478</v>
-      </c>
-      <c r="CJ163" s="8"/>
+      <c r="CI163" s="26">
+        <v>4.8854067990745502</v>
+      </c>
+      <c r="CJ163" s="26">
+        <v>5.0274290146901661</v>
+      </c>
       <c r="CK163" s="8"/>
       <c r="CL163" s="8"/>
       <c r="CM163" s="8"/>
@@ -25330,25 +25478,27 @@
       <c r="CC164" s="15">
         <v>0.4889466192213584</v>
       </c>
-      <c r="CD164" s="27">
+      <c r="CD164" s="26">
         <v>0.38115461292617325</v>
       </c>
-      <c r="CE164" s="27">
+      <c r="CE164" s="26">
         <v>0.56784503048790369</v>
       </c>
-      <c r="CF164" s="27">
+      <c r="CF164" s="26">
         <v>0.74331246641650306</v>
       </c>
-      <c r="CG164" s="27">
+      <c r="CG164" s="26">
         <v>0.7018455266359237</v>
       </c>
-      <c r="CH164" s="27">
+      <c r="CH164" s="26">
         <v>0.57714533359673659</v>
       </c>
-      <c r="CI164" s="27">
-        <v>0.58392628833592031</v>
-      </c>
-      <c r="CJ164" s="8"/>
+      <c r="CI164" s="26">
+        <v>0.59219479541194553</v>
+      </c>
+      <c r="CJ164" s="26">
+        <v>0.84574163978297856</v>
+      </c>
       <c r="CK164" s="8"/>
       <c r="CL164" s="8"/>
       <c r="CM164" s="8"/>
@@ -25657,25 +25807,27 @@
       <c r="CC165" s="15">
         <v>12.331296000094479</v>
       </c>
-      <c r="CD165" s="27">
+      <c r="CD165" s="26">
         <v>16.282797342086027</v>
       </c>
-      <c r="CE165" s="27">
+      <c r="CE165" s="26">
         <v>18.229566651218533</v>
       </c>
-      <c r="CF165" s="27">
+      <c r="CF165" s="26">
         <v>15.045236854245292</v>
       </c>
-      <c r="CG165" s="27">
+      <c r="CG165" s="26">
         <v>15.36471586725664</v>
       </c>
-      <c r="CH165" s="27">
+      <c r="CH165" s="26">
         <v>20.142466979842126</v>
       </c>
-      <c r="CI165" s="27">
-        <v>18.782911838847109</v>
-      </c>
-      <c r="CJ165" s="8"/>
+      <c r="CI165" s="26">
+        <v>18.179911435005668</v>
+      </c>
+      <c r="CJ165" s="26">
+        <v>16.717817255162352</v>
+      </c>
       <c r="CK165" s="8"/>
       <c r="CL165" s="8"/>
       <c r="CM165" s="8"/>
@@ -25984,25 +26136,27 @@
       <c r="CC166" s="15">
         <v>49.282665541919236</v>
       </c>
-      <c r="CD166" s="27">
+      <c r="CD166" s="26">
         <v>50.360791994195488</v>
       </c>
-      <c r="CE166" s="27">
+      <c r="CE166" s="26">
         <v>63.616408505240663</v>
       </c>
-      <c r="CF166" s="27">
+      <c r="CF166" s="26">
         <v>62.391408382997739</v>
       </c>
-      <c r="CG166" s="27">
+      <c r="CG166" s="26">
         <v>64.624449886671144</v>
       </c>
-      <c r="CH166" s="27">
+      <c r="CH166" s="26">
         <v>61.452275513088836</v>
       </c>
-      <c r="CI166" s="27">
-        <v>61.54474686974082</v>
-      </c>
-      <c r="CJ166" s="8"/>
+      <c r="CI166" s="26">
+        <v>60.080874527536608</v>
+      </c>
+      <c r="CJ166" s="26">
+        <v>56.891200878552773</v>
+      </c>
       <c r="CK166" s="8"/>
       <c r="CL166" s="8"/>
       <c r="CM166" s="8"/>
@@ -26311,25 +26465,27 @@
       <c r="CC167" s="15">
         <v>8.6803901470086657</v>
       </c>
-      <c r="CD167" s="27">
+      <c r="CD167" s="26">
         <v>10.623920298718568</v>
       </c>
-      <c r="CE167" s="27">
+      <c r="CE167" s="26">
         <v>12.271249078439107</v>
       </c>
-      <c r="CF167" s="27">
+      <c r="CF167" s="26">
         <v>11.335154901125579</v>
       </c>
-      <c r="CG167" s="27">
+      <c r="CG167" s="26">
         <v>10.314528231019395</v>
       </c>
-      <c r="CH167" s="27">
+      <c r="CH167" s="26">
         <v>12.912992511907071</v>
       </c>
-      <c r="CI167" s="27">
-        <v>12.125255012932316</v>
-      </c>
-      <c r="CJ167" s="8"/>
+      <c r="CI167" s="26">
+        <v>12.345104807082677</v>
+      </c>
+      <c r="CJ167" s="26">
+        <v>13.278288754225656</v>
+      </c>
       <c r="CK167" s="8"/>
       <c r="CL167" s="8"/>
       <c r="CM167" s="8"/>
@@ -26638,25 +26794,27 @@
       <c r="CC168" s="15">
         <v>1.4704774648675385</v>
       </c>
-      <c r="CD168" s="27">
+      <c r="CD168" s="26">
         <v>0.92401504047481176</v>
       </c>
-      <c r="CE168" s="27">
+      <c r="CE168" s="26">
         <v>1.2642579155929465</v>
       </c>
-      <c r="CF168" s="27">
+      <c r="CF168" s="26">
         <v>1.3929967382652435</v>
       </c>
-      <c r="CG168" s="27">
+      <c r="CG168" s="26">
         <v>1.3816242059522525</v>
       </c>
-      <c r="CH168" s="27">
+      <c r="CH168" s="26">
         <v>0.97322851721739834</v>
       </c>
-      <c r="CI168" s="27">
-        <v>1.1275439539416647</v>
-      </c>
-      <c r="CJ168" s="8"/>
+      <c r="CI168" s="26">
+        <v>1.1231780973229573</v>
+      </c>
+      <c r="CJ168" s="26">
+        <v>1.5114805978903125</v>
+      </c>
       <c r="CK168" s="8"/>
       <c r="CL168" s="8"/>
       <c r="CM168" s="8"/>
@@ -26802,13 +26960,13 @@
       <c r="CA169" s="8"/>
       <c r="CB169" s="8"/>
       <c r="CC169" s="8"/>
-      <c r="CD169" s="22"/>
-      <c r="CE169" s="22"/>
-      <c r="CF169" s="22"/>
-      <c r="CG169" s="22"/>
-      <c r="CH169" s="22"/>
-      <c r="CI169" s="22"/>
-      <c r="CJ169" s="8"/>
+      <c r="CD169" s="21"/>
+      <c r="CE169" s="21"/>
+      <c r="CF169" s="21"/>
+      <c r="CG169" s="21"/>
+      <c r="CH169" s="21"/>
+      <c r="CI169" s="21"/>
+      <c r="CJ169" s="21"/>
       <c r="CK169" s="8"/>
       <c r="CL169" s="8"/>
       <c r="CM169" s="8"/>
@@ -27117,25 +27275,27 @@
       <c r="CC170" s="14">
         <v>100</v>
       </c>
-      <c r="CD170" s="26">
+      <c r="CD170" s="25">
         <v>100</v>
       </c>
-      <c r="CE170" s="26">
+      <c r="CE170" s="25">
         <v>100</v>
       </c>
-      <c r="CF170" s="26">
+      <c r="CF170" s="25">
         <v>100</v>
       </c>
-      <c r="CG170" s="26">
+      <c r="CG170" s="25">
         <v>100</v>
       </c>
-      <c r="CH170" s="26">
+      <c r="CH170" s="25">
         <v>100</v>
       </c>
-      <c r="CI170" s="26">
+      <c r="CI170" s="25">
         <v>100</v>
       </c>
-      <c r="CJ170" s="8"/>
+      <c r="CJ170" s="25">
+        <v>100</v>
+      </c>
       <c r="CK170" s="8"/>
       <c r="CL170" s="8"/>
       <c r="CM170" s="8"/>
@@ -27282,12 +27442,13 @@
       <c r="CA171" s="11"/>
       <c r="CB171" s="11"/>
       <c r="CC171" s="11"/>
-      <c r="CD171" s="24"/>
-      <c r="CE171" s="24"/>
-      <c r="CF171" s="24"/>
-      <c r="CG171" s="24"/>
-      <c r="CH171" s="24"/>
-      <c r="CI171" s="24"/>
+      <c r="CD171" s="23"/>
+      <c r="CE171" s="23"/>
+      <c r="CF171" s="23"/>
+      <c r="CG171" s="23"/>
+      <c r="CH171" s="23"/>
+      <c r="CI171" s="23"/>
+      <c r="CJ171" s="23"/>
     </row>
     <row r="172" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
@@ -27382,7 +27543,7 @@
       <c r="CG173" s="18"/>
       <c r="CH173" s="18"/>
       <c r="CI173" s="18"/>
-      <c r="CJ173" s="16"/>
+      <c r="CJ173" s="18"/>
       <c r="CK173" s="16"/>
       <c r="CL173" s="16"/>
       <c r="CM173" s="16"/>
@@ -27535,7 +27696,7 @@
       <c r="CG174" s="18"/>
       <c r="CH174" s="18"/>
       <c r="CI174" s="18"/>
-      <c r="CJ174" s="16"/>
+      <c r="CJ174" s="18"/>
       <c r="CK174" s="16"/>
       <c r="CL174" s="16"/>
       <c r="CM174" s="16"/>
@@ -27602,11 +27763,6 @@
     </row>
   </sheetData>
   <mergeCells count="152">
-    <mergeCell ref="AD158:AG158"/>
-    <mergeCell ref="AH158:AK158"/>
-    <mergeCell ref="BZ59:CC59"/>
-    <mergeCell ref="BZ84:CC84"/>
-    <mergeCell ref="CD9:CG9"/>
     <mergeCell ref="CD158:CG158"/>
     <mergeCell ref="CD133:CG133"/>
     <mergeCell ref="CD108:CG108"/>
@@ -27622,10 +27778,10 @@
     <mergeCell ref="BB108:BE108"/>
     <mergeCell ref="BF108:BI108"/>
     <mergeCell ref="BZ34:CC34"/>
-    <mergeCell ref="BV9:BY9"/>
-    <mergeCell ref="BZ9:CC9"/>
-    <mergeCell ref="BR9:BU9"/>
     <mergeCell ref="BR59:BU59"/>
+    <mergeCell ref="BB133:BE133"/>
+    <mergeCell ref="B108:E108"/>
+    <mergeCell ref="F108:I108"/>
     <mergeCell ref="J108:M108"/>
     <mergeCell ref="N108:Q108"/>
     <mergeCell ref="B158:E158"/>
@@ -27635,14 +27791,8 @@
     <mergeCell ref="R158:U158"/>
     <mergeCell ref="V158:Y158"/>
     <mergeCell ref="Z158:AC158"/>
-    <mergeCell ref="AT108:AW108"/>
-    <mergeCell ref="AX108:BA108"/>
-    <mergeCell ref="AL158:AO158"/>
-    <mergeCell ref="AP158:AS158"/>
-    <mergeCell ref="AT158:AW158"/>
-    <mergeCell ref="AX158:BA158"/>
-    <mergeCell ref="BJ108:BM108"/>
-    <mergeCell ref="BN108:BQ108"/>
+    <mergeCell ref="AD158:AG158"/>
+    <mergeCell ref="AH158:AK158"/>
     <mergeCell ref="B133:E133"/>
     <mergeCell ref="F133:I133"/>
     <mergeCell ref="J133:M133"/>
@@ -27652,16 +27802,6 @@
     <mergeCell ref="Z133:AC133"/>
     <mergeCell ref="AD133:AG133"/>
     <mergeCell ref="AH133:AK133"/>
-    <mergeCell ref="AL133:AO133"/>
-    <mergeCell ref="AP133:AS133"/>
-    <mergeCell ref="AT133:AW133"/>
-    <mergeCell ref="AX133:BA133"/>
-    <mergeCell ref="BB133:BE133"/>
-    <mergeCell ref="B108:E108"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="AH84:AK84"/>
-    <mergeCell ref="AL84:AO84"/>
-    <mergeCell ref="AP84:AS84"/>
     <mergeCell ref="R108:U108"/>
     <mergeCell ref="V108:Y108"/>
     <mergeCell ref="Z108:AC108"/>
@@ -27669,6 +27809,15 @@
     <mergeCell ref="AH108:AK108"/>
     <mergeCell ref="AL108:AO108"/>
     <mergeCell ref="AP108:AS108"/>
+    <mergeCell ref="AT108:AW108"/>
+    <mergeCell ref="AX108:BA108"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="R34:U34"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
     <mergeCell ref="BB34:BE34"/>
     <mergeCell ref="BF34:BI34"/>
     <mergeCell ref="V34:Y34"/>
@@ -27676,28 +27825,24 @@
     <mergeCell ref="AD34:AG34"/>
     <mergeCell ref="AH34:AK34"/>
     <mergeCell ref="AL34:AO34"/>
-    <mergeCell ref="BF59:BI59"/>
-    <mergeCell ref="BJ59:BM59"/>
     <mergeCell ref="AP34:AS34"/>
+    <mergeCell ref="AT34:AW34"/>
+    <mergeCell ref="AX34:BA34"/>
+    <mergeCell ref="AD59:AG59"/>
+    <mergeCell ref="AH59:AK59"/>
+    <mergeCell ref="BJ34:BM34"/>
+    <mergeCell ref="BN34:BQ34"/>
+    <mergeCell ref="AL59:AO59"/>
+    <mergeCell ref="AP59:AS59"/>
+    <mergeCell ref="AT59:AW59"/>
+    <mergeCell ref="AX59:BA59"/>
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="R9:U9"/>
     <mergeCell ref="V9:Y9"/>
     <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="R34:U34"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="AT34:AW34"/>
-    <mergeCell ref="AX34:BA34"/>
-    <mergeCell ref="BZ158:CC158"/>
-    <mergeCell ref="BR158:BU158"/>
-    <mergeCell ref="BV158:BY158"/>
-    <mergeCell ref="BR84:BU84"/>
-    <mergeCell ref="BV84:BY84"/>
+    <mergeCell ref="BF59:BI59"/>
+    <mergeCell ref="BJ59:BM59"/>
     <mergeCell ref="AD9:AG9"/>
     <mergeCell ref="AH9:AK9"/>
     <mergeCell ref="AL9:AO9"/>
@@ -27707,14 +27852,36 @@
     <mergeCell ref="BB9:BE9"/>
     <mergeCell ref="BF9:BI9"/>
     <mergeCell ref="BJ9:BM9"/>
-    <mergeCell ref="AD59:AG59"/>
-    <mergeCell ref="AH59:AK59"/>
-    <mergeCell ref="BJ34:BM34"/>
-    <mergeCell ref="BN34:BQ34"/>
-    <mergeCell ref="AL59:AO59"/>
-    <mergeCell ref="AP59:AS59"/>
-    <mergeCell ref="AT59:AW59"/>
-    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="AX84:BA84"/>
+    <mergeCell ref="BB84:BE84"/>
+    <mergeCell ref="BF84:BI84"/>
+    <mergeCell ref="BJ84:BM84"/>
+    <mergeCell ref="Z84:AC84"/>
+    <mergeCell ref="AD84:AG84"/>
+    <mergeCell ref="BZ158:CC158"/>
+    <mergeCell ref="BR158:BU158"/>
+    <mergeCell ref="BV158:BY158"/>
+    <mergeCell ref="BR84:BU84"/>
+    <mergeCell ref="BV84:BY84"/>
+    <mergeCell ref="AH84:AK84"/>
+    <mergeCell ref="AL84:AO84"/>
+    <mergeCell ref="AP84:AS84"/>
+    <mergeCell ref="AL158:AO158"/>
+    <mergeCell ref="AP158:AS158"/>
+    <mergeCell ref="AT158:AW158"/>
+    <mergeCell ref="AX158:BA158"/>
+    <mergeCell ref="BJ108:BM108"/>
+    <mergeCell ref="BN108:BQ108"/>
+    <mergeCell ref="AL133:AO133"/>
+    <mergeCell ref="AP133:AS133"/>
+    <mergeCell ref="AT133:AW133"/>
+    <mergeCell ref="AX133:BA133"/>
+    <mergeCell ref="CH9:CJ9"/>
+    <mergeCell ref="CH34:CJ34"/>
+    <mergeCell ref="CD84:CF84"/>
+    <mergeCell ref="CH108:CJ108"/>
+    <mergeCell ref="CH133:CJ133"/>
+    <mergeCell ref="CH158:CJ158"/>
     <mergeCell ref="B84:E84"/>
     <mergeCell ref="BR133:BU133"/>
     <mergeCell ref="BV133:BY133"/>
@@ -27733,19 +27900,7 @@
     <mergeCell ref="V84:Y84"/>
     <mergeCell ref="BB59:BE59"/>
     <mergeCell ref="AT84:AW84"/>
-    <mergeCell ref="AX84:BA84"/>
-    <mergeCell ref="BB84:BE84"/>
-    <mergeCell ref="BF84:BI84"/>
-    <mergeCell ref="BJ84:BM84"/>
-    <mergeCell ref="Z84:AC84"/>
-    <mergeCell ref="AD84:AG84"/>
-    <mergeCell ref="CH9:CI9"/>
-    <mergeCell ref="CH34:CI34"/>
     <mergeCell ref="CD59:CE59"/>
-    <mergeCell ref="CD84:CE84"/>
-    <mergeCell ref="CH108:CI108"/>
-    <mergeCell ref="CH133:CI133"/>
-    <mergeCell ref="CH158:CI158"/>
     <mergeCell ref="BN59:BQ59"/>
     <mergeCell ref="BZ108:CC108"/>
     <mergeCell ref="BR108:BU108"/>
@@ -27754,14 +27909,20 @@
     <mergeCell ref="BV108:BY108"/>
     <mergeCell ref="BV59:BY59"/>
     <mergeCell ref="BN9:BQ9"/>
+    <mergeCell ref="BZ59:CC59"/>
+    <mergeCell ref="BZ84:CC84"/>
+    <mergeCell ref="CD9:CG9"/>
+    <mergeCell ref="BV9:BY9"/>
+    <mergeCell ref="BZ9:CC9"/>
+    <mergeCell ref="BR9:BU9"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="50" max="86" man="1"/>
-    <brk id="100" max="86" man="1"/>
-    <brk id="124" max="86" man="1"/>
+    <brk id="50" max="87" man="1"/>
+    <brk id="100" max="87" man="1"/>
+    <brk id="124" max="87" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q3 2023 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2023\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of November 2023\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948E9536-37C6-4E2F-9EEC-A6ADE40659E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BE28AD-7329-4F5C-B184-D99C1A6BB816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="1560" windowWidth="28770" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="975" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EOS" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt" localSheetId="0">EOS!$A$37:$A$48</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EOS!$A$1:$CQ$174</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EOS!$A$1:$CR$174</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="57">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -219,13 +219,13 @@
     <t>2022 - 2023</t>
   </si>
   <si>
-    <t>As of August 2023</t>
+    <t>As of November 2023</t>
   </si>
   <si>
-    <t>Q1 2000 to Q2 2023</t>
+    <t>Q1 2000 to Q3 2023</t>
   </si>
   <si>
-    <t>Q1 2001 to Q2 2023</t>
+    <t>Q1 2001 to Q3 2023</t>
   </si>
 </sst>
 </file>
@@ -316,7 +316,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -351,10 +351,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -695,19 +706,20 @@
   <dimension ref="A1:EU174"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="70" zoomScaleNormal="95" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="BX14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="BX3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="topRight" activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="bottomLeft" activeCell="P1" sqref="P1:AF1048576"/>
-      <selection pane="bottomRight" activeCell="CQ5" sqref="CQ5"/>
+      <selection pane="bottomRight" activeCell="CU17" sqref="CU17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.77734375" style="1" customWidth="1"/>
     <col min="2" max="73" width="8.77734375" style="1" customWidth="1"/>
-    <col min="74" max="95" width="10" style="1" customWidth="1"/>
-    <col min="96" max="16384" width="7.77734375" style="1"/>
+    <col min="74" max="89" width="10" style="1" customWidth="1"/>
+    <col min="90" max="96" width="11.109375" style="22" customWidth="1"/>
+    <col min="97" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:151" x14ac:dyDescent="0.2">
@@ -742,148 +754,149 @@
     </row>
     <row r="9" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="22">
+      <c r="B9" s="32">
         <v>2000</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32">
         <v>2001</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22">
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32">
         <v>2002</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22">
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32">
         <v>2003</v>
       </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22">
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32">
         <v>2004</v>
       </c>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22">
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32">
         <v>2005</v>
       </c>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="22">
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32">
         <v>2006</v>
       </c>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22">
+      <c r="AA9" s="32"/>
+      <c r="AB9" s="32"/>
+      <c r="AC9" s="32"/>
+      <c r="AD9" s="32">
         <v>2007</v>
       </c>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="22">
+      <c r="AE9" s="32"/>
+      <c r="AF9" s="32"/>
+      <c r="AG9" s="32"/>
+      <c r="AH9" s="32">
         <v>2008</v>
       </c>
-      <c r="AI9" s="22"/>
-      <c r="AJ9" s="22"/>
-      <c r="AK9" s="22"/>
-      <c r="AL9" s="22">
+      <c r="AI9" s="32"/>
+      <c r="AJ9" s="32"/>
+      <c r="AK9" s="32"/>
+      <c r="AL9" s="32">
         <v>2009</v>
       </c>
-      <c r="AM9" s="22"/>
-      <c r="AN9" s="22"/>
-      <c r="AO9" s="22"/>
-      <c r="AP9" s="22">
+      <c r="AM9" s="32"/>
+      <c r="AN9" s="32"/>
+      <c r="AO9" s="32"/>
+      <c r="AP9" s="32">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="22"/>
-      <c r="AR9" s="22"/>
-      <c r="AS9" s="22"/>
-      <c r="AT9" s="22">
+      <c r="AQ9" s="32"/>
+      <c r="AR9" s="32"/>
+      <c r="AS9" s="32"/>
+      <c r="AT9" s="32">
         <v>2011</v>
       </c>
-      <c r="AU9" s="22"/>
-      <c r="AV9" s="22"/>
-      <c r="AW9" s="22"/>
-      <c r="AX9" s="22">
+      <c r="AU9" s="32"/>
+      <c r="AV9" s="32"/>
+      <c r="AW9" s="32"/>
+      <c r="AX9" s="32">
         <v>2012</v>
       </c>
-      <c r="AY9" s="22"/>
-      <c r="AZ9" s="22"/>
-      <c r="BA9" s="22"/>
-      <c r="BB9" s="22">
+      <c r="AY9" s="32"/>
+      <c r="AZ9" s="32"/>
+      <c r="BA9" s="32"/>
+      <c r="BB9" s="32">
         <v>2013</v>
       </c>
-      <c r="BC9" s="22"/>
-      <c r="BD9" s="22"/>
-      <c r="BE9" s="22"/>
-      <c r="BF9" s="22">
+      <c r="BC9" s="32"/>
+      <c r="BD9" s="32"/>
+      <c r="BE9" s="32"/>
+      <c r="BF9" s="32">
         <v>2014</v>
       </c>
-      <c r="BG9" s="22"/>
-      <c r="BH9" s="22"/>
-      <c r="BI9" s="22"/>
-      <c r="BJ9" s="22">
+      <c r="BG9" s="32"/>
+      <c r="BH9" s="32"/>
+      <c r="BI9" s="32"/>
+      <c r="BJ9" s="32">
         <v>2015</v>
       </c>
-      <c r="BK9" s="22"/>
-      <c r="BL9" s="22"/>
-      <c r="BM9" s="22"/>
-      <c r="BN9" s="22">
+      <c r="BK9" s="32"/>
+      <c r="BL9" s="32"/>
+      <c r="BM9" s="32"/>
+      <c r="BN9" s="32">
         <v>2016</v>
       </c>
-      <c r="BO9" s="22"/>
-      <c r="BP9" s="22"/>
-      <c r="BQ9" s="22"/>
-      <c r="BR9" s="22">
+      <c r="BO9" s="32"/>
+      <c r="BP9" s="32"/>
+      <c r="BQ9" s="32"/>
+      <c r="BR9" s="32">
         <v>2017</v>
       </c>
-      <c r="BS9" s="22"/>
-      <c r="BT9" s="22"/>
-      <c r="BU9" s="22"/>
-      <c r="BV9" s="22">
+      <c r="BS9" s="32"/>
+      <c r="BT9" s="32"/>
+      <c r="BU9" s="32"/>
+      <c r="BV9" s="32">
         <v>2018</v>
       </c>
-      <c r="BW9" s="22"/>
-      <c r="BX9" s="22"/>
-      <c r="BY9" s="22"/>
-      <c r="BZ9" s="22">
+      <c r="BW9" s="32"/>
+      <c r="BX9" s="32"/>
+      <c r="BY9" s="32"/>
+      <c r="BZ9" s="32">
         <v>2019</v>
       </c>
-      <c r="CA9" s="22"/>
-      <c r="CB9" s="22"/>
-      <c r="CC9" s="22"/>
-      <c r="CD9" s="22">
+      <c r="CA9" s="32"/>
+      <c r="CB9" s="32"/>
+      <c r="CC9" s="32"/>
+      <c r="CD9" s="32">
         <v>2020</v>
       </c>
-      <c r="CE9" s="22"/>
-      <c r="CF9" s="22"/>
-      <c r="CG9" s="22"/>
-      <c r="CH9" s="22">
+      <c r="CE9" s="32"/>
+      <c r="CF9" s="32"/>
+      <c r="CG9" s="32"/>
+      <c r="CH9" s="32">
         <v>2021</v>
       </c>
-      <c r="CI9" s="22"/>
-      <c r="CJ9" s="22"/>
-      <c r="CK9" s="22"/>
-      <c r="CL9" s="22">
+      <c r="CI9" s="32"/>
+      <c r="CJ9" s="32"/>
+      <c r="CK9" s="32"/>
+      <c r="CL9" s="31">
         <v>2022</v>
       </c>
-      <c r="CM9" s="22"/>
-      <c r="CN9" s="22"/>
-      <c r="CO9" s="22"/>
-      <c r="CP9" s="22">
+      <c r="CM9" s="31"/>
+      <c r="CN9" s="31"/>
+      <c r="CO9" s="31"/>
+      <c r="CP9" s="31">
         <v>2023</v>
       </c>
-      <c r="CQ9" s="23"/>
+      <c r="CQ9" s="31"/>
+      <c r="CR9" s="31"/>
     </row>
     <row r="10" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -1151,23 +1164,26 @@
       <c r="CK10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CL10" s="5" t="s">
+      <c r="CL10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CM10" s="5" t="s">
+      <c r="CM10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CN10" s="5" t="s">
+      <c r="CN10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="CO10" s="5" t="s">
+      <c r="CO10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP10" s="5" t="s">
+      <c r="CP10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ10" s="5" t="s">
+      <c r="CQ10" s="13" t="s">
         <v>8</v>
+      </c>
+      <c r="CR10" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1441,25 +1457,27 @@
       <c r="CK12" s="18">
         <v>30220.178862962039</v>
       </c>
-      <c r="CL12" s="18">
+      <c r="CL12" s="23">
         <v>50141.526896531599</v>
       </c>
-      <c r="CM12" s="18">
+      <c r="CM12" s="23">
         <v>33174.177713591889</v>
       </c>
-      <c r="CN12" s="18">
+      <c r="CN12" s="23">
         <v>45433.318337045661</v>
       </c>
-      <c r="CO12" s="18">
+      <c r="CO12" s="23">
         <v>57101.427341662231</v>
       </c>
-      <c r="CP12" s="18">
+      <c r="CP12" s="23">
         <v>90759.354467504862</v>
       </c>
-      <c r="CQ12" s="18">
-        <v>36688.044009385638</v>
-      </c>
-      <c r="CR12" s="8"/>
+      <c r="CQ12" s="23">
+        <v>34722.619909424669</v>
+      </c>
+      <c r="CR12" s="23">
+        <v>54722.458757352855</v>
+      </c>
       <c r="CS12" s="8"/>
       <c r="CT12" s="8"/>
       <c r="CU12" s="8"/>
@@ -1784,25 +1802,27 @@
       <c r="CK13" s="18">
         <v>827.28506832280971</v>
       </c>
-      <c r="CL13" s="18">
+      <c r="CL13" s="23">
         <v>574.23768992813712</v>
       </c>
-      <c r="CM13" s="18">
+      <c r="CM13" s="23">
         <v>434.56660096089865</v>
       </c>
-      <c r="CN13" s="18">
+      <c r="CN13" s="23">
         <v>901.3910259754723</v>
       </c>
-      <c r="CO13" s="18">
+      <c r="CO13" s="23">
         <v>1017.4234524259053</v>
       </c>
-      <c r="CP13" s="18">
+      <c r="CP13" s="23">
         <v>474.27613087101957</v>
       </c>
-      <c r="CQ13" s="18">
-        <v>455.9713996188803</v>
-      </c>
-      <c r="CR13" s="8"/>
+      <c r="CQ13" s="23">
+        <v>470.71334369924239</v>
+      </c>
+      <c r="CR13" s="23">
+        <v>954.34872015458097</v>
+      </c>
       <c r="CS13" s="8"/>
       <c r="CT13" s="8"/>
       <c r="CU13" s="8"/>
@@ -2127,25 +2147,27 @@
       <c r="CK14" s="18">
         <v>13235.535014912855</v>
       </c>
-      <c r="CL14" s="18">
+      <c r="CL14" s="23">
         <v>17456.163863680598</v>
       </c>
-      <c r="CM14" s="18">
+      <c r="CM14" s="23">
         <v>66283.591438967225</v>
       </c>
-      <c r="CN14" s="18">
+      <c r="CN14" s="23">
         <v>105311.49157059008</v>
       </c>
-      <c r="CO14" s="18">
+      <c r="CO14" s="23">
         <v>64203.136054041541</v>
       </c>
-      <c r="CP14" s="18">
+      <c r="CP14" s="23">
         <v>128049.61270907105</v>
       </c>
-      <c r="CQ14" s="18">
+      <c r="CQ14" s="23">
         <v>132330.33872905793</v>
       </c>
-      <c r="CR14" s="8"/>
+      <c r="CR14" s="23">
+        <v>174583.24150521151</v>
+      </c>
       <c r="CS14" s="8"/>
       <c r="CT14" s="8"/>
       <c r="CU14" s="8"/>
@@ -2470,25 +2492,27 @@
       <c r="CK15" s="18">
         <v>4195.2180605646736</v>
       </c>
-      <c r="CL15" s="18">
+      <c r="CL15" s="23">
         <v>3729.5283113630962</v>
       </c>
-      <c r="CM15" s="18">
+      <c r="CM15" s="23">
         <v>4331.5359392082883</v>
       </c>
-      <c r="CN15" s="18">
+      <c r="CN15" s="23">
         <v>4463.2768148689938</v>
       </c>
-      <c r="CO15" s="18">
+      <c r="CO15" s="23">
         <v>4595.0686874499042</v>
       </c>
-      <c r="CP15" s="18">
+      <c r="CP15" s="23">
         <v>4570.1940500558103</v>
       </c>
-      <c r="CQ15" s="18">
-        <v>5219.9633965336925</v>
-      </c>
-      <c r="CR15" s="8"/>
+      <c r="CQ15" s="23">
+        <v>5139.0553496337761</v>
+      </c>
+      <c r="CR15" s="23">
+        <v>5303.5480278897912</v>
+      </c>
       <c r="CS15" s="8"/>
       <c r="CT15" s="8"/>
       <c r="CU15" s="8"/>
@@ -2813,25 +2837,27 @@
       <c r="CK16" s="18">
         <v>71751.796558186717</v>
       </c>
-      <c r="CL16" s="18">
+      <c r="CL16" s="23">
         <v>119217.8979954884</v>
       </c>
-      <c r="CM16" s="18">
+      <c r="CM16" s="23">
         <v>118035.67759448505</v>
       </c>
-      <c r="CN16" s="18">
+      <c r="CN16" s="23">
         <v>85298.716941900639</v>
       </c>
-      <c r="CO16" s="18">
+      <c r="CO16" s="23">
         <v>88349.252531254111</v>
       </c>
-      <c r="CP16" s="18">
+      <c r="CP16" s="23">
         <v>135502.32232032763</v>
       </c>
-      <c r="CQ16" s="18">
-        <v>128987.3449783593</v>
-      </c>
-      <c r="CR16" s="8"/>
+      <c r="CQ16" s="23">
+        <v>132006.04495852461</v>
+      </c>
+      <c r="CR16" s="23">
+        <v>90807.764514924245</v>
+      </c>
       <c r="CS16" s="8"/>
       <c r="CT16" s="8"/>
       <c r="CU16" s="8"/>
@@ -3156,25 +3182,27 @@
       <c r="CK17" s="18">
         <v>292354.81528290245</v>
       </c>
-      <c r="CL17" s="18">
+      <c r="CL17" s="23">
         <v>407354.16197559203</v>
       </c>
-      <c r="CM17" s="18">
+      <c r="CM17" s="23">
         <v>417649.08107765322</v>
       </c>
-      <c r="CN17" s="18">
+      <c r="CN17" s="23">
         <v>328602.19931776245</v>
       </c>
-      <c r="CO17" s="18">
+      <c r="CO17" s="23">
         <v>330617.25478872925</v>
       </c>
-      <c r="CP17" s="18">
+      <c r="CP17" s="23">
         <v>438458.15859506308</v>
       </c>
-      <c r="CQ17" s="18">
-        <v>441409.99578828533</v>
-      </c>
-      <c r="CR17" s="8"/>
+      <c r="CQ17" s="23">
+        <v>442320.61266757827</v>
+      </c>
+      <c r="CR17" s="23">
+        <v>339614.21704754344</v>
+      </c>
       <c r="CS17" s="8"/>
       <c r="CT17" s="8"/>
       <c r="CU17" s="8"/>
@@ -3499,25 +3527,27 @@
       <c r="CK18" s="18">
         <v>55767.085148338512</v>
       </c>
-      <c r="CL18" s="18">
+      <c r="CL18" s="23">
         <v>86134.983310187468</v>
       </c>
-      <c r="CM18" s="18">
+      <c r="CM18" s="23">
         <v>79391.782907497327</v>
       </c>
-      <c r="CN18" s="18">
+      <c r="CN18" s="23">
         <v>58500.276885178675</v>
       </c>
-      <c r="CO18" s="18">
+      <c r="CO18" s="23">
         <v>67519.422955250629</v>
       </c>
-      <c r="CP18" s="18">
+      <c r="CP18" s="23">
         <v>67323.097737259697</v>
       </c>
-      <c r="CQ18" s="18">
-        <v>72565.429562570003</v>
-      </c>
-      <c r="CR18" s="8"/>
+      <c r="CQ18" s="23">
+        <v>78879.443606324872</v>
+      </c>
+      <c r="CR18" s="23">
+        <v>63688.062502897381</v>
+      </c>
       <c r="CS18" s="8"/>
       <c r="CT18" s="8"/>
       <c r="CU18" s="8"/>
@@ -3842,25 +3872,27 @@
       <c r="CK19" s="18">
         <v>7425.0266070361704</v>
       </c>
-      <c r="CL19" s="18">
+      <c r="CL19" s="23">
         <v>6985.328235938412</v>
       </c>
-      <c r="CM19" s="18">
+      <c r="CM19" s="23">
         <v>9386.617492368041</v>
       </c>
-      <c r="CN19" s="18">
+      <c r="CN19" s="23">
         <v>9326.1589327401853</v>
       </c>
-      <c r="CO19" s="18">
+      <c r="CO19" s="23">
         <v>11124.599699881461</v>
       </c>
-      <c r="CP19" s="18">
+      <c r="CP19" s="23">
         <v>8730.0729440266932</v>
       </c>
-      <c r="CQ19" s="18">
-        <v>14091.47674314199</v>
-      </c>
-      <c r="CR19" s="8"/>
+      <c r="CQ19" s="23">
+        <v>10916.291705433185</v>
+      </c>
+      <c r="CR19" s="23">
+        <v>8832.2082543798206</v>
+      </c>
       <c r="CS19" s="8"/>
       <c r="CT19" s="8"/>
       <c r="CU19" s="8"/>
@@ -4006,13 +4038,13 @@
       <c r="CI20" s="8"/>
       <c r="CJ20" s="8"/>
       <c r="CK20" s="8"/>
-      <c r="CL20" s="8"/>
-      <c r="CM20" s="8"/>
-      <c r="CN20" s="8"/>
-      <c r="CO20" s="8"/>
-      <c r="CP20" s="8"/>
-      <c r="CQ20" s="8"/>
-      <c r="CR20" s="8"/>
+      <c r="CL20" s="24"/>
+      <c r="CM20" s="24"/>
+      <c r="CN20" s="24"/>
+      <c r="CO20" s="24"/>
+      <c r="CP20" s="24"/>
+      <c r="CQ20" s="24"/>
+      <c r="CR20" s="24"/>
       <c r="CS20" s="8"/>
       <c r="CT20" s="8"/>
       <c r="CU20" s="8"/>
@@ -4337,25 +4369,27 @@
       <c r="CK21" s="19">
         <v>475776.94060322625</v>
       </c>
-      <c r="CL21" s="19">
+      <c r="CL21" s="25">
         <v>691593.82827870979</v>
       </c>
-      <c r="CM21" s="19">
+      <c r="CM21" s="25">
         <v>728687.03076473204</v>
       </c>
-      <c r="CN21" s="19">
+      <c r="CN21" s="25">
         <v>637836.8298260622</v>
       </c>
-      <c r="CO21" s="19">
+      <c r="CO21" s="25">
         <v>624527.585510695</v>
       </c>
-      <c r="CP21" s="19">
+      <c r="CP21" s="25">
         <v>873867.08895417978</v>
       </c>
-      <c r="CQ21" s="19">
-        <v>831748.56460695283</v>
-      </c>
-      <c r="CR21" s="8"/>
+      <c r="CQ21" s="25">
+        <v>836785.12026967644</v>
+      </c>
+      <c r="CR21" s="25">
+        <v>738505.84933035367</v>
+      </c>
       <c r="CS21" s="8"/>
       <c r="CT21" s="8"/>
       <c r="CU21" s="8"/>
@@ -4502,12 +4536,13 @@
       <c r="CI22" s="11"/>
       <c r="CJ22" s="11"/>
       <c r="CK22" s="11"/>
-      <c r="CL22" s="11"/>
-      <c r="CM22" s="11"/>
-      <c r="CN22" s="11"/>
-      <c r="CO22" s="11"/>
-      <c r="CP22" s="11"/>
-      <c r="CQ22" s="11"/>
+      <c r="CL22" s="26"/>
+      <c r="CM22" s="26"/>
+      <c r="CN22" s="26"/>
+      <c r="CO22" s="26"/>
+      <c r="CP22" s="26"/>
+      <c r="CQ22" s="26"/>
+      <c r="CR22" s="26"/>
     </row>
     <row r="23" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
@@ -4603,13 +4638,13 @@
       <c r="CI24" s="8"/>
       <c r="CJ24" s="8"/>
       <c r="CK24" s="8"/>
-      <c r="CL24" s="8"/>
-      <c r="CM24" s="8"/>
-      <c r="CN24" s="8"/>
-      <c r="CO24" s="8"/>
-      <c r="CP24" s="8"/>
-      <c r="CQ24" s="8"/>
-      <c r="CR24" s="8"/>
+      <c r="CL24" s="24"/>
+      <c r="CM24" s="24"/>
+      <c r="CN24" s="24"/>
+      <c r="CO24" s="24"/>
+      <c r="CP24" s="24"/>
+      <c r="CQ24" s="24"/>
+      <c r="CR24" s="24"/>
       <c r="CS24" s="8"/>
       <c r="CT24" s="8"/>
       <c r="CU24" s="8"/>
@@ -4755,13 +4790,13 @@
       <c r="CI25" s="8"/>
       <c r="CJ25" s="8"/>
       <c r="CK25" s="8"/>
-      <c r="CL25" s="8"/>
-      <c r="CM25" s="8"/>
-      <c r="CN25" s="8"/>
-      <c r="CO25" s="8"/>
-      <c r="CP25" s="8"/>
-      <c r="CQ25" s="8"/>
-      <c r="CR25" s="8"/>
+      <c r="CL25" s="24"/>
+      <c r="CM25" s="24"/>
+      <c r="CN25" s="24"/>
+      <c r="CO25" s="24"/>
+      <c r="CP25" s="24"/>
+      <c r="CQ25" s="24"/>
+      <c r="CR25" s="24"/>
       <c r="CS25" s="8"/>
       <c r="CT25" s="8"/>
       <c r="CU25" s="8"/>
@@ -4850,148 +4885,149 @@
     </row>
     <row r="34" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-      <c r="B34" s="21">
+      <c r="B34" s="31">
         <v>2000</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31">
         <v>2001</v>
       </c>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21">
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31">
         <v>2002</v>
       </c>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21">
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31">
         <v>2003</v>
       </c>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21">
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31">
         <v>2004</v>
       </c>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-      <c r="V34" s="21">
+      <c r="S34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="31"/>
+      <c r="V34" s="31">
         <v>2005</v>
       </c>
-      <c r="W34" s="21"/>
-      <c r="X34" s="21"/>
-      <c r="Y34" s="21"/>
-      <c r="Z34" s="21">
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="31"/>
+      <c r="Z34" s="31">
         <v>2006</v>
       </c>
-      <c r="AA34" s="21"/>
-      <c r="AB34" s="21"/>
-      <c r="AC34" s="21"/>
-      <c r="AD34" s="21">
+      <c r="AA34" s="31"/>
+      <c r="AB34" s="31"/>
+      <c r="AC34" s="31"/>
+      <c r="AD34" s="31">
         <v>2007</v>
       </c>
-      <c r="AE34" s="21"/>
-      <c r="AF34" s="21"/>
-      <c r="AG34" s="21"/>
-      <c r="AH34" s="21">
+      <c r="AE34" s="31"/>
+      <c r="AF34" s="31"/>
+      <c r="AG34" s="31"/>
+      <c r="AH34" s="31">
         <v>2008</v>
       </c>
-      <c r="AI34" s="21"/>
-      <c r="AJ34" s="21"/>
-      <c r="AK34" s="21"/>
-      <c r="AL34" s="21">
+      <c r="AI34" s="31"/>
+      <c r="AJ34" s="31"/>
+      <c r="AK34" s="31"/>
+      <c r="AL34" s="31">
         <v>2009</v>
       </c>
-      <c r="AM34" s="21"/>
-      <c r="AN34" s="21"/>
-      <c r="AO34" s="21"/>
-      <c r="AP34" s="21">
+      <c r="AM34" s="31"/>
+      <c r="AN34" s="31"/>
+      <c r="AO34" s="31"/>
+      <c r="AP34" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ34" s="21"/>
-      <c r="AR34" s="21"/>
-      <c r="AS34" s="21"/>
-      <c r="AT34" s="21">
+      <c r="AQ34" s="31"/>
+      <c r="AR34" s="31"/>
+      <c r="AS34" s="31"/>
+      <c r="AT34" s="31">
         <v>2011</v>
       </c>
-      <c r="AU34" s="21"/>
-      <c r="AV34" s="21"/>
-      <c r="AW34" s="21"/>
-      <c r="AX34" s="21">
+      <c r="AU34" s="31"/>
+      <c r="AV34" s="31"/>
+      <c r="AW34" s="31"/>
+      <c r="AX34" s="31">
         <v>2012</v>
       </c>
-      <c r="AY34" s="21"/>
-      <c r="AZ34" s="21"/>
-      <c r="BA34" s="21"/>
-      <c r="BB34" s="21">
+      <c r="AY34" s="31"/>
+      <c r="AZ34" s="31"/>
+      <c r="BA34" s="31"/>
+      <c r="BB34" s="31">
         <v>2013</v>
       </c>
-      <c r="BC34" s="21"/>
-      <c r="BD34" s="21"/>
-      <c r="BE34" s="21"/>
-      <c r="BF34" s="21">
+      <c r="BC34" s="31"/>
+      <c r="BD34" s="31"/>
+      <c r="BE34" s="31"/>
+      <c r="BF34" s="31">
         <v>2014</v>
       </c>
-      <c r="BG34" s="21"/>
-      <c r="BH34" s="21"/>
-      <c r="BI34" s="21"/>
-      <c r="BJ34" s="21">
+      <c r="BG34" s="31"/>
+      <c r="BH34" s="31"/>
+      <c r="BI34" s="31"/>
+      <c r="BJ34" s="31">
         <v>2015</v>
       </c>
-      <c r="BK34" s="21"/>
-      <c r="BL34" s="21"/>
-      <c r="BM34" s="21"/>
-      <c r="BN34" s="21">
+      <c r="BK34" s="31"/>
+      <c r="BL34" s="31"/>
+      <c r="BM34" s="31"/>
+      <c r="BN34" s="31">
         <v>2016</v>
       </c>
-      <c r="BO34" s="21"/>
-      <c r="BP34" s="21"/>
-      <c r="BQ34" s="21"/>
-      <c r="BR34" s="21">
+      <c r="BO34" s="31"/>
+      <c r="BP34" s="31"/>
+      <c r="BQ34" s="31"/>
+      <c r="BR34" s="31">
         <v>2017</v>
       </c>
-      <c r="BS34" s="21"/>
-      <c r="BT34" s="21"/>
-      <c r="BU34" s="21"/>
-      <c r="BV34" s="21">
+      <c r="BS34" s="31"/>
+      <c r="BT34" s="31"/>
+      <c r="BU34" s="31"/>
+      <c r="BV34" s="31">
         <v>2018</v>
       </c>
-      <c r="BW34" s="21"/>
-      <c r="BX34" s="21"/>
-      <c r="BY34" s="21"/>
-      <c r="BZ34" s="21">
+      <c r="BW34" s="31"/>
+      <c r="BX34" s="31"/>
+      <c r="BY34" s="31"/>
+      <c r="BZ34" s="31">
         <v>2019</v>
       </c>
-      <c r="CA34" s="21"/>
-      <c r="CB34" s="21"/>
-      <c r="CC34" s="21"/>
-      <c r="CD34" s="22">
+      <c r="CA34" s="31"/>
+      <c r="CB34" s="31"/>
+      <c r="CC34" s="31"/>
+      <c r="CD34" s="32">
         <v>2020</v>
       </c>
-      <c r="CE34" s="22"/>
-      <c r="CF34" s="22"/>
-      <c r="CG34" s="22"/>
-      <c r="CH34" s="22">
+      <c r="CE34" s="32"/>
+      <c r="CF34" s="32"/>
+      <c r="CG34" s="32"/>
+      <c r="CH34" s="32">
         <v>2021</v>
       </c>
-      <c r="CI34" s="22"/>
-      <c r="CJ34" s="22"/>
-      <c r="CK34" s="22"/>
-      <c r="CL34" s="22">
+      <c r="CI34" s="32"/>
+      <c r="CJ34" s="32"/>
+      <c r="CK34" s="32"/>
+      <c r="CL34" s="31">
         <v>2022</v>
       </c>
-      <c r="CM34" s="22"/>
-      <c r="CN34" s="22"/>
-      <c r="CO34" s="22"/>
-      <c r="CP34" s="22">
+      <c r="CM34" s="31"/>
+      <c r="CN34" s="31"/>
+      <c r="CO34" s="31"/>
+      <c r="CP34" s="31">
         <v>2023</v>
       </c>
-      <c r="CQ34" s="23"/>
+      <c r="CQ34" s="31"/>
+      <c r="CR34" s="31"/>
     </row>
     <row r="35" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
@@ -5259,23 +5295,26 @@
       <c r="CK35" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CL35" s="13" t="s">
+      <c r="CL35" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CM35" s="13" t="s">
+      <c r="CM35" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="CN35" s="13" t="s">
+      <c r="CN35" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="CO35" s="13" t="s">
+      <c r="CO35" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="CP35" s="13" t="s">
+      <c r="CP35" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CQ35" s="13" t="s">
+      <c r="CQ35" s="27" t="s">
         <v>8</v>
+      </c>
+      <c r="CR35" s="27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -5549,25 +5588,27 @@
       <c r="CK37" s="18">
         <v>25473.984362080206</v>
       </c>
-      <c r="CL37" s="18">
+      <c r="CL37" s="23">
         <v>39764.430508135309</v>
       </c>
-      <c r="CM37" s="18">
+      <c r="CM37" s="23">
         <v>26620.30384489982</v>
       </c>
-      <c r="CN37" s="18">
+      <c r="CN37" s="23">
         <v>35357.329087856539</v>
       </c>
-      <c r="CO37" s="18">
+      <c r="CO37" s="23">
         <v>42923.047723132688</v>
       </c>
-      <c r="CP37" s="18">
+      <c r="CP37" s="23">
         <v>66380.3538554962</v>
       </c>
-      <c r="CQ37" s="18">
-        <v>25899.265033307081</v>
-      </c>
-      <c r="CR37" s="8"/>
+      <c r="CQ37" s="23">
+        <v>24511.809227412497</v>
+      </c>
+      <c r="CR37" s="23">
+        <v>42003.108653506613</v>
+      </c>
       <c r="CS37" s="8"/>
       <c r="CT37" s="8"/>
       <c r="CU37" s="8"/>
@@ -5892,25 +5933,27 @@
       <c r="CK38" s="18">
         <v>770.19546330619676</v>
       </c>
-      <c r="CL38" s="18">
+      <c r="CL38" s="23">
         <v>513.260353030533</v>
       </c>
-      <c r="CM38" s="18">
+      <c r="CM38" s="23">
         <v>382.06821091022977</v>
       </c>
-      <c r="CN38" s="18">
+      <c r="CN38" s="23">
         <v>776.70768745237024</v>
       </c>
-      <c r="CO38" s="18">
+      <c r="CO38" s="23">
         <v>889.21572221660801</v>
       </c>
-      <c r="CP38" s="18">
+      <c r="CP38" s="23">
         <v>396.58022379505599</v>
       </c>
-      <c r="CQ38" s="18">
-        <v>382.30657292821888</v>
-      </c>
-      <c r="CR38" s="8"/>
+      <c r="CQ38" s="23">
+        <v>394.66687035997319</v>
+      </c>
+      <c r="CR38" s="23">
+        <v>795.16883248606666</v>
+      </c>
       <c r="CS38" s="8"/>
       <c r="CT38" s="8"/>
       <c r="CU38" s="8"/>
@@ -6235,25 +6278,27 @@
       <c r="CK39" s="18">
         <v>12202.689945533572</v>
       </c>
-      <c r="CL39" s="18">
+      <c r="CL39" s="23">
         <v>15389.064093647212</v>
       </c>
-      <c r="CM39" s="18">
+      <c r="CM39" s="23">
         <v>57321.791102132127</v>
       </c>
-      <c r="CN39" s="18">
+      <c r="CN39" s="23">
         <v>88956.594041921373</v>
       </c>
-      <c r="CO39" s="18">
+      <c r="CO39" s="23">
         <v>54857.258251901527</v>
       </c>
-      <c r="CP39" s="18">
+      <c r="CP39" s="23">
         <v>104952.98838100983</v>
       </c>
-      <c r="CQ39" s="18">
+      <c r="CQ39" s="23">
         <v>107908.32982931691</v>
       </c>
-      <c r="CR39" s="8"/>
+      <c r="CR39" s="23">
+        <v>139971.22516500723</v>
+      </c>
       <c r="CS39" s="8"/>
       <c r="CT39" s="8"/>
       <c r="CU39" s="8"/>
@@ -6578,25 +6623,27 @@
       <c r="CK40" s="18">
         <v>3847.7974661865246</v>
       </c>
-      <c r="CL40" s="18">
+      <c r="CL40" s="23">
         <v>3434.5919735030589</v>
       </c>
-      <c r="CM40" s="18">
+      <c r="CM40" s="23">
         <v>3938.4675463402086</v>
       </c>
-      <c r="CN40" s="18">
+      <c r="CN40" s="23">
         <v>3966.0472849247194</v>
       </c>
-      <c r="CO40" s="18">
+      <c r="CO40" s="23">
         <v>3977.1461621146914</v>
       </c>
-      <c r="CP40" s="18">
+      <c r="CP40" s="23">
         <v>3948.5227029077737</v>
       </c>
-      <c r="CQ40" s="18">
-        <v>4480.5580480484614</v>
-      </c>
-      <c r="CR40" s="8"/>
+      <c r="CQ40" s="23">
+        <v>4411.1105877597502</v>
+      </c>
+      <c r="CR40" s="23">
+        <v>4489.0256045275964</v>
+      </c>
       <c r="CS40" s="8"/>
       <c r="CT40" s="8"/>
       <c r="CU40" s="8"/>
@@ -6921,25 +6968,27 @@
       <c r="CK41" s="18">
         <v>72338.577129792466</v>
       </c>
-      <c r="CL41" s="18">
+      <c r="CL41" s="23">
         <v>116677.43002870887</v>
       </c>
-      <c r="CM41" s="18">
+      <c r="CM41" s="23">
         <v>114398.77827366724</v>
       </c>
-      <c r="CN41" s="18">
+      <c r="CN41" s="23">
         <v>83482.535941170252</v>
       </c>
-      <c r="CO41" s="18">
+      <c r="CO41" s="23">
         <v>85486.339096444455</v>
       </c>
-      <c r="CP41" s="18">
+      <c r="CP41" s="23">
         <v>131657.7994655674</v>
       </c>
-      <c r="CQ41" s="18">
-        <v>124483.47918496309</v>
-      </c>
-      <c r="CR41" s="8"/>
+      <c r="CQ41" s="23">
+        <v>127397.97452047074</v>
+      </c>
+      <c r="CR41" s="23">
+        <v>88544.277655303624</v>
+      </c>
       <c r="CS41" s="8"/>
       <c r="CT41" s="8"/>
       <c r="CU41" s="8"/>
@@ -7264,25 +7313,27 @@
       <c r="CK42" s="18">
         <v>267343.98843610822</v>
       </c>
-      <c r="CL42" s="18">
+      <c r="CL42" s="23">
         <v>357362.75456158456</v>
       </c>
-      <c r="CM42" s="18">
+      <c r="CM42" s="23">
         <v>362411.57167247194</v>
       </c>
-      <c r="CN42" s="18">
+      <c r="CN42" s="23">
         <v>282000.18209253578</v>
       </c>
-      <c r="CO42" s="18">
+      <c r="CO42" s="23">
         <v>282568.33591674821</v>
       </c>
-      <c r="CP42" s="18">
+      <c r="CP42" s="23">
         <v>369595.05173715425</v>
       </c>
-      <c r="CQ42" s="18">
-        <v>369271.05106020212</v>
-      </c>
-      <c r="CR42" s="8"/>
+      <c r="CQ42" s="23">
+        <v>370084.79216041439</v>
+      </c>
+      <c r="CR42" s="23">
+        <v>281734.9483746647</v>
+      </c>
       <c r="CS42" s="8"/>
       <c r="CT42" s="8"/>
       <c r="CU42" s="8"/>
@@ -7607,25 +7658,27 @@
       <c r="CK43" s="18">
         <v>52037.635302078721</v>
       </c>
-      <c r="CL43" s="18">
+      <c r="CL43" s="23">
         <v>76295.067345606396</v>
       </c>
-      <c r="CM43" s="18">
+      <c r="CM43" s="23">
         <v>69855.480841691693</v>
       </c>
-      <c r="CN43" s="18">
+      <c r="CN43" s="23">
         <v>48935.143393238061</v>
       </c>
-      <c r="CO43" s="18">
+      <c r="CO43" s="23">
         <v>57321.148454949551</v>
       </c>
-      <c r="CP43" s="18">
+      <c r="CP43" s="23">
         <v>55787.222374251556</v>
       </c>
-      <c r="CQ43" s="18">
-        <v>60889.765891529736</v>
-      </c>
-      <c r="CR43" s="8"/>
+      <c r="CQ43" s="23">
+        <v>66187.864990199887</v>
+      </c>
+      <c r="CR43" s="23">
+        <v>51514.425499060904</v>
+      </c>
       <c r="CS43" s="8"/>
       <c r="CT43" s="8"/>
       <c r="CU43" s="8"/>
@@ -7950,25 +8003,27 @@
       <c r="CK44" s="18">
         <v>6921.6089579479312</v>
       </c>
-      <c r="CL44" s="18">
+      <c r="CL44" s="23">
         <v>6236.6807855633124</v>
       </c>
-      <c r="CM44" s="18">
+      <c r="CM44" s="23">
         <v>8296.7941167833451</v>
       </c>
-      <c r="CN44" s="18">
+      <c r="CN44" s="23">
         <v>8381.4864233369353</v>
       </c>
-      <c r="CO44" s="18">
+      <c r="CO44" s="23">
         <v>9735.3833275709912</v>
       </c>
-      <c r="CP44" s="18">
+      <c r="CP44" s="23">
         <v>7291.860155735676</v>
       </c>
-      <c r="CQ44" s="18">
-        <v>11878.108919901721</v>
-      </c>
-      <c r="CR44" s="8"/>
+      <c r="CQ44" s="23">
+        <v>9201.6546059773391</v>
+      </c>
+      <c r="CR44" s="23">
+        <v>7593.185856089387</v>
+      </c>
       <c r="CS44" s="8"/>
       <c r="CT44" s="8"/>
       <c r="CU44" s="8"/>
@@ -8114,13 +8169,13 @@
       <c r="CI45" s="8"/>
       <c r="CJ45" s="8"/>
       <c r="CK45" s="8"/>
-      <c r="CL45" s="8"/>
-      <c r="CM45" s="8"/>
-      <c r="CN45" s="8"/>
-      <c r="CO45" s="8"/>
-      <c r="CP45" s="8"/>
-      <c r="CQ45" s="8"/>
-      <c r="CR45" s="8"/>
+      <c r="CL45" s="24"/>
+      <c r="CM45" s="24"/>
+      <c r="CN45" s="24"/>
+      <c r="CO45" s="24"/>
+      <c r="CP45" s="24"/>
+      <c r="CQ45" s="24"/>
+      <c r="CR45" s="24"/>
       <c r="CS45" s="8"/>
       <c r="CT45" s="8"/>
       <c r="CU45" s="8"/>
@@ -8445,25 +8500,27 @@
       <c r="CK46" s="19">
         <v>440936.47706303385</v>
       </c>
-      <c r="CL46" s="19">
+      <c r="CL46" s="25">
         <v>615673.2796497792</v>
       </c>
-      <c r="CM46" s="19">
+      <c r="CM46" s="25">
         <v>643225.25560889661</v>
       </c>
-      <c r="CN46" s="19">
+      <c r="CN46" s="25">
         <v>551856.02595243603</v>
       </c>
-      <c r="CO46" s="19">
+      <c r="CO46" s="25">
         <v>537757.87465507863</v>
       </c>
-      <c r="CP46" s="19">
+      <c r="CP46" s="25">
         <v>740010.37889591767</v>
       </c>
-      <c r="CQ46" s="19">
-        <v>705192.86454019742</v>
-      </c>
-      <c r="CR46" s="8"/>
+      <c r="CQ46" s="25">
+        <v>710098.20279191155</v>
+      </c>
+      <c r="CR46" s="25">
+        <v>616645.36564064596</v>
+      </c>
       <c r="CS46" s="8"/>
       <c r="CT46" s="8"/>
       <c r="CU46" s="8"/>
@@ -8610,12 +8667,13 @@
       <c r="CI47" s="11"/>
       <c r="CJ47" s="11"/>
       <c r="CK47" s="11"/>
-      <c r="CL47" s="11"/>
-      <c r="CM47" s="11"/>
-      <c r="CN47" s="11"/>
-      <c r="CO47" s="11"/>
-      <c r="CP47" s="11"/>
-      <c r="CQ47" s="11"/>
+      <c r="CL47" s="26"/>
+      <c r="CM47" s="26"/>
+      <c r="CN47" s="26"/>
+      <c r="CO47" s="26"/>
+      <c r="CP47" s="26"/>
+      <c r="CQ47" s="26"/>
+      <c r="CR47" s="26"/>
     </row>
     <row r="48" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
@@ -8711,13 +8769,13 @@
       <c r="CI49" s="8"/>
       <c r="CJ49" s="8"/>
       <c r="CK49" s="8"/>
-      <c r="CL49" s="8"/>
-      <c r="CM49" s="8"/>
-      <c r="CN49" s="8"/>
-      <c r="CO49" s="8"/>
-      <c r="CP49" s="8"/>
-      <c r="CQ49" s="8"/>
-      <c r="CR49" s="8"/>
+      <c r="CL49" s="24"/>
+      <c r="CM49" s="24"/>
+      <c r="CN49" s="24"/>
+      <c r="CO49" s="24"/>
+      <c r="CP49" s="24"/>
+      <c r="CQ49" s="24"/>
+      <c r="CR49" s="24"/>
       <c r="CS49" s="8"/>
       <c r="CT49" s="8"/>
       <c r="CU49" s="8"/>
@@ -8863,13 +8921,13 @@
       <c r="CI50" s="8"/>
       <c r="CJ50" s="8"/>
       <c r="CK50" s="8"/>
-      <c r="CL50" s="8"/>
-      <c r="CM50" s="8"/>
-      <c r="CN50" s="8"/>
-      <c r="CO50" s="8"/>
-      <c r="CP50" s="8"/>
-      <c r="CQ50" s="8"/>
-      <c r="CR50" s="8"/>
+      <c r="CL50" s="24"/>
+      <c r="CM50" s="24"/>
+      <c r="CN50" s="24"/>
+      <c r="CO50" s="24"/>
+      <c r="CP50" s="24"/>
+      <c r="CQ50" s="24"/>
+      <c r="CR50" s="24"/>
       <c r="CS50" s="8"/>
       <c r="CT50" s="8"/>
       <c r="CU50" s="8"/>
@@ -8958,148 +9016,147 @@
     </row>
     <row r="59" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22" t="s">
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22" t="s">
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="22" t="s">
+      <c r="K59" s="32"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+      <c r="N59" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22" t="s">
+      <c r="O59" s="32"/>
+      <c r="P59" s="32"/>
+      <c r="Q59" s="32"/>
+      <c r="R59" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="S59" s="22"/>
-      <c r="T59" s="22"/>
-      <c r="U59" s="22"/>
-      <c r="V59" s="22" t="s">
+      <c r="S59" s="32"/>
+      <c r="T59" s="32"/>
+      <c r="U59" s="32"/>
+      <c r="V59" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="W59" s="22"/>
-      <c r="X59" s="22"/>
-      <c r="Y59" s="22"/>
-      <c r="Z59" s="22" t="s">
+      <c r="W59" s="32"/>
+      <c r="X59" s="32"/>
+      <c r="Y59" s="32"/>
+      <c r="Z59" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AA59" s="22"/>
-      <c r="AB59" s="22"/>
-      <c r="AC59" s="22"/>
-      <c r="AD59" s="22" t="s">
+      <c r="AA59" s="32"/>
+      <c r="AB59" s="32"/>
+      <c r="AC59" s="32"/>
+      <c r="AD59" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="AE59" s="22"/>
-      <c r="AF59" s="22"/>
-      <c r="AG59" s="22"/>
-      <c r="AH59" s="22" t="s">
+      <c r="AE59" s="32"/>
+      <c r="AF59" s="32"/>
+      <c r="AG59" s="32"/>
+      <c r="AH59" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="AI59" s="22"/>
-      <c r="AJ59" s="22"/>
-      <c r="AK59" s="22"/>
-      <c r="AL59" s="22" t="s">
+      <c r="AI59" s="32"/>
+      <c r="AJ59" s="32"/>
+      <c r="AK59" s="32"/>
+      <c r="AL59" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="AM59" s="22"/>
-      <c r="AN59" s="22"/>
-      <c r="AO59" s="22"/>
-      <c r="AP59" s="22" t="s">
+      <c r="AM59" s="32"/>
+      <c r="AN59" s="32"/>
+      <c r="AO59" s="32"/>
+      <c r="AP59" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="AQ59" s="22"/>
-      <c r="AR59" s="22"/>
-      <c r="AS59" s="22"/>
-      <c r="AT59" s="22" t="s">
+      <c r="AQ59" s="32"/>
+      <c r="AR59" s="32"/>
+      <c r="AS59" s="32"/>
+      <c r="AT59" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="AU59" s="22"/>
-      <c r="AV59" s="22"/>
-      <c r="AW59" s="22"/>
-      <c r="AX59" s="22" t="s">
+      <c r="AU59" s="32"/>
+      <c r="AV59" s="32"/>
+      <c r="AW59" s="32"/>
+      <c r="AX59" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AY59" s="22"/>
-      <c r="AZ59" s="22"/>
-      <c r="BA59" s="22"/>
-      <c r="BB59" s="22" t="s">
+      <c r="AY59" s="32"/>
+      <c r="AZ59" s="32"/>
+      <c r="BA59" s="32"/>
+      <c r="BB59" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="BC59" s="22"/>
-      <c r="BD59" s="22"/>
-      <c r="BE59" s="22"/>
-      <c r="BF59" s="22" t="s">
+      <c r="BC59" s="32"/>
+      <c r="BD59" s="32"/>
+      <c r="BE59" s="32"/>
+      <c r="BF59" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="BG59" s="22"/>
-      <c r="BH59" s="22"/>
-      <c r="BI59" s="22"/>
-      <c r="BJ59" s="22" t="s">
+      <c r="BG59" s="32"/>
+      <c r="BH59" s="32"/>
+      <c r="BI59" s="32"/>
+      <c r="BJ59" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="BK59" s="22"/>
-      <c r="BL59" s="22"/>
-      <c r="BM59" s="22"/>
-      <c r="BN59" s="22" t="s">
+      <c r="BK59" s="32"/>
+      <c r="BL59" s="32"/>
+      <c r="BM59" s="32"/>
+      <c r="BN59" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="BO59" s="22"/>
-      <c r="BP59" s="22"/>
-      <c r="BQ59" s="22"/>
-      <c r="BR59" s="22" t="s">
+      <c r="BO59" s="32"/>
+      <c r="BP59" s="32"/>
+      <c r="BQ59" s="32"/>
+      <c r="BR59" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="BS59" s="22"/>
-      <c r="BT59" s="22"/>
-      <c r="BU59" s="22"/>
-      <c r="BV59" s="22" t="s">
+      <c r="BS59" s="32"/>
+      <c r="BT59" s="32"/>
+      <c r="BU59" s="32"/>
+      <c r="BV59" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="BW59" s="22"/>
-      <c r="BX59" s="22"/>
-      <c r="BY59" s="22"/>
-      <c r="BZ59" s="22" t="s">
+      <c r="BW59" s="32"/>
+      <c r="BX59" s="32"/>
+      <c r="BY59" s="32"/>
+      <c r="BZ59" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="CA59" s="22"/>
-      <c r="CB59" s="22"/>
-      <c r="CC59" s="22"/>
-      <c r="CD59" s="22" t="s">
+      <c r="CA59" s="32"/>
+      <c r="CB59" s="32"/>
+      <c r="CC59" s="32"/>
+      <c r="CD59" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="CE59" s="22"/>
-      <c r="CF59" s="22"/>
-      <c r="CG59" s="22"/>
-      <c r="CH59" s="22" t="s">
+      <c r="CE59" s="32"/>
+      <c r="CF59" s="32"/>
+      <c r="CG59" s="32"/>
+      <c r="CH59" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="CI59" s="22"/>
-      <c r="CJ59" s="22"/>
-      <c r="CK59" s="22"/>
-      <c r="CL59" s="22" t="s">
+      <c r="CI59" s="32"/>
+      <c r="CJ59" s="32"/>
+      <c r="CK59" s="32"/>
+      <c r="CL59" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="CM59" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN59" s="22"/>
-      <c r="CO59" s="22"/>
-      <c r="CP59" s="22"/>
-      <c r="CQ59" s="23"/>
+      <c r="CM59" s="31"/>
+      <c r="CN59" s="31"/>
+      <c r="CO59" s="28"/>
+      <c r="CP59" s="21"/>
+      <c r="CQ59" s="21"/>
+      <c r="CR59" s="21"/>
     </row>
     <row r="60" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
@@ -9367,16 +9424,19 @@
       <c r="CK60" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CL60" s="13" t="s">
+      <c r="CL60" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CM60" s="13" t="s">
+      <c r="CM60" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="CN60" s="13"/>
-      <c r="CO60" s="13"/>
-      <c r="CP60" s="13"/>
-      <c r="CQ60" s="13"/>
+      <c r="CN60" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO60" s="27"/>
+      <c r="CP60" s="27"/>
+      <c r="CQ60" s="27"/>
+      <c r="CR60" s="27"/>
     </row>
     <row r="61" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
@@ -9649,17 +9709,19 @@
       <c r="CK62" s="14">
         <v>88.951321567609739</v>
       </c>
-      <c r="CL62" s="14">
+      <c r="CL62" s="29">
         <v>81.00636355727508</v>
       </c>
-      <c r="CM62" s="14">
-        <v>10.592173003142975</v>
-      </c>
-      <c r="CN62" s="14"/>
-      <c r="CO62" s="14"/>
-      <c r="CP62" s="14"/>
-      <c r="CQ62" s="14"/>
-      <c r="CR62" s="8"/>
+      <c r="CM62" s="29">
+        <v>4.6676128921753701</v>
+      </c>
+      <c r="CN62" s="29">
+        <v>20.445656976661922</v>
+      </c>
+      <c r="CO62" s="29"/>
+      <c r="CP62" s="29"/>
+      <c r="CQ62" s="29"/>
+      <c r="CR62" s="29"/>
       <c r="CS62" s="8"/>
       <c r="CT62" s="8"/>
       <c r="CU62" s="8"/>
@@ -9980,17 +10042,19 @@
       <c r="CK63" s="14">
         <v>22.983417854811677</v>
       </c>
-      <c r="CL63" s="14">
+      <c r="CL63" s="29">
         <v>-17.407697336903681</v>
       </c>
-      <c r="CM63" s="14">
-        <v>4.9255507925947626</v>
-      </c>
-      <c r="CN63" s="14"/>
-      <c r="CO63" s="14"/>
-      <c r="CP63" s="14"/>
-      <c r="CQ63" s="14"/>
-      <c r="CR63" s="8"/>
+      <c r="CM63" s="29">
+        <v>8.3178833022181919</v>
+      </c>
+      <c r="CN63" s="29">
+        <v>5.8751077671090286</v>
+      </c>
+      <c r="CO63" s="29"/>
+      <c r="CP63" s="29"/>
+      <c r="CQ63" s="29"/>
+      <c r="CR63" s="29"/>
       <c r="CS63" s="8"/>
       <c r="CT63" s="8"/>
       <c r="CU63" s="8"/>
@@ -10311,17 +10375,19 @@
       <c r="CK64" s="14">
         <v>385.08153226675034</v>
       </c>
-      <c r="CL64" s="14">
+      <c r="CL64" s="29">
         <v>633.54955710224431</v>
       </c>
-      <c r="CM64" s="14">
+      <c r="CM64" s="29">
         <v>99.642680573374463</v>
       </c>
-      <c r="CN64" s="14"/>
-      <c r="CO64" s="14"/>
-      <c r="CP64" s="14"/>
-      <c r="CQ64" s="14"/>
-      <c r="CR64" s="8"/>
+      <c r="CN64" s="29">
+        <v>65.777959177597154</v>
+      </c>
+      <c r="CO64" s="29"/>
+      <c r="CP64" s="29"/>
+      <c r="CQ64" s="29"/>
+      <c r="CR64" s="29"/>
       <c r="CS64" s="8"/>
       <c r="CT64" s="8"/>
       <c r="CU64" s="8"/>
@@ -10642,17 +10708,19 @@
       <c r="CK65" s="14">
         <v>9.5311047271619174</v>
       </c>
-      <c r="CL65" s="14">
+      <c r="CL65" s="29">
         <v>22.540805927960932</v>
       </c>
-      <c r="CM65" s="14">
-        <v>20.510679578657488</v>
-      </c>
-      <c r="CN65" s="14"/>
-      <c r="CO65" s="14"/>
-      <c r="CP65" s="14"/>
-      <c r="CQ65" s="14"/>
-      <c r="CR65" s="8"/>
+      <c r="CM65" s="29">
+        <v>18.642796037220123</v>
+      </c>
+      <c r="CN65" s="29">
+        <v>18.826329799252221</v>
+      </c>
+      <c r="CO65" s="29"/>
+      <c r="CP65" s="29"/>
+      <c r="CQ65" s="29"/>
+      <c r="CR65" s="29"/>
       <c r="CS65" s="8"/>
       <c r="CT65" s="8"/>
       <c r="CU65" s="8"/>
@@ -10973,17 +11041,19 @@
       <c r="CK66" s="14">
         <v>23.131763620173302</v>
       </c>
-      <c r="CL66" s="14">
+      <c r="CL66" s="29">
         <v>13.659378833751518</v>
       </c>
-      <c r="CM66" s="14">
-        <v>9.2782687464200535</v>
-      </c>
-      <c r="CN66" s="14"/>
-      <c r="CO66" s="14"/>
-      <c r="CP66" s="14"/>
-      <c r="CQ66" s="14"/>
-      <c r="CR66" s="8"/>
+      <c r="CM66" s="29">
+        <v>11.835715818089469</v>
+      </c>
+      <c r="CN66" s="29">
+        <v>6.4585350993919093</v>
+      </c>
+      <c r="CO66" s="29"/>
+      <c r="CP66" s="29"/>
+      <c r="CQ66" s="29"/>
+      <c r="CR66" s="29"/>
       <c r="CS66" s="8"/>
       <c r="CT66" s="8"/>
       <c r="CU66" s="8"/>
@@ -11304,17 +11374,19 @@
       <c r="CK67" s="14">
         <v>13.08767207025528</v>
       </c>
-      <c r="CL67" s="14">
+      <c r="CL67" s="29">
         <v>7.6356152760591556</v>
       </c>
-      <c r="CM67" s="14">
-        <v>5.6892055524993026</v>
-      </c>
-      <c r="CN67" s="14"/>
-      <c r="CO67" s="14"/>
-      <c r="CP67" s="14"/>
-      <c r="CQ67" s="14"/>
-      <c r="CR67" s="8"/>
+      <c r="CM67" s="29">
+        <v>5.9072395242114624</v>
+      </c>
+      <c r="CN67" s="29">
+        <v>3.3511698195094084</v>
+      </c>
+      <c r="CO67" s="29"/>
+      <c r="CP67" s="29"/>
+      <c r="CQ67" s="29"/>
+      <c r="CR67" s="29"/>
       <c r="CS67" s="8"/>
       <c r="CT67" s="8"/>
       <c r="CU67" s="8"/>
@@ -11635,17 +11707,19 @@
       <c r="CK68" s="14">
         <v>21.073968229917895</v>
       </c>
-      <c r="CL68" s="14">
+      <c r="CL68" s="29">
         <v>-21.840006057913556</v>
       </c>
-      <c r="CM68" s="14">
-        <v>-8.5983121866415217</v>
-      </c>
-      <c r="CN68" s="14"/>
-      <c r="CO68" s="14"/>
-      <c r="CP68" s="14"/>
-      <c r="CQ68" s="14"/>
-      <c r="CR68" s="8"/>
+      <c r="CM68" s="29">
+        <v>-0.64533038862397518</v>
+      </c>
+      <c r="CN68" s="29">
+        <v>8.867967630137926</v>
+      </c>
+      <c r="CO68" s="29"/>
+      <c r="CP68" s="29"/>
+      <c r="CQ68" s="29"/>
+      <c r="CR68" s="29"/>
       <c r="CS68" s="8"/>
       <c r="CT68" s="8"/>
       <c r="CU68" s="8"/>
@@ -11966,17 +12040,19 @@
       <c r="CK69" s="14">
         <v>49.825721692895598</v>
       </c>
-      <c r="CL69" s="14">
+      <c r="CL69" s="29">
         <v>24.977275929738639</v>
       </c>
-      <c r="CM69" s="14">
-        <v>50.123052895244939</v>
-      </c>
-      <c r="CN69" s="14"/>
-      <c r="CO69" s="14"/>
-      <c r="CP69" s="14"/>
-      <c r="CQ69" s="14"/>
-      <c r="CR69" s="8"/>
+      <c r="CM69" s="29">
+        <v>16.296330539823018</v>
+      </c>
+      <c r="CN69" s="29">
+        <v>-5.2963999640442978</v>
+      </c>
+      <c r="CO69" s="29"/>
+      <c r="CP69" s="29"/>
+      <c r="CQ69" s="29"/>
+      <c r="CR69" s="29"/>
       <c r="CS69" s="8"/>
       <c r="CT69" s="8"/>
       <c r="CU69" s="8"/>
@@ -12118,13 +12194,13 @@
       <c r="CI70" s="8"/>
       <c r="CJ70" s="8"/>
       <c r="CK70" s="8"/>
-      <c r="CL70" s="8"/>
-      <c r="CM70" s="8"/>
-      <c r="CN70" s="8"/>
-      <c r="CO70" s="8"/>
-      <c r="CP70" s="8"/>
-      <c r="CQ70" s="8"/>
-      <c r="CR70" s="8"/>
+      <c r="CL70" s="24"/>
+      <c r="CM70" s="24"/>
+      <c r="CN70" s="24"/>
+      <c r="CO70" s="24"/>
+      <c r="CP70" s="24"/>
+      <c r="CQ70" s="24"/>
+      <c r="CR70" s="24"/>
       <c r="CS70" s="8"/>
       <c r="CT70" s="8"/>
       <c r="CU70" s="8"/>
@@ -12445,17 +12521,19 @@
       <c r="CK71" s="14">
         <v>31.264786544482661</v>
       </c>
-      <c r="CL71" s="14">
+      <c r="CL71" s="29">
         <v>26.355536041888229</v>
       </c>
-      <c r="CM71" s="14">
-        <v>14.143456585752759</v>
-      </c>
-      <c r="CN71" s="14"/>
-      <c r="CO71" s="14"/>
-      <c r="CP71" s="14"/>
-      <c r="CQ71" s="14"/>
-      <c r="CR71" s="8"/>
+      <c r="CM71" s="29">
+        <v>14.834638869790112</v>
+      </c>
+      <c r="CN71" s="29">
+        <v>15.782879695382874</v>
+      </c>
+      <c r="CO71" s="29"/>
+      <c r="CP71" s="29"/>
+      <c r="CQ71" s="29"/>
+      <c r="CR71" s="29"/>
       <c r="CS71" s="8"/>
       <c r="CT71" s="8"/>
       <c r="CU71" s="8"/>
@@ -12598,12 +12676,13 @@
       <c r="CI72" s="11"/>
       <c r="CJ72" s="11"/>
       <c r="CK72" s="11"/>
-      <c r="CL72" s="11"/>
-      <c r="CM72" s="11"/>
-      <c r="CN72" s="11"/>
-      <c r="CO72" s="11"/>
-      <c r="CP72" s="11"/>
-      <c r="CQ72" s="11"/>
+      <c r="CL72" s="26"/>
+      <c r="CM72" s="26"/>
+      <c r="CN72" s="26"/>
+      <c r="CO72" s="26"/>
+      <c r="CP72" s="26"/>
+      <c r="CQ72" s="26"/>
+      <c r="CR72" s="26"/>
     </row>
     <row r="73" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
@@ -12699,13 +12778,13 @@
       <c r="CI74" s="8"/>
       <c r="CJ74" s="8"/>
       <c r="CK74" s="8"/>
-      <c r="CL74" s="8"/>
-      <c r="CM74" s="8"/>
-      <c r="CN74" s="8"/>
-      <c r="CO74" s="8"/>
-      <c r="CP74" s="8"/>
-      <c r="CQ74" s="8"/>
-      <c r="CR74" s="8"/>
+      <c r="CL74" s="24"/>
+      <c r="CM74" s="24"/>
+      <c r="CN74" s="24"/>
+      <c r="CO74" s="24"/>
+      <c r="CP74" s="24"/>
+      <c r="CQ74" s="24"/>
+      <c r="CR74" s="24"/>
       <c r="CS74" s="8"/>
       <c r="CT74" s="8"/>
       <c r="CU74" s="8"/>
@@ -12847,13 +12926,13 @@
       <c r="CI75" s="8"/>
       <c r="CJ75" s="8"/>
       <c r="CK75" s="8"/>
-      <c r="CL75" s="8"/>
-      <c r="CM75" s="8"/>
-      <c r="CN75" s="8"/>
-      <c r="CO75" s="8"/>
-      <c r="CP75" s="8"/>
-      <c r="CQ75" s="8"/>
-      <c r="CR75" s="8"/>
+      <c r="CL75" s="24"/>
+      <c r="CM75" s="24"/>
+      <c r="CN75" s="24"/>
+      <c r="CO75" s="24"/>
+      <c r="CP75" s="24"/>
+      <c r="CQ75" s="24"/>
+      <c r="CR75" s="24"/>
       <c r="CS75" s="8"/>
       <c r="CT75" s="8"/>
       <c r="CU75" s="8"/>
@@ -12938,148 +13017,147 @@
     </row>
     <row r="84" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
-      <c r="B84" s="22" t="s">
+      <c r="B84" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22" t="s">
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G84" s="22"/>
-      <c r="H84" s="22"/>
-      <c r="I84" s="22"/>
-      <c r="J84" s="22" t="s">
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="32"/>
+      <c r="J84" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K84" s="22"/>
-      <c r="L84" s="22"/>
-      <c r="M84" s="22"/>
-      <c r="N84" s="22" t="s">
+      <c r="K84" s="32"/>
+      <c r="L84" s="32"/>
+      <c r="M84" s="32"/>
+      <c r="N84" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="O84" s="22"/>
-      <c r="P84" s="22"/>
-      <c r="Q84" s="22"/>
-      <c r="R84" s="22" t="s">
+      <c r="O84" s="32"/>
+      <c r="P84" s="32"/>
+      <c r="Q84" s="32"/>
+      <c r="R84" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="S84" s="22"/>
-      <c r="T84" s="22"/>
-      <c r="U84" s="22"/>
-      <c r="V84" s="22" t="s">
+      <c r="S84" s="32"/>
+      <c r="T84" s="32"/>
+      <c r="U84" s="32"/>
+      <c r="V84" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="W84" s="22"/>
-      <c r="X84" s="22"/>
-      <c r="Y84" s="22"/>
-      <c r="Z84" s="22" t="s">
+      <c r="W84" s="32"/>
+      <c r="X84" s="32"/>
+      <c r="Y84" s="32"/>
+      <c r="Z84" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AA84" s="22"/>
-      <c r="AB84" s="22"/>
-      <c r="AC84" s="22"/>
-      <c r="AD84" s="22" t="s">
+      <c r="AA84" s="32"/>
+      <c r="AB84" s="32"/>
+      <c r="AC84" s="32"/>
+      <c r="AD84" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="AE84" s="22"/>
-      <c r="AF84" s="22"/>
-      <c r="AG84" s="22"/>
-      <c r="AH84" s="22" t="s">
+      <c r="AE84" s="32"/>
+      <c r="AF84" s="32"/>
+      <c r="AG84" s="32"/>
+      <c r="AH84" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="AI84" s="22"/>
-      <c r="AJ84" s="22"/>
-      <c r="AK84" s="22"/>
-      <c r="AL84" s="22" t="s">
+      <c r="AI84" s="32"/>
+      <c r="AJ84" s="32"/>
+      <c r="AK84" s="32"/>
+      <c r="AL84" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="AM84" s="22"/>
-      <c r="AN84" s="22"/>
-      <c r="AO84" s="22"/>
-      <c r="AP84" s="22" t="s">
+      <c r="AM84" s="32"/>
+      <c r="AN84" s="32"/>
+      <c r="AO84" s="32"/>
+      <c r="AP84" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="AQ84" s="22"/>
-      <c r="AR84" s="22"/>
-      <c r="AS84" s="22"/>
-      <c r="AT84" s="22" t="s">
+      <c r="AQ84" s="32"/>
+      <c r="AR84" s="32"/>
+      <c r="AS84" s="32"/>
+      <c r="AT84" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="AU84" s="22"/>
-      <c r="AV84" s="22"/>
-      <c r="AW84" s="22"/>
-      <c r="AX84" s="22" t="s">
+      <c r="AU84" s="32"/>
+      <c r="AV84" s="32"/>
+      <c r="AW84" s="32"/>
+      <c r="AX84" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AY84" s="22"/>
-      <c r="AZ84" s="22"/>
-      <c r="BA84" s="22"/>
-      <c r="BB84" s="22" t="s">
+      <c r="AY84" s="32"/>
+      <c r="AZ84" s="32"/>
+      <c r="BA84" s="32"/>
+      <c r="BB84" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="BC84" s="22"/>
-      <c r="BD84" s="22"/>
-      <c r="BE84" s="22"/>
-      <c r="BF84" s="22" t="s">
+      <c r="BC84" s="32"/>
+      <c r="BD84" s="32"/>
+      <c r="BE84" s="32"/>
+      <c r="BF84" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="BG84" s="22"/>
-      <c r="BH84" s="22"/>
-      <c r="BI84" s="22"/>
-      <c r="BJ84" s="22" t="s">
+      <c r="BG84" s="32"/>
+      <c r="BH84" s="32"/>
+      <c r="BI84" s="32"/>
+      <c r="BJ84" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="BK84" s="22"/>
-      <c r="BL84" s="22"/>
-      <c r="BM84" s="22"/>
-      <c r="BN84" s="22" t="s">
+      <c r="BK84" s="32"/>
+      <c r="BL84" s="32"/>
+      <c r="BM84" s="32"/>
+      <c r="BN84" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="BO84" s="22"/>
-      <c r="BP84" s="22"/>
-      <c r="BQ84" s="22"/>
-      <c r="BR84" s="22" t="s">
+      <c r="BO84" s="32"/>
+      <c r="BP84" s="32"/>
+      <c r="BQ84" s="32"/>
+      <c r="BR84" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="BS84" s="22"/>
-      <c r="BT84" s="22"/>
-      <c r="BU84" s="22"/>
-      <c r="BV84" s="22" t="s">
+      <c r="BS84" s="32"/>
+      <c r="BT84" s="32"/>
+      <c r="BU84" s="32"/>
+      <c r="BV84" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="BW84" s="22"/>
-      <c r="BX84" s="22"/>
-      <c r="BY84" s="22"/>
-      <c r="BZ84" s="22" t="s">
+      <c r="BW84" s="32"/>
+      <c r="BX84" s="32"/>
+      <c r="BY84" s="32"/>
+      <c r="BZ84" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="CA84" s="22"/>
-      <c r="CB84" s="22"/>
-      <c r="CC84" s="22"/>
-      <c r="CD84" s="22" t="s">
+      <c r="CA84" s="32"/>
+      <c r="CB84" s="32"/>
+      <c r="CC84" s="32"/>
+      <c r="CD84" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="CE84" s="22"/>
-      <c r="CF84" s="22"/>
-      <c r="CG84" s="22"/>
-      <c r="CH84" s="22" t="s">
+      <c r="CE84" s="32"/>
+      <c r="CF84" s="32"/>
+      <c r="CG84" s="32"/>
+      <c r="CH84" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="CI84" s="22"/>
-      <c r="CJ84" s="22"/>
-      <c r="CK84" s="22"/>
-      <c r="CL84" s="22" t="s">
+      <c r="CI84" s="32"/>
+      <c r="CJ84" s="32"/>
+      <c r="CK84" s="32"/>
+      <c r="CL84" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="CM84" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN84" s="22"/>
-      <c r="CO84" s="22"/>
-      <c r="CP84" s="22"/>
-      <c r="CQ84" s="23"/>
+      <c r="CM84" s="31"/>
+      <c r="CN84" s="31"/>
+      <c r="CO84" s="28"/>
+      <c r="CP84" s="21"/>
+      <c r="CQ84" s="21"/>
+      <c r="CR84" s="21"/>
     </row>
     <row r="85" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
@@ -13347,16 +13425,19 @@
       <c r="CK85" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CL85" s="5" t="s">
+      <c r="CL85" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CM85" s="5" t="s">
+      <c r="CM85" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CN85" s="5"/>
-      <c r="CO85" s="5"/>
-      <c r="CP85" s="5"/>
-      <c r="CQ85" s="5"/>
+      <c r="CN85" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO85" s="13"/>
+      <c r="CP85" s="13"/>
+      <c r="CQ85" s="13"/>
+      <c r="CR85" s="13"/>
     </row>
     <row r="86" spans="1:147" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
@@ -13629,17 +13710,19 @@
       <c r="CK87" s="14">
         <v>68.497582133349454</v>
       </c>
-      <c r="CL87" s="14">
+      <c r="CL87" s="29">
         <v>66.933998569187622</v>
       </c>
-      <c r="CM87" s="14">
-        <v>-2.7086047394266757</v>
-      </c>
-      <c r="CN87" s="14"/>
-      <c r="CO87" s="14"/>
-      <c r="CP87" s="14"/>
-      <c r="CQ87" s="14"/>
-      <c r="CR87" s="8"/>
+      <c r="CM87" s="29">
+        <v>-7.9206256614208002</v>
+      </c>
+      <c r="CN87" s="29">
+        <v>18.79604522484297</v>
+      </c>
+      <c r="CO87" s="29"/>
+      <c r="CP87" s="29"/>
+      <c r="CQ87" s="29"/>
+      <c r="CR87" s="29"/>
       <c r="CS87" s="8"/>
       <c r="CT87" s="8"/>
       <c r="CU87" s="8"/>
@@ -13960,17 +14043,19 @@
       <c r="CK88" s="14">
         <v>15.453253697379125</v>
       </c>
-      <c r="CL88" s="14">
+      <c r="CL88" s="29">
         <v>-22.733127261153541</v>
       </c>
-      <c r="CM88" s="14">
-        <v>6.2387293991619686E-2</v>
-      </c>
-      <c r="CN88" s="14"/>
-      <c r="CO88" s="14"/>
-      <c r="CP88" s="14"/>
-      <c r="CQ88" s="14"/>
-      <c r="CR88" s="8"/>
+      <c r="CM88" s="29">
+        <v>3.2974895816976471</v>
+      </c>
+      <c r="CN88" s="29">
+        <v>2.3768459269728197</v>
+      </c>
+      <c r="CO88" s="29"/>
+      <c r="CP88" s="29"/>
+      <c r="CQ88" s="29"/>
+      <c r="CR88" s="29"/>
       <c r="CS88" s="8"/>
       <c r="CT88" s="8"/>
       <c r="CU88" s="8"/>
@@ -14291,17 +14376,19 @@
       <c r="CK89" s="14">
         <v>349.55053760077203</v>
       </c>
-      <c r="CL89" s="14">
+      <c r="CL89" s="29">
         <v>581.9972140107966</v>
       </c>
-      <c r="CM89" s="14">
+      <c r="CM89" s="29">
         <v>88.250101321944186</v>
       </c>
-      <c r="CN89" s="14"/>
-      <c r="CO89" s="14"/>
-      <c r="CP89" s="14"/>
-      <c r="CQ89" s="14"/>
-      <c r="CR89" s="8"/>
+      <c r="CN89" s="29">
+        <v>57.34777918660518</v>
+      </c>
+      <c r="CO89" s="29"/>
+      <c r="CP89" s="29"/>
+      <c r="CQ89" s="29"/>
+      <c r="CR89" s="29"/>
       <c r="CS89" s="8"/>
       <c r="CT89" s="8"/>
       <c r="CU89" s="8"/>
@@ -14622,17 +14709,19 @@
       <c r="CK90" s="14">
         <v>3.3616295313059226</v>
       </c>
-      <c r="CL90" s="14">
+      <c r="CL90" s="29">
         <v>14.963370710976747</v>
       </c>
-      <c r="CM90" s="14">
-        <v>13.763995648814898</v>
-      </c>
-      <c r="CN90" s="14"/>
-      <c r="CO90" s="14"/>
-      <c r="CP90" s="14"/>
-      <c r="CQ90" s="14"/>
-      <c r="CR90" s="8"/>
+      <c r="CM90" s="29">
+        <v>12.000683917244444</v>
+      </c>
+      <c r="CN90" s="29">
+        <v>13.186386395108343</v>
+      </c>
+      <c r="CO90" s="29"/>
+      <c r="CP90" s="29"/>
+      <c r="CQ90" s="29"/>
+      <c r="CR90" s="29"/>
       <c r="CS90" s="8"/>
       <c r="CT90" s="8"/>
       <c r="CU90" s="8"/>
@@ -14953,17 +15042,19 @@
       <c r="CK91" s="14">
         <v>18.175311829899286</v>
       </c>
-      <c r="CL91" s="14">
+      <c r="CL91" s="29">
         <v>12.839132155355642</v>
       </c>
-      <c r="CM91" s="14">
-        <v>8.8153921427124118</v>
-      </c>
-      <c r="CN91" s="14"/>
-      <c r="CO91" s="14"/>
-      <c r="CP91" s="14"/>
-      <c r="CQ91" s="14"/>
-      <c r="CR91" s="8"/>
+      <c r="CM91" s="29">
+        <v>11.363055133077154</v>
+      </c>
+      <c r="CN91" s="29">
+        <v>6.0632342526110676</v>
+      </c>
+      <c r="CO91" s="29"/>
+      <c r="CP91" s="29"/>
+      <c r="CQ91" s="29"/>
+      <c r="CR91" s="29"/>
       <c r="CS91" s="8"/>
       <c r="CT91" s="8"/>
       <c r="CU91" s="8"/>
@@ -15284,17 +15375,19 @@
       <c r="CK92" s="14">
         <v>5.6946661002921388</v>
       </c>
-      <c r="CL92" s="14">
+      <c r="CL92" s="29">
         <v>3.4229356639520034</v>
       </c>
-      <c r="CM92" s="14">
-        <v>1.8927318893474592</v>
-      </c>
-      <c r="CN92" s="14"/>
-      <c r="CO92" s="14"/>
-      <c r="CP92" s="14"/>
-      <c r="CQ92" s="14"/>
-      <c r="CR92" s="8"/>
+      <c r="CM92" s="29">
+        <v>2.1172669659889038</v>
+      </c>
+      <c r="CN92" s="29">
+        <v>-9.4054449150689834E-2</v>
+      </c>
+      <c r="CO92" s="29"/>
+      <c r="CP92" s="29"/>
+      <c r="CQ92" s="29"/>
+      <c r="CR92" s="29"/>
       <c r="CS92" s="8"/>
       <c r="CT92" s="8"/>
       <c r="CU92" s="8"/>
@@ -15615,17 +15708,19 @@
       <c r="CK93" s="14">
         <v>10.153253740682118</v>
       </c>
-      <c r="CL93" s="14">
+      <c r="CL93" s="29">
         <v>-26.879647249614521</v>
       </c>
-      <c r="CM93" s="14">
-        <v>-12.834662136934242</v>
-      </c>
-      <c r="CN93" s="14"/>
-      <c r="CO93" s="14"/>
-      <c r="CP93" s="14"/>
-      <c r="CQ93" s="14"/>
-      <c r="CR93" s="8"/>
+      <c r="CM93" s="29">
+        <v>-5.2502907535679952</v>
+      </c>
+      <c r="CN93" s="29">
+        <v>5.2708175085868021</v>
+      </c>
+      <c r="CO93" s="29"/>
+      <c r="CP93" s="29"/>
+      <c r="CQ93" s="29"/>
+      <c r="CR93" s="29"/>
       <c r="CS93" s="8"/>
       <c r="CT93" s="8"/>
       <c r="CU93" s="8"/>
@@ -15946,17 +16041,19 @@
       <c r="CK94" s="14">
         <v>40.652027393024923</v>
       </c>
-      <c r="CL94" s="14">
+      <c r="CL94" s="29">
         <v>16.918925410049781</v>
       </c>
-      <c r="CM94" s="14">
-        <v>43.165043662754471</v>
-      </c>
-      <c r="CN94" s="14"/>
-      <c r="CO94" s="14"/>
-      <c r="CP94" s="14"/>
-      <c r="CQ94" s="14"/>
-      <c r="CR94" s="8"/>
+      <c r="CM94" s="29">
+        <v>10.906146114480265</v>
+      </c>
+      <c r="CN94" s="29">
+        <v>-9.4052597287833066</v>
+      </c>
+      <c r="CO94" s="29"/>
+      <c r="CP94" s="29"/>
+      <c r="CQ94" s="29"/>
+      <c r="CR94" s="29"/>
       <c r="CS94" s="8"/>
       <c r="CT94" s="8"/>
       <c r="CU94" s="8"/>
@@ -16098,13 +16195,13 @@
       <c r="CI95" s="8"/>
       <c r="CJ95" s="8"/>
       <c r="CK95" s="8"/>
-      <c r="CL95" s="8"/>
-      <c r="CM95" s="8"/>
-      <c r="CN95" s="8"/>
-      <c r="CO95" s="8"/>
-      <c r="CP95" s="8"/>
-      <c r="CQ95" s="8"/>
-      <c r="CR95" s="8"/>
+      <c r="CL95" s="24"/>
+      <c r="CM95" s="24"/>
+      <c r="CN95" s="24"/>
+      <c r="CO95" s="24"/>
+      <c r="CP95" s="24"/>
+      <c r="CQ95" s="24"/>
+      <c r="CR95" s="24"/>
       <c r="CS95" s="8"/>
       <c r="CT95" s="8"/>
       <c r="CU95" s="8"/>
@@ -16425,17 +16522,19 @@
       <c r="CK96" s="14">
         <v>21.958128353759164</v>
       </c>
-      <c r="CL96" s="14">
+      <c r="CL96" s="29">
         <v>20.195305425122001</v>
       </c>
-      <c r="CM96" s="14">
-        <v>9.6338892776590939</v>
-      </c>
-      <c r="CN96" s="14"/>
-      <c r="CO96" s="14"/>
-      <c r="CP96" s="14"/>
-      <c r="CQ96" s="14"/>
-      <c r="CR96" s="8"/>
+      <c r="CM96" s="29">
+        <v>10.396505205584774</v>
+      </c>
+      <c r="CN96" s="29">
+        <v>11.740261343779196</v>
+      </c>
+      <c r="CO96" s="29"/>
+      <c r="CP96" s="29"/>
+      <c r="CQ96" s="29"/>
+      <c r="CR96" s="29"/>
       <c r="CS96" s="8"/>
       <c r="CT96" s="8"/>
       <c r="CU96" s="8"/>
@@ -16578,12 +16677,13 @@
       <c r="CI97" s="11"/>
       <c r="CJ97" s="11"/>
       <c r="CK97" s="11"/>
-      <c r="CL97" s="11"/>
-      <c r="CM97" s="11"/>
-      <c r="CN97" s="11"/>
-      <c r="CO97" s="11"/>
-      <c r="CP97" s="11"/>
-      <c r="CQ97" s="11"/>
+      <c r="CL97" s="26"/>
+      <c r="CM97" s="26"/>
+      <c r="CN97" s="26"/>
+      <c r="CO97" s="26"/>
+      <c r="CP97" s="26"/>
+      <c r="CQ97" s="26"/>
+      <c r="CR97" s="26"/>
     </row>
     <row r="98" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="s">
@@ -16679,13 +16779,13 @@
       <c r="CI99" s="8"/>
       <c r="CJ99" s="8"/>
       <c r="CK99" s="8"/>
-      <c r="CL99" s="8"/>
-      <c r="CM99" s="8"/>
-      <c r="CN99" s="8"/>
-      <c r="CO99" s="8"/>
-      <c r="CP99" s="8"/>
-      <c r="CQ99" s="8"/>
-      <c r="CR99" s="8"/>
+      <c r="CL99" s="24"/>
+      <c r="CM99" s="24"/>
+      <c r="CN99" s="24"/>
+      <c r="CO99" s="24"/>
+      <c r="CP99" s="24"/>
+      <c r="CQ99" s="24"/>
+      <c r="CR99" s="24"/>
       <c r="CS99" s="8"/>
       <c r="CT99" s="8"/>
       <c r="CU99" s="8"/>
@@ -16827,13 +16927,13 @@
       <c r="CI100" s="8"/>
       <c r="CJ100" s="8"/>
       <c r="CK100" s="8"/>
-      <c r="CL100" s="8"/>
-      <c r="CM100" s="8"/>
-      <c r="CN100" s="8"/>
-      <c r="CO100" s="8"/>
-      <c r="CP100" s="8"/>
-      <c r="CQ100" s="8"/>
-      <c r="CR100" s="8"/>
+      <c r="CL100" s="24"/>
+      <c r="CM100" s="24"/>
+      <c r="CN100" s="24"/>
+      <c r="CO100" s="24"/>
+      <c r="CP100" s="24"/>
+      <c r="CQ100" s="24"/>
+      <c r="CR100" s="24"/>
       <c r="CS100" s="8"/>
       <c r="CT100" s="8"/>
       <c r="CU100" s="8"/>
@@ -16913,148 +17013,149 @@
     </row>
     <row r="108" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
-      <c r="B108" s="21">
+      <c r="B108" s="31">
         <v>2000</v>
       </c>
-      <c r="C108" s="21"/>
-      <c r="D108" s="21"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21">
+      <c r="C108" s="31"/>
+      <c r="D108" s="31"/>
+      <c r="E108" s="31"/>
+      <c r="F108" s="31">
         <v>2001</v>
       </c>
-      <c r="G108" s="21"/>
-      <c r="H108" s="21"/>
-      <c r="I108" s="21"/>
-      <c r="J108" s="21">
+      <c r="G108" s="31"/>
+      <c r="H108" s="31"/>
+      <c r="I108" s="31"/>
+      <c r="J108" s="31">
         <v>2002</v>
       </c>
-      <c r="K108" s="21"/>
-      <c r="L108" s="21"/>
-      <c r="M108" s="21"/>
-      <c r="N108" s="21">
+      <c r="K108" s="31"/>
+      <c r="L108" s="31"/>
+      <c r="M108" s="31"/>
+      <c r="N108" s="31">
         <v>2003</v>
       </c>
-      <c r="O108" s="21"/>
-      <c r="P108" s="21"/>
-      <c r="Q108" s="21"/>
-      <c r="R108" s="21">
+      <c r="O108" s="31"/>
+      <c r="P108" s="31"/>
+      <c r="Q108" s="31"/>
+      <c r="R108" s="31">
         <v>2004</v>
       </c>
-      <c r="S108" s="21"/>
-      <c r="T108" s="21"/>
-      <c r="U108" s="21"/>
-      <c r="V108" s="21">
+      <c r="S108" s="31"/>
+      <c r="T108" s="31"/>
+      <c r="U108" s="31"/>
+      <c r="V108" s="31">
         <v>2005</v>
       </c>
-      <c r="W108" s="21"/>
-      <c r="X108" s="21"/>
-      <c r="Y108" s="21"/>
-      <c r="Z108" s="21">
+      <c r="W108" s="31"/>
+      <c r="X108" s="31"/>
+      <c r="Y108" s="31"/>
+      <c r="Z108" s="31">
         <v>2006</v>
       </c>
-      <c r="AA108" s="21"/>
-      <c r="AB108" s="21"/>
-      <c r="AC108" s="21"/>
-      <c r="AD108" s="21">
+      <c r="AA108" s="31"/>
+      <c r="AB108" s="31"/>
+      <c r="AC108" s="31"/>
+      <c r="AD108" s="31">
         <v>2007</v>
       </c>
-      <c r="AE108" s="21"/>
-      <c r="AF108" s="21"/>
-      <c r="AG108" s="21"/>
-      <c r="AH108" s="21">
+      <c r="AE108" s="31"/>
+      <c r="AF108" s="31"/>
+      <c r="AG108" s="31"/>
+      <c r="AH108" s="31">
         <v>2008</v>
       </c>
-      <c r="AI108" s="21"/>
-      <c r="AJ108" s="21"/>
-      <c r="AK108" s="21"/>
-      <c r="AL108" s="21">
+      <c r="AI108" s="31"/>
+      <c r="AJ108" s="31"/>
+      <c r="AK108" s="31"/>
+      <c r="AL108" s="31">
         <v>2009</v>
       </c>
-      <c r="AM108" s="21"/>
-      <c r="AN108" s="21"/>
-      <c r="AO108" s="21"/>
-      <c r="AP108" s="21">
+      <c r="AM108" s="31"/>
+      <c r="AN108" s="31"/>
+      <c r="AO108" s="31"/>
+      <c r="AP108" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ108" s="21"/>
-      <c r="AR108" s="21"/>
-      <c r="AS108" s="21"/>
-      <c r="AT108" s="21">
+      <c r="AQ108" s="31"/>
+      <c r="AR108" s="31"/>
+      <c r="AS108" s="31"/>
+      <c r="AT108" s="31">
         <v>2011</v>
       </c>
-      <c r="AU108" s="21"/>
-      <c r="AV108" s="21"/>
-      <c r="AW108" s="21"/>
-      <c r="AX108" s="21">
+      <c r="AU108" s="31"/>
+      <c r="AV108" s="31"/>
+      <c r="AW108" s="31"/>
+      <c r="AX108" s="31">
         <v>2012</v>
       </c>
-      <c r="AY108" s="21"/>
-      <c r="AZ108" s="21"/>
-      <c r="BA108" s="21"/>
-      <c r="BB108" s="21">
+      <c r="AY108" s="31"/>
+      <c r="AZ108" s="31"/>
+      <c r="BA108" s="31"/>
+      <c r="BB108" s="31">
         <v>2013</v>
       </c>
-      <c r="BC108" s="21"/>
-      <c r="BD108" s="21"/>
-      <c r="BE108" s="21"/>
-      <c r="BF108" s="21">
+      <c r="BC108" s="31"/>
+      <c r="BD108" s="31"/>
+      <c r="BE108" s="31"/>
+      <c r="BF108" s="31">
         <v>2014</v>
       </c>
-      <c r="BG108" s="21"/>
-      <c r="BH108" s="21"/>
-      <c r="BI108" s="21"/>
-      <c r="BJ108" s="21">
+      <c r="BG108" s="31"/>
+      <c r="BH108" s="31"/>
+      <c r="BI108" s="31"/>
+      <c r="BJ108" s="31">
         <v>2015</v>
       </c>
-      <c r="BK108" s="21"/>
-      <c r="BL108" s="21"/>
-      <c r="BM108" s="21"/>
-      <c r="BN108" s="21">
+      <c r="BK108" s="31"/>
+      <c r="BL108" s="31"/>
+      <c r="BM108" s="31"/>
+      <c r="BN108" s="31">
         <v>2016</v>
       </c>
-      <c r="BO108" s="21"/>
-      <c r="BP108" s="21"/>
-      <c r="BQ108" s="21"/>
-      <c r="BR108" s="21">
+      <c r="BO108" s="31"/>
+      <c r="BP108" s="31"/>
+      <c r="BQ108" s="31"/>
+      <c r="BR108" s="31">
         <v>2017</v>
       </c>
-      <c r="BS108" s="21"/>
-      <c r="BT108" s="21"/>
-      <c r="BU108" s="21"/>
-      <c r="BV108" s="21">
+      <c r="BS108" s="31"/>
+      <c r="BT108" s="31"/>
+      <c r="BU108" s="31"/>
+      <c r="BV108" s="31">
         <v>2018</v>
       </c>
-      <c r="BW108" s="21"/>
-      <c r="BX108" s="21"/>
-      <c r="BY108" s="21"/>
-      <c r="BZ108" s="21">
+      <c r="BW108" s="31"/>
+      <c r="BX108" s="31"/>
+      <c r="BY108" s="31"/>
+      <c r="BZ108" s="31">
         <v>2019</v>
       </c>
-      <c r="CA108" s="21"/>
-      <c r="CB108" s="21"/>
-      <c r="CC108" s="21"/>
-      <c r="CD108" s="22">
+      <c r="CA108" s="31"/>
+      <c r="CB108" s="31"/>
+      <c r="CC108" s="31"/>
+      <c r="CD108" s="32">
         <v>2020</v>
       </c>
-      <c r="CE108" s="22"/>
-      <c r="CF108" s="22"/>
-      <c r="CG108" s="22"/>
-      <c r="CH108" s="22">
+      <c r="CE108" s="32"/>
+      <c r="CF108" s="32"/>
+      <c r="CG108" s="32"/>
+      <c r="CH108" s="32">
         <v>2021</v>
       </c>
-      <c r="CI108" s="22"/>
-      <c r="CJ108" s="22"/>
-      <c r="CK108" s="22"/>
-      <c r="CL108" s="22">
+      <c r="CI108" s="32"/>
+      <c r="CJ108" s="32"/>
+      <c r="CK108" s="32"/>
+      <c r="CL108" s="31">
         <v>2022</v>
       </c>
-      <c r="CM108" s="22"/>
-      <c r="CN108" s="22"/>
-      <c r="CO108" s="22"/>
-      <c r="CP108" s="22">
+      <c r="CM108" s="31"/>
+      <c r="CN108" s="31"/>
+      <c r="CO108" s="31"/>
+      <c r="CP108" s="31">
         <v>2023</v>
       </c>
-      <c r="CQ108" s="23"/>
+      <c r="CQ108" s="31"/>
+      <c r="CR108" s="31"/>
     </row>
     <row r="109" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
@@ -17322,23 +17423,26 @@
       <c r="CK109" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CL109" s="13" t="s">
+      <c r="CL109" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CM109" s="13" t="s">
+      <c r="CM109" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="CN109" s="13" t="s">
+      <c r="CN109" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="CO109" s="13" t="s">
+      <c r="CO109" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="CP109" s="13" t="s">
+      <c r="CP109" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CQ109" s="13" t="s">
+      <c r="CQ109" s="27" t="s">
         <v>8</v>
+      </c>
+      <c r="CR109" s="27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -17612,25 +17716,27 @@
       <c r="CK111" s="14">
         <v>118.63153574023102</v>
       </c>
-      <c r="CL111" s="14">
+      <c r="CL111" s="29">
         <v>126.09642903416727</v>
       </c>
-      <c r="CM111" s="14">
+      <c r="CM111" s="29">
         <v>124.61983118929622</v>
       </c>
-      <c r="CN111" s="14">
+      <c r="CN111" s="29">
         <v>128.49759727085754</v>
       </c>
-      <c r="CO111" s="14">
+      <c r="CO111" s="29">
         <v>133.0320896828776</v>
       </c>
-      <c r="CP111" s="14">
+      <c r="CP111" s="29">
         <v>136.72622876503408</v>
       </c>
-      <c r="CQ111" s="14">
-        <v>141.65669937816355</v>
-      </c>
-      <c r="CR111" s="8"/>
+      <c r="CQ111" s="29">
+        <v>141.65669937816352</v>
+      </c>
+      <c r="CR111" s="29">
+        <v>130.28192558024958</v>
+      </c>
       <c r="CS111" s="8"/>
       <c r="CT111" s="8"/>
       <c r="CU111" s="8"/>
@@ -17955,25 +18061,27 @@
       <c r="CK112" s="14">
         <v>107.41235280347485</v>
       </c>
-      <c r="CL112" s="14">
+      <c r="CL112" s="29">
         <v>111.88039102135299</v>
       </c>
-      <c r="CM112" s="14">
+      <c r="CM112" s="29">
         <v>113.74058049100657</v>
       </c>
-      <c r="CN112" s="14">
+      <c r="CN112" s="29">
         <v>116.05280088472769</v>
       </c>
-      <c r="CO112" s="14">
+      <c r="CO112" s="29">
         <v>114.41806830514707</v>
       </c>
-      <c r="CP112" s="14">
+      <c r="CP112" s="29">
         <v>119.59147290110843</v>
       </c>
-      <c r="CQ112" s="14">
+      <c r="CQ112" s="29">
         <v>119.26852215132922</v>
       </c>
-      <c r="CR112" s="8"/>
+      <c r="CR112" s="29">
+        <v>120.01837611904935</v>
+      </c>
       <c r="CS112" s="8"/>
       <c r="CT112" s="8"/>
       <c r="CU112" s="8"/>
@@ -18298,25 +18406,27 @@
       <c r="CK113" s="14">
         <v>108.46407696982685</v>
       </c>
-      <c r="CL113" s="14">
+      <c r="CL113" s="29">
         <v>113.43226434989448</v>
       </c>
-      <c r="CM113" s="14">
+      <c r="CM113" s="29">
         <v>115.6341945436903</v>
       </c>
-      <c r="CN113" s="14">
+      <c r="CN113" s="29">
         <v>118.385255983341</v>
       </c>
-      <c r="CO113" s="14">
+      <c r="CO113" s="29">
         <v>117.03672057255258</v>
       </c>
-      <c r="CP113" s="14">
+      <c r="CP113" s="29">
         <v>122.00663809992125</v>
       </c>
-      <c r="CQ113" s="14">
+      <c r="CQ113" s="29">
         <v>122.63218135093956</v>
       </c>
-      <c r="CR113" s="8"/>
+      <c r="CR113" s="29">
+        <v>124.72795126241223</v>
+      </c>
       <c r="CS113" s="8"/>
       <c r="CT113" s="8"/>
       <c r="CU113" s="8"/>
@@ -18641,25 +18751,27 @@
       <c r="CK114" s="14">
         <v>109.02907695717339</v>
       </c>
-      <c r="CL114" s="14">
+      <c r="CL114" s="29">
         <v>108.58723074343011</v>
       </c>
-      <c r="CM114" s="14">
+      <c r="CM114" s="29">
         <v>109.98023693843398</v>
       </c>
-      <c r="CN114" s="14">
+      <c r="CN114" s="29">
         <v>112.53715586887442</v>
       </c>
-      <c r="CO114" s="14">
+      <c r="CO114" s="29">
         <v>115.53683219443604</v>
       </c>
-      <c r="CP114" s="14">
+      <c r="CP114" s="29">
         <v>115.7444035129955</v>
       </c>
-      <c r="CQ114" s="14">
+      <c r="CQ114" s="29">
         <v>116.50252804574832</v>
       </c>
-      <c r="CR114" s="8"/>
+      <c r="CR114" s="29">
+        <v>118.14474888583113</v>
+      </c>
       <c r="CS114" s="8"/>
       <c r="CT114" s="8"/>
       <c r="CU114" s="8"/>
@@ -18984,25 +19096,27 @@
       <c r="CK115" s="14">
         <v>99.188841424745021</v>
       </c>
-      <c r="CL115" s="14">
+      <c r="CL115" s="29">
         <v>102.1773430955365</v>
       </c>
-      <c r="CM115" s="14">
+      <c r="CM115" s="29">
         <v>103.17914174932667</v>
       </c>
-      <c r="CN115" s="14">
+      <c r="CN115" s="29">
         <v>102.17552207806702</v>
       </c>
-      <c r="CO115" s="14">
+      <c r="CO115" s="29">
         <v>103.34897185336216</v>
       </c>
-      <c r="CP115" s="14">
+      <c r="CP115" s="29">
         <v>102.92008743148232</v>
       </c>
-      <c r="CQ115" s="14">
-        <v>103.61804299083268</v>
-      </c>
-      <c r="CR115" s="8"/>
+      <c r="CQ115" s="29">
+        <v>103.61706726923939</v>
+      </c>
+      <c r="CR115" s="29">
+        <v>102.55633330527832</v>
+      </c>
       <c r="CS115" s="8"/>
       <c r="CT115" s="8"/>
       <c r="CU115" s="8"/>
@@ -19327,25 +19441,27 @@
       <c r="CK116" s="14">
         <v>109.3552980162752</v>
       </c>
-      <c r="CL116" s="14">
+      <c r="CL116" s="29">
         <v>113.98898088171985</v>
       </c>
-      <c r="CM116" s="14">
+      <c r="CM116" s="29">
         <v>115.24165168078628</v>
       </c>
-      <c r="CN116" s="14">
+      <c r="CN116" s="29">
         <v>116.52552735229604</v>
       </c>
-      <c r="CO116" s="14">
+      <c r="CO116" s="29">
         <v>117.00435355436905</v>
       </c>
-      <c r="CP116" s="14">
+      <c r="CP116" s="29">
         <v>118.63204242974616</v>
       </c>
-      <c r="CQ116" s="14">
-        <v>119.53549960685177</v>
-      </c>
-      <c r="CR116" s="8"/>
+      <c r="CQ116" s="29">
+        <v>119.51872166523746</v>
+      </c>
+      <c r="CR116" s="29">
+        <v>120.54387253224547</v>
+      </c>
       <c r="CS116" s="8"/>
       <c r="CT116" s="8"/>
       <c r="CU116" s="8"/>
@@ -19670,25 +19786,27 @@
       <c r="CK117" s="14">
         <v>107.16683189889456</v>
       </c>
-      <c r="CL117" s="14">
+      <c r="CL117" s="29">
         <v>112.89718497790633</v>
       </c>
-      <c r="CM117" s="14">
+      <c r="CM117" s="29">
         <v>113.65147294228359</v>
       </c>
-      <c r="CN117" s="14">
+      <c r="CN117" s="29">
         <v>119.54655249515902</v>
       </c>
-      <c r="CO117" s="14">
+      <c r="CO117" s="29">
         <v>117.79146924859019</v>
       </c>
-      <c r="CP117" s="14">
+      <c r="CP117" s="29">
         <v>120.67834689029524</v>
       </c>
-      <c r="CQ117" s="14">
+      <c r="CQ117" s="29">
         <v>119.17508385865621</v>
       </c>
-      <c r="CR117" s="8"/>
+      <c r="CR117" s="29">
+        <v>123.63151075820188</v>
+      </c>
       <c r="CS117" s="8"/>
       <c r="CT117" s="8"/>
       <c r="CU117" s="8"/>
@@ -20013,25 +20131,27 @@
       <c r="CK118" s="14">
         <v>107.27313045488039</v>
       </c>
-      <c r="CL118" s="14">
+      <c r="CL118" s="29">
         <v>112.00394049520814</v>
       </c>
-      <c r="CM118" s="14">
+      <c r="CM118" s="29">
         <v>113.13547570597326</v>
       </c>
-      <c r="CN118" s="14">
+      <c r="CN118" s="29">
         <v>111.27094242821842</v>
       </c>
-      <c r="CO118" s="14">
+      <c r="CO118" s="29">
         <v>114.26976550965541</v>
       </c>
-      <c r="CP118" s="14">
+      <c r="CP118" s="29">
         <v>119.72353771979209</v>
       </c>
-      <c r="CQ118" s="14">
-        <v>118.63400847867105</v>
-      </c>
-      <c r="CR118" s="8"/>
+      <c r="CQ118" s="29">
+        <v>118.63400847867109</v>
+      </c>
+      <c r="CR118" s="29">
+        <v>116.31755657998013</v>
+      </c>
       <c r="CS118" s="8"/>
       <c r="CT118" s="8"/>
       <c r="CU118" s="8"/>
@@ -20177,13 +20297,13 @@
       <c r="CI119" s="8"/>
       <c r="CJ119" s="8"/>
       <c r="CK119" s="8"/>
-      <c r="CL119" s="8"/>
-      <c r="CM119" s="8"/>
-      <c r="CN119" s="8"/>
-      <c r="CO119" s="8"/>
-      <c r="CP119" s="8"/>
-      <c r="CQ119" s="8"/>
-      <c r="CR119" s="8"/>
+      <c r="CL119" s="24"/>
+      <c r="CM119" s="24"/>
+      <c r="CN119" s="24"/>
+      <c r="CO119" s="24"/>
+      <c r="CP119" s="24"/>
+      <c r="CQ119" s="24"/>
+      <c r="CR119" s="24"/>
       <c r="CS119" s="8"/>
       <c r="CT119" s="8"/>
       <c r="CU119" s="8"/>
@@ -20508,25 +20628,27 @@
       <c r="CK120" s="14">
         <v>107.90147001950392</v>
       </c>
-      <c r="CL120" s="14">
+      <c r="CL120" s="29">
         <v>112.33130479076783</v>
       </c>
-      <c r="CM120" s="14">
+      <c r="CM120" s="29">
         <v>113.28644583069654</v>
       </c>
-      <c r="CN120" s="14">
+      <c r="CN120" s="29">
         <v>115.58029627840591</v>
       </c>
-      <c r="CO120" s="14">
+      <c r="CO120" s="29">
         <v>116.13546076127123</v>
       </c>
-      <c r="CP120" s="14">
+      <c r="CP120" s="29">
         <v>118.08849090170519</v>
       </c>
-      <c r="CQ120" s="14">
-        <v>117.94625363222767</v>
-      </c>
-      <c r="CR120" s="8"/>
+      <c r="CQ120" s="29">
+        <v>117.84076019058585</v>
+      </c>
+      <c r="CR120" s="29">
+        <v>119.7618421348394</v>
+      </c>
       <c r="CS120" s="8"/>
       <c r="CT120" s="8"/>
       <c r="CU120" s="8"/>
@@ -20673,12 +20795,13 @@
       <c r="CI121" s="11"/>
       <c r="CJ121" s="11"/>
       <c r="CK121" s="11"/>
-      <c r="CL121" s="11"/>
-      <c r="CM121" s="11"/>
-      <c r="CN121" s="11"/>
-      <c r="CO121" s="11"/>
-      <c r="CP121" s="11"/>
-      <c r="CQ121" s="11"/>
+      <c r="CL121" s="26"/>
+      <c r="CM121" s="26"/>
+      <c r="CN121" s="26"/>
+      <c r="CO121" s="26"/>
+      <c r="CP121" s="26"/>
+      <c r="CQ121" s="26"/>
+      <c r="CR121" s="26"/>
     </row>
     <row r="122" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
@@ -20717,148 +20840,149 @@
     </row>
     <row r="133" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
-      <c r="B133" s="21">
+      <c r="B133" s="31">
         <v>2000</v>
       </c>
-      <c r="C133" s="21"/>
-      <c r="D133" s="21"/>
-      <c r="E133" s="21"/>
-      <c r="F133" s="21">
+      <c r="C133" s="31"/>
+      <c r="D133" s="31"/>
+      <c r="E133" s="31"/>
+      <c r="F133" s="31">
         <v>2001</v>
       </c>
-      <c r="G133" s="21"/>
-      <c r="H133" s="21"/>
-      <c r="I133" s="21"/>
-      <c r="J133" s="21">
+      <c r="G133" s="31"/>
+      <c r="H133" s="31"/>
+      <c r="I133" s="31"/>
+      <c r="J133" s="31">
         <v>2002</v>
       </c>
-      <c r="K133" s="21"/>
-      <c r="L133" s="21"/>
-      <c r="M133" s="21"/>
-      <c r="N133" s="21">
+      <c r="K133" s="31"/>
+      <c r="L133" s="31"/>
+      <c r="M133" s="31"/>
+      <c r="N133" s="31">
         <v>2003</v>
       </c>
-      <c r="O133" s="21"/>
-      <c r="P133" s="21"/>
-      <c r="Q133" s="21"/>
-      <c r="R133" s="21">
+      <c r="O133" s="31"/>
+      <c r="P133" s="31"/>
+      <c r="Q133" s="31"/>
+      <c r="R133" s="31">
         <v>2004</v>
       </c>
-      <c r="S133" s="21"/>
-      <c r="T133" s="21"/>
-      <c r="U133" s="21"/>
-      <c r="V133" s="21">
+      <c r="S133" s="31"/>
+      <c r="T133" s="31"/>
+      <c r="U133" s="31"/>
+      <c r="V133" s="31">
         <v>2005</v>
       </c>
-      <c r="W133" s="21"/>
-      <c r="X133" s="21"/>
-      <c r="Y133" s="21"/>
-      <c r="Z133" s="21">
+      <c r="W133" s="31"/>
+      <c r="X133" s="31"/>
+      <c r="Y133" s="31"/>
+      <c r="Z133" s="31">
         <v>2006</v>
       </c>
-      <c r="AA133" s="21"/>
-      <c r="AB133" s="21"/>
-      <c r="AC133" s="21"/>
-      <c r="AD133" s="21">
+      <c r="AA133" s="31"/>
+      <c r="AB133" s="31"/>
+      <c r="AC133" s="31"/>
+      <c r="AD133" s="31">
         <v>2007</v>
       </c>
-      <c r="AE133" s="21"/>
-      <c r="AF133" s="21"/>
-      <c r="AG133" s="21"/>
-      <c r="AH133" s="21">
+      <c r="AE133" s="31"/>
+      <c r="AF133" s="31"/>
+      <c r="AG133" s="31"/>
+      <c r="AH133" s="31">
         <v>2008</v>
       </c>
-      <c r="AI133" s="21"/>
-      <c r="AJ133" s="21"/>
-      <c r="AK133" s="21"/>
-      <c r="AL133" s="21">
+      <c r="AI133" s="31"/>
+      <c r="AJ133" s="31"/>
+      <c r="AK133" s="31"/>
+      <c r="AL133" s="31">
         <v>2009</v>
       </c>
-      <c r="AM133" s="21"/>
-      <c r="AN133" s="21"/>
-      <c r="AO133" s="21"/>
-      <c r="AP133" s="21">
+      <c r="AM133" s="31"/>
+      <c r="AN133" s="31"/>
+      <c r="AO133" s="31"/>
+      <c r="AP133" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ133" s="21"/>
-      <c r="AR133" s="21"/>
-      <c r="AS133" s="21"/>
-      <c r="AT133" s="21">
+      <c r="AQ133" s="31"/>
+      <c r="AR133" s="31"/>
+      <c r="AS133" s="31"/>
+      <c r="AT133" s="31">
         <v>2011</v>
       </c>
-      <c r="AU133" s="21"/>
-      <c r="AV133" s="21"/>
-      <c r="AW133" s="21"/>
-      <c r="AX133" s="21">
+      <c r="AU133" s="31"/>
+      <c r="AV133" s="31"/>
+      <c r="AW133" s="31"/>
+      <c r="AX133" s="31">
         <v>2012</v>
       </c>
-      <c r="AY133" s="21"/>
-      <c r="AZ133" s="21"/>
-      <c r="BA133" s="21"/>
-      <c r="BB133" s="21">
+      <c r="AY133" s="31"/>
+      <c r="AZ133" s="31"/>
+      <c r="BA133" s="31"/>
+      <c r="BB133" s="31">
         <v>2013</v>
       </c>
-      <c r="BC133" s="21"/>
-      <c r="BD133" s="21"/>
-      <c r="BE133" s="21"/>
-      <c r="BF133" s="21">
+      <c r="BC133" s="31"/>
+      <c r="BD133" s="31"/>
+      <c r="BE133" s="31"/>
+      <c r="BF133" s="31">
         <v>2014</v>
       </c>
-      <c r="BG133" s="21"/>
-      <c r="BH133" s="21"/>
-      <c r="BI133" s="21"/>
-      <c r="BJ133" s="21">
+      <c r="BG133" s="31"/>
+      <c r="BH133" s="31"/>
+      <c r="BI133" s="31"/>
+      <c r="BJ133" s="31">
         <v>2015</v>
       </c>
-      <c r="BK133" s="21"/>
-      <c r="BL133" s="21"/>
-      <c r="BM133" s="21"/>
-      <c r="BN133" s="21">
+      <c r="BK133" s="31"/>
+      <c r="BL133" s="31"/>
+      <c r="BM133" s="31"/>
+      <c r="BN133" s="31">
         <v>2016</v>
       </c>
-      <c r="BO133" s="21"/>
-      <c r="BP133" s="21"/>
-      <c r="BQ133" s="21"/>
-      <c r="BR133" s="21">
+      <c r="BO133" s="31"/>
+      <c r="BP133" s="31"/>
+      <c r="BQ133" s="31"/>
+      <c r="BR133" s="31">
         <v>2017</v>
       </c>
-      <c r="BS133" s="21"/>
-      <c r="BT133" s="21"/>
-      <c r="BU133" s="21"/>
-      <c r="BV133" s="21">
+      <c r="BS133" s="31"/>
+      <c r="BT133" s="31"/>
+      <c r="BU133" s="31"/>
+      <c r="BV133" s="31">
         <v>2018</v>
       </c>
-      <c r="BW133" s="21"/>
-      <c r="BX133" s="21"/>
-      <c r="BY133" s="21"/>
-      <c r="BZ133" s="21">
+      <c r="BW133" s="31"/>
+      <c r="BX133" s="31"/>
+      <c r="BY133" s="31"/>
+      <c r="BZ133" s="31">
         <v>2019</v>
       </c>
-      <c r="CA133" s="21"/>
-      <c r="CB133" s="21"/>
-      <c r="CC133" s="21"/>
-      <c r="CD133" s="22">
+      <c r="CA133" s="31"/>
+      <c r="CB133" s="31"/>
+      <c r="CC133" s="31"/>
+      <c r="CD133" s="32">
         <v>2020</v>
       </c>
-      <c r="CE133" s="22"/>
-      <c r="CF133" s="22"/>
-      <c r="CG133" s="22"/>
-      <c r="CH133" s="22">
+      <c r="CE133" s="32"/>
+      <c r="CF133" s="32"/>
+      <c r="CG133" s="32"/>
+      <c r="CH133" s="32">
         <v>2021</v>
       </c>
-      <c r="CI133" s="22"/>
-      <c r="CJ133" s="22"/>
-      <c r="CK133" s="22"/>
-      <c r="CL133" s="22">
+      <c r="CI133" s="32"/>
+      <c r="CJ133" s="32"/>
+      <c r="CK133" s="32"/>
+      <c r="CL133" s="31">
         <v>2022</v>
       </c>
-      <c r="CM133" s="22"/>
-      <c r="CN133" s="22"/>
-      <c r="CO133" s="22"/>
-      <c r="CP133" s="22">
+      <c r="CM133" s="31"/>
+      <c r="CN133" s="31"/>
+      <c r="CO133" s="31"/>
+      <c r="CP133" s="31">
         <v>2023</v>
       </c>
-      <c r="CQ133" s="23"/>
+      <c r="CQ133" s="31"/>
+      <c r="CR133" s="31"/>
     </row>
     <row r="134" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
@@ -21126,23 +21250,26 @@
       <c r="CK134" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CL134" s="13" t="s">
+      <c r="CL134" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CM134" s="13" t="s">
+      <c r="CM134" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="CN134" s="13" t="s">
+      <c r="CN134" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="CO134" s="13" t="s">
+      <c r="CO134" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="CP134" s="13" t="s">
+      <c r="CP134" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CQ134" s="13" t="s">
+      <c r="CQ134" s="27" t="s">
         <v>8</v>
+      </c>
+      <c r="CR134" s="27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -21416,25 +21543,27 @@
       <c r="CK136" s="20">
         <v>6.3517535811312325</v>
       </c>
-      <c r="CL136" s="20">
+      <c r="CL136" s="30">
         <v>7.2501408841845167</v>
       </c>
-      <c r="CM136" s="20">
+      <c r="CM136" s="30">
         <v>4.5525961507475614</v>
       </c>
-      <c r="CN136" s="20">
+      <c r="CN136" s="30">
         <v>7.123031504693027</v>
       </c>
-      <c r="CO136" s="20">
+      <c r="CO136" s="30">
         <v>9.1431393370668612</v>
       </c>
-      <c r="CP136" s="20">
+      <c r="CP136" s="30">
         <v>10.385944912529338</v>
       </c>
-      <c r="CQ136" s="20">
-        <v>4.4109536908816631</v>
-      </c>
-      <c r="CR136" s="8"/>
+      <c r="CQ136" s="30">
+        <v>4.1495264516934016</v>
+      </c>
+      <c r="CR136" s="30">
+        <v>7.4098883315511861</v>
+      </c>
       <c r="CS136" s="8"/>
       <c r="CT136" s="8"/>
       <c r="CU136" s="8"/>
@@ -21759,25 +21888,27 @@
       <c r="CK137" s="20">
         <v>0.17388086679314779</v>
       </c>
-      <c r="CL137" s="20">
+      <c r="CL137" s="30">
         <v>8.303106049360541E-2</v>
       </c>
-      <c r="CM137" s="20">
+      <c r="CM137" s="30">
         <v>5.9636933637316959E-2</v>
       </c>
-      <c r="CN137" s="20">
+      <c r="CN137" s="30">
         <v>0.14132000283227314</v>
       </c>
-      <c r="CO137" s="20">
+      <c r="CO137" s="30">
         <v>0.16291089073254109</v>
       </c>
-      <c r="CP137" s="20">
+      <c r="CP137" s="30">
         <v>5.4273256982205413E-2</v>
       </c>
-      <c r="CQ137" s="20">
-        <v>5.4820821943269836E-2</v>
-      </c>
-      <c r="CR137" s="8"/>
+      <c r="CQ137" s="30">
+        <v>5.6252594877349446E-2</v>
+      </c>
+      <c r="CR137" s="30">
+        <v>0.12922696834695957</v>
+      </c>
       <c r="CS137" s="8"/>
       <c r="CT137" s="8"/>
       <c r="CU137" s="8"/>
@@ -22102,25 +22233,27 @@
       <c r="CK138" s="20">
         <v>2.7818782049697144</v>
       </c>
-      <c r="CL138" s="20">
+      <c r="CL138" s="30">
         <v>2.5240485310759349</v>
       </c>
-      <c r="CM138" s="20">
+      <c r="CM138" s="30">
         <v>9.0963045368606146</v>
       </c>
-      <c r="CN138" s="20">
+      <c r="CN138" s="30">
         <v>16.510726042475234</v>
       </c>
-      <c r="CO138" s="20">
+      <c r="CO138" s="30">
         <v>10.280272247948936</v>
       </c>
-      <c r="CP138" s="20">
+      <c r="CP138" s="30">
         <v>14.653213781321977</v>
       </c>
-      <c r="CQ138" s="20">
-        <v>15.909896855859479</v>
-      </c>
-      <c r="CR138" s="8"/>
+      <c r="CQ138" s="30">
+        <v>15.814136212939701</v>
+      </c>
+      <c r="CR138" s="30">
+        <v>23.640062115082273</v>
+      </c>
       <c r="CS138" s="8"/>
       <c r="CT138" s="8"/>
       <c r="CU138" s="8"/>
@@ -22445,25 +22578,27 @@
       <c r="CK139" s="20">
         <v>0.88176153624546327</v>
       </c>
-      <c r="CL139" s="20">
+      <c r="CL139" s="30">
         <v>0.53926570175523747</v>
       </c>
-      <c r="CM139" s="20">
+      <c r="CM139" s="30">
         <v>0.59443022262417511</v>
       </c>
-      <c r="CN139" s="20">
+      <c r="CN139" s="30">
         <v>0.69975213191846064</v>
       </c>
-      <c r="CO139" s="20">
+      <c r="CO139" s="30">
         <v>0.73576712927618371</v>
       </c>
-      <c r="CP139" s="20">
+      <c r="CP139" s="30">
         <v>0.52298502916791312</v>
       </c>
-      <c r="CQ139" s="20">
-        <v>0.62758910789349109</v>
-      </c>
-      <c r="CR139" s="8"/>
+      <c r="CQ139" s="30">
+        <v>0.61414277395104466</v>
+      </c>
+      <c r="CR139" s="30">
+        <v>0.71814570361207397</v>
+      </c>
       <c r="CS139" s="8"/>
       <c r="CT139" s="8"/>
       <c r="CU139" s="8"/>
@@ -22788,25 +22923,27 @@
       <c r="CK140" s="20">
         <v>15.080973968014156</v>
       </c>
-      <c r="CL140" s="20">
+      <c r="CL140" s="30">
         <v>17.238137924424048</v>
       </c>
-      <c r="CM140" s="20">
+      <c r="CM140" s="30">
         <v>16.198405160389729</v>
       </c>
-      <c r="CN140" s="20">
+      <c r="CN140" s="30">
         <v>13.373125061649633</v>
       </c>
-      <c r="CO140" s="20">
+      <c r="CO140" s="30">
         <v>14.14657327890621</v>
       </c>
-      <c r="CP140" s="20">
+      <c r="CP140" s="30">
         <v>15.506056245062746</v>
       </c>
-      <c r="CQ140" s="20">
-        <v>15.507973258638918</v>
-      </c>
-      <c r="CR140" s="8"/>
+      <c r="CQ140" s="30">
+        <v>15.775381488139049</v>
+      </c>
+      <c r="CR140" s="30">
+        <v>12.296146956353148</v>
+      </c>
       <c r="CS140" s="8"/>
       <c r="CT140" s="8"/>
       <c r="CU140" s="8"/>
@@ -23131,25 +23268,27 @@
       <c r="CK141" s="20">
         <v>61.447874063049959</v>
       </c>
-      <c r="CL141" s="20">
+      <c r="CL141" s="30">
         <v>58.900780388605469</v>
       </c>
-      <c r="CM141" s="20">
+      <c r="CM141" s="30">
         <v>57.315289478851419</v>
       </c>
-      <c r="CN141" s="20">
+      <c r="CN141" s="30">
         <v>51.518222835669761</v>
       </c>
-      <c r="CO141" s="20">
+      <c r="CO141" s="30">
         <v>52.938775237345773</v>
       </c>
-      <c r="CP141" s="20">
+      <c r="CP141" s="30">
         <v>50.174467506242607</v>
       </c>
-      <c r="CQ141" s="20">
-        <v>53.070124142249163</v>
-      </c>
-      <c r="CR141" s="8"/>
+      <c r="CQ141" s="30">
+        <v>52.859521752134953</v>
+      </c>
+      <c r="CR141" s="30">
+        <v>45.986665827425938</v>
+      </c>
       <c r="CS141" s="8"/>
       <c r="CT141" s="8"/>
       <c r="CU141" s="8"/>
@@ -23474,25 +23613,27 @@
       <c r="CK142" s="20">
         <v>11.721266919248494</v>
       </c>
-      <c r="CL142" s="20">
+      <c r="CL142" s="30">
         <v>12.454562170481861</v>
       </c>
-      <c r="CM142" s="20">
+      <c r="CM142" s="30">
         <v>10.895182644348477</v>
       </c>
-      <c r="CN142" s="20">
+      <c r="CN142" s="30">
         <v>9.1716680739699008</v>
       </c>
-      <c r="CO142" s="20">
+      <c r="CO142" s="30">
         <v>10.811279520989928</v>
       </c>
-      <c r="CP142" s="20">
+      <c r="CP142" s="30">
         <v>7.7040431649428687</v>
       </c>
-      <c r="CQ142" s="20">
-        <v>8.7244430168462248</v>
-      </c>
-      <c r="CR142" s="8"/>
+      <c r="CQ142" s="30">
+        <v>9.4264873616423603</v>
+      </c>
+      <c r="CR142" s="30">
+        <v>8.6239076590452282</v>
+      </c>
       <c r="CS142" s="8"/>
       <c r="CT142" s="8"/>
       <c r="CU142" s="8"/>
@@ -23817,25 +23958,27 @@
       <c r="CK143" s="20">
         <v>1.5606108605478348</v>
       </c>
-      <c r="CL143" s="20">
+      <c r="CL143" s="30">
         <v>1.0100333389793279</v>
       </c>
-      <c r="CM143" s="20">
+      <c r="CM143" s="30">
         <v>1.2881548725406995</v>
       </c>
-      <c r="CN143" s="20">
+      <c r="CN143" s="30">
         <v>1.462154346791706</v>
       </c>
-      <c r="CO143" s="20">
+      <c r="CO143" s="30">
         <v>1.7812823577335724</v>
       </c>
-      <c r="CP143" s="20">
+      <c r="CP143" s="30">
         <v>0.99901610375035477</v>
       </c>
-      <c r="CQ143" s="20">
-        <v>1.6941991056877856</v>
-      </c>
-      <c r="CR143" s="8"/>
+      <c r="CQ143" s="30">
+        <v>1.3045513646221525</v>
+      </c>
+      <c r="CR143" s="30">
+        <v>1.1959564385831878</v>
+      </c>
       <c r="CS143" s="8"/>
       <c r="CT143" s="8"/>
       <c r="CU143" s="8"/>
@@ -23981,13 +24124,13 @@
       <c r="CI144" s="8"/>
       <c r="CJ144" s="8"/>
       <c r="CK144" s="8"/>
-      <c r="CL144" s="8"/>
-      <c r="CM144" s="8"/>
-      <c r="CN144" s="8"/>
-      <c r="CO144" s="8"/>
-      <c r="CP144" s="8"/>
-      <c r="CQ144" s="8"/>
-      <c r="CR144" s="8"/>
+      <c r="CL144" s="24"/>
+      <c r="CM144" s="24"/>
+      <c r="CN144" s="24"/>
+      <c r="CO144" s="24"/>
+      <c r="CP144" s="24"/>
+      <c r="CQ144" s="24"/>
+      <c r="CR144" s="24"/>
       <c r="CS144" s="8"/>
       <c r="CT144" s="8"/>
       <c r="CU144" s="8"/>
@@ -24312,25 +24455,27 @@
       <c r="CK145" s="14">
         <v>100</v>
       </c>
-      <c r="CL145" s="14">
+      <c r="CL145" s="29">
         <v>100</v>
       </c>
-      <c r="CM145" s="14">
+      <c r="CM145" s="29">
         <v>100</v>
       </c>
-      <c r="CN145" s="14">
+      <c r="CN145" s="29">
         <v>100</v>
       </c>
-      <c r="CO145" s="14">
+      <c r="CO145" s="29">
         <v>100</v>
       </c>
-      <c r="CP145" s="14">
+      <c r="CP145" s="29">
         <v>100</v>
       </c>
-      <c r="CQ145" s="14">
+      <c r="CQ145" s="29">
         <v>100</v>
       </c>
-      <c r="CR145" s="8"/>
+      <c r="CR145" s="29">
+        <v>100</v>
+      </c>
       <c r="CS145" s="8"/>
       <c r="CT145" s="8"/>
       <c r="CU145" s="8"/>
@@ -24477,12 +24622,13 @@
       <c r="CI146" s="11"/>
       <c r="CJ146" s="11"/>
       <c r="CK146" s="11"/>
-      <c r="CL146" s="11"/>
-      <c r="CM146" s="11"/>
-      <c r="CN146" s="11"/>
-      <c r="CO146" s="11"/>
-      <c r="CP146" s="11"/>
-      <c r="CQ146" s="11"/>
+      <c r="CL146" s="26"/>
+      <c r="CM146" s="26"/>
+      <c r="CN146" s="26"/>
+      <c r="CO146" s="26"/>
+      <c r="CP146" s="26"/>
+      <c r="CQ146" s="26"/>
+      <c r="CR146" s="26"/>
     </row>
     <row r="147" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="s">
@@ -24578,13 +24724,13 @@
       <c r="CI148" s="8"/>
       <c r="CJ148" s="8"/>
       <c r="CK148" s="8"/>
-      <c r="CL148" s="8"/>
-      <c r="CM148" s="8"/>
-      <c r="CN148" s="8"/>
-      <c r="CO148" s="8"/>
-      <c r="CP148" s="8"/>
-      <c r="CQ148" s="8"/>
-      <c r="CR148" s="8"/>
+      <c r="CL148" s="24"/>
+      <c r="CM148" s="24"/>
+      <c r="CN148" s="24"/>
+      <c r="CO148" s="24"/>
+      <c r="CP148" s="24"/>
+      <c r="CQ148" s="24"/>
+      <c r="CR148" s="24"/>
       <c r="CS148" s="8"/>
       <c r="CT148" s="8"/>
       <c r="CU148" s="8"/>
@@ -24730,13 +24876,13 @@
       <c r="CI149" s="8"/>
       <c r="CJ149" s="8"/>
       <c r="CK149" s="8"/>
-      <c r="CL149" s="8"/>
-      <c r="CM149" s="8"/>
-      <c r="CN149" s="8"/>
-      <c r="CO149" s="8"/>
-      <c r="CP149" s="8"/>
-      <c r="CQ149" s="8"/>
-      <c r="CR149" s="8"/>
+      <c r="CL149" s="24"/>
+      <c r="CM149" s="24"/>
+      <c r="CN149" s="24"/>
+      <c r="CO149" s="24"/>
+      <c r="CP149" s="24"/>
+      <c r="CQ149" s="24"/>
+      <c r="CR149" s="24"/>
       <c r="CS149" s="8"/>
       <c r="CT149" s="8"/>
       <c r="CU149" s="8"/>
@@ -24825,148 +24971,149 @@
     </row>
     <row r="158" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
-      <c r="B158" s="21">
+      <c r="B158" s="31">
         <v>2000</v>
       </c>
-      <c r="C158" s="21"/>
-      <c r="D158" s="21"/>
-      <c r="E158" s="21"/>
-      <c r="F158" s="21">
+      <c r="C158" s="31"/>
+      <c r="D158" s="31"/>
+      <c r="E158" s="31"/>
+      <c r="F158" s="31">
         <v>2001</v>
       </c>
-      <c r="G158" s="21"/>
-      <c r="H158" s="21"/>
-      <c r="I158" s="21"/>
-      <c r="J158" s="21">
+      <c r="G158" s="31"/>
+      <c r="H158" s="31"/>
+      <c r="I158" s="31"/>
+      <c r="J158" s="31">
         <v>2002</v>
       </c>
-      <c r="K158" s="21"/>
-      <c r="L158" s="21"/>
-      <c r="M158" s="21"/>
-      <c r="N158" s="21">
+      <c r="K158" s="31"/>
+      <c r="L158" s="31"/>
+      <c r="M158" s="31"/>
+      <c r="N158" s="31">
         <v>2003</v>
       </c>
-      <c r="O158" s="21"/>
-      <c r="P158" s="21"/>
-      <c r="Q158" s="21"/>
-      <c r="R158" s="21">
+      <c r="O158" s="31"/>
+      <c r="P158" s="31"/>
+      <c r="Q158" s="31"/>
+      <c r="R158" s="31">
         <v>2004</v>
       </c>
-      <c r="S158" s="21"/>
-      <c r="T158" s="21"/>
-      <c r="U158" s="21"/>
-      <c r="V158" s="21">
+      <c r="S158" s="31"/>
+      <c r="T158" s="31"/>
+      <c r="U158" s="31"/>
+      <c r="V158" s="31">
         <v>2005</v>
       </c>
-      <c r="W158" s="21"/>
-      <c r="X158" s="21"/>
-      <c r="Y158" s="21"/>
-      <c r="Z158" s="21">
+      <c r="W158" s="31"/>
+      <c r="X158" s="31"/>
+      <c r="Y158" s="31"/>
+      <c r="Z158" s="31">
         <v>2006</v>
       </c>
-      <c r="AA158" s="21"/>
-      <c r="AB158" s="21"/>
-      <c r="AC158" s="21"/>
-      <c r="AD158" s="21">
+      <c r="AA158" s="31"/>
+      <c r="AB158" s="31"/>
+      <c r="AC158" s="31"/>
+      <c r="AD158" s="31">
         <v>2007</v>
       </c>
-      <c r="AE158" s="21"/>
-      <c r="AF158" s="21"/>
-      <c r="AG158" s="21"/>
-      <c r="AH158" s="21">
+      <c r="AE158" s="31"/>
+      <c r="AF158" s="31"/>
+      <c r="AG158" s="31"/>
+      <c r="AH158" s="31">
         <v>2008</v>
       </c>
-      <c r="AI158" s="21"/>
-      <c r="AJ158" s="21"/>
-      <c r="AK158" s="21"/>
-      <c r="AL158" s="21">
+      <c r="AI158" s="31"/>
+      <c r="AJ158" s="31"/>
+      <c r="AK158" s="31"/>
+      <c r="AL158" s="31">
         <v>2009</v>
       </c>
-      <c r="AM158" s="21"/>
-      <c r="AN158" s="21"/>
-      <c r="AO158" s="21"/>
-      <c r="AP158" s="21">
+      <c r="AM158" s="31"/>
+      <c r="AN158" s="31"/>
+      <c r="AO158" s="31"/>
+      <c r="AP158" s="31">
         <v>2010</v>
       </c>
-      <c r="AQ158" s="21"/>
-      <c r="AR158" s="21"/>
-      <c r="AS158" s="21"/>
-      <c r="AT158" s="21">
+      <c r="AQ158" s="31"/>
+      <c r="AR158" s="31"/>
+      <c r="AS158" s="31"/>
+      <c r="AT158" s="31">
         <v>2011</v>
       </c>
-      <c r="AU158" s="21"/>
-      <c r="AV158" s="21"/>
-      <c r="AW158" s="21"/>
-      <c r="AX158" s="21">
+      <c r="AU158" s="31"/>
+      <c r="AV158" s="31"/>
+      <c r="AW158" s="31"/>
+      <c r="AX158" s="31">
         <v>2012</v>
       </c>
-      <c r="AY158" s="21"/>
-      <c r="AZ158" s="21"/>
-      <c r="BA158" s="21"/>
-      <c r="BB158" s="21">
+      <c r="AY158" s="31"/>
+      <c r="AZ158" s="31"/>
+      <c r="BA158" s="31"/>
+      <c r="BB158" s="31">
         <v>2013</v>
       </c>
-      <c r="BC158" s="21"/>
-      <c r="BD158" s="21"/>
-      <c r="BE158" s="21"/>
-      <c r="BF158" s="21">
+      <c r="BC158" s="31"/>
+      <c r="BD158" s="31"/>
+      <c r="BE158" s="31"/>
+      <c r="BF158" s="31">
         <v>2014</v>
       </c>
-      <c r="BG158" s="21"/>
-      <c r="BH158" s="21"/>
-      <c r="BI158" s="21"/>
-      <c r="BJ158" s="21">
+      <c r="BG158" s="31"/>
+      <c r="BH158" s="31"/>
+      <c r="BI158" s="31"/>
+      <c r="BJ158" s="31">
         <v>2015</v>
       </c>
-      <c r="BK158" s="21"/>
-      <c r="BL158" s="21"/>
-      <c r="BM158" s="21"/>
-      <c r="BN158" s="21">
+      <c r="BK158" s="31"/>
+      <c r="BL158" s="31"/>
+      <c r="BM158" s="31"/>
+      <c r="BN158" s="31">
         <v>2016</v>
       </c>
-      <c r="BO158" s="21"/>
-      <c r="BP158" s="21"/>
-      <c r="BQ158" s="21"/>
-      <c r="BR158" s="21">
+      <c r="BO158" s="31"/>
+      <c r="BP158" s="31"/>
+      <c r="BQ158" s="31"/>
+      <c r="BR158" s="31">
         <v>2017</v>
       </c>
-      <c r="BS158" s="21"/>
-      <c r="BT158" s="21"/>
-      <c r="BU158" s="21"/>
-      <c r="BV158" s="21">
+      <c r="BS158" s="31"/>
+      <c r="BT158" s="31"/>
+      <c r="BU158" s="31"/>
+      <c r="BV158" s="31">
         <v>2018</v>
       </c>
-      <c r="BW158" s="21"/>
-      <c r="BX158" s="21"/>
-      <c r="BY158" s="21"/>
-      <c r="BZ158" s="21">
+      <c r="BW158" s="31"/>
+      <c r="BX158" s="31"/>
+      <c r="BY158" s="31"/>
+      <c r="BZ158" s="31">
         <v>2019</v>
       </c>
-      <c r="CA158" s="21"/>
-      <c r="CB158" s="21"/>
-      <c r="CC158" s="21"/>
-      <c r="CD158" s="22">
+      <c r="CA158" s="31"/>
+      <c r="CB158" s="31"/>
+      <c r="CC158" s="31"/>
+      <c r="CD158" s="32">
         <v>2020</v>
       </c>
-      <c r="CE158" s="22"/>
-      <c r="CF158" s="22"/>
-      <c r="CG158" s="22"/>
-      <c r="CH158" s="22">
+      <c r="CE158" s="32"/>
+      <c r="CF158" s="32"/>
+      <c r="CG158" s="32"/>
+      <c r="CH158" s="32">
         <v>2021</v>
       </c>
-      <c r="CI158" s="22"/>
-      <c r="CJ158" s="22"/>
-      <c r="CK158" s="22"/>
-      <c r="CL158" s="22">
+      <c r="CI158" s="32"/>
+      <c r="CJ158" s="32"/>
+      <c r="CK158" s="32"/>
+      <c r="CL158" s="31">
         <v>2022</v>
       </c>
-      <c r="CM158" s="22"/>
-      <c r="CN158" s="22"/>
-      <c r="CO158" s="22"/>
-      <c r="CP158" s="22">
+      <c r="CM158" s="31"/>
+      <c r="CN158" s="31"/>
+      <c r="CO158" s="31"/>
+      <c r="CP158" s="31">
         <v>2023</v>
       </c>
-      <c r="CQ158" s="23"/>
+      <c r="CQ158" s="31"/>
+      <c r="CR158" s="31"/>
     </row>
     <row r="159" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A159" s="4"/>
@@ -25234,23 +25381,26 @@
       <c r="CK159" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CL159" s="13" t="s">
+      <c r="CL159" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CM159" s="13" t="s">
+      <c r="CM159" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="CN159" s="13" t="s">
+      <c r="CN159" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="CO159" s="13" t="s">
+      <c r="CO159" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="CP159" s="13" t="s">
+      <c r="CP159" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="CQ159" s="13" t="s">
+      <c r="CQ159" s="27" t="s">
         <v>8</v>
+      </c>
+      <c r="CR159" s="27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -25524,25 +25674,27 @@
       <c r="CK161" s="20">
         <v>5.7772458590307521</v>
       </c>
-      <c r="CL161" s="20">
+      <c r="CL161" s="30">
         <v>6.4586903187929448</v>
       </c>
-      <c r="CM161" s="20">
+      <c r="CM161" s="30">
         <v>4.1385663284785403</v>
       </c>
-      <c r="CN161" s="20">
+      <c r="CN161" s="30">
         <v>6.4069843265431619</v>
       </c>
-      <c r="CO161" s="20">
+      <c r="CO161" s="30">
         <v>7.9818538688371241</v>
       </c>
-      <c r="CP161" s="20">
+      <c r="CP161" s="30">
         <v>8.9701922768346183</v>
       </c>
-      <c r="CQ161" s="20">
-        <v>3.6726498998531447</v>
-      </c>
-      <c r="CR161" s="8"/>
+      <c r="CQ161" s="30">
+        <v>3.4518900528178751</v>
+      </c>
+      <c r="CR161" s="30">
+        <v>6.8115502027439527</v>
+      </c>
       <c r="CS161" s="8"/>
       <c r="CT161" s="8"/>
       <c r="CU161" s="8"/>
@@ -25867,25 +26019,27 @@
       <c r="CK162" s="20">
         <v>0.17467265771166715</v>
       </c>
-      <c r="CL162" s="20">
+      <c r="CL162" s="30">
         <v>8.3365702231303115E-2</v>
       </c>
-      <c r="CM162" s="20">
+      <c r="CM162" s="30">
         <v>5.9398819865764195E-2</v>
       </c>
-      <c r="CN162" s="20">
+      <c r="CN162" s="30">
         <v>0.14074462376520538</v>
       </c>
-      <c r="CO162" s="20">
+      <c r="CO162" s="30">
         <v>0.16535615081173041</v>
       </c>
-      <c r="CP162" s="20">
+      <c r="CP162" s="30">
         <v>5.3591170489628352E-2</v>
       </c>
-      <c r="CQ162" s="20">
-        <v>5.4213051797892466E-2</v>
-      </c>
-      <c r="CR162" s="8"/>
+      <c r="CQ162" s="30">
+        <v>5.5579195779999334E-2</v>
+      </c>
+      <c r="CR162" s="30">
+        <v>0.12895075140310977</v>
+      </c>
       <c r="CS162" s="8"/>
       <c r="CT162" s="8"/>
       <c r="CU162" s="8"/>
@@ -26210,25 +26364,27 @@
       <c r="CK163" s="20">
         <v>2.7674485056923839</v>
       </c>
-      <c r="CL163" s="20">
+      <c r="CL163" s="30">
         <v>2.4995504275256444</v>
       </c>
-      <c r="CM163" s="20">
+      <c r="CM163" s="30">
         <v>8.911620089896747</v>
       </c>
-      <c r="CN163" s="20">
+      <c r="CN163" s="30">
         <v>16.119529344341789</v>
       </c>
-      <c r="CO163" s="20">
+      <c r="CO163" s="30">
         <v>10.2011073825906</v>
       </c>
-      <c r="CP163" s="20">
+      <c r="CP163" s="30">
         <v>14.182637348627166</v>
       </c>
-      <c r="CQ163" s="20">
-        <v>15.30195996802601</v>
-      </c>
-      <c r="CR163" s="8"/>
+      <c r="CQ163" s="30">
+        <v>15.196254462418146</v>
+      </c>
+      <c r="CR163" s="30">
+        <v>22.69882058054359</v>
+      </c>
       <c r="CS163" s="8"/>
       <c r="CT163" s="8"/>
       <c r="CU163" s="8"/>
@@ -26553,25 +26709,27 @@
       <c r="CK164" s="20">
         <v>0.87264213018068471</v>
       </c>
-      <c r="CL164" s="20">
+      <c r="CL164" s="30">
         <v>0.55785951527030686</v>
       </c>
-      <c r="CM164" s="20">
+      <c r="CM164" s="30">
         <v>0.61229989214461655</v>
       </c>
-      <c r="CN164" s="20">
+      <c r="CN164" s="30">
         <v>0.71867427343568591</v>
       </c>
-      <c r="CO164" s="20">
+      <c r="CO164" s="30">
         <v>0.73957934408039272</v>
       </c>
-      <c r="CP164" s="20">
+      <c r="CP164" s="30">
         <v>0.53357666534338333</v>
       </c>
-      <c r="CQ164" s="20">
-        <v>0.63536633357314132</v>
-      </c>
-      <c r="CR164" s="8"/>
+      <c r="CQ164" s="30">
+        <v>0.6211972612261899</v>
+      </c>
+      <c r="CR164" s="30">
+        <v>0.72797524390114443</v>
+      </c>
       <c r="CS164" s="8"/>
       <c r="CT164" s="8"/>
       <c r="CU164" s="8"/>
@@ -26896,25 +27054,27 @@
       <c r="CK165" s="20">
         <v>16.405668592360829</v>
       </c>
-      <c r="CL165" s="20">
+      <c r="CL165" s="30">
         <v>18.951192764948299</v>
       </c>
-      <c r="CM165" s="20">
+      <c r="CM165" s="30">
         <v>17.785181361601524</v>
       </c>
-      <c r="CN165" s="20">
+      <c r="CN165" s="30">
         <v>15.127593432922945</v>
       </c>
-      <c r="CO165" s="20">
+      <c r="CO165" s="30">
         <v>15.896808419825733</v>
       </c>
-      <c r="CP165" s="20">
+      <c r="CP165" s="30">
         <v>17.791344989241704</v>
       </c>
-      <c r="CQ165" s="20">
-        <v>17.652401980290779</v>
-      </c>
-      <c r="CR165" s="8"/>
+      <c r="CQ165" s="30">
+        <v>17.940895219784647</v>
+      </c>
+      <c r="CR165" s="30">
+        <v>14.359027504133287</v>
+      </c>
       <c r="CS165" s="8"/>
       <c r="CT165" s="8"/>
       <c r="CU165" s="8"/>
@@ -27239,25 +27399,27 @@
       <c r="CK166" s="20">
         <v>60.630953060817014</v>
       </c>
-      <c r="CL166" s="20">
+      <c r="CL166" s="30">
         <v>58.044220266448377</v>
       </c>
-      <c r="CM166" s="20">
+      <c r="CM166" s="30">
         <v>56.342870326104055</v>
       </c>
-      <c r="CN166" s="20">
+      <c r="CN166" s="30">
         <v>51.100317624662694</v>
       </c>
-      <c r="CO166" s="20">
+      <c r="CO166" s="30">
         <v>52.545643538551502</v>
       </c>
-      <c r="CP166" s="20">
+      <c r="CP166" s="30">
         <v>49.944576762366964</v>
       </c>
-      <c r="CQ166" s="20">
-        <v>52.364547293168606</v>
-      </c>
-      <c r="CR166" s="8"/>
+      <c r="CQ166" s="30">
+        <v>52.11741005755858</v>
+      </c>
+      <c r="CR166" s="30">
+        <v>45.688326560593588</v>
+      </c>
       <c r="CS166" s="8"/>
       <c r="CT166" s="8"/>
       <c r="CU166" s="8"/>
@@ -27582,25 +27744,27 @@
       <c r="CK167" s="20">
         <v>11.801617241714322</v>
       </c>
-      <c r="CL167" s="20">
+      <c r="CL167" s="30">
         <v>12.392135547770765</v>
       </c>
-      <c r="CM167" s="20">
+      <c r="CM167" s="30">
         <v>10.860189371072559</v>
       </c>
-      <c r="CN167" s="20">
+      <c r="CN167" s="30">
         <v>8.8673750202839567</v>
       </c>
-      <c r="CO167" s="20">
+      <c r="CO167" s="30">
         <v>10.659285741136884</v>
       </c>
-      <c r="CP167" s="20">
+      <c r="CP167" s="30">
         <v>7.5387080999438281</v>
       </c>
-      <c r="CQ167" s="20">
-        <v>8.6344841182179728</v>
-      </c>
-      <c r="CR167" s="8"/>
+      <c r="CQ167" s="30">
+        <v>9.3209452903791821</v>
+      </c>
+      <c r="CR167" s="30">
+        <v>8.3539791863255921</v>
+      </c>
       <c r="CS167" s="8"/>
       <c r="CT167" s="8"/>
       <c r="CU167" s="8"/>
@@ -27925,25 +28089,27 @@
       <c r="CK168" s="20">
         <v>1.5697519524923442</v>
       </c>
-      <c r="CL168" s="20">
+      <c r="CL168" s="30">
         <v>1.012985457012362</v>
       </c>
-      <c r="CM168" s="20">
+      <c r="CM168" s="30">
         <v>1.2898738108361971</v>
       </c>
-      <c r="CN168" s="20">
+      <c r="CN168" s="30">
         <v>1.5187813540445654</v>
       </c>
-      <c r="CO168" s="20">
+      <c r="CO168" s="30">
         <v>1.8103655541660508</v>
       </c>
-      <c r="CP168" s="20">
+      <c r="CP168" s="30">
         <v>0.98537268715271287</v>
       </c>
-      <c r="CQ168" s="20">
-        <v>1.6843773550724355</v>
-      </c>
-      <c r="CR168" s="8"/>
+      <c r="CQ168" s="30">
+        <v>1.2958284600353802</v>
+      </c>
+      <c r="CR168" s="30">
+        <v>1.2313699703557595</v>
+      </c>
       <c r="CS168" s="8"/>
       <c r="CT168" s="8"/>
       <c r="CU168" s="8"/>
@@ -28089,13 +28255,13 @@
       <c r="CI169" s="8"/>
       <c r="CJ169" s="8"/>
       <c r="CK169" s="8"/>
-      <c r="CL169" s="8"/>
-      <c r="CM169" s="8"/>
-      <c r="CN169" s="8"/>
-      <c r="CO169" s="8"/>
-      <c r="CP169" s="8"/>
-      <c r="CQ169" s="8"/>
-      <c r="CR169" s="8"/>
+      <c r="CL169" s="24"/>
+      <c r="CM169" s="24"/>
+      <c r="CN169" s="24"/>
+      <c r="CO169" s="24"/>
+      <c r="CP169" s="24"/>
+      <c r="CQ169" s="24"/>
+      <c r="CR169" s="24"/>
       <c r="CS169" s="8"/>
       <c r="CT169" s="8"/>
       <c r="CU169" s="8"/>
@@ -28420,25 +28586,27 @@
       <c r="CK170" s="14">
         <v>100</v>
       </c>
-      <c r="CL170" s="14">
+      <c r="CL170" s="29">
         <v>100</v>
       </c>
-      <c r="CM170" s="14">
+      <c r="CM170" s="29">
         <v>100</v>
       </c>
-      <c r="CN170" s="14">
+      <c r="CN170" s="29">
         <v>100</v>
       </c>
-      <c r="CO170" s="14">
+      <c r="CO170" s="29">
         <v>100</v>
       </c>
-      <c r="CP170" s="14">
+      <c r="CP170" s="29">
         <v>100</v>
       </c>
-      <c r="CQ170" s="14">
+      <c r="CQ170" s="29">
         <v>100</v>
       </c>
-      <c r="CR170" s="8"/>
+      <c r="CR170" s="29">
+        <v>100</v>
+      </c>
       <c r="CS170" s="8"/>
       <c r="CT170" s="8"/>
       <c r="CU170" s="8"/>
@@ -28585,12 +28753,13 @@
       <c r="CI171" s="11"/>
       <c r="CJ171" s="11"/>
       <c r="CK171" s="11"/>
-      <c r="CL171" s="11"/>
-      <c r="CM171" s="11"/>
-      <c r="CN171" s="11"/>
-      <c r="CO171" s="11"/>
-      <c r="CP171" s="11"/>
-      <c r="CQ171" s="11"/>
+      <c r="CL171" s="26"/>
+      <c r="CM171" s="26"/>
+      <c r="CN171" s="26"/>
+      <c r="CO171" s="26"/>
+      <c r="CP171" s="26"/>
+      <c r="CQ171" s="26"/>
+      <c r="CR171" s="26"/>
     </row>
     <row r="172" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A172" s="12" t="s">
@@ -28687,13 +28856,13 @@
       <c r="CI173" s="1"/>
       <c r="CJ173" s="1"/>
       <c r="CK173" s="1"/>
-      <c r="CL173" s="1"/>
-      <c r="CM173" s="1"/>
-      <c r="CN173" s="1"/>
-      <c r="CO173" s="1"/>
-      <c r="CP173" s="1"/>
-      <c r="CQ173" s="1"/>
-      <c r="CR173" s="16"/>
+      <c r="CL173" s="22"/>
+      <c r="CM173" s="22"/>
+      <c r="CN173" s="22"/>
+      <c r="CO173" s="22"/>
+      <c r="CP173" s="22"/>
+      <c r="CQ173" s="22"/>
+      <c r="CR173" s="22"/>
       <c r="CS173" s="16"/>
       <c r="CT173" s="16"/>
       <c r="CU173" s="16"/>
@@ -28840,13 +29009,13 @@
       <c r="CI174" s="1"/>
       <c r="CJ174" s="1"/>
       <c r="CK174" s="1"/>
-      <c r="CL174" s="1"/>
-      <c r="CM174" s="1"/>
-      <c r="CN174" s="1"/>
-      <c r="CO174" s="1"/>
-      <c r="CP174" s="1"/>
-      <c r="CQ174" s="1"/>
-      <c r="CR174" s="16"/>
+      <c r="CL174" s="22"/>
+      <c r="CM174" s="22"/>
+      <c r="CN174" s="22"/>
+      <c r="CO174" s="22"/>
+      <c r="CP174" s="22"/>
+      <c r="CQ174" s="22"/>
+      <c r="CR174" s="22"/>
       <c r="CS174" s="16"/>
       <c r="CT174" s="16"/>
       <c r="CU174" s="16"/>
@@ -28904,16 +29073,12 @@
       <c r="EU174" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="168">
-    <mergeCell ref="CP9:CQ9"/>
-    <mergeCell ref="CP34:CQ34"/>
-    <mergeCell ref="CP108:CQ108"/>
-    <mergeCell ref="CP133:CQ133"/>
-    <mergeCell ref="CP158:CQ158"/>
-    <mergeCell ref="CL59:CO59"/>
-    <mergeCell ref="CP59:CQ59"/>
-    <mergeCell ref="CL84:CO84"/>
-    <mergeCell ref="CP84:CQ84"/>
+  <mergeCells count="166">
+    <mergeCell ref="CP9:CR9"/>
+    <mergeCell ref="CP34:CR34"/>
+    <mergeCell ref="CP108:CR108"/>
+    <mergeCell ref="CP133:CR133"/>
+    <mergeCell ref="CP158:CR158"/>
     <mergeCell ref="CH133:CK133"/>
     <mergeCell ref="CH158:CK158"/>
     <mergeCell ref="CL9:CO9"/>
@@ -28924,6 +29089,8 @@
     <mergeCell ref="CD9:CG9"/>
     <mergeCell ref="BV9:BY9"/>
     <mergeCell ref="BZ9:CC9"/>
+    <mergeCell ref="CL59:CN59"/>
+    <mergeCell ref="CL84:CN84"/>
     <mergeCell ref="BR9:BU9"/>
     <mergeCell ref="CH9:CK9"/>
     <mergeCell ref="CH34:CK34"/>
@@ -29078,9 +29245,9 @@
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="50" max="94" man="1"/>
-    <brk id="100" max="94" man="1"/>
-    <brk id="124" max="94" man="1"/>
+    <brk id="50" max="95" man="1"/>
+    <brk id="100" max="95" man="1"/>
+    <brk id="124" max="95" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q2 2024 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of May 2024\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2024\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56DB849-85C0-4F6D-AB81-BA9890FF7A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CC2A88-56D7-439B-8BAE-7B3458D5F98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="975" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="58">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -222,13 +222,13 @@
     <t>2023 - 2024</t>
   </si>
   <si>
-    <t>Q1 2000 to Q1 2024</t>
+    <t>As of August 2024</t>
   </si>
   <si>
-    <t>Q1 2001 to Q1 2024</t>
+    <t>Q1 2000 to Q2 2024</t>
   </si>
   <si>
-    <t>As of May 2024</t>
+    <t>Q1 2001 to Q2 2024</t>
   </si>
 </sst>
 </file>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -354,35 +354,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -727,16 +711,15 @@
       <selection activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="topRight" activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="bottomLeft" activeCell="P1" sqref="P1:AF1048576"/>
-      <selection pane="bottomRight" activeCell="CX12" sqref="CX12"/>
+      <selection pane="bottomRight" activeCell="CP1" sqref="CP1:CU1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.77734375" style="1" customWidth="1"/>
     <col min="2" max="73" width="8.77734375" style="1" customWidth="1"/>
-    <col min="74" max="93" width="10" style="1" customWidth="1"/>
-    <col min="94" max="98" width="9.6640625" style="23" customWidth="1"/>
-    <col min="99" max="16384" width="7.77734375" style="1"/>
+    <col min="74" max="99" width="10" style="1" customWidth="1"/>
+    <col min="100" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:151" x14ac:dyDescent="0.2">
@@ -751,7 +734,7 @@
     </row>
     <row r="3" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:151" x14ac:dyDescent="0.2">
@@ -761,7 +744,7 @@
     </row>
     <row r="6" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:151" x14ac:dyDescent="0.2">
@@ -771,132 +754,132 @@
     </row>
     <row r="9" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="36">
+      <c r="B9" s="25">
         <v>2000</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25">
         <v>2001</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36">
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25">
         <v>2002</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36">
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25">
         <v>2003</v>
       </c>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36">
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25">
         <v>2004</v>
       </c>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="36"/>
-      <c r="V9" s="36">
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25">
         <v>2005</v>
       </c>
-      <c r="W9" s="36"/>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="36">
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25">
         <v>2006</v>
       </c>
-      <c r="AA9" s="36"/>
-      <c r="AB9" s="36"/>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36">
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AD9" s="25">
         <v>2007</v>
       </c>
-      <c r="AE9" s="36"/>
-      <c r="AF9" s="36"/>
-      <c r="AG9" s="36"/>
-      <c r="AH9" s="36">
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25">
         <v>2008</v>
       </c>
-      <c r="AI9" s="36"/>
-      <c r="AJ9" s="36"/>
-      <c r="AK9" s="36"/>
-      <c r="AL9" s="36">
+      <c r="AI9" s="25"/>
+      <c r="AJ9" s="25"/>
+      <c r="AK9" s="25"/>
+      <c r="AL9" s="25">
         <v>2009</v>
       </c>
-      <c r="AM9" s="36"/>
-      <c r="AN9" s="36"/>
-      <c r="AO9" s="36"/>
-      <c r="AP9" s="36">
+      <c r="AM9" s="25"/>
+      <c r="AN9" s="25"/>
+      <c r="AO9" s="25"/>
+      <c r="AP9" s="25">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="36"/>
-      <c r="AR9" s="36"/>
-      <c r="AS9" s="36"/>
-      <c r="AT9" s="36">
+      <c r="AQ9" s="25"/>
+      <c r="AR9" s="25"/>
+      <c r="AS9" s="25"/>
+      <c r="AT9" s="25">
         <v>2011</v>
       </c>
-      <c r="AU9" s="36"/>
-      <c r="AV9" s="36"/>
-      <c r="AW9" s="36"/>
-      <c r="AX9" s="36">
+      <c r="AU9" s="25"/>
+      <c r="AV9" s="25"/>
+      <c r="AW9" s="25"/>
+      <c r="AX9" s="25">
         <v>2012</v>
       </c>
-      <c r="AY9" s="36"/>
-      <c r="AZ9" s="36"/>
-      <c r="BA9" s="36"/>
-      <c r="BB9" s="36">
+      <c r="AY9" s="25"/>
+      <c r="AZ9" s="25"/>
+      <c r="BA9" s="25"/>
+      <c r="BB9" s="25">
         <v>2013</v>
       </c>
-      <c r="BC9" s="36"/>
-      <c r="BD9" s="36"/>
-      <c r="BE9" s="36"/>
-      <c r="BF9" s="36">
+      <c r="BC9" s="25"/>
+      <c r="BD9" s="25"/>
+      <c r="BE9" s="25"/>
+      <c r="BF9" s="25">
         <v>2014</v>
       </c>
-      <c r="BG9" s="36"/>
-      <c r="BH9" s="36"/>
-      <c r="BI9" s="36"/>
-      <c r="BJ9" s="36">
+      <c r="BG9" s="25"/>
+      <c r="BH9" s="25"/>
+      <c r="BI9" s="25"/>
+      <c r="BJ9" s="25">
         <v>2015</v>
       </c>
-      <c r="BK9" s="36"/>
-      <c r="BL9" s="36"/>
-      <c r="BM9" s="36"/>
-      <c r="BN9" s="36">
+      <c r="BK9" s="25"/>
+      <c r="BL9" s="25"/>
+      <c r="BM9" s="25"/>
+      <c r="BN9" s="25">
         <v>2016</v>
       </c>
-      <c r="BO9" s="36"/>
-      <c r="BP9" s="36"/>
-      <c r="BQ9" s="36"/>
-      <c r="BR9" s="36">
+      <c r="BO9" s="25"/>
+      <c r="BP9" s="25"/>
+      <c r="BQ9" s="25"/>
+      <c r="BR9" s="25">
         <v>2017</v>
       </c>
-      <c r="BS9" s="36"/>
-      <c r="BT9" s="36"/>
-      <c r="BU9" s="36"/>
-      <c r="BV9" s="36">
+      <c r="BS9" s="25"/>
+      <c r="BT9" s="25"/>
+      <c r="BU9" s="25"/>
+      <c r="BV9" s="25">
         <v>2018</v>
       </c>
-      <c r="BW9" s="36"/>
-      <c r="BX9" s="36"/>
-      <c r="BY9" s="36"/>
-      <c r="BZ9" s="36">
+      <c r="BW9" s="25"/>
+      <c r="BX9" s="25"/>
+      <c r="BY9" s="25"/>
+      <c r="BZ9" s="25">
         <v>2019</v>
       </c>
-      <c r="CA9" s="36"/>
-      <c r="CB9" s="36"/>
-      <c r="CC9" s="36"/>
-      <c r="CD9" s="36">
+      <c r="CA9" s="25"/>
+      <c r="CB9" s="25"/>
+      <c r="CC9" s="25"/>
+      <c r="CD9" s="25">
         <v>2020</v>
       </c>
-      <c r="CE9" s="36"/>
-      <c r="CF9" s="36"/>
-      <c r="CG9" s="36"/>
+      <c r="CE9" s="25"/>
+      <c r="CF9" s="25"/>
+      <c r="CG9" s="25"/>
       <c r="CH9" s="21">
         <v>2021</v>
       </c>
@@ -909,15 +892,16 @@
       <c r="CM9" s="21"/>
       <c r="CN9" s="21"/>
       <c r="CO9" s="21"/>
-      <c r="CP9" s="24">
+      <c r="CP9" s="21">
         <v>2023</v>
       </c>
-      <c r="CQ9" s="24"/>
-      <c r="CR9" s="24"/>
-      <c r="CS9" s="24"/>
-      <c r="CT9" s="24">
+      <c r="CQ9" s="21"/>
+      <c r="CR9" s="21"/>
+      <c r="CS9" s="21"/>
+      <c r="CT9" s="21">
         <v>2024</v>
       </c>
+      <c r="CU9" s="21"/>
     </row>
     <row r="10" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -1197,20 +1181,23 @@
       <c r="CO10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CP10" s="13" t="s">
+      <c r="CP10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="CQ10" s="13" t="s">
+      <c r="CQ10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="CR10" s="13" t="s">
+      <c r="CR10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="CS10" s="13" t="s">
+      <c r="CS10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CT10" s="13" t="s">
+      <c r="CT10" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="CU10" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1496,22 +1483,24 @@
       <c r="CO12" s="18">
         <v>54545.476736266144</v>
       </c>
-      <c r="CP12" s="25">
+      <c r="CP12" s="18">
         <v>91388.504694742951</v>
       </c>
-      <c r="CQ12" s="25">
+      <c r="CQ12" s="18">
         <v>34472.852940256031</v>
       </c>
-      <c r="CR12" s="25">
+      <c r="CR12" s="18">
         <v>51853.834593934924</v>
       </c>
-      <c r="CS12" s="25">
+      <c r="CS12" s="18">
         <v>61415.796931664518</v>
       </c>
-      <c r="CT12" s="25">
-        <v>100665.95681405888</v>
-      </c>
-      <c r="CU12" s="8"/>
+      <c r="CT12" s="18">
+        <v>102696.07234617718</v>
+      </c>
+      <c r="CU12" s="18">
+        <v>38145.561898129105</v>
+      </c>
       <c r="CV12" s="8"/>
       <c r="CW12" s="8"/>
       <c r="CX12" s="8"/>
@@ -1845,22 +1834,24 @@
       <c r="CO13" s="18">
         <v>1000.4370497140442</v>
       </c>
-      <c r="CP13" s="25">
+      <c r="CP13" s="18">
         <v>480.04158316722192</v>
       </c>
-      <c r="CQ13" s="25">
+      <c r="CQ13" s="18">
         <v>464.05012427240712</v>
       </c>
-      <c r="CR13" s="25">
+      <c r="CR13" s="18">
         <v>930.61252590324239</v>
       </c>
-      <c r="CS13" s="25">
+      <c r="CS13" s="18">
         <v>942.90067939335495</v>
       </c>
-      <c r="CT13" s="25">
-        <v>554.11170074826589</v>
-      </c>
-      <c r="CU13" s="8"/>
+      <c r="CT13" s="18">
+        <v>534.38963333813354</v>
+      </c>
+      <c r="CU13" s="18">
+        <v>519.70697381865602</v>
+      </c>
       <c r="CV13" s="8"/>
       <c r="CW13" s="8"/>
       <c r="CX13" s="8"/>
@@ -2194,22 +2185,24 @@
       <c r="CO14" s="18">
         <v>64203.136054041541</v>
       </c>
-      <c r="CP14" s="25">
+      <c r="CP14" s="18">
         <v>128049.61270907105</v>
       </c>
-      <c r="CQ14" s="25">
+      <c r="CQ14" s="18">
         <v>132330.33872905793</v>
       </c>
-      <c r="CR14" s="25">
+      <c r="CR14" s="18">
         <v>174583.24150521151</v>
       </c>
-      <c r="CS14" s="25">
+      <c r="CS14" s="18">
         <v>107496.30220590543</v>
       </c>
-      <c r="CT14" s="25">
+      <c r="CT14" s="18">
         <v>151426.10425368711</v>
       </c>
-      <c r="CU14" s="8"/>
+      <c r="CU14" s="18">
+        <v>167362.97894372992</v>
+      </c>
       <c r="CV14" s="8"/>
       <c r="CW14" s="8"/>
       <c r="CX14" s="8"/>
@@ -2543,22 +2536,24 @@
       <c r="CO15" s="18">
         <v>4595.0686874499042</v>
       </c>
-      <c r="CP15" s="25">
+      <c r="CP15" s="18">
         <v>4570.1940500558103</v>
       </c>
-      <c r="CQ15" s="25">
+      <c r="CQ15" s="18">
         <v>5139.0553496337761</v>
       </c>
-      <c r="CR15" s="25">
+      <c r="CR15" s="18">
         <v>5303.5480278897912</v>
       </c>
-      <c r="CS15" s="25">
+      <c r="CS15" s="18">
         <v>5496.1059442223577</v>
       </c>
-      <c r="CT15" s="25">
-        <v>5221.04502611514</v>
-      </c>
-      <c r="CU15" s="8"/>
+      <c r="CT15" s="18">
+        <v>4977.9404636384443</v>
+      </c>
+      <c r="CU15" s="18">
+        <v>5391.142877497583</v>
+      </c>
       <c r="CV15" s="8"/>
       <c r="CW15" s="8"/>
       <c r="CX15" s="8"/>
@@ -2892,22 +2887,24 @@
       <c r="CO16" s="18">
         <v>88349.252531254111</v>
       </c>
-      <c r="CP16" s="25">
+      <c r="CP16" s="18">
         <v>136255.87042386705</v>
       </c>
-      <c r="CQ16" s="25">
+      <c r="CQ16" s="18">
         <v>132006.04495852461</v>
       </c>
-      <c r="CR16" s="25">
+      <c r="CR16" s="18">
         <v>90834.805619856139</v>
       </c>
-      <c r="CS16" s="25">
+      <c r="CS16" s="18">
         <v>100998.99676650774</v>
       </c>
-      <c r="CT16" s="25">
-        <v>146104.69416379082</v>
-      </c>
-      <c r="CU16" s="8"/>
+      <c r="CT16" s="18">
+        <v>144427.11597770988</v>
+      </c>
+      <c r="CU16" s="18">
+        <v>142487.33049555379</v>
+      </c>
       <c r="CV16" s="8"/>
       <c r="CW16" s="8"/>
       <c r="CX16" s="8"/>
@@ -3241,22 +3238,24 @@
       <c r="CO17" s="18">
         <v>330617.25478872925</v>
       </c>
-      <c r="CP17" s="25">
+      <c r="CP17" s="18">
         <v>438940.2579160161</v>
       </c>
-      <c r="CQ17" s="25">
+      <c r="CQ17" s="18">
         <v>442320.61266757833</v>
       </c>
-      <c r="CR17" s="25">
+      <c r="CR17" s="18">
         <v>334923.1459927574</v>
       </c>
-      <c r="CS17" s="25">
+      <c r="CS17" s="18">
         <v>354637.50058273773</v>
       </c>
-      <c r="CT17" s="25">
-        <v>490017.52442568971</v>
-      </c>
-      <c r="CU17" s="8"/>
+      <c r="CT17" s="18">
+        <v>489463.82320816326</v>
+      </c>
+      <c r="CU17" s="18">
+        <v>472218.42256727559</v>
+      </c>
       <c r="CV17" s="8"/>
       <c r="CW17" s="8"/>
       <c r="CX17" s="8"/>
@@ -3590,22 +3589,24 @@
       <c r="CO18" s="18">
         <v>66718.593327664843</v>
       </c>
-      <c r="CP18" s="25">
+      <c r="CP18" s="18">
         <v>68561.433407578908</v>
       </c>
-      <c r="CQ18" s="25">
+      <c r="CQ18" s="18">
         <v>79162.752002960682</v>
       </c>
-      <c r="CR18" s="25">
+      <c r="CR18" s="18">
         <v>65974.839012592245</v>
       </c>
-      <c r="CS18" s="25">
+      <c r="CS18" s="18">
         <v>72001.17877859922</v>
       </c>
-      <c r="CT18" s="25">
-        <v>71295.046251172957</v>
-      </c>
-      <c r="CU18" s="8"/>
+      <c r="CT18" s="18">
+        <v>74272.253945248944</v>
+      </c>
+      <c r="CU18" s="18">
+        <v>83334.967220423583</v>
+      </c>
       <c r="CV18" s="8"/>
       <c r="CW18" s="8"/>
       <c r="CX18" s="8"/>
@@ -3939,22 +3940,24 @@
       <c r="CO19" s="18">
         <v>11024.543795387575</v>
       </c>
-      <c r="CP19" s="25">
+      <c r="CP19" s="18">
         <v>8484.317640903666</v>
       </c>
-      <c r="CQ19" s="25">
+      <c r="CQ19" s="18">
         <v>11183.54873158895</v>
       </c>
-      <c r="CR19" s="25">
+      <c r="CR19" s="18">
         <v>9272.9031053682593</v>
       </c>
-      <c r="CS19" s="25">
+      <c r="CS19" s="18">
         <v>12603.042609203625</v>
       </c>
-      <c r="CT19" s="25">
-        <v>8753.4010204739516</v>
-      </c>
-      <c r="CU19" s="8"/>
+      <c r="CT19" s="18">
+        <v>9152.9725122828659</v>
+      </c>
+      <c r="CU19" s="18">
+        <v>14514.532929209307</v>
+      </c>
       <c r="CV19" s="8"/>
       <c r="CW19" s="8"/>
       <c r="CX19" s="8"/>
@@ -4101,11 +4104,11 @@
       <c r="CM20" s="8"/>
       <c r="CN20" s="8"/>
       <c r="CO20" s="8"/>
-      <c r="CP20" s="26"/>
-      <c r="CQ20" s="26"/>
-      <c r="CR20" s="26"/>
-      <c r="CS20" s="26"/>
-      <c r="CT20" s="26"/>
+      <c r="CP20" s="8"/>
+      <c r="CQ20" s="8"/>
+      <c r="CR20" s="8"/>
+      <c r="CS20" s="8"/>
+      <c r="CT20" s="8"/>
       <c r="CU20" s="8"/>
       <c r="CV20" s="8"/>
       <c r="CW20" s="8"/>
@@ -4440,22 +4443,24 @@
       <c r="CO21" s="19">
         <v>621053.76297050749</v>
       </c>
-      <c r="CP21" s="27">
+      <c r="CP21" s="19">
         <v>876730.23242540262</v>
       </c>
-      <c r="CQ21" s="27">
+      <c r="CQ21" s="19">
         <v>837079.25550387276</v>
       </c>
-      <c r="CR21" s="27">
+      <c r="CR21" s="19">
         <v>733676.93038351345</v>
       </c>
-      <c r="CS21" s="27">
+      <c r="CS21" s="19">
         <v>715591.82449823397</v>
       </c>
-      <c r="CT21" s="27">
-        <v>974037.8836557368</v>
-      </c>
-      <c r="CU21" s="8"/>
+      <c r="CT21" s="19">
+        <v>976950.6723402458</v>
+      </c>
+      <c r="CU21" s="19">
+        <v>923974.64390563755</v>
+      </c>
       <c r="CV21" s="8"/>
       <c r="CW21" s="8"/>
       <c r="CX21" s="8"/>
@@ -4603,11 +4608,12 @@
       <c r="CM22" s="11"/>
       <c r="CN22" s="11"/>
       <c r="CO22" s="11"/>
-      <c r="CP22" s="28"/>
-      <c r="CQ22" s="28"/>
-      <c r="CR22" s="28"/>
-      <c r="CS22" s="28"/>
-      <c r="CT22" s="28"/>
+      <c r="CP22" s="11"/>
+      <c r="CQ22" s="11"/>
+      <c r="CR22" s="11"/>
+      <c r="CS22" s="11"/>
+      <c r="CT22" s="11"/>
+      <c r="CU22" s="11"/>
     </row>
     <row r="23" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
@@ -4707,11 +4713,11 @@
       <c r="CM24" s="8"/>
       <c r="CN24" s="8"/>
       <c r="CO24" s="8"/>
-      <c r="CP24" s="26"/>
-      <c r="CQ24" s="26"/>
-      <c r="CR24" s="26"/>
-      <c r="CS24" s="26"/>
-      <c r="CT24" s="26"/>
+      <c r="CP24" s="8"/>
+      <c r="CQ24" s="8"/>
+      <c r="CR24" s="8"/>
+      <c r="CS24" s="8"/>
+      <c r="CT24" s="8"/>
       <c r="CU24" s="8"/>
       <c r="CV24" s="8"/>
       <c r="CW24" s="8"/>
@@ -4859,11 +4865,11 @@
       <c r="CM25" s="8"/>
       <c r="CN25" s="8"/>
       <c r="CO25" s="8"/>
-      <c r="CP25" s="26"/>
-      <c r="CQ25" s="26"/>
-      <c r="CR25" s="26"/>
-      <c r="CS25" s="26"/>
-      <c r="CT25" s="26"/>
+      <c r="CP25" s="8"/>
+      <c r="CQ25" s="8"/>
+      <c r="CR25" s="8"/>
+      <c r="CS25" s="8"/>
+      <c r="CT25" s="8"/>
       <c r="CU25" s="8"/>
       <c r="CV25" s="8"/>
       <c r="CW25" s="8"/>
@@ -4930,7 +4936,7 @@
     </row>
     <row r="28" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:151" x14ac:dyDescent="0.2">
@@ -4940,7 +4946,7 @@
     </row>
     <row r="31" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:151" x14ac:dyDescent="0.2">
@@ -4950,132 +4956,132 @@
     </row>
     <row r="34" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-      <c r="B34" s="35">
+      <c r="B34" s="26">
         <v>2000</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26">
         <v>2001</v>
       </c>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35">
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26">
         <v>2002</v>
       </c>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35">
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26">
         <v>2003</v>
       </c>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35">
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26">
         <v>2004</v>
       </c>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35">
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26">
         <v>2005</v>
       </c>
-      <c r="W34" s="35"/>
-      <c r="X34" s="35"/>
-      <c r="Y34" s="35"/>
-      <c r="Z34" s="35">
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+      <c r="Y34" s="26"/>
+      <c r="Z34" s="26">
         <v>2006</v>
       </c>
-      <c r="AA34" s="35"/>
-      <c r="AB34" s="35"/>
-      <c r="AC34" s="35"/>
-      <c r="AD34" s="35">
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="26"/>
+      <c r="AC34" s="26"/>
+      <c r="AD34" s="26">
         <v>2007</v>
       </c>
-      <c r="AE34" s="35"/>
-      <c r="AF34" s="35"/>
-      <c r="AG34" s="35"/>
-      <c r="AH34" s="35">
+      <c r="AE34" s="26"/>
+      <c r="AF34" s="26"/>
+      <c r="AG34" s="26"/>
+      <c r="AH34" s="26">
         <v>2008</v>
       </c>
-      <c r="AI34" s="35"/>
-      <c r="AJ34" s="35"/>
-      <c r="AK34" s="35"/>
-      <c r="AL34" s="35">
+      <c r="AI34" s="26"/>
+      <c r="AJ34" s="26"/>
+      <c r="AK34" s="26"/>
+      <c r="AL34" s="26">
         <v>2009</v>
       </c>
-      <c r="AM34" s="35"/>
-      <c r="AN34" s="35"/>
-      <c r="AO34" s="35"/>
-      <c r="AP34" s="35">
+      <c r="AM34" s="26"/>
+      <c r="AN34" s="26"/>
+      <c r="AO34" s="26"/>
+      <c r="AP34" s="26">
         <v>2010</v>
       </c>
-      <c r="AQ34" s="35"/>
-      <c r="AR34" s="35"/>
-      <c r="AS34" s="35"/>
-      <c r="AT34" s="35">
+      <c r="AQ34" s="26"/>
+      <c r="AR34" s="26"/>
+      <c r="AS34" s="26"/>
+      <c r="AT34" s="26">
         <v>2011</v>
       </c>
-      <c r="AU34" s="35"/>
-      <c r="AV34" s="35"/>
-      <c r="AW34" s="35"/>
-      <c r="AX34" s="35">
+      <c r="AU34" s="26"/>
+      <c r="AV34" s="26"/>
+      <c r="AW34" s="26"/>
+      <c r="AX34" s="26">
         <v>2012</v>
       </c>
-      <c r="AY34" s="35"/>
-      <c r="AZ34" s="35"/>
-      <c r="BA34" s="35"/>
-      <c r="BB34" s="35">
+      <c r="AY34" s="26"/>
+      <c r="AZ34" s="26"/>
+      <c r="BA34" s="26"/>
+      <c r="BB34" s="26">
         <v>2013</v>
       </c>
-      <c r="BC34" s="35"/>
-      <c r="BD34" s="35"/>
-      <c r="BE34" s="35"/>
-      <c r="BF34" s="35">
+      <c r="BC34" s="26"/>
+      <c r="BD34" s="26"/>
+      <c r="BE34" s="26"/>
+      <c r="BF34" s="26">
         <v>2014</v>
       </c>
-      <c r="BG34" s="35"/>
-      <c r="BH34" s="35"/>
-      <c r="BI34" s="35"/>
-      <c r="BJ34" s="35">
+      <c r="BG34" s="26"/>
+      <c r="BH34" s="26"/>
+      <c r="BI34" s="26"/>
+      <c r="BJ34" s="26">
         <v>2015</v>
       </c>
-      <c r="BK34" s="35"/>
-      <c r="BL34" s="35"/>
-      <c r="BM34" s="35"/>
-      <c r="BN34" s="35">
+      <c r="BK34" s="26"/>
+      <c r="BL34" s="26"/>
+      <c r="BM34" s="26"/>
+      <c r="BN34" s="26">
         <v>2016</v>
       </c>
-      <c r="BO34" s="35"/>
-      <c r="BP34" s="35"/>
-      <c r="BQ34" s="35"/>
-      <c r="BR34" s="35">
+      <c r="BO34" s="26"/>
+      <c r="BP34" s="26"/>
+      <c r="BQ34" s="26"/>
+      <c r="BR34" s="26">
         <v>2017</v>
       </c>
-      <c r="BS34" s="35"/>
-      <c r="BT34" s="35"/>
-      <c r="BU34" s="35"/>
-      <c r="BV34" s="35">
+      <c r="BS34" s="26"/>
+      <c r="BT34" s="26"/>
+      <c r="BU34" s="26"/>
+      <c r="BV34" s="26">
         <v>2018</v>
       </c>
-      <c r="BW34" s="35"/>
-      <c r="BX34" s="35"/>
-      <c r="BY34" s="35"/>
-      <c r="BZ34" s="35">
+      <c r="BW34" s="26"/>
+      <c r="BX34" s="26"/>
+      <c r="BY34" s="26"/>
+      <c r="BZ34" s="26">
         <v>2019</v>
       </c>
-      <c r="CA34" s="35"/>
-      <c r="CB34" s="35"/>
-      <c r="CC34" s="35"/>
-      <c r="CD34" s="36">
+      <c r="CA34" s="26"/>
+      <c r="CB34" s="26"/>
+      <c r="CC34" s="26"/>
+      <c r="CD34" s="25">
         <v>2020</v>
       </c>
-      <c r="CE34" s="36"/>
-      <c r="CF34" s="36"/>
-      <c r="CG34" s="36"/>
+      <c r="CE34" s="25"/>
+      <c r="CF34" s="25"/>
+      <c r="CG34" s="25"/>
       <c r="CH34" s="21">
         <v>2021</v>
       </c>
@@ -5088,15 +5094,16 @@
       <c r="CM34" s="21"/>
       <c r="CN34" s="21"/>
       <c r="CO34" s="21"/>
-      <c r="CP34" s="24">
+      <c r="CP34" s="21">
         <v>2023</v>
       </c>
-      <c r="CQ34" s="24"/>
-      <c r="CR34" s="24"/>
-      <c r="CS34" s="24"/>
-      <c r="CT34" s="24">
+      <c r="CQ34" s="21"/>
+      <c r="CR34" s="21"/>
+      <c r="CS34" s="21"/>
+      <c r="CT34" s="21">
         <v>2024</v>
       </c>
+      <c r="CU34" s="21"/>
     </row>
     <row r="35" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
@@ -5376,20 +5383,23 @@
       <c r="CO35" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP35" s="29" t="s">
+      <c r="CP35" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ35" s="29" t="s">
+      <c r="CQ35" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CR35" s="29" t="s">
+      <c r="CR35" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="CS35" s="29" t="s">
+      <c r="CS35" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CT35" s="29" t="s">
+      <c r="CT35" s="13" t="s">
         <v>7</v>
+      </c>
+      <c r="CU35" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -5675,22 +5685,24 @@
       <c r="CO37" s="18">
         <v>41001.743914789178</v>
       </c>
-      <c r="CP37" s="25">
+      <c r="CP37" s="18">
         <v>66840.507136195039</v>
       </c>
-      <c r="CQ37" s="25">
+      <c r="CQ37" s="18">
         <v>24335.490726229673</v>
       </c>
-      <c r="CR37" s="25">
+      <c r="CR37" s="18">
         <v>39801.249761229999</v>
       </c>
-      <c r="CS37" s="25">
+      <c r="CS37" s="18">
         <v>45097.200111910657</v>
       </c>
-      <c r="CT37" s="25">
-        <v>72305.397080042458</v>
-      </c>
-      <c r="CU37" s="8"/>
+      <c r="CT37" s="18">
+        <v>73763.569378939006</v>
+      </c>
+      <c r="CU37" s="18">
+        <v>26958.75242415956</v>
+      </c>
       <c r="CV37" s="8"/>
       <c r="CW37" s="8"/>
       <c r="CX37" s="8"/>
@@ -6024,22 +6036,24 @@
       <c r="CO38" s="18">
         <v>874.3698128567687</v>
       </c>
-      <c r="CP38" s="25">
+      <c r="CP38" s="18">
         <v>401.40117980165178</v>
       </c>
-      <c r="CQ38" s="25">
+      <c r="CQ38" s="18">
         <v>389.08013271399068</v>
       </c>
-      <c r="CR38" s="25">
+      <c r="CR38" s="18">
         <v>775.39169916792036</v>
       </c>
-      <c r="CS38" s="25">
+      <c r="CS38" s="18">
         <v>800.26199980740012</v>
       </c>
-      <c r="CT38" s="25">
-        <v>453.13602828715932</v>
-      </c>
-      <c r="CU38" s="8"/>
+      <c r="CT38" s="18">
+        <v>437.00790956349607</v>
+      </c>
+      <c r="CU38" s="18">
+        <v>425.47272384273145</v>
+      </c>
       <c r="CV38" s="8"/>
       <c r="CW38" s="8"/>
       <c r="CX38" s="8"/>
@@ -6373,22 +6387,24 @@
       <c r="CO39" s="18">
         <v>54857.258251901527</v>
       </c>
-      <c r="CP39" s="25">
+      <c r="CP39" s="18">
         <v>104952.98838100983</v>
       </c>
-      <c r="CQ39" s="25">
+      <c r="CQ39" s="18">
         <v>107908.32982931691</v>
       </c>
-      <c r="CR39" s="25">
+      <c r="CR39" s="18">
         <v>139971.22516500723</v>
       </c>
-      <c r="CS39" s="25">
+      <c r="CS39" s="18">
         <v>88041.043596806237</v>
       </c>
-      <c r="CT39" s="25">
+      <c r="CT39" s="18">
         <v>120172.09772732317</v>
       </c>
-      <c r="CU39" s="8"/>
+      <c r="CU39" s="18">
+        <v>132251.56752630067</v>
+      </c>
       <c r="CV39" s="8"/>
       <c r="CW39" s="8"/>
       <c r="CX39" s="8"/>
@@ -6722,22 +6738,24 @@
       <c r="CO40" s="18">
         <v>3977.1461621146914</v>
       </c>
-      <c r="CP40" s="25">
+      <c r="CP40" s="18">
         <v>3948.5227029077732</v>
       </c>
-      <c r="CQ40" s="25">
+      <c r="CQ40" s="18">
         <v>4411.1105877597493</v>
       </c>
-      <c r="CR40" s="25">
+      <c r="CR40" s="18">
         <v>4489.0256045275964</v>
       </c>
-      <c r="CS40" s="25">
+      <c r="CS40" s="18">
         <v>4564.4944289546966</v>
       </c>
-      <c r="CT40" s="25">
-        <v>4356.5529553400547</v>
-      </c>
-      <c r="CU40" s="8"/>
+      <c r="CT40" s="18">
+        <v>4153.7012475273468</v>
+      </c>
+      <c r="CU40" s="18">
+        <v>4540.1651977513411</v>
+      </c>
       <c r="CV40" s="8"/>
       <c r="CW40" s="8"/>
       <c r="CX40" s="8"/>
@@ -7071,22 +7089,24 @@
       <c r="CO41" s="18">
         <v>85486.339096444455</v>
       </c>
-      <c r="CP41" s="25">
+      <c r="CP41" s="18">
         <v>132389.96761888449</v>
       </c>
-      <c r="CQ41" s="25">
+      <c r="CQ41" s="18">
         <v>127397.97452047073</v>
       </c>
-      <c r="CR41" s="25">
+      <c r="CR41" s="18">
         <v>88570.644729925349</v>
       </c>
-      <c r="CS41" s="25">
+      <c r="CS41" s="18">
         <v>97408.840224678061</v>
       </c>
-      <c r="CT41" s="25">
-        <v>141361.49065992335</v>
-      </c>
-      <c r="CU41" s="8"/>
+      <c r="CT41" s="18">
+        <v>139628.09619555547</v>
+      </c>
+      <c r="CU41" s="18">
+        <v>136933.7534025386</v>
+      </c>
       <c r="CV41" s="8"/>
       <c r="CW41" s="8"/>
       <c r="CX41" s="8"/>
@@ -7420,22 +7440,24 @@
       <c r="CO42" s="18">
         <v>282568.33591674821</v>
       </c>
-      <c r="CP42" s="25">
+      <c r="CP42" s="18">
         <v>370976.65010641125</v>
       </c>
-      <c r="CQ42" s="25">
+      <c r="CQ42" s="18">
         <v>372232.40369391814</v>
       </c>
-      <c r="CR42" s="25">
+      <c r="CR42" s="18">
         <v>279294.63152185868</v>
       </c>
-      <c r="CS42" s="25">
+      <c r="CS42" s="18">
         <v>294572.86033506453</v>
       </c>
-      <c r="CT42" s="25">
-        <v>405890.48919580912</v>
-      </c>
-      <c r="CU42" s="8"/>
+      <c r="CT42" s="18">
+        <v>405436.75997405779</v>
+      </c>
+      <c r="CU42" s="18">
+        <v>388024.31549253245</v>
+      </c>
       <c r="CV42" s="8"/>
       <c r="CW42" s="8"/>
       <c r="CX42" s="8"/>
@@ -7769,22 +7791,24 @@
       <c r="CO43" s="18">
         <v>56641.27780498279</v>
       </c>
-      <c r="CP43" s="25">
+      <c r="CP43" s="18">
         <v>56722.129138118144</v>
       </c>
-      <c r="CQ43" s="25">
+      <c r="CQ43" s="18">
         <v>66425.589510680875</v>
       </c>
-      <c r="CR43" s="25">
+      <c r="CR43" s="18">
         <v>54458.070986274273</v>
       </c>
-      <c r="CS43" s="25">
+      <c r="CS43" s="18">
         <v>60129.24129404522</v>
       </c>
-      <c r="CT43" s="25">
-        <v>57685.077201933127</v>
-      </c>
-      <c r="CU43" s="8"/>
+      <c r="CT43" s="18">
+        <v>60093.946607444414</v>
+      </c>
+      <c r="CU43" s="18">
+        <v>68278.004479713622</v>
+      </c>
       <c r="CV43" s="8"/>
       <c r="CW43" s="8"/>
       <c r="CX43" s="8"/>
@@ -8118,22 +8142,24 @@
       <c r="CO44" s="18">
         <v>9647.8221918255676</v>
       </c>
-      <c r="CP44" s="25">
+      <c r="CP44" s="18">
         <v>7111.5053813856466</v>
       </c>
-      <c r="CQ44" s="25">
+      <c r="CQ44" s="18">
         <v>9426.9331998502021</v>
       </c>
-      <c r="CR44" s="25">
+      <c r="CR44" s="18">
         <v>7972.0580263325928</v>
       </c>
-      <c r="CS44" s="25">
+      <c r="CS44" s="18">
         <v>10710.381145611891</v>
       </c>
-      <c r="CT44" s="25">
-        <v>7180.5097103007411</v>
-      </c>
-      <c r="CU44" s="8"/>
+      <c r="CT44" s="18">
+        <v>7509.6085256193328</v>
+      </c>
+      <c r="CU44" s="18">
+        <v>11946.285158690835</v>
+      </c>
       <c r="CV44" s="8"/>
       <c r="CW44" s="8"/>
       <c r="CX44" s="8"/>
@@ -8280,11 +8306,11 @@
       <c r="CM45" s="8"/>
       <c r="CN45" s="8"/>
       <c r="CO45" s="8"/>
-      <c r="CP45" s="26"/>
-      <c r="CQ45" s="26"/>
-      <c r="CR45" s="26"/>
-      <c r="CS45" s="26"/>
-      <c r="CT45" s="26"/>
+      <c r="CP45" s="8"/>
+      <c r="CQ45" s="8"/>
+      <c r="CR45" s="8"/>
+      <c r="CS45" s="8"/>
+      <c r="CT45" s="8"/>
       <c r="CU45" s="8"/>
       <c r="CV45" s="8"/>
       <c r="CW45" s="8"/>
@@ -8619,22 +8645,24 @@
       <c r="CO46" s="19">
         <v>535054.29315166315</v>
       </c>
-      <c r="CP46" s="27">
+      <c r="CP46" s="19">
         <v>743343.67164471385</v>
       </c>
-      <c r="CQ46" s="27">
+      <c r="CQ46" s="19">
         <v>712526.91220094031</v>
       </c>
-      <c r="CR46" s="27">
+      <c r="CR46" s="19">
         <v>615332.29749432369</v>
       </c>
-      <c r="CS46" s="27">
+      <c r="CS46" s="19">
         <v>601324.32313687867</v>
       </c>
-      <c r="CT46" s="27">
-        <v>809404.75055895909</v>
-      </c>
-      <c r="CU46" s="8"/>
+      <c r="CT46" s="19">
+        <v>811194.78756603005</v>
+      </c>
+      <c r="CU46" s="19">
+        <v>769358.31640552985</v>
+      </c>
       <c r="CV46" s="8"/>
       <c r="CW46" s="8"/>
       <c r="CX46" s="8"/>
@@ -8782,11 +8810,12 @@
       <c r="CM47" s="11"/>
       <c r="CN47" s="11"/>
       <c r="CO47" s="11"/>
-      <c r="CP47" s="28"/>
-      <c r="CQ47" s="28"/>
-      <c r="CR47" s="28"/>
-      <c r="CS47" s="28"/>
-      <c r="CT47" s="28"/>
+      <c r="CP47" s="11"/>
+      <c r="CQ47" s="11"/>
+      <c r="CR47" s="11"/>
+      <c r="CS47" s="11"/>
+      <c r="CT47" s="11"/>
+      <c r="CU47" s="11"/>
     </row>
     <row r="48" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
@@ -8886,11 +8915,11 @@
       <c r="CM49" s="8"/>
       <c r="CN49" s="8"/>
       <c r="CO49" s="8"/>
-      <c r="CP49" s="26"/>
-      <c r="CQ49" s="26"/>
-      <c r="CR49" s="26"/>
-      <c r="CS49" s="26"/>
-      <c r="CT49" s="26"/>
+      <c r="CP49" s="8"/>
+      <c r="CQ49" s="8"/>
+      <c r="CR49" s="8"/>
+      <c r="CS49" s="8"/>
+      <c r="CT49" s="8"/>
       <c r="CU49" s="8"/>
       <c r="CV49" s="8"/>
       <c r="CW49" s="8"/>
@@ -9038,11 +9067,11 @@
       <c r="CM50" s="8"/>
       <c r="CN50" s="8"/>
       <c r="CO50" s="8"/>
-      <c r="CP50" s="26"/>
-      <c r="CQ50" s="26"/>
-      <c r="CR50" s="26"/>
-      <c r="CS50" s="26"/>
-      <c r="CT50" s="26"/>
+      <c r="CP50" s="8"/>
+      <c r="CQ50" s="8"/>
+      <c r="CR50" s="8"/>
+      <c r="CS50" s="8"/>
+      <c r="CT50" s="8"/>
       <c r="CU50" s="8"/>
       <c r="CV50" s="8"/>
       <c r="CW50" s="8"/>
@@ -9109,172 +9138,172 @@
     </row>
     <row r="53" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="CP55" s="30"/>
-      <c r="CQ55" s="30"/>
-      <c r="CR55" s="30"/>
-      <c r="CS55" s="30"/>
-      <c r="CT55" s="30"/>
+      <c r="CP55" s="6"/>
+      <c r="CQ55" s="6"/>
+      <c r="CR55" s="6"/>
+      <c r="CS55" s="6"/>
+      <c r="CT55" s="6"/>
+      <c r="CU55" s="6"/>
     </row>
     <row r="56" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CP56" s="30"/>
-      <c r="CQ56" s="30"/>
-      <c r="CR56" s="30"/>
-      <c r="CS56" s="30"/>
-      <c r="CT56" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="CP56" s="6"/>
+      <c r="CQ56" s="6"/>
+      <c r="CR56" s="6"/>
+      <c r="CS56" s="6"/>
+      <c r="CT56" s="6"/>
+      <c r="CU56" s="6"/>
     </row>
     <row r="57" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="CQ57" s="30"/>
-      <c r="CR57" s="30"/>
-      <c r="CS57" s="30"/>
-      <c r="CT57" s="30"/>
+      <c r="CR57" s="6"/>
+      <c r="CS57" s="6"/>
+      <c r="CU57" s="6"/>
     </row>
     <row r="58" spans="1:151" x14ac:dyDescent="0.2">
-      <c r="CQ58" s="30"/>
-      <c r="CR58" s="30"/>
-      <c r="CS58" s="30"/>
-      <c r="CT58" s="30"/>
+      <c r="CR58" s="6"/>
+      <c r="CS58" s="6"/>
+      <c r="CU58" s="6"/>
     </row>
     <row r="59" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
-      <c r="B59" s="36" t="s">
+      <c r="B59" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36" t="s">
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36" t="s">
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="K59" s="36"/>
-      <c r="L59" s="36"/>
-      <c r="M59" s="36"/>
-      <c r="N59" s="36" t="s">
+      <c r="K59" s="25"/>
+      <c r="L59" s="25"/>
+      <c r="M59" s="25"/>
+      <c r="N59" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="O59" s="36"/>
-      <c r="P59" s="36"/>
-      <c r="Q59" s="36"/>
-      <c r="R59" s="36" t="s">
+      <c r="O59" s="25"/>
+      <c r="P59" s="25"/>
+      <c r="Q59" s="25"/>
+      <c r="R59" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="S59" s="36"/>
-      <c r="T59" s="36"/>
-      <c r="U59" s="36"/>
-      <c r="V59" s="36" t="s">
+      <c r="S59" s="25"/>
+      <c r="T59" s="25"/>
+      <c r="U59" s="25"/>
+      <c r="V59" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="W59" s="36"/>
-      <c r="X59" s="36"/>
-      <c r="Y59" s="36"/>
-      <c r="Z59" s="36" t="s">
+      <c r="W59" s="25"/>
+      <c r="X59" s="25"/>
+      <c r="Y59" s="25"/>
+      <c r="Z59" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AA59" s="36"/>
-      <c r="AB59" s="36"/>
-      <c r="AC59" s="36"/>
-      <c r="AD59" s="36" t="s">
+      <c r="AA59" s="25"/>
+      <c r="AB59" s="25"/>
+      <c r="AC59" s="25"/>
+      <c r="AD59" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AE59" s="36"/>
-      <c r="AF59" s="36"/>
-      <c r="AG59" s="36"/>
-      <c r="AH59" s="36" t="s">
+      <c r="AE59" s="25"/>
+      <c r="AF59" s="25"/>
+      <c r="AG59" s="25"/>
+      <c r="AH59" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="AI59" s="36"/>
-      <c r="AJ59" s="36"/>
-      <c r="AK59" s="36"/>
-      <c r="AL59" s="36" t="s">
+      <c r="AI59" s="25"/>
+      <c r="AJ59" s="25"/>
+      <c r="AK59" s="25"/>
+      <c r="AL59" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AM59" s="36"/>
-      <c r="AN59" s="36"/>
-      <c r="AO59" s="36"/>
-      <c r="AP59" s="36" t="s">
+      <c r="AM59" s="25"/>
+      <c r="AN59" s="25"/>
+      <c r="AO59" s="25"/>
+      <c r="AP59" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AQ59" s="36"/>
-      <c r="AR59" s="36"/>
-      <c r="AS59" s="36"/>
-      <c r="AT59" s="36" t="s">
+      <c r="AQ59" s="25"/>
+      <c r="AR59" s="25"/>
+      <c r="AS59" s="25"/>
+      <c r="AT59" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AU59" s="36"/>
-      <c r="AV59" s="36"/>
-      <c r="AW59" s="36"/>
-      <c r="AX59" s="36" t="s">
+      <c r="AU59" s="25"/>
+      <c r="AV59" s="25"/>
+      <c r="AW59" s="25"/>
+      <c r="AX59" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AY59" s="36"/>
-      <c r="AZ59" s="36"/>
-      <c r="BA59" s="36"/>
-      <c r="BB59" s="36" t="s">
+      <c r="AY59" s="25"/>
+      <c r="AZ59" s="25"/>
+      <c r="BA59" s="25"/>
+      <c r="BB59" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="BC59" s="36"/>
-      <c r="BD59" s="36"/>
-      <c r="BE59" s="36"/>
-      <c r="BF59" s="36" t="s">
+      <c r="BC59" s="25"/>
+      <c r="BD59" s="25"/>
+      <c r="BE59" s="25"/>
+      <c r="BF59" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="BG59" s="36"/>
-      <c r="BH59" s="36"/>
-      <c r="BI59" s="36"/>
-      <c r="BJ59" s="36" t="s">
+      <c r="BG59" s="25"/>
+      <c r="BH59" s="25"/>
+      <c r="BI59" s="25"/>
+      <c r="BJ59" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="BK59" s="36"/>
-      <c r="BL59" s="36"/>
-      <c r="BM59" s="36"/>
-      <c r="BN59" s="36" t="s">
+      <c r="BK59" s="25"/>
+      <c r="BL59" s="25"/>
+      <c r="BM59" s="25"/>
+      <c r="BN59" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="BO59" s="36"/>
-      <c r="BP59" s="36"/>
-      <c r="BQ59" s="36"/>
-      <c r="BR59" s="36" t="s">
+      <c r="BO59" s="25"/>
+      <c r="BP59" s="25"/>
+      <c r="BQ59" s="25"/>
+      <c r="BR59" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="BS59" s="36"/>
-      <c r="BT59" s="36"/>
-      <c r="BU59" s="36"/>
-      <c r="BV59" s="36" t="s">
+      <c r="BS59" s="25"/>
+      <c r="BT59" s="25"/>
+      <c r="BU59" s="25"/>
+      <c r="BV59" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="BW59" s="36"/>
-      <c r="BX59" s="36"/>
-      <c r="BY59" s="36"/>
-      <c r="BZ59" s="36" t="s">
+      <c r="BW59" s="25"/>
+      <c r="BX59" s="25"/>
+      <c r="BY59" s="25"/>
+      <c r="BZ59" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="CA59" s="36"/>
-      <c r="CB59" s="36"/>
-      <c r="CC59" s="36"/>
-      <c r="CD59" s="36" t="s">
+      <c r="CA59" s="25"/>
+      <c r="CB59" s="25"/>
+      <c r="CC59" s="25"/>
+      <c r="CD59" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="CE59" s="36"/>
-      <c r="CF59" s="36"/>
-      <c r="CG59" s="36"/>
+      <c r="CE59" s="25"/>
+      <c r="CF59" s="25"/>
+      <c r="CG59" s="25"/>
       <c r="CH59" s="21" t="s">
         <v>52</v>
       </c>
@@ -9287,13 +9316,14 @@
       <c r="CM59" s="21"/>
       <c r="CN59" s="21"/>
       <c r="CO59" s="21"/>
-      <c r="CP59" s="24" t="s">
+      <c r="CP59" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="CQ59" s="22"/>
+      <c r="CQ59" s="21"/>
       <c r="CR59" s="22"/>
       <c r="CS59" s="22"/>
-      <c r="CT59" s="22"/>
+      <c r="CT59" s="21"/>
+      <c r="CU59" s="22"/>
     </row>
     <row r="60" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
@@ -9573,20 +9603,22 @@
       <c r="CO60" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP60" s="29" t="s">
+      <c r="CP60" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ60" s="29"/>
-      <c r="CR60" s="29"/>
-      <c r="CS60" s="29"/>
-      <c r="CT60" s="29"/>
+      <c r="CQ60" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="CR60" s="13"/>
+      <c r="CS60" s="13"/>
+      <c r="CT60" s="13"/>
+      <c r="CU60" s="13"/>
     </row>
     <row r="61" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
-      <c r="CQ61" s="30"/>
-      <c r="CR61" s="30"/>
-      <c r="CS61" s="30"/>
-      <c r="CT61" s="30"/>
+      <c r="CR61" s="6"/>
+      <c r="CS61" s="6"/>
+      <c r="CU61" s="6"/>
     </row>
     <row r="62" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -9868,14 +9900,16 @@
       <c r="CO62" s="14">
         <v>12.595581900616963</v>
       </c>
-      <c r="CP62" s="31">
-        <v>10.15166201734516</v>
-      </c>
-      <c r="CQ62" s="32"/>
-      <c r="CR62" s="32"/>
-      <c r="CS62" s="32"/>
-      <c r="CT62" s="32"/>
-      <c r="CU62" s="8"/>
+      <c r="CP62" s="14">
+        <v>12.373074369915457</v>
+      </c>
+      <c r="CQ62" s="14">
+        <v>10.653916472298206</v>
+      </c>
+      <c r="CR62" s="23"/>
+      <c r="CS62" s="23"/>
+      <c r="CT62" s="14"/>
+      <c r="CU62" s="23"/>
       <c r="CV62" s="8"/>
       <c r="CW62" s="8"/>
       <c r="CX62" s="8"/>
@@ -10205,14 +10239,16 @@
       <c r="CO63" s="14">
         <v>-5.7511235051855465</v>
       </c>
-      <c r="CP63" s="31">
-        <v>15.429937775878415</v>
-      </c>
-      <c r="CQ63" s="32"/>
-      <c r="CR63" s="32"/>
-      <c r="CS63" s="32"/>
-      <c r="CT63" s="32"/>
-      <c r="CU63" s="8"/>
+      <c r="CP63" s="14">
+        <v>11.321529650063567</v>
+      </c>
+      <c r="CQ63" s="14">
+        <v>11.993715039622984</v>
+      </c>
+      <c r="CR63" s="23"/>
+      <c r="CS63" s="23"/>
+      <c r="CT63" s="14"/>
+      <c r="CU63" s="23"/>
       <c r="CV63" s="8"/>
       <c r="CW63" s="8"/>
       <c r="CX63" s="8"/>
@@ -10542,14 +10578,16 @@
       <c r="CO64" s="14">
         <v>67.431544333633241</v>
       </c>
-      <c r="CP64" s="31">
+      <c r="CP64" s="14">
         <v>18.255808080987705</v>
       </c>
-      <c r="CQ64" s="32"/>
-      <c r="CR64" s="32"/>
-      <c r="CS64" s="32"/>
-      <c r="CT64" s="32"/>
-      <c r="CU64" s="8"/>
+      <c r="CQ64" s="14">
+        <v>26.473626948390262</v>
+      </c>
+      <c r="CR64" s="23"/>
+      <c r="CS64" s="23"/>
+      <c r="CT64" s="14"/>
+      <c r="CU64" s="23"/>
       <c r="CV64" s="8"/>
       <c r="CW64" s="8"/>
       <c r="CX64" s="8"/>
@@ -10879,14 +10917,16 @@
       <c r="CO65" s="14">
         <v>19.608787551606682</v>
       </c>
-      <c r="CP65" s="31">
-        <v>14.241210962396252</v>
-      </c>
-      <c r="CQ65" s="32"/>
-      <c r="CR65" s="32"/>
-      <c r="CS65" s="32"/>
-      <c r="CT65" s="32"/>
-      <c r="CU65" s="8"/>
+      <c r="CP65" s="14">
+        <v>8.9218621598278673</v>
+      </c>
+      <c r="CQ65" s="14">
+        <v>4.9053281335405643</v>
+      </c>
+      <c r="CR65" s="23"/>
+      <c r="CS65" s="23"/>
+      <c r="CT65" s="14"/>
+      <c r="CU65" s="23"/>
       <c r="CV65" s="8"/>
       <c r="CW65" s="8"/>
       <c r="CX65" s="8"/>
@@ -11216,14 +11256,16 @@
       <c r="CO66" s="14">
         <v>14.317884840937054</v>
       </c>
-      <c r="CP66" s="31">
-        <v>7.2281830568370395</v>
-      </c>
-      <c r="CQ66" s="32"/>
-      <c r="CR66" s="32"/>
-      <c r="CS66" s="32"/>
-      <c r="CT66" s="32"/>
-      <c r="CU66" s="8"/>
+      <c r="CP66" s="14">
+        <v>5.9969860589665416</v>
+      </c>
+      <c r="CQ66" s="14">
+        <v>7.9400042174752912</v>
+      </c>
+      <c r="CR66" s="23"/>
+      <c r="CS66" s="23"/>
+      <c r="CT66" s="14"/>
+      <c r="CU66" s="23"/>
       <c r="CV66" s="8"/>
       <c r="CW66" s="8"/>
       <c r="CX66" s="8"/>
@@ -11553,14 +11595,16 @@
       <c r="CO67" s="14">
         <v>7.2652728936842408</v>
       </c>
-      <c r="CP67" s="31">
-        <v>11.636496217543652</v>
-      </c>
-      <c r="CQ67" s="32"/>
-      <c r="CR67" s="32"/>
-      <c r="CS67" s="32"/>
-      <c r="CT67" s="32"/>
-      <c r="CU67" s="8"/>
+      <c r="CP67" s="14">
+        <v>11.510351210896232</v>
+      </c>
+      <c r="CQ67" s="14">
+        <v>6.7593073990803703</v>
+      </c>
+      <c r="CR67" s="23"/>
+      <c r="CS67" s="23"/>
+      <c r="CT67" s="14"/>
+      <c r="CU67" s="23"/>
       <c r="CV67" s="8"/>
       <c r="CW67" s="8"/>
       <c r="CX67" s="8"/>
@@ -11890,14 +11934,16 @@
       <c r="CO68" s="14">
         <v>7.917711071920877</v>
       </c>
-      <c r="CP68" s="31">
-        <v>3.9870999011112787</v>
-      </c>
-      <c r="CQ68" s="32"/>
-      <c r="CR68" s="32"/>
-      <c r="CS68" s="32"/>
-      <c r="CT68" s="32"/>
-      <c r="CU68" s="8"/>
+      <c r="CP68" s="14">
+        <v>8.3294940811998117</v>
+      </c>
+      <c r="CQ68" s="14">
+        <v>5.2704272045858858</v>
+      </c>
+      <c r="CR68" s="23"/>
+      <c r="CS68" s="23"/>
+      <c r="CT68" s="14"/>
+      <c r="CU68" s="23"/>
       <c r="CV68" s="8"/>
       <c r="CW68" s="8"/>
       <c r="CX68" s="8"/>
@@ -12227,14 +12273,16 @@
       <c r="CO69" s="14">
         <v>14.318042026160384</v>
       </c>
-      <c r="CP69" s="31">
-        <v>3.1715382539782695</v>
-      </c>
-      <c r="CQ69" s="32"/>
-      <c r="CR69" s="32"/>
-      <c r="CS69" s="32"/>
-      <c r="CT69" s="32"/>
-      <c r="CU69" s="8"/>
+      <c r="CP69" s="14">
+        <v>7.8810683390206293</v>
+      </c>
+      <c r="CQ69" s="14">
+        <v>29.784679957728343</v>
+      </c>
+      <c r="CR69" s="23"/>
+      <c r="CS69" s="23"/>
+      <c r="CT69" s="14"/>
+      <c r="CU69" s="23"/>
       <c r="CV69" s="8"/>
       <c r="CW69" s="8"/>
       <c r="CX69" s="8"/>
@@ -12377,12 +12425,12 @@
       <c r="CM70" s="8"/>
       <c r="CN70" s="8"/>
       <c r="CO70" s="8"/>
-      <c r="CP70" s="26"/>
-      <c r="CQ70" s="33"/>
-      <c r="CR70" s="33"/>
-      <c r="CS70" s="33"/>
-      <c r="CT70" s="33"/>
-      <c r="CU70" s="8"/>
+      <c r="CP70" s="8"/>
+      <c r="CQ70" s="8"/>
+      <c r="CR70" s="24"/>
+      <c r="CS70" s="24"/>
+      <c r="CT70" s="8"/>
+      <c r="CU70" s="24"/>
       <c r="CV70" s="8"/>
       <c r="CW70" s="8"/>
       <c r="CX70" s="8"/>
@@ -12712,14 +12760,16 @@
       <c r="CO71" s="14">
         <v>15.22220251521378</v>
       </c>
-      <c r="CP71" s="31">
-        <v>11.098927313267225</v>
-      </c>
-      <c r="CQ71" s="32"/>
-      <c r="CR71" s="32"/>
-      <c r="CS71" s="32"/>
-      <c r="CT71" s="32"/>
-      <c r="CU71" s="8"/>
+      <c r="CP71" s="14">
+        <v>11.431160487940687</v>
+      </c>
+      <c r="CQ71" s="14">
+        <v>10.380783878040177</v>
+      </c>
+      <c r="CR71" s="23"/>
+      <c r="CS71" s="23"/>
+      <c r="CT71" s="14"/>
+      <c r="CU71" s="23"/>
       <c r="CV71" s="8"/>
       <c r="CW71" s="8"/>
       <c r="CX71" s="8"/>
@@ -12863,20 +12913,20 @@
       <c r="CM72" s="11"/>
       <c r="CN72" s="11"/>
       <c r="CO72" s="11"/>
-      <c r="CP72" s="28"/>
-      <c r="CQ72" s="13"/>
-      <c r="CR72" s="13"/>
-      <c r="CS72" s="13"/>
-      <c r="CT72" s="13"/>
+      <c r="CP72" s="11"/>
+      <c r="CQ72" s="11"/>
+      <c r="CR72" s="5"/>
+      <c r="CS72" s="5"/>
+      <c r="CT72" s="11"/>
+      <c r="CU72" s="5"/>
     </row>
     <row r="73" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="CQ73" s="30"/>
-      <c r="CR73" s="30"/>
-      <c r="CS73" s="30"/>
-      <c r="CT73" s="30"/>
+      <c r="CR73" s="6"/>
+      <c r="CS73" s="6"/>
+      <c r="CU73" s="6"/>
     </row>
     <row r="74" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="8"/>
@@ -12971,12 +13021,12 @@
       <c r="CM74" s="8"/>
       <c r="CN74" s="8"/>
       <c r="CO74" s="8"/>
-      <c r="CP74" s="26"/>
-      <c r="CQ74" s="33"/>
-      <c r="CR74" s="33"/>
-      <c r="CS74" s="33"/>
-      <c r="CT74" s="33"/>
-      <c r="CU74" s="8"/>
+      <c r="CP74" s="8"/>
+      <c r="CQ74" s="8"/>
+      <c r="CR74" s="24"/>
+      <c r="CS74" s="24"/>
+      <c r="CT74" s="8"/>
+      <c r="CU74" s="24"/>
       <c r="CV74" s="8"/>
       <c r="CW74" s="8"/>
       <c r="CX74" s="8"/>
@@ -13119,12 +13169,12 @@
       <c r="CM75" s="8"/>
       <c r="CN75" s="8"/>
       <c r="CO75" s="8"/>
-      <c r="CP75" s="26"/>
-      <c r="CQ75" s="33"/>
-      <c r="CR75" s="33"/>
-      <c r="CS75" s="33"/>
-      <c r="CT75" s="33"/>
-      <c r="CU75" s="8"/>
+      <c r="CP75" s="8"/>
+      <c r="CQ75" s="8"/>
+      <c r="CR75" s="24"/>
+      <c r="CS75" s="24"/>
+      <c r="CT75" s="8"/>
+      <c r="CU75" s="24"/>
       <c r="CV75" s="8"/>
       <c r="CW75" s="8"/>
       <c r="CX75" s="8"/>
@@ -13178,196 +13228,188 @@
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="CQ76" s="30"/>
-      <c r="CR76" s="30"/>
-      <c r="CS76" s="30"/>
-      <c r="CT76" s="30"/>
+      <c r="CR76" s="6"/>
+      <c r="CS76" s="6"/>
+      <c r="CU76" s="6"/>
     </row>
     <row r="77" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="CQ77" s="30"/>
-      <c r="CR77" s="30"/>
-      <c r="CS77" s="30"/>
-      <c r="CT77" s="30"/>
+      <c r="CR77" s="6"/>
+      <c r="CS77" s="6"/>
+      <c r="CU77" s="6"/>
     </row>
     <row r="78" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="CQ78" s="30"/>
-      <c r="CR78" s="30"/>
-      <c r="CS78" s="30"/>
-      <c r="CT78" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="CR78" s="6"/>
+      <c r="CS78" s="6"/>
+      <c r="CU78" s="6"/>
     </row>
     <row r="79" spans="1:147" x14ac:dyDescent="0.2">
-      <c r="CQ79" s="30"/>
-      <c r="CR79" s="30"/>
-      <c r="CS79" s="30"/>
-      <c r="CT79" s="30"/>
+      <c r="CR79" s="6"/>
+      <c r="CS79" s="6"/>
+      <c r="CU79" s="6"/>
     </row>
     <row r="80" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="CQ80" s="30"/>
-      <c r="CR80" s="30"/>
-      <c r="CS80" s="30"/>
-      <c r="CT80" s="30"/>
+      <c r="CR80" s="6"/>
+      <c r="CS80" s="6"/>
+      <c r="CU80" s="6"/>
     </row>
     <row r="81" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CQ81" s="30"/>
-      <c r="CR81" s="30"/>
-      <c r="CS81" s="30"/>
-      <c r="CT81" s="30"/>
+        <v>57</v>
+      </c>
+      <c r="CR81" s="6"/>
+      <c r="CS81" s="6"/>
+      <c r="CU81" s="6"/>
     </row>
     <row r="82" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="CQ82" s="30"/>
-      <c r="CR82" s="30"/>
-      <c r="CS82" s="30"/>
-      <c r="CT82" s="30"/>
+      <c r="CR82" s="6"/>
+      <c r="CS82" s="6"/>
+      <c r="CU82" s="6"/>
     </row>
     <row r="83" spans="1:147" x14ac:dyDescent="0.2">
-      <c r="CQ83" s="30"/>
-      <c r="CR83" s="30"/>
-      <c r="CS83" s="30"/>
-      <c r="CT83" s="30"/>
+      <c r="CR83" s="6"/>
+      <c r="CS83" s="6"/>
+      <c r="CU83" s="6"/>
     </row>
     <row r="84" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
-      <c r="B84" s="36" t="s">
+      <c r="B84" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36" t="s">
+      <c r="C84" s="25"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G84" s="36"/>
-      <c r="H84" s="36"/>
-      <c r="I84" s="36"/>
-      <c r="J84" s="36" t="s">
+      <c r="G84" s="25"/>
+      <c r="H84" s="25"/>
+      <c r="I84" s="25"/>
+      <c r="J84" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="K84" s="36"/>
-      <c r="L84" s="36"/>
-      <c r="M84" s="36"/>
-      <c r="N84" s="36" t="s">
+      <c r="K84" s="25"/>
+      <c r="L84" s="25"/>
+      <c r="M84" s="25"/>
+      <c r="N84" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="O84" s="36"/>
-      <c r="P84" s="36"/>
-      <c r="Q84" s="36"/>
-      <c r="R84" s="36" t="s">
+      <c r="O84" s="25"/>
+      <c r="P84" s="25"/>
+      <c r="Q84" s="25"/>
+      <c r="R84" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="S84" s="36"/>
-      <c r="T84" s="36"/>
-      <c r="U84" s="36"/>
-      <c r="V84" s="36" t="s">
+      <c r="S84" s="25"/>
+      <c r="T84" s="25"/>
+      <c r="U84" s="25"/>
+      <c r="V84" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="W84" s="36"/>
-      <c r="X84" s="36"/>
-      <c r="Y84" s="36"/>
-      <c r="Z84" s="36" t="s">
+      <c r="W84" s="25"/>
+      <c r="X84" s="25"/>
+      <c r="Y84" s="25"/>
+      <c r="Z84" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AA84" s="36"/>
-      <c r="AB84" s="36"/>
-      <c r="AC84" s="36"/>
-      <c r="AD84" s="36" t="s">
+      <c r="AA84" s="25"/>
+      <c r="AB84" s="25"/>
+      <c r="AC84" s="25"/>
+      <c r="AD84" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AE84" s="36"/>
-      <c r="AF84" s="36"/>
-      <c r="AG84" s="36"/>
-      <c r="AH84" s="36" t="s">
+      <c r="AE84" s="25"/>
+      <c r="AF84" s="25"/>
+      <c r="AG84" s="25"/>
+      <c r="AH84" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="AI84" s="36"/>
-      <c r="AJ84" s="36"/>
-      <c r="AK84" s="36"/>
-      <c r="AL84" s="36" t="s">
+      <c r="AI84" s="25"/>
+      <c r="AJ84" s="25"/>
+      <c r="AK84" s="25"/>
+      <c r="AL84" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AM84" s="36"/>
-      <c r="AN84" s="36"/>
-      <c r="AO84" s="36"/>
-      <c r="AP84" s="36" t="s">
+      <c r="AM84" s="25"/>
+      <c r="AN84" s="25"/>
+      <c r="AO84" s="25"/>
+      <c r="AP84" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AQ84" s="36"/>
-      <c r="AR84" s="36"/>
-      <c r="AS84" s="36"/>
-      <c r="AT84" s="36" t="s">
+      <c r="AQ84" s="25"/>
+      <c r="AR84" s="25"/>
+      <c r="AS84" s="25"/>
+      <c r="AT84" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AU84" s="36"/>
-      <c r="AV84" s="36"/>
-      <c r="AW84" s="36"/>
-      <c r="AX84" s="36" t="s">
+      <c r="AU84" s="25"/>
+      <c r="AV84" s="25"/>
+      <c r="AW84" s="25"/>
+      <c r="AX84" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AY84" s="36"/>
-      <c r="AZ84" s="36"/>
-      <c r="BA84" s="36"/>
-      <c r="BB84" s="36" t="s">
+      <c r="AY84" s="25"/>
+      <c r="AZ84" s="25"/>
+      <c r="BA84" s="25"/>
+      <c r="BB84" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="BC84" s="36"/>
-      <c r="BD84" s="36"/>
-      <c r="BE84" s="36"/>
-      <c r="BF84" s="36" t="s">
+      <c r="BC84" s="25"/>
+      <c r="BD84" s="25"/>
+      <c r="BE84" s="25"/>
+      <c r="BF84" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="BG84" s="36"/>
-      <c r="BH84" s="36"/>
-      <c r="BI84" s="36"/>
-      <c r="BJ84" s="36" t="s">
+      <c r="BG84" s="25"/>
+      <c r="BH84" s="25"/>
+      <c r="BI84" s="25"/>
+      <c r="BJ84" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="BK84" s="36"/>
-      <c r="BL84" s="36"/>
-      <c r="BM84" s="36"/>
-      <c r="BN84" s="36" t="s">
+      <c r="BK84" s="25"/>
+      <c r="BL84" s="25"/>
+      <c r="BM84" s="25"/>
+      <c r="BN84" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="BO84" s="36"/>
-      <c r="BP84" s="36"/>
-      <c r="BQ84" s="36"/>
-      <c r="BR84" s="36" t="s">
+      <c r="BO84" s="25"/>
+      <c r="BP84" s="25"/>
+      <c r="BQ84" s="25"/>
+      <c r="BR84" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="BS84" s="36"/>
-      <c r="BT84" s="36"/>
-      <c r="BU84" s="36"/>
-      <c r="BV84" s="36" t="s">
+      <c r="BS84" s="25"/>
+      <c r="BT84" s="25"/>
+      <c r="BU84" s="25"/>
+      <c r="BV84" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="BW84" s="36"/>
-      <c r="BX84" s="36"/>
-      <c r="BY84" s="36"/>
-      <c r="BZ84" s="36" t="s">
+      <c r="BW84" s="25"/>
+      <c r="BX84" s="25"/>
+      <c r="BY84" s="25"/>
+      <c r="BZ84" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="CA84" s="36"/>
-      <c r="CB84" s="36"/>
-      <c r="CC84" s="36"/>
-      <c r="CD84" s="36" t="s">
+      <c r="CA84" s="25"/>
+      <c r="CB84" s="25"/>
+      <c r="CC84" s="25"/>
+      <c r="CD84" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="CE84" s="36"/>
-      <c r="CF84" s="36"/>
-      <c r="CG84" s="36"/>
+      <c r="CE84" s="25"/>
+      <c r="CF84" s="25"/>
+      <c r="CG84" s="25"/>
       <c r="CH84" s="21" t="s">
         <v>52</v>
       </c>
@@ -13380,13 +13422,14 @@
       <c r="CM84" s="21"/>
       <c r="CN84" s="21"/>
       <c r="CO84" s="21"/>
-      <c r="CP84" s="24" t="s">
+      <c r="CP84" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="CQ84" s="22"/>
+      <c r="CQ84" s="21"/>
       <c r="CR84" s="22"/>
       <c r="CS84" s="22"/>
-      <c r="CT84" s="22"/>
+      <c r="CT84" s="21"/>
+      <c r="CU84" s="22"/>
     </row>
     <row r="85" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
@@ -13666,20 +13709,22 @@
       <c r="CO85" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CP85" s="13" t="s">
+      <c r="CP85" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="CQ85" s="13"/>
-      <c r="CR85" s="13"/>
-      <c r="CS85" s="13"/>
-      <c r="CT85" s="13"/>
+      <c r="CQ85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="CR85" s="5"/>
+      <c r="CS85" s="5"/>
+      <c r="CT85" s="5"/>
+      <c r="CU85" s="5"/>
     </row>
     <row r="86" spans="1:147" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
-      <c r="CQ86" s="30"/>
-      <c r="CR86" s="30"/>
-      <c r="CS86" s="30"/>
-      <c r="CT86" s="30"/>
+      <c r="CR86" s="6"/>
+      <c r="CS86" s="6"/>
+      <c r="CU86" s="6"/>
     </row>
     <row r="87" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
@@ -13961,14 +14006,16 @@
       <c r="CO87" s="14">
         <v>9.9884926983417017</v>
       </c>
-      <c r="CP87" s="31">
-        <v>8.1760150812621504</v>
-      </c>
-      <c r="CQ87" s="32"/>
-      <c r="CR87" s="32"/>
-      <c r="CS87" s="32"/>
-      <c r="CT87" s="32"/>
-      <c r="CU87" s="8"/>
+      <c r="CP87" s="14">
+        <v>10.357584852905816</v>
+      </c>
+      <c r="CQ87" s="14">
+        <v>10.779571809096254</v>
+      </c>
+      <c r="CR87" s="23"/>
+      <c r="CS87" s="23"/>
+      <c r="CT87" s="14"/>
+      <c r="CU87" s="23"/>
       <c r="CV87" s="8"/>
       <c r="CW87" s="8"/>
       <c r="CX87" s="8"/>
@@ -14298,14 +14345,16 @@
       <c r="CO88" s="14">
         <v>-8.4755685706075781</v>
       </c>
-      <c r="CP88" s="31">
-        <v>12.888564132041608</v>
-      </c>
-      <c r="CQ88" s="32"/>
-      <c r="CR88" s="32"/>
-      <c r="CS88" s="32"/>
-      <c r="CT88" s="32"/>
-      <c r="CU88" s="8"/>
+      <c r="CP88" s="14">
+        <v>8.8706091445568234</v>
+      </c>
+      <c r="CQ88" s="14">
+        <v>9.3534950949275526</v>
+      </c>
+      <c r="CR88" s="23"/>
+      <c r="CS88" s="23"/>
+      <c r="CT88" s="14"/>
+      <c r="CU88" s="23"/>
       <c r="CV88" s="8"/>
       <c r="CW88" s="8"/>
       <c r="CX88" s="8"/>
@@ -14635,14 +14684,16 @@
       <c r="CO89" s="14">
         <v>60.491148122143812</v>
       </c>
-      <c r="CP89" s="31">
+      <c r="CP89" s="14">
         <v>14.500882329394528</v>
       </c>
-      <c r="CQ89" s="32"/>
-      <c r="CR89" s="32"/>
-      <c r="CS89" s="32"/>
-      <c r="CT89" s="32"/>
-      <c r="CU89" s="8"/>
+      <c r="CQ89" s="14">
+        <v>22.559183091322495</v>
+      </c>
+      <c r="CR89" s="23"/>
+      <c r="CS89" s="23"/>
+      <c r="CT89" s="14"/>
+      <c r="CU89" s="23"/>
       <c r="CV89" s="8"/>
       <c r="CW89" s="8"/>
       <c r="CX89" s="8"/>
@@ -14972,14 +15023,16 @@
       <c r="CO90" s="14">
         <v>14.768083517647383</v>
       </c>
-      <c r="CP90" s="31">
-        <v>10.33374462129342</v>
-      </c>
-      <c r="CQ90" s="32"/>
-      <c r="CR90" s="32"/>
-      <c r="CS90" s="32"/>
-      <c r="CT90" s="32"/>
-      <c r="CU90" s="8"/>
+      <c r="CP90" s="14">
+        <v>5.1963369608708518</v>
+      </c>
+      <c r="CQ90" s="14">
+        <v>2.9256716063682688</v>
+      </c>
+      <c r="CR90" s="23"/>
+      <c r="CS90" s="23"/>
+      <c r="CT90" s="14"/>
+      <c r="CU90" s="23"/>
       <c r="CV90" s="8"/>
       <c r="CW90" s="8"/>
       <c r="CX90" s="8"/>
@@ -15309,14 +15362,16 @@
       <c r="CO91" s="14">
         <v>13.94667411688178</v>
       </c>
-      <c r="CP91" s="31">
-        <v>6.77658828867267</v>
-      </c>
-      <c r="CQ91" s="32"/>
-      <c r="CR91" s="32"/>
-      <c r="CS91" s="32"/>
-      <c r="CT91" s="32"/>
-      <c r="CU91" s="8"/>
+      <c r="CP91" s="14">
+        <v>5.4672787574868522</v>
+      </c>
+      <c r="CQ91" s="14">
+        <v>7.4850317816753176</v>
+      </c>
+      <c r="CR91" s="23"/>
+      <c r="CS91" s="23"/>
+      <c r="CT91" s="14"/>
+      <c r="CU91" s="23"/>
       <c r="CV91" s="8"/>
       <c r="CW91" s="8"/>
       <c r="CX91" s="8"/>
@@ -15646,14 +15701,16 @@
       <c r="CO92" s="14">
         <v>4.2483615085071591</v>
       </c>
-      <c r="CP92" s="31">
-        <v>9.4113306267074108</v>
-      </c>
-      <c r="CQ92" s="32"/>
-      <c r="CR92" s="32"/>
-      <c r="CS92" s="32"/>
-      <c r="CT92" s="32"/>
-      <c r="CU92" s="8"/>
+      <c r="CP92" s="14">
+        <v>9.2890239473999259</v>
+      </c>
+      <c r="CQ92" s="14">
+        <v>4.2424871241461943</v>
+      </c>
+      <c r="CR92" s="23"/>
+      <c r="CS92" s="23"/>
+      <c r="CT92" s="14"/>
+      <c r="CU92" s="23"/>
       <c r="CV92" s="8"/>
       <c r="CW92" s="8"/>
       <c r="CX92" s="8"/>
@@ -15983,14 +16040,16 @@
       <c r="CO93" s="14">
         <v>6.157988704053551</v>
       </c>
-      <c r="CP93" s="31">
-        <v>1.6976585301835314</v>
-      </c>
-      <c r="CQ93" s="32"/>
-      <c r="CR93" s="32"/>
-      <c r="CS93" s="32"/>
-      <c r="CT93" s="32"/>
-      <c r="CU93" s="8"/>
+      <c r="CP93" s="14">
+        <v>5.9444479968583579</v>
+      </c>
+      <c r="CQ93" s="14">
+        <v>2.7887068563160966</v>
+      </c>
+      <c r="CR93" s="23"/>
+      <c r="CS93" s="23"/>
+      <c r="CT93" s="14"/>
+      <c r="CU93" s="23"/>
       <c r="CV93" s="8"/>
       <c r="CW93" s="8"/>
       <c r="CX93" s="8"/>
@@ -16320,14 +16379,16 @@
       <c r="CO94" s="14">
         <v>11.013459127455832</v>
       </c>
-      <c r="CP94" s="31">
-        <v>0.97031957672018621</v>
-      </c>
-      <c r="CQ94" s="32"/>
-      <c r="CR94" s="32"/>
-      <c r="CS94" s="32"/>
-      <c r="CT94" s="32"/>
-      <c r="CU94" s="8"/>
+      <c r="CP94" s="14">
+        <v>5.5980150879969699</v>
+      </c>
+      <c r="CQ94" s="14">
+        <v>26.725043080613602</v>
+      </c>
+      <c r="CR94" s="23"/>
+      <c r="CS94" s="23"/>
+      <c r="CT94" s="14"/>
+      <c r="CU94" s="23"/>
       <c r="CV94" s="8"/>
       <c r="CW94" s="8"/>
       <c r="CX94" s="8"/>
@@ -16470,12 +16531,12 @@
       <c r="CM95" s="8"/>
       <c r="CN95" s="8"/>
       <c r="CO95" s="8"/>
-      <c r="CP95" s="26"/>
-      <c r="CQ95" s="33"/>
-      <c r="CR95" s="33"/>
-      <c r="CS95" s="33"/>
-      <c r="CT95" s="33"/>
-      <c r="CU95" s="8"/>
+      <c r="CP95" s="8"/>
+      <c r="CQ95" s="8"/>
+      <c r="CR95" s="24"/>
+      <c r="CS95" s="24"/>
+      <c r="CT95" s="8"/>
+      <c r="CU95" s="24"/>
       <c r="CV95" s="8"/>
       <c r="CW95" s="8"/>
       <c r="CX95" s="8"/>
@@ -16805,14 +16866,16 @@
       <c r="CO96" s="14">
         <v>12.385664564031657</v>
       </c>
-      <c r="CP96" s="31">
-        <v>8.8870170601007743</v>
-      </c>
-      <c r="CQ96" s="32"/>
-      <c r="CR96" s="32"/>
-      <c r="CS96" s="32"/>
-      <c r="CT96" s="32"/>
-      <c r="CU96" s="8"/>
+      <c r="CP96" s="14">
+        <v>9.1278258643393713</v>
+      </c>
+      <c r="CQ96" s="14">
+        <v>7.9760361652925837</v>
+      </c>
+      <c r="CR96" s="23"/>
+      <c r="CS96" s="23"/>
+      <c r="CT96" s="14"/>
+      <c r="CU96" s="23"/>
       <c r="CV96" s="8"/>
       <c r="CW96" s="8"/>
       <c r="CX96" s="8"/>
@@ -16956,20 +17019,20 @@
       <c r="CM97" s="11"/>
       <c r="CN97" s="11"/>
       <c r="CO97" s="11"/>
-      <c r="CP97" s="28"/>
-      <c r="CQ97" s="13"/>
-      <c r="CR97" s="13"/>
-      <c r="CS97" s="13"/>
-      <c r="CT97" s="13"/>
+      <c r="CP97" s="11"/>
+      <c r="CQ97" s="11"/>
+      <c r="CR97" s="5"/>
+      <c r="CS97" s="5"/>
+      <c r="CT97" s="11"/>
+      <c r="CU97" s="5"/>
     </row>
     <row r="98" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="CQ98" s="30"/>
-      <c r="CR98" s="30"/>
-      <c r="CS98" s="30"/>
-      <c r="CT98" s="30"/>
+      <c r="CR98" s="6"/>
+      <c r="CS98" s="6"/>
+      <c r="CU98" s="6"/>
     </row>
     <row r="99" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="8"/>
@@ -17064,12 +17127,12 @@
       <c r="CM99" s="8"/>
       <c r="CN99" s="8"/>
       <c r="CO99" s="8"/>
-      <c r="CP99" s="26"/>
-      <c r="CQ99" s="33"/>
-      <c r="CR99" s="33"/>
-      <c r="CS99" s="33"/>
-      <c r="CT99" s="33"/>
-      <c r="CU99" s="8"/>
+      <c r="CP99" s="8"/>
+      <c r="CQ99" s="8"/>
+      <c r="CR99" s="24"/>
+      <c r="CS99" s="24"/>
+      <c r="CT99" s="8"/>
+      <c r="CU99" s="24"/>
       <c r="CV99" s="8"/>
       <c r="CW99" s="8"/>
       <c r="CX99" s="8"/>
@@ -17212,12 +17275,12 @@
       <c r="CM100" s="8"/>
       <c r="CN100" s="8"/>
       <c r="CO100" s="8"/>
-      <c r="CP100" s="26"/>
-      <c r="CQ100" s="33"/>
-      <c r="CR100" s="33"/>
-      <c r="CS100" s="33"/>
-      <c r="CT100" s="33"/>
-      <c r="CU100" s="8"/>
+      <c r="CP100" s="8"/>
+      <c r="CQ100" s="8"/>
+      <c r="CR100" s="24"/>
+      <c r="CS100" s="24"/>
+      <c r="CT100" s="8"/>
+      <c r="CU100" s="24"/>
       <c r="CV100" s="8"/>
       <c r="CW100" s="8"/>
       <c r="CX100" s="8"/>
@@ -17274,7 +17337,7 @@
     </row>
     <row r="102" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="104" spans="1:151" x14ac:dyDescent="0.2">
@@ -17284,7 +17347,7 @@
     </row>
     <row r="105" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="1:151" x14ac:dyDescent="0.2">
@@ -17294,132 +17357,132 @@
     </row>
     <row r="108" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
-      <c r="B108" s="35">
+      <c r="B108" s="26">
         <v>2000</v>
       </c>
-      <c r="C108" s="35"/>
-      <c r="D108" s="35"/>
-      <c r="E108" s="35"/>
-      <c r="F108" s="35">
+      <c r="C108" s="26"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="26">
         <v>2001</v>
       </c>
-      <c r="G108" s="35"/>
-      <c r="H108" s="35"/>
-      <c r="I108" s="35"/>
-      <c r="J108" s="35">
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="26">
         <v>2002</v>
       </c>
-      <c r="K108" s="35"/>
-      <c r="L108" s="35"/>
-      <c r="M108" s="35"/>
-      <c r="N108" s="35">
+      <c r="K108" s="26"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
+      <c r="N108" s="26">
         <v>2003</v>
       </c>
-      <c r="O108" s="35"/>
-      <c r="P108" s="35"/>
-      <c r="Q108" s="35"/>
-      <c r="R108" s="35">
+      <c r="O108" s="26"/>
+      <c r="P108" s="26"/>
+      <c r="Q108" s="26"/>
+      <c r="R108" s="26">
         <v>2004</v>
       </c>
-      <c r="S108" s="35"/>
-      <c r="T108" s="35"/>
-      <c r="U108" s="35"/>
-      <c r="V108" s="35">
+      <c r="S108" s="26"/>
+      <c r="T108" s="26"/>
+      <c r="U108" s="26"/>
+      <c r="V108" s="26">
         <v>2005</v>
       </c>
-      <c r="W108" s="35"/>
-      <c r="X108" s="35"/>
-      <c r="Y108" s="35"/>
-      <c r="Z108" s="35">
+      <c r="W108" s="26"/>
+      <c r="X108" s="26"/>
+      <c r="Y108" s="26"/>
+      <c r="Z108" s="26">
         <v>2006</v>
       </c>
-      <c r="AA108" s="35"/>
-      <c r="AB108" s="35"/>
-      <c r="AC108" s="35"/>
-      <c r="AD108" s="35">
+      <c r="AA108" s="26"/>
+      <c r="AB108" s="26"/>
+      <c r="AC108" s="26"/>
+      <c r="AD108" s="26">
         <v>2007</v>
       </c>
-      <c r="AE108" s="35"/>
-      <c r="AF108" s="35"/>
-      <c r="AG108" s="35"/>
-      <c r="AH108" s="35">
+      <c r="AE108" s="26"/>
+      <c r="AF108" s="26"/>
+      <c r="AG108" s="26"/>
+      <c r="AH108" s="26">
         <v>2008</v>
       </c>
-      <c r="AI108" s="35"/>
-      <c r="AJ108" s="35"/>
-      <c r="AK108" s="35"/>
-      <c r="AL108" s="35">
+      <c r="AI108" s="26"/>
+      <c r="AJ108" s="26"/>
+      <c r="AK108" s="26"/>
+      <c r="AL108" s="26">
         <v>2009</v>
       </c>
-      <c r="AM108" s="35"/>
-      <c r="AN108" s="35"/>
-      <c r="AO108" s="35"/>
-      <c r="AP108" s="35">
+      <c r="AM108" s="26"/>
+      <c r="AN108" s="26"/>
+      <c r="AO108" s="26"/>
+      <c r="AP108" s="26">
         <v>2010</v>
       </c>
-      <c r="AQ108" s="35"/>
-      <c r="AR108" s="35"/>
-      <c r="AS108" s="35"/>
-      <c r="AT108" s="35">
+      <c r="AQ108" s="26"/>
+      <c r="AR108" s="26"/>
+      <c r="AS108" s="26"/>
+      <c r="AT108" s="26">
         <v>2011</v>
       </c>
-      <c r="AU108" s="35"/>
-      <c r="AV108" s="35"/>
-      <c r="AW108" s="35"/>
-      <c r="AX108" s="35">
+      <c r="AU108" s="26"/>
+      <c r="AV108" s="26"/>
+      <c r="AW108" s="26"/>
+      <c r="AX108" s="26">
         <v>2012</v>
       </c>
-      <c r="AY108" s="35"/>
-      <c r="AZ108" s="35"/>
-      <c r="BA108" s="35"/>
-      <c r="BB108" s="35">
+      <c r="AY108" s="26"/>
+      <c r="AZ108" s="26"/>
+      <c r="BA108" s="26"/>
+      <c r="BB108" s="26">
         <v>2013</v>
       </c>
-      <c r="BC108" s="35"/>
-      <c r="BD108" s="35"/>
-      <c r="BE108" s="35"/>
-      <c r="BF108" s="35">
+      <c r="BC108" s="26"/>
+      <c r="BD108" s="26"/>
+      <c r="BE108" s="26"/>
+      <c r="BF108" s="26">
         <v>2014</v>
       </c>
-      <c r="BG108" s="35"/>
-      <c r="BH108" s="35"/>
-      <c r="BI108" s="35"/>
-      <c r="BJ108" s="35">
+      <c r="BG108" s="26"/>
+      <c r="BH108" s="26"/>
+      <c r="BI108" s="26"/>
+      <c r="BJ108" s="26">
         <v>2015</v>
       </c>
-      <c r="BK108" s="35"/>
-      <c r="BL108" s="35"/>
-      <c r="BM108" s="35"/>
-      <c r="BN108" s="35">
+      <c r="BK108" s="26"/>
+      <c r="BL108" s="26"/>
+      <c r="BM108" s="26"/>
+      <c r="BN108" s="26">
         <v>2016</v>
       </c>
-      <c r="BO108" s="35"/>
-      <c r="BP108" s="35"/>
-      <c r="BQ108" s="35"/>
-      <c r="BR108" s="35">
+      <c r="BO108" s="26"/>
+      <c r="BP108" s="26"/>
+      <c r="BQ108" s="26"/>
+      <c r="BR108" s="26">
         <v>2017</v>
       </c>
-      <c r="BS108" s="35"/>
-      <c r="BT108" s="35"/>
-      <c r="BU108" s="35"/>
-      <c r="BV108" s="35">
+      <c r="BS108" s="26"/>
+      <c r="BT108" s="26"/>
+      <c r="BU108" s="26"/>
+      <c r="BV108" s="26">
         <v>2018</v>
       </c>
-      <c r="BW108" s="35"/>
-      <c r="BX108" s="35"/>
-      <c r="BY108" s="35"/>
-      <c r="BZ108" s="35">
+      <c r="BW108" s="26"/>
+      <c r="BX108" s="26"/>
+      <c r="BY108" s="26"/>
+      <c r="BZ108" s="26">
         <v>2019</v>
       </c>
-      <c r="CA108" s="35"/>
-      <c r="CB108" s="35"/>
-      <c r="CC108" s="35"/>
-      <c r="CD108" s="36">
+      <c r="CA108" s="26"/>
+      <c r="CB108" s="26"/>
+      <c r="CC108" s="26"/>
+      <c r="CD108" s="25">
         <v>2020</v>
       </c>
-      <c r="CE108" s="36"/>
-      <c r="CF108" s="36"/>
-      <c r="CG108" s="36"/>
+      <c r="CE108" s="25"/>
+      <c r="CF108" s="25"/>
+      <c r="CG108" s="25"/>
       <c r="CH108" s="21">
         <v>2021</v>
       </c>
@@ -17432,15 +17495,16 @@
       <c r="CM108" s="21"/>
       <c r="CN108" s="21"/>
       <c r="CO108" s="21"/>
-      <c r="CP108" s="24">
+      <c r="CP108" s="21">
         <v>2023</v>
       </c>
-      <c r="CQ108" s="24"/>
-      <c r="CR108" s="24"/>
-      <c r="CS108" s="24"/>
-      <c r="CT108" s="24">
+      <c r="CQ108" s="21"/>
+      <c r="CR108" s="21"/>
+      <c r="CS108" s="21"/>
+      <c r="CT108" s="21">
         <v>2024</v>
       </c>
+      <c r="CU108" s="21"/>
     </row>
     <row r="109" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
@@ -17720,20 +17784,23 @@
       <c r="CO109" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP109" s="29" t="s">
+      <c r="CP109" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ109" s="29" t="s">
+      <c r="CQ109" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CR109" s="29" t="s">
+      <c r="CR109" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="CS109" s="29" t="s">
+      <c r="CS109" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CT109" s="29" t="s">
+      <c r="CT109" s="13" t="s">
         <v>7</v>
+      </c>
+      <c r="CU109" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -18019,22 +18086,24 @@
       <c r="CO111" s="14">
         <v>133.0320896828776</v>
       </c>
-      <c r="CP111" s="31">
+      <c r="CP111" s="14">
         <v>136.72622876503405</v>
       </c>
-      <c r="CQ111" s="31">
+      <c r="CQ111" s="14">
         <v>141.65669937816352</v>
       </c>
-      <c r="CR111" s="31">
+      <c r="CR111" s="14">
         <v>130.28192558024955</v>
       </c>
-      <c r="CS111" s="31">
+      <c r="CS111" s="14">
         <v>136.18538796035799</v>
       </c>
-      <c r="CT111" s="31">
+      <c r="CT111" s="14">
         <v>139.22329574183948</v>
       </c>
-      <c r="CU111" s="8"/>
+      <c r="CU111" s="14">
+        <v>141.49602065392421</v>
+      </c>
       <c r="CV111" s="8"/>
       <c r="CW111" s="8"/>
       <c r="CX111" s="8"/>
@@ -18368,22 +18437,24 @@
       <c r="CO112" s="14">
         <v>114.41806830514707</v>
       </c>
-      <c r="CP112" s="31">
+      <c r="CP112" s="14">
         <v>119.59147290110843</v>
       </c>
-      <c r="CQ112" s="31">
+      <c r="CQ112" s="14">
         <v>119.26852215132922</v>
       </c>
-      <c r="CR112" s="31">
+      <c r="CR112" s="14">
         <v>120.01837611904935</v>
       </c>
-      <c r="CS112" s="31">
+      <c r="CS112" s="14">
         <v>117.82399759332367</v>
       </c>
-      <c r="CT112" s="31">
+      <c r="CT112" s="14">
         <v>122.28374398804517</v>
       </c>
-      <c r="CU112" s="8"/>
+      <c r="CU112" s="14">
+        <v>122.14812952633753</v>
+      </c>
       <c r="CV112" s="8"/>
       <c r="CW112" s="8"/>
       <c r="CX112" s="8"/>
@@ -18717,22 +18788,24 @@
       <c r="CO113" s="14">
         <v>117.03672057255258</v>
       </c>
-      <c r="CP113" s="31">
+      <c r="CP113" s="14">
         <v>122.00663809992125</v>
       </c>
-      <c r="CQ113" s="31">
+      <c r="CQ113" s="14">
         <v>122.63218135093956</v>
       </c>
-      <c r="CR113" s="31">
+      <c r="CR113" s="14">
         <v>124.72795126241223</v>
       </c>
-      <c r="CS113" s="31">
+      <c r="CS113" s="14">
         <v>122.09794183971367</v>
       </c>
-      <c r="CT113" s="31">
+      <c r="CT113" s="14">
         <v>126.00770654539204</v>
       </c>
-      <c r="CU113" s="8"/>
+      <c r="CU113" s="14">
+        <v>126.54895671497179</v>
+      </c>
       <c r="CV113" s="8"/>
       <c r="CW113" s="8"/>
       <c r="CX113" s="8"/>
@@ -19066,22 +19139,24 @@
       <c r="CO114" s="14">
         <v>115.53683219443604</v>
       </c>
-      <c r="CP114" s="31">
+      <c r="CP114" s="14">
         <v>115.7444035129955</v>
       </c>
-      <c r="CQ114" s="31">
+      <c r="CQ114" s="14">
         <v>116.50252804574835</v>
       </c>
-      <c r="CR114" s="31">
+      <c r="CR114" s="14">
         <v>118.14474888583113</v>
       </c>
-      <c r="CS114" s="31">
+      <c r="CS114" s="14">
         <v>120.40996061596701</v>
       </c>
-      <c r="CT114" s="31">
+      <c r="CT114" s="14">
         <v>119.8434881806138</v>
       </c>
-      <c r="CU114" s="8"/>
+      <c r="CU114" s="14">
+        <v>118.7433197401653</v>
+      </c>
       <c r="CV114" s="8"/>
       <c r="CW114" s="8"/>
       <c r="CX114" s="8"/>
@@ -19415,22 +19490,24 @@
       <c r="CO115" s="14">
         <v>103.34897185336216</v>
       </c>
-      <c r="CP115" s="31">
+      <c r="CP115" s="14">
         <v>102.92008743148232</v>
       </c>
-      <c r="CQ115" s="31">
+      <c r="CQ115" s="14">
         <v>103.61706726923939</v>
       </c>
-      <c r="CR115" s="31">
+      <c r="CR115" s="14">
         <v>102.55633330527829</v>
       </c>
-      <c r="CS115" s="31">
+      <c r="CS115" s="14">
         <v>103.68565782484302</v>
       </c>
-      <c r="CT115" s="31">
-        <v>103.35537173647829</v>
-      </c>
-      <c r="CU115" s="8"/>
+      <c r="CT115" s="14">
+        <v>103.43700151539213</v>
+      </c>
+      <c r="CU115" s="14">
+        <v>104.05566703242958</v>
+      </c>
       <c r="CV115" s="8"/>
       <c r="CW115" s="8"/>
       <c r="CX115" s="8"/>
@@ -19764,22 +19841,24 @@
       <c r="CO116" s="14">
         <v>117.00435355436905</v>
       </c>
-      <c r="CP116" s="31">
+      <c r="CP116" s="14">
         <v>118.32018478524459</v>
       </c>
-      <c r="CQ116" s="31">
+      <c r="CQ116" s="14">
         <v>118.82915304474481</v>
       </c>
-      <c r="CR116" s="31">
+      <c r="CR116" s="14">
         <v>119.9175022333163</v>
       </c>
-      <c r="CS116" s="31">
+      <c r="CS116" s="14">
         <v>120.3904189202468</v>
       </c>
-      <c r="CT116" s="31">
-        <v>120.72653522790384</v>
-      </c>
-      <c r="CU116" s="8"/>
+      <c r="CT116" s="14">
+        <v>120.72507269431662</v>
+      </c>
+      <c r="CU116" s="14">
+        <v>121.69815233560111</v>
+      </c>
       <c r="CV116" s="8"/>
       <c r="CW116" s="8"/>
       <c r="CX116" s="8"/>
@@ -20113,22 +20192,24 @@
       <c r="CO117" s="14">
         <v>117.79146924859019</v>
       </c>
-      <c r="CP117" s="31">
+      <c r="CP117" s="14">
         <v>120.87246097661833</v>
       </c>
-      <c r="CQ117" s="31">
+      <c r="CQ117" s="14">
         <v>119.17508385865622</v>
       </c>
-      <c r="CR117" s="31">
+      <c r="CR117" s="14">
         <v>121.14795441289259</v>
       </c>
-      <c r="CS117" s="31">
+      <c r="CS117" s="14">
         <v>119.74403340048416</v>
       </c>
-      <c r="CT117" s="31">
+      <c r="CT117" s="14">
         <v>123.59356996541166</v>
       </c>
-      <c r="CU117" s="8"/>
+      <c r="CU117" s="14">
+        <v>122.05243526878937</v>
+      </c>
       <c r="CV117" s="8"/>
       <c r="CW117" s="8"/>
       <c r="CX117" s="8"/>
@@ -20462,22 +20543,24 @@
       <c r="CO118" s="14">
         <v>114.26976550965544</v>
       </c>
-      <c r="CP118" s="31">
+      <c r="CP118" s="14">
         <v>119.3041020978674</v>
       </c>
-      <c r="CQ118" s="31">
+      <c r="CQ118" s="14">
         <v>118.63400847867109</v>
       </c>
-      <c r="CR118" s="31">
+      <c r="CR118" s="14">
         <v>116.31755657998011</v>
       </c>
-      <c r="CS118" s="31">
+      <c r="CS118" s="14">
         <v>117.67128020805468</v>
       </c>
-      <c r="CT118" s="31">
-        <v>121.90500916553087</v>
-      </c>
-      <c r="CU118" s="8"/>
+      <c r="CT118" s="14">
+        <v>121.88348408651571</v>
+      </c>
+      <c r="CU118" s="14">
+        <v>121.49829621846997</v>
+      </c>
       <c r="CV118" s="8"/>
       <c r="CW118" s="8"/>
       <c r="CX118" s="8"/>
@@ -20624,11 +20707,11 @@
       <c r="CM119" s="8"/>
       <c r="CN119" s="8"/>
       <c r="CO119" s="8"/>
-      <c r="CP119" s="26"/>
-      <c r="CQ119" s="26"/>
-      <c r="CR119" s="26"/>
-      <c r="CS119" s="26"/>
-      <c r="CT119" s="26"/>
+      <c r="CP119" s="8"/>
+      <c r="CQ119" s="8"/>
+      <c r="CR119" s="8"/>
+      <c r="CS119" s="8"/>
+      <c r="CT119" s="8"/>
       <c r="CU119" s="8"/>
       <c r="CV119" s="8"/>
       <c r="CW119" s="8"/>
@@ -20963,22 +21046,24 @@
       <c r="CO120" s="14">
         <v>116.07303612354485</v>
       </c>
-      <c r="CP120" s="31">
+      <c r="CP120" s="14">
         <v>117.94413080635491</v>
       </c>
-      <c r="CQ120" s="31">
+      <c r="CQ120" s="14">
         <v>117.48037037902188</v>
       </c>
-      <c r="CR120" s="31">
+      <c r="CR120" s="14">
         <v>119.232637937436</v>
       </c>
-      <c r="CS120" s="31">
+      <c r="CS120" s="14">
         <v>119.00264083203311</v>
       </c>
-      <c r="CT120" s="31">
-        <v>120.34002555372764</v>
-      </c>
-      <c r="CU120" s="8"/>
+      <c r="CT120" s="14">
+        <v>120.43354904579233</v>
+      </c>
+      <c r="CU120" s="14">
+        <v>120.09679029954219</v>
+      </c>
       <c r="CV120" s="8"/>
       <c r="CW120" s="8"/>
       <c r="CX120" s="8"/>
@@ -21126,11 +21211,12 @@
       <c r="CM121" s="11"/>
       <c r="CN121" s="11"/>
       <c r="CO121" s="11"/>
-      <c r="CP121" s="28"/>
-      <c r="CQ121" s="28"/>
-      <c r="CR121" s="28"/>
-      <c r="CS121" s="28"/>
-      <c r="CT121" s="28"/>
+      <c r="CP121" s="11"/>
+      <c r="CQ121" s="11"/>
+      <c r="CR121" s="11"/>
+      <c r="CS121" s="11"/>
+      <c r="CT121" s="11"/>
+      <c r="CU121" s="11"/>
     </row>
     <row r="122" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
@@ -21149,7 +21235,7 @@
     </row>
     <row r="127" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="129" spans="1:151" x14ac:dyDescent="0.2">
@@ -21159,7 +21245,7 @@
     </row>
     <row r="130" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="131" spans="1:151" x14ac:dyDescent="0.2">
@@ -21169,132 +21255,132 @@
     </row>
     <row r="133" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
-      <c r="B133" s="35">
+      <c r="B133" s="26">
         <v>2000</v>
       </c>
-      <c r="C133" s="35"/>
-      <c r="D133" s="35"/>
-      <c r="E133" s="35"/>
-      <c r="F133" s="35">
+      <c r="C133" s="26"/>
+      <c r="D133" s="26"/>
+      <c r="E133" s="26"/>
+      <c r="F133" s="26">
         <v>2001</v>
       </c>
-      <c r="G133" s="35"/>
-      <c r="H133" s="35"/>
-      <c r="I133" s="35"/>
-      <c r="J133" s="35">
+      <c r="G133" s="26"/>
+      <c r="H133" s="26"/>
+      <c r="I133" s="26"/>
+      <c r="J133" s="26">
         <v>2002</v>
       </c>
-      <c r="K133" s="35"/>
-      <c r="L133" s="35"/>
-      <c r="M133" s="35"/>
-      <c r="N133" s="35">
+      <c r="K133" s="26"/>
+      <c r="L133" s="26"/>
+      <c r="M133" s="26"/>
+      <c r="N133" s="26">
         <v>2003</v>
       </c>
-      <c r="O133" s="35"/>
-      <c r="P133" s="35"/>
-      <c r="Q133" s="35"/>
-      <c r="R133" s="35">
+      <c r="O133" s="26"/>
+      <c r="P133" s="26"/>
+      <c r="Q133" s="26"/>
+      <c r="R133" s="26">
         <v>2004</v>
       </c>
-      <c r="S133" s="35"/>
-      <c r="T133" s="35"/>
-      <c r="U133" s="35"/>
-      <c r="V133" s="35">
+      <c r="S133" s="26"/>
+      <c r="T133" s="26"/>
+      <c r="U133" s="26"/>
+      <c r="V133" s="26">
         <v>2005</v>
       </c>
-      <c r="W133" s="35"/>
-      <c r="X133" s="35"/>
-      <c r="Y133" s="35"/>
-      <c r="Z133" s="35">
+      <c r="W133" s="26"/>
+      <c r="X133" s="26"/>
+      <c r="Y133" s="26"/>
+      <c r="Z133" s="26">
         <v>2006</v>
       </c>
-      <c r="AA133" s="35"/>
-      <c r="AB133" s="35"/>
-      <c r="AC133" s="35"/>
-      <c r="AD133" s="35">
+      <c r="AA133" s="26"/>
+      <c r="AB133" s="26"/>
+      <c r="AC133" s="26"/>
+      <c r="AD133" s="26">
         <v>2007</v>
       </c>
-      <c r="AE133" s="35"/>
-      <c r="AF133" s="35"/>
-      <c r="AG133" s="35"/>
-      <c r="AH133" s="35">
+      <c r="AE133" s="26"/>
+      <c r="AF133" s="26"/>
+      <c r="AG133" s="26"/>
+      <c r="AH133" s="26">
         <v>2008</v>
       </c>
-      <c r="AI133" s="35"/>
-      <c r="AJ133" s="35"/>
-      <c r="AK133" s="35"/>
-      <c r="AL133" s="35">
+      <c r="AI133" s="26"/>
+      <c r="AJ133" s="26"/>
+      <c r="AK133" s="26"/>
+      <c r="AL133" s="26">
         <v>2009</v>
       </c>
-      <c r="AM133" s="35"/>
-      <c r="AN133" s="35"/>
-      <c r="AO133" s="35"/>
-      <c r="AP133" s="35">
+      <c r="AM133" s="26"/>
+      <c r="AN133" s="26"/>
+      <c r="AO133" s="26"/>
+      <c r="AP133" s="26">
         <v>2010</v>
       </c>
-      <c r="AQ133" s="35"/>
-      <c r="AR133" s="35"/>
-      <c r="AS133" s="35"/>
-      <c r="AT133" s="35">
+      <c r="AQ133" s="26"/>
+      <c r="AR133" s="26"/>
+      <c r="AS133" s="26"/>
+      <c r="AT133" s="26">
         <v>2011</v>
       </c>
-      <c r="AU133" s="35"/>
-      <c r="AV133" s="35"/>
-      <c r="AW133" s="35"/>
-      <c r="AX133" s="35">
+      <c r="AU133" s="26"/>
+      <c r="AV133" s="26"/>
+      <c r="AW133" s="26"/>
+      <c r="AX133" s="26">
         <v>2012</v>
       </c>
-      <c r="AY133" s="35"/>
-      <c r="AZ133" s="35"/>
-      <c r="BA133" s="35"/>
-      <c r="BB133" s="35">
+      <c r="AY133" s="26"/>
+      <c r="AZ133" s="26"/>
+      <c r="BA133" s="26"/>
+      <c r="BB133" s="26">
         <v>2013</v>
       </c>
-      <c r="BC133" s="35"/>
-      <c r="BD133" s="35"/>
-      <c r="BE133" s="35"/>
-      <c r="BF133" s="35">
+      <c r="BC133" s="26"/>
+      <c r="BD133" s="26"/>
+      <c r="BE133" s="26"/>
+      <c r="BF133" s="26">
         <v>2014</v>
       </c>
-      <c r="BG133" s="35"/>
-      <c r="BH133" s="35"/>
-      <c r="BI133" s="35"/>
-      <c r="BJ133" s="35">
+      <c r="BG133" s="26"/>
+      <c r="BH133" s="26"/>
+      <c r="BI133" s="26"/>
+      <c r="BJ133" s="26">
         <v>2015</v>
       </c>
-      <c r="BK133" s="35"/>
-      <c r="BL133" s="35"/>
-      <c r="BM133" s="35"/>
-      <c r="BN133" s="35">
+      <c r="BK133" s="26"/>
+      <c r="BL133" s="26"/>
+      <c r="BM133" s="26"/>
+      <c r="BN133" s="26">
         <v>2016</v>
       </c>
-      <c r="BO133" s="35"/>
-      <c r="BP133" s="35"/>
-      <c r="BQ133" s="35"/>
-      <c r="BR133" s="35">
+      <c r="BO133" s="26"/>
+      <c r="BP133" s="26"/>
+      <c r="BQ133" s="26"/>
+      <c r="BR133" s="26">
         <v>2017</v>
       </c>
-      <c r="BS133" s="35"/>
-      <c r="BT133" s="35"/>
-      <c r="BU133" s="35"/>
-      <c r="BV133" s="35">
+      <c r="BS133" s="26"/>
+      <c r="BT133" s="26"/>
+      <c r="BU133" s="26"/>
+      <c r="BV133" s="26">
         <v>2018</v>
       </c>
-      <c r="BW133" s="35"/>
-      <c r="BX133" s="35"/>
-      <c r="BY133" s="35"/>
-      <c r="BZ133" s="35">
+      <c r="BW133" s="26"/>
+      <c r="BX133" s="26"/>
+      <c r="BY133" s="26"/>
+      <c r="BZ133" s="26">
         <v>2019</v>
       </c>
-      <c r="CA133" s="35"/>
-      <c r="CB133" s="35"/>
-      <c r="CC133" s="35"/>
-      <c r="CD133" s="36">
+      <c r="CA133" s="26"/>
+      <c r="CB133" s="26"/>
+      <c r="CC133" s="26"/>
+      <c r="CD133" s="25">
         <v>2020</v>
       </c>
-      <c r="CE133" s="36"/>
-      <c r="CF133" s="36"/>
-      <c r="CG133" s="36"/>
+      <c r="CE133" s="25"/>
+      <c r="CF133" s="25"/>
+      <c r="CG133" s="25"/>
       <c r="CH133" s="21">
         <v>2021</v>
       </c>
@@ -21307,15 +21393,16 @@
       <c r="CM133" s="21"/>
       <c r="CN133" s="21"/>
       <c r="CO133" s="21"/>
-      <c r="CP133" s="24">
+      <c r="CP133" s="21">
         <v>2023</v>
       </c>
-      <c r="CQ133" s="24"/>
-      <c r="CR133" s="24"/>
-      <c r="CS133" s="24"/>
-      <c r="CT133" s="24">
+      <c r="CQ133" s="21"/>
+      <c r="CR133" s="21"/>
+      <c r="CS133" s="21"/>
+      <c r="CT133" s="21">
         <v>2024</v>
       </c>
+      <c r="CU133" s="21"/>
     </row>
     <row r="134" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
@@ -21595,20 +21682,23 @@
       <c r="CO134" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP134" s="29" t="s">
+      <c r="CP134" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ134" s="29" t="s">
+      <c r="CQ134" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CR134" s="29" t="s">
+      <c r="CR134" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="CS134" s="29" t="s">
+      <c r="CS134" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CT134" s="29" t="s">
+      <c r="CT134" s="13" t="s">
         <v>7</v>
+      </c>
+      <c r="CU134" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -21894,22 +21984,24 @@
       <c r="CO136" s="20">
         <v>8.7827302543622761</v>
       </c>
-      <c r="CP136" s="34">
+      <c r="CP136" s="20">
         <v>10.423788448805297</v>
       </c>
-      <c r="CQ136" s="34">
+      <c r="CQ136" s="20">
         <v>4.1182304678552075</v>
       </c>
-      <c r="CR136" s="34">
+      <c r="CR136" s="20">
         <v>7.0676659503017865</v>
       </c>
-      <c r="CS136" s="34">
+      <c r="CS136" s="20">
         <v>8.5825179703148056</v>
       </c>
-      <c r="CT136" s="34">
-        <v>10.334911865670122</v>
-      </c>
-      <c r="CU136" s="8"/>
+      <c r="CT136" s="20">
+        <v>10.511899449352228</v>
+      </c>
+      <c r="CU136" s="20">
+        <v>4.1284208554563735</v>
+      </c>
       <c r="CV136" s="8"/>
       <c r="CW136" s="8"/>
       <c r="CX136" s="8"/>
@@ -22243,22 +22335,24 @@
       <c r="CO137" s="20">
         <v>0.16108702810670397</v>
       </c>
-      <c r="CP137" s="34">
+      <c r="CP137" s="20">
         <v>5.4753624936512799E-2</v>
       </c>
-      <c r="CQ137" s="34">
+      <c r="CQ137" s="20">
         <v>5.5436820494742294E-2</v>
       </c>
-      <c r="CR137" s="34">
+      <c r="CR137" s="20">
         <v>0.12684227721550209</v>
       </c>
-      <c r="CS137" s="34">
+      <c r="CS137" s="20">
         <v>0.13176515537394626</v>
       </c>
-      <c r="CT137" s="34">
-        <v>5.6888105693444539E-2</v>
-      </c>
-      <c r="CU137" s="8"/>
+      <c r="CT137" s="20">
+        <v>5.4699755931179699E-2</v>
+      </c>
+      <c r="CU137" s="20">
+        <v>5.6246886994848304E-2</v>
+      </c>
       <c r="CV137" s="8"/>
       <c r="CW137" s="8"/>
       <c r="CX137" s="8"/>
@@ -22592,22 +22686,24 @@
       <c r="CO138" s="20">
         <v>10.337774260791397</v>
       </c>
-      <c r="CP138" s="34">
+      <c r="CP138" s="20">
         <v>14.605360688296587</v>
       </c>
-      <c r="CQ138" s="34">
+      <c r="CQ138" s="20">
         <v>15.808579397825692</v>
       </c>
-      <c r="CR138" s="34">
+      <c r="CR138" s="20">
         <v>23.795656408870862</v>
       </c>
-      <c r="CS138" s="34">
+      <c r="CS138" s="20">
         <v>15.022013741043057</v>
       </c>
-      <c r="CT138" s="34">
-        <v>15.546223282954674</v>
-      </c>
-      <c r="CU138" s="8"/>
+      <c r="CT138" s="20">
+        <v>15.499872055049821</v>
+      </c>
+      <c r="CU138" s="20">
+        <v>18.113373570110884</v>
+      </c>
       <c r="CV138" s="8"/>
       <c r="CW138" s="8"/>
       <c r="CX138" s="8"/>
@@ -22941,22 +23037,24 @@
       <c r="CO139" s="20">
         <v>0.73988259333163631</v>
       </c>
-      <c r="CP139" s="34">
+      <c r="CP139" s="20">
         <v>0.52127711364677609</v>
       </c>
-      <c r="CQ139" s="34">
+      <c r="CQ139" s="20">
         <v>0.6139269747570516</v>
       </c>
-      <c r="CR139" s="34">
+      <c r="CR139" s="20">
         <v>0.72287239904319722</v>
       </c>
-      <c r="CS139" s="34">
+      <c r="CS139" s="20">
         <v>0.7680504103126351</v>
       </c>
-      <c r="CT139" s="34">
-        <v>0.53602073530442496</v>
-      </c>
-      <c r="CU139" s="8"/>
+      <c r="CT139" s="20">
+        <v>0.50953856776760176</v>
+      </c>
+      <c r="CU139" s="20">
+        <v>0.58347303284311358</v>
+      </c>
       <c r="CV139" s="8"/>
       <c r="CW139" s="8"/>
       <c r="CX139" s="8"/>
@@ -23290,22 +23388,24 @@
       <c r="CO140" s="20">
         <v>14.225701187072531</v>
       </c>
-      <c r="CP140" s="34">
+      <c r="CP140" s="20">
         <v>15.541367844351198</v>
       </c>
-      <c r="CQ140" s="34">
+      <c r="CQ140" s="20">
         <v>15.7698382907679</v>
       </c>
-      <c r="CR140" s="34">
+      <c r="CR140" s="20">
         <v>12.380763502046364</v>
       </c>
-      <c r="CS140" s="34">
+      <c r="CS140" s="20">
         <v>14.114051238263833</v>
       </c>
-      <c r="CT140" s="34">
-        <v>14.999898527091576</v>
-      </c>
-      <c r="CU140" s="8"/>
+      <c r="CT140" s="20">
+        <v>14.783460420958672</v>
+      </c>
+      <c r="CU140" s="20">
+        <v>15.421129945001558</v>
+      </c>
       <c r="CV140" s="8"/>
       <c r="CW140" s="8"/>
       <c r="CX140" s="8"/>
@@ -23639,22 +23739,24 @@
       <c r="CO141" s="20">
         <v>53.234884723567731</v>
       </c>
-      <c r="CP141" s="34">
+      <c r="CP141" s="20">
         <v>50.065600760877572</v>
       </c>
-      <c r="CQ141" s="34">
+      <c r="CQ141" s="20">
         <v>52.840947826538496</v>
       </c>
-      <c r="CR141" s="34">
+      <c r="CR141" s="20">
         <v>45.6499491973509</v>
       </c>
-      <c r="CS141" s="34">
+      <c r="CS141" s="20">
         <v>49.55862943674714</v>
       </c>
-      <c r="CT141" s="34">
-        <v>50.307850715884598</v>
-      </c>
-      <c r="CU141" s="8"/>
+      <c r="CT141" s="20">
+        <v>50.10118085447165</v>
+      </c>
+      <c r="CU141" s="20">
+        <v>51.107292357202574</v>
+      </c>
       <c r="CV141" s="8"/>
       <c r="CW141" s="8"/>
       <c r="CX141" s="8"/>
@@ -23988,22 +24090,24 @@
       <c r="CO142" s="20">
         <v>10.742804778856668</v>
       </c>
-      <c r="CP142" s="34">
+      <c r="CP142" s="20">
         <v>7.8201288003847322</v>
       </c>
-      <c r="CQ142" s="34">
+      <c r="CQ142" s="20">
         <v>9.4570199276183633</v>
       </c>
-      <c r="CR142" s="34">
+      <c r="CR142" s="20">
         <v>8.992355665061643</v>
       </c>
-      <c r="CS142" s="34">
+      <c r="CS142" s="20">
         <v>10.061766542551789</v>
       </c>
-      <c r="CT142" s="34">
-        <v>7.3195352508867533</v>
-      </c>
-      <c r="CU142" s="8"/>
+      <c r="CT142" s="20">
+        <v>7.6024569149773722</v>
+      </c>
+      <c r="CU142" s="20">
+        <v>9.0191833477341952</v>
+      </c>
       <c r="CV142" s="8"/>
       <c r="CW142" s="8"/>
       <c r="CX142" s="8"/>
@@ -24337,22 +24441,24 @@
       <c r="CO143" s="20">
         <v>1.7751351739110399</v>
       </c>
-      <c r="CP143" s="34">
+      <c r="CP143" s="20">
         <v>0.96772271870133808</v>
       </c>
-      <c r="CQ143" s="34">
+      <c r="CQ143" s="20">
         <v>1.336020294142531</v>
       </c>
-      <c r="CR143" s="34">
+      <c r="CR143" s="20">
         <v>1.2638946001097586</v>
       </c>
-      <c r="CS143" s="34">
+      <c r="CS143" s="20">
         <v>1.7612055053927922</v>
       </c>
-      <c r="CT143" s="34">
-        <v>0.8986715165144179</v>
-      </c>
-      <c r="CU143" s="8"/>
+      <c r="CT143" s="20">
+        <v>0.93689198149148001</v>
+      </c>
+      <c r="CU143" s="20">
+        <v>1.5708800046564511</v>
+      </c>
       <c r="CV143" s="8"/>
       <c r="CW143" s="8"/>
       <c r="CX143" s="8"/>
@@ -24499,11 +24605,11 @@
       <c r="CM144" s="8"/>
       <c r="CN144" s="8"/>
       <c r="CO144" s="8"/>
-      <c r="CP144" s="26"/>
-      <c r="CQ144" s="26"/>
-      <c r="CR144" s="26"/>
-      <c r="CS144" s="26"/>
-      <c r="CT144" s="26"/>
+      <c r="CP144" s="8"/>
+      <c r="CQ144" s="8"/>
+      <c r="CR144" s="8"/>
+      <c r="CS144" s="8"/>
+      <c r="CT144" s="8"/>
       <c r="CU144" s="8"/>
       <c r="CV144" s="8"/>
       <c r="CW144" s="8"/>
@@ -24838,22 +24944,24 @@
       <c r="CO145" s="14">
         <v>100</v>
       </c>
-      <c r="CP145" s="31">
+      <c r="CP145" s="14">
         <v>100</v>
       </c>
-      <c r="CQ145" s="31">
+      <c r="CQ145" s="14">
         <v>100</v>
       </c>
-      <c r="CR145" s="31">
+      <c r="CR145" s="14">
         <v>100</v>
       </c>
-      <c r="CS145" s="31">
+      <c r="CS145" s="14">
         <v>100</v>
       </c>
-      <c r="CT145" s="31">
+      <c r="CT145" s="14">
         <v>100</v>
       </c>
-      <c r="CU145" s="8"/>
+      <c r="CU145" s="14">
+        <v>100</v>
+      </c>
       <c r="CV145" s="8"/>
       <c r="CW145" s="8"/>
       <c r="CX145" s="8"/>
@@ -25001,11 +25109,12 @@
       <c r="CM146" s="11"/>
       <c r="CN146" s="11"/>
       <c r="CO146" s="11"/>
-      <c r="CP146" s="28"/>
-      <c r="CQ146" s="28"/>
-      <c r="CR146" s="28"/>
-      <c r="CS146" s="28"/>
-      <c r="CT146" s="28"/>
+      <c r="CP146" s="11"/>
+      <c r="CQ146" s="11"/>
+      <c r="CR146" s="11"/>
+      <c r="CS146" s="11"/>
+      <c r="CT146" s="11"/>
+      <c r="CU146" s="11"/>
     </row>
     <row r="147" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="s">
@@ -25105,11 +25214,11 @@
       <c r="CM148" s="8"/>
       <c r="CN148" s="8"/>
       <c r="CO148" s="8"/>
-      <c r="CP148" s="26"/>
-      <c r="CQ148" s="26"/>
-      <c r="CR148" s="26"/>
-      <c r="CS148" s="26"/>
-      <c r="CT148" s="26"/>
+      <c r="CP148" s="8"/>
+      <c r="CQ148" s="8"/>
+      <c r="CR148" s="8"/>
+      <c r="CS148" s="8"/>
+      <c r="CT148" s="8"/>
       <c r="CU148" s="8"/>
       <c r="CV148" s="8"/>
       <c r="CW148" s="8"/>
@@ -25257,11 +25366,11 @@
       <c r="CM149" s="8"/>
       <c r="CN149" s="8"/>
       <c r="CO149" s="8"/>
-      <c r="CP149" s="26"/>
-      <c r="CQ149" s="26"/>
-      <c r="CR149" s="26"/>
-      <c r="CS149" s="26"/>
-      <c r="CT149" s="26"/>
+      <c r="CP149" s="8"/>
+      <c r="CQ149" s="8"/>
+      <c r="CR149" s="8"/>
+      <c r="CS149" s="8"/>
+      <c r="CT149" s="8"/>
       <c r="CU149" s="8"/>
       <c r="CV149" s="8"/>
       <c r="CW149" s="8"/>
@@ -25328,7 +25437,7 @@
     </row>
     <row r="152" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="154" spans="1:151" x14ac:dyDescent="0.2">
@@ -25338,7 +25447,7 @@
     </row>
     <row r="155" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="156" spans="1:151" x14ac:dyDescent="0.2">
@@ -25348,132 +25457,132 @@
     </row>
     <row r="158" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
-      <c r="B158" s="35">
+      <c r="B158" s="26">
         <v>2000</v>
       </c>
-      <c r="C158" s="35"/>
-      <c r="D158" s="35"/>
-      <c r="E158" s="35"/>
-      <c r="F158" s="35">
+      <c r="C158" s="26"/>
+      <c r="D158" s="26"/>
+      <c r="E158" s="26"/>
+      <c r="F158" s="26">
         <v>2001</v>
       </c>
-      <c r="G158" s="35"/>
-      <c r="H158" s="35"/>
-      <c r="I158" s="35"/>
-      <c r="J158" s="35">
+      <c r="G158" s="26"/>
+      <c r="H158" s="26"/>
+      <c r="I158" s="26"/>
+      <c r="J158" s="26">
         <v>2002</v>
       </c>
-      <c r="K158" s="35"/>
-      <c r="L158" s="35"/>
-      <c r="M158" s="35"/>
-      <c r="N158" s="35">
+      <c r="K158" s="26"/>
+      <c r="L158" s="26"/>
+      <c r="M158" s="26"/>
+      <c r="N158" s="26">
         <v>2003</v>
       </c>
-      <c r="O158" s="35"/>
-      <c r="P158" s="35"/>
-      <c r="Q158" s="35"/>
-      <c r="R158" s="35">
+      <c r="O158" s="26"/>
+      <c r="P158" s="26"/>
+      <c r="Q158" s="26"/>
+      <c r="R158" s="26">
         <v>2004</v>
       </c>
-      <c r="S158" s="35"/>
-      <c r="T158" s="35"/>
-      <c r="U158" s="35"/>
-      <c r="V158" s="35">
+      <c r="S158" s="26"/>
+      <c r="T158" s="26"/>
+      <c r="U158" s="26"/>
+      <c r="V158" s="26">
         <v>2005</v>
       </c>
-      <c r="W158" s="35"/>
-      <c r="X158" s="35"/>
-      <c r="Y158" s="35"/>
-      <c r="Z158" s="35">
+      <c r="W158" s="26"/>
+      <c r="X158" s="26"/>
+      <c r="Y158" s="26"/>
+      <c r="Z158" s="26">
         <v>2006</v>
       </c>
-      <c r="AA158" s="35"/>
-      <c r="AB158" s="35"/>
-      <c r="AC158" s="35"/>
-      <c r="AD158" s="35">
+      <c r="AA158" s="26"/>
+      <c r="AB158" s="26"/>
+      <c r="AC158" s="26"/>
+      <c r="AD158" s="26">
         <v>2007</v>
       </c>
-      <c r="AE158" s="35"/>
-      <c r="AF158" s="35"/>
-      <c r="AG158" s="35"/>
-      <c r="AH158" s="35">
+      <c r="AE158" s="26"/>
+      <c r="AF158" s="26"/>
+      <c r="AG158" s="26"/>
+      <c r="AH158" s="26">
         <v>2008</v>
       </c>
-      <c r="AI158" s="35"/>
-      <c r="AJ158" s="35"/>
-      <c r="AK158" s="35"/>
-      <c r="AL158" s="35">
+      <c r="AI158" s="26"/>
+      <c r="AJ158" s="26"/>
+      <c r="AK158" s="26"/>
+      <c r="AL158" s="26">
         <v>2009</v>
       </c>
-      <c r="AM158" s="35"/>
-      <c r="AN158" s="35"/>
-      <c r="AO158" s="35"/>
-      <c r="AP158" s="35">
+      <c r="AM158" s="26"/>
+      <c r="AN158" s="26"/>
+      <c r="AO158" s="26"/>
+      <c r="AP158" s="26">
         <v>2010</v>
       </c>
-      <c r="AQ158" s="35"/>
-      <c r="AR158" s="35"/>
-      <c r="AS158" s="35"/>
-      <c r="AT158" s="35">
+      <c r="AQ158" s="26"/>
+      <c r="AR158" s="26"/>
+      <c r="AS158" s="26"/>
+      <c r="AT158" s="26">
         <v>2011</v>
       </c>
-      <c r="AU158" s="35"/>
-      <c r="AV158" s="35"/>
-      <c r="AW158" s="35"/>
-      <c r="AX158" s="35">
+      <c r="AU158" s="26"/>
+      <c r="AV158" s="26"/>
+      <c r="AW158" s="26"/>
+      <c r="AX158" s="26">
         <v>2012</v>
       </c>
-      <c r="AY158" s="35"/>
-      <c r="AZ158" s="35"/>
-      <c r="BA158" s="35"/>
-      <c r="BB158" s="35">
+      <c r="AY158" s="26"/>
+      <c r="AZ158" s="26"/>
+      <c r="BA158" s="26"/>
+      <c r="BB158" s="26">
         <v>2013</v>
       </c>
-      <c r="BC158" s="35"/>
-      <c r="BD158" s="35"/>
-      <c r="BE158" s="35"/>
-      <c r="BF158" s="35">
+      <c r="BC158" s="26"/>
+      <c r="BD158" s="26"/>
+      <c r="BE158" s="26"/>
+      <c r="BF158" s="26">
         <v>2014</v>
       </c>
-      <c r="BG158" s="35"/>
-      <c r="BH158" s="35"/>
-      <c r="BI158" s="35"/>
-      <c r="BJ158" s="35">
+      <c r="BG158" s="26"/>
+      <c r="BH158" s="26"/>
+      <c r="BI158" s="26"/>
+      <c r="BJ158" s="26">
         <v>2015</v>
       </c>
-      <c r="BK158" s="35"/>
-      <c r="BL158" s="35"/>
-      <c r="BM158" s="35"/>
-      <c r="BN158" s="35">
+      <c r="BK158" s="26"/>
+      <c r="BL158" s="26"/>
+      <c r="BM158" s="26"/>
+      <c r="BN158" s="26">
         <v>2016</v>
       </c>
-      <c r="BO158" s="35"/>
-      <c r="BP158" s="35"/>
-      <c r="BQ158" s="35"/>
-      <c r="BR158" s="35">
+      <c r="BO158" s="26"/>
+      <c r="BP158" s="26"/>
+      <c r="BQ158" s="26"/>
+      <c r="BR158" s="26">
         <v>2017</v>
       </c>
-      <c r="BS158" s="35"/>
-      <c r="BT158" s="35"/>
-      <c r="BU158" s="35"/>
-      <c r="BV158" s="35">
+      <c r="BS158" s="26"/>
+      <c r="BT158" s="26"/>
+      <c r="BU158" s="26"/>
+      <c r="BV158" s="26">
         <v>2018</v>
       </c>
-      <c r="BW158" s="35"/>
-      <c r="BX158" s="35"/>
-      <c r="BY158" s="35"/>
-      <c r="BZ158" s="35">
+      <c r="BW158" s="26"/>
+      <c r="BX158" s="26"/>
+      <c r="BY158" s="26"/>
+      <c r="BZ158" s="26">
         <v>2019</v>
       </c>
-      <c r="CA158" s="35"/>
-      <c r="CB158" s="35"/>
-      <c r="CC158" s="35"/>
-      <c r="CD158" s="36">
+      <c r="CA158" s="26"/>
+      <c r="CB158" s="26"/>
+      <c r="CC158" s="26"/>
+      <c r="CD158" s="25">
         <v>2020</v>
       </c>
-      <c r="CE158" s="36"/>
-      <c r="CF158" s="36"/>
-      <c r="CG158" s="36"/>
+      <c r="CE158" s="25"/>
+      <c r="CF158" s="25"/>
+      <c r="CG158" s="25"/>
       <c r="CH158" s="21">
         <v>2021</v>
       </c>
@@ -25486,15 +25595,16 @@
       <c r="CM158" s="21"/>
       <c r="CN158" s="21"/>
       <c r="CO158" s="21"/>
-      <c r="CP158" s="24">
+      <c r="CP158" s="21">
         <v>2023</v>
       </c>
-      <c r="CQ158" s="24"/>
-      <c r="CR158" s="24"/>
-      <c r="CS158" s="24"/>
-      <c r="CT158" s="24">
+      <c r="CQ158" s="21"/>
+      <c r="CR158" s="21"/>
+      <c r="CS158" s="21"/>
+      <c r="CT158" s="21">
         <v>2024</v>
       </c>
+      <c r="CU158" s="21"/>
     </row>
     <row r="159" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A159" s="4"/>
@@ -25774,20 +25884,23 @@
       <c r="CO159" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP159" s="29" t="s">
+      <c r="CP159" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ159" s="29" t="s">
+      <c r="CQ159" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CR159" s="29" t="s">
+      <c r="CR159" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="CS159" s="29" t="s">
+      <c r="CS159" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CT159" s="29" t="s">
+      <c r="CT159" s="13" t="s">
         <v>7</v>
+      </c>
+      <c r="CU159" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="160" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -26073,22 +26186,24 @@
       <c r="CO161" s="20">
         <v>7.6630996965324938</v>
       </c>
-      <c r="CP161" s="34">
+      <c r="CP161" s="20">
         <v>8.9918714163940461</v>
       </c>
-      <c r="CQ161" s="34">
+      <c r="CQ161" s="20">
         <v>3.4153784663458158</v>
       </c>
-      <c r="CR161" s="34">
+      <c r="CR161" s="20">
         <v>6.4682529948945442</v>
       </c>
-      <c r="CS161" s="34">
+      <c r="CS161" s="20">
         <v>7.4996467591159188</v>
       </c>
-      <c r="CT161" s="34">
-        <v>8.9331569934707904</v>
-      </c>
-      <c r="CU161" s="8"/>
+      <c r="CT161" s="20">
+        <v>9.0932006109487933</v>
+      </c>
+      <c r="CU161" s="20">
+        <v>3.5040568028317205</v>
+      </c>
       <c r="CV161" s="8"/>
       <c r="CW161" s="8"/>
       <c r="CX161" s="8"/>
@@ -26422,22 +26537,24 @@
       <c r="CO162" s="20">
         <v>0.16341702590711205</v>
       </c>
-      <c r="CP162" s="34">
+      <c r="CP162" s="20">
         <v>5.3999407691669186E-2</v>
       </c>
-      <c r="CQ162" s="34">
+      <c r="CQ162" s="20">
         <v>5.4605675385951721E-2</v>
       </c>
-      <c r="CR162" s="34">
+      <c r="CR162" s="20">
         <v>0.12601186421147886</v>
       </c>
-      <c r="CS162" s="34">
+      <c r="CS162" s="20">
         <v>0.13308325790527478</v>
       </c>
-      <c r="CT162" s="34">
-        <v>5.5983860729039756E-2</v>
-      </c>
-      <c r="CU162" s="8"/>
+      <c r="CT162" s="20">
+        <v>5.3872129883221702E-2</v>
+      </c>
+      <c r="CU162" s="20">
+        <v>5.5302284354389719E-2</v>
+      </c>
       <c r="CV162" s="8"/>
       <c r="CW162" s="8"/>
       <c r="CX162" s="8"/>
@@ -26771,22 +26888,24 @@
       <c r="CO163" s="20">
         <v>10.252652666100939</v>
       </c>
-      <c r="CP163" s="34">
+      <c r="CP163" s="20">
         <v>14.119039736867878</v>
       </c>
-      <c r="CQ163" s="34">
+      <c r="CQ163" s="20">
         <v>15.144456718974508</v>
       </c>
-      <c r="CR163" s="34">
+      <c r="CR163" s="20">
         <v>22.747257983203529</v>
       </c>
-      <c r="CS163" s="34">
+      <c r="CS163" s="20">
         <v>14.64119115247656</v>
       </c>
-      <c r="CT163" s="34">
-        <v>14.846972129127566</v>
-      </c>
-      <c r="CU163" s="8"/>
+      <c r="CT163" s="20">
+        <v>14.814209801310064</v>
+      </c>
+      <c r="CU163" s="20">
+        <v>17.189853505995075</v>
+      </c>
       <c r="CV163" s="8"/>
       <c r="CW163" s="8"/>
       <c r="CX163" s="8"/>
@@ -27120,22 +27239,24 @@
       <c r="CO164" s="20">
         <v>0.74331637237930814</v>
       </c>
-      <c r="CP164" s="34">
+      <c r="CP164" s="20">
         <v>0.53118400728041659</v>
       </c>
-      <c r="CQ164" s="34">
+      <c r="CQ164" s="20">
         <v>0.61907985680627431</v>
       </c>
-      <c r="CR164" s="34">
+      <c r="CR164" s="20">
         <v>0.72952868276331728</v>
       </c>
-      <c r="CS164" s="34">
+      <c r="CS164" s="20">
         <v>0.75907364018529599</v>
       </c>
-      <c r="CT164" s="34">
-        <v>0.53824158461282867</v>
-      </c>
-      <c r="CU164" s="8"/>
+      <c r="CT164" s="20">
+        <v>0.51204732959273869</v>
+      </c>
+      <c r="CU164" s="20">
+        <v>0.59012362652595463</v>
+      </c>
       <c r="CV164" s="8"/>
       <c r="CW164" s="8"/>
       <c r="CX164" s="8"/>
@@ -27469,22 +27590,24 @@
       <c r="CO165" s="20">
         <v>15.977133571417401</v>
       </c>
-      <c r="CP165" s="34">
+      <c r="CP165" s="20">
         <v>17.810061842049443</v>
       </c>
-      <c r="CQ165" s="34">
+      <c r="CQ165" s="20">
         <v>17.879742131696933</v>
       </c>
-      <c r="CR165" s="34">
+      <c r="CR165" s="20">
         <v>14.393953493192416</v>
       </c>
-      <c r="CS165" s="34">
+      <c r="CS165" s="20">
         <v>16.199052071689611</v>
       </c>
-      <c r="CT165" s="34">
-        <v>17.464870395472953</v>
-      </c>
-      <c r="CU165" s="8"/>
+      <c r="CT165" s="20">
+        <v>17.212647114573571</v>
+      </c>
+      <c r="CU165" s="20">
+        <v>17.79843675990897</v>
+      </c>
       <c r="CV165" s="8"/>
       <c r="CW165" s="8"/>
       <c r="CX165" s="8"/>
@@ -27818,22 +27941,24 @@
       <c r="CO166" s="20">
         <v>52.81115197717947</v>
       </c>
-      <c r="CP166" s="34">
+      <c r="CP166" s="20">
         <v>49.906478558644686</v>
       </c>
-      <c r="CQ166" s="34">
+      <c r="CQ166" s="20">
         <v>52.241171150170473</v>
       </c>
-      <c r="CR166" s="34">
+      <c r="CR166" s="20">
         <v>45.389236459579003</v>
       </c>
-      <c r="CS166" s="34">
+      <c r="CS166" s="20">
         <v>48.987351583982289</v>
       </c>
-      <c r="CT166" s="34">
-        <v>50.146788601810044</v>
-      </c>
-      <c r="CU166" s="8"/>
+      <c r="CT166" s="20">
+        <v>49.980197874614156</v>
+      </c>
+      <c r="CU166" s="20">
+        <v>50.434798353177776</v>
+      </c>
       <c r="CV166" s="8"/>
       <c r="CW166" s="8"/>
       <c r="CX166" s="8"/>
@@ -28167,22 +28292,24 @@
       <c r="CO167" s="20">
         <v>10.586080427716073</v>
       </c>
-      <c r="CP167" s="34">
+      <c r="CP167" s="20">
         <v>7.6306735769493264</v>
       </c>
-      <c r="CQ167" s="34">
+      <c r="CQ167" s="20">
         <v>9.3225376295608804</v>
       </c>
-      <c r="CR167" s="34">
+      <c r="CR167" s="20">
         <v>8.850188947993038</v>
       </c>
-      <c r="CS167" s="34">
+      <c r="CS167" s="20">
         <v>9.9994693346801604</v>
       </c>
-      <c r="CT167" s="34">
-        <v>7.126851820686368</v>
-      </c>
-      <c r="CU167" s="8"/>
+      <c r="CT167" s="20">
+        <v>7.4080784946553733</v>
+      </c>
+      <c r="CU167" s="20">
+        <v>8.874669061707289</v>
+      </c>
       <c r="CV167" s="8"/>
       <c r="CW167" s="8"/>
       <c r="CX167" s="8"/>
@@ -28516,22 +28643,24 @@
       <c r="CO168" s="20">
         <v>1.8031482627672057</v>
       </c>
-      <c r="CP168" s="34">
+      <c r="CP168" s="20">
         <v>0.95669145412253398</v>
       </c>
-      <c r="CQ168" s="34">
+      <c r="CQ168" s="20">
         <v>1.3230283710591559</v>
       </c>
-      <c r="CR168" s="34">
+      <c r="CR168" s="20">
         <v>1.2955695741626716</v>
       </c>
-      <c r="CS168" s="34">
+      <c r="CS168" s="20">
         <v>1.7811321999648935</v>
       </c>
-      <c r="CT168" s="34">
-        <v>0.88713461409041916</v>
-      </c>
-      <c r="CU168" s="8"/>
+      <c r="CT168" s="20">
+        <v>0.92574664442207877</v>
+      </c>
+      <c r="CU168" s="20">
+        <v>1.5527596054988155</v>
+      </c>
       <c r="CV168" s="8"/>
       <c r="CW168" s="8"/>
       <c r="CX168" s="8"/>
@@ -28678,11 +28807,11 @@
       <c r="CM169" s="8"/>
       <c r="CN169" s="8"/>
       <c r="CO169" s="8"/>
-      <c r="CP169" s="26"/>
-      <c r="CQ169" s="26"/>
-      <c r="CR169" s="26"/>
-      <c r="CS169" s="26"/>
-      <c r="CT169" s="26"/>
+      <c r="CP169" s="8"/>
+      <c r="CQ169" s="8"/>
+      <c r="CR169" s="8"/>
+      <c r="CS169" s="8"/>
+      <c r="CT169" s="8"/>
       <c r="CU169" s="8"/>
       <c r="CV169" s="8"/>
       <c r="CW169" s="8"/>
@@ -29017,22 +29146,24 @@
       <c r="CO170" s="14">
         <v>100</v>
       </c>
-      <c r="CP170" s="31">
+      <c r="CP170" s="14">
         <v>100</v>
       </c>
-      <c r="CQ170" s="31">
+      <c r="CQ170" s="14">
         <v>100</v>
       </c>
-      <c r="CR170" s="31">
+      <c r="CR170" s="14">
         <v>100</v>
       </c>
-      <c r="CS170" s="31">
+      <c r="CS170" s="14">
         <v>100</v>
       </c>
-      <c r="CT170" s="31">
+      <c r="CT170" s="14">
         <v>100</v>
       </c>
-      <c r="CU170" s="8"/>
+      <c r="CU170" s="14">
+        <v>100</v>
+      </c>
       <c r="CV170" s="8"/>
       <c r="CW170" s="8"/>
       <c r="CX170" s="8"/>
@@ -29180,11 +29311,12 @@
       <c r="CM171" s="11"/>
       <c r="CN171" s="11"/>
       <c r="CO171" s="11"/>
-      <c r="CP171" s="28"/>
-      <c r="CQ171" s="28"/>
-      <c r="CR171" s="28"/>
-      <c r="CS171" s="28"/>
-      <c r="CT171" s="28"/>
+      <c r="CP171" s="11"/>
+      <c r="CQ171" s="11"/>
+      <c r="CR171" s="11"/>
+      <c r="CS171" s="11"/>
+      <c r="CT171" s="11"/>
+      <c r="CU171" s="11"/>
     </row>
     <row r="172" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A172" s="12" t="s">
@@ -29285,12 +29417,12 @@
       <c r="CM173" s="1"/>
       <c r="CN173" s="1"/>
       <c r="CO173" s="1"/>
-      <c r="CP173" s="23"/>
-      <c r="CQ173" s="23"/>
-      <c r="CR173" s="23"/>
-      <c r="CS173" s="23"/>
-      <c r="CT173" s="23"/>
-      <c r="CU173" s="16"/>
+      <c r="CP173" s="1"/>
+      <c r="CQ173" s="1"/>
+      <c r="CR173" s="1"/>
+      <c r="CS173" s="1"/>
+      <c r="CT173" s="1"/>
+      <c r="CU173" s="1"/>
       <c r="CV173" s="16"/>
       <c r="CW173" s="16"/>
       <c r="CX173" s="16"/>
@@ -29438,12 +29570,12 @@
       <c r="CM174" s="1"/>
       <c r="CN174" s="1"/>
       <c r="CO174" s="1"/>
-      <c r="CP174" s="23"/>
-      <c r="CQ174" s="23"/>
-      <c r="CR174" s="23"/>
-      <c r="CS174" s="23"/>
-      <c r="CT174" s="23"/>
-      <c r="CU174" s="16"/>
+      <c r="CP174" s="1"/>
+      <c r="CQ174" s="1"/>
+      <c r="CR174" s="1"/>
+      <c r="CS174" s="1"/>
+      <c r="CT174" s="1"/>
+      <c r="CU174" s="1"/>
       <c r="CV174" s="16"/>
       <c r="CW174" s="16"/>
       <c r="CX174" s="16"/>
@@ -29499,24 +29631,111 @@
     </row>
   </sheetData>
   <mergeCells count="147">
-    <mergeCell ref="CD158:CG158"/>
-    <mergeCell ref="CD133:CG133"/>
-    <mergeCell ref="CD108:CG108"/>
-    <mergeCell ref="BN9:BQ9"/>
-    <mergeCell ref="BZ59:CC59"/>
-    <mergeCell ref="BZ84:CC84"/>
-    <mergeCell ref="CD9:CG9"/>
-    <mergeCell ref="BV9:BY9"/>
-    <mergeCell ref="BZ9:CC9"/>
-    <mergeCell ref="BR9:BU9"/>
-    <mergeCell ref="CD59:CG59"/>
-    <mergeCell ref="CD84:CG84"/>
-    <mergeCell ref="CD34:CG34"/>
-    <mergeCell ref="BZ34:CC34"/>
-    <mergeCell ref="BR59:BU59"/>
-    <mergeCell ref="BR34:BU34"/>
-    <mergeCell ref="BV34:BY34"/>
-    <mergeCell ref="BV59:BY59"/>
+    <mergeCell ref="BJ34:BM34"/>
+    <mergeCell ref="BN34:BQ34"/>
+    <mergeCell ref="BF59:BI59"/>
+    <mergeCell ref="BJ59:BM59"/>
+    <mergeCell ref="BB59:BE59"/>
+    <mergeCell ref="BN59:BQ59"/>
+    <mergeCell ref="BZ108:CC108"/>
+    <mergeCell ref="BB158:BE158"/>
+    <mergeCell ref="BF158:BI158"/>
+    <mergeCell ref="BJ158:BM158"/>
+    <mergeCell ref="BN158:BQ158"/>
+    <mergeCell ref="BF133:BI133"/>
+    <mergeCell ref="BJ133:BM133"/>
+    <mergeCell ref="BN133:BQ133"/>
+    <mergeCell ref="BN84:BQ84"/>
+    <mergeCell ref="BB108:BE108"/>
+    <mergeCell ref="BF108:BI108"/>
+    <mergeCell ref="BB133:BE133"/>
+    <mergeCell ref="BR108:BU108"/>
+    <mergeCell ref="BV108:BY108"/>
+    <mergeCell ref="V158:Y158"/>
+    <mergeCell ref="Z158:AC158"/>
+    <mergeCell ref="AD158:AG158"/>
+    <mergeCell ref="AH158:AK158"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="F133:I133"/>
+    <mergeCell ref="J133:M133"/>
+    <mergeCell ref="N133:Q133"/>
+    <mergeCell ref="R133:U133"/>
+    <mergeCell ref="V133:Y133"/>
+    <mergeCell ref="Z133:AC133"/>
+    <mergeCell ref="AD133:AG133"/>
+    <mergeCell ref="AH133:AK133"/>
+    <mergeCell ref="B158:E158"/>
+    <mergeCell ref="F158:I158"/>
+    <mergeCell ref="J158:M158"/>
+    <mergeCell ref="N158:Q158"/>
+    <mergeCell ref="R158:U158"/>
+    <mergeCell ref="AT108:AW108"/>
+    <mergeCell ref="AX108:BA108"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="R34:U34"/>
+    <mergeCell ref="AD59:AG59"/>
+    <mergeCell ref="AH59:AK59"/>
+    <mergeCell ref="AL59:AO59"/>
+    <mergeCell ref="AP59:AS59"/>
+    <mergeCell ref="AT59:AW59"/>
+    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="AT84:AW84"/>
+    <mergeCell ref="B108:E108"/>
+    <mergeCell ref="F108:I108"/>
+    <mergeCell ref="J108:M108"/>
+    <mergeCell ref="N108:Q108"/>
+    <mergeCell ref="R108:U108"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="BB34:BE34"/>
+    <mergeCell ref="BF34:BI34"/>
+    <mergeCell ref="V34:Y34"/>
+    <mergeCell ref="Z34:AC34"/>
+    <mergeCell ref="AD34:AG34"/>
+    <mergeCell ref="AH34:AK34"/>
+    <mergeCell ref="AL34:AO34"/>
+    <mergeCell ref="AP34:AS34"/>
+    <mergeCell ref="AT34:AW34"/>
+    <mergeCell ref="AX34:BA34"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="AD9:AG9"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="AX9:BA9"/>
+    <mergeCell ref="BB9:BE9"/>
+    <mergeCell ref="BF9:BI9"/>
+    <mergeCell ref="BJ9:BM9"/>
+    <mergeCell ref="AX84:BA84"/>
+    <mergeCell ref="BB84:BE84"/>
+    <mergeCell ref="BF84:BI84"/>
+    <mergeCell ref="BJ84:BM84"/>
+    <mergeCell ref="Z84:AC84"/>
+    <mergeCell ref="AD84:AG84"/>
+    <mergeCell ref="BZ158:CC158"/>
+    <mergeCell ref="BR158:BU158"/>
+    <mergeCell ref="BV158:BY158"/>
+    <mergeCell ref="BR84:BU84"/>
+    <mergeCell ref="BV84:BY84"/>
+    <mergeCell ref="AH84:AK84"/>
+    <mergeCell ref="AL84:AO84"/>
+    <mergeCell ref="AP84:AS84"/>
+    <mergeCell ref="AL158:AO158"/>
+    <mergeCell ref="AP158:AS158"/>
+    <mergeCell ref="AT158:AW158"/>
+    <mergeCell ref="AX158:BA158"/>
+    <mergeCell ref="BJ108:BM108"/>
+    <mergeCell ref="BN108:BQ108"/>
+    <mergeCell ref="AL133:AO133"/>
+    <mergeCell ref="AP133:AS133"/>
     <mergeCell ref="AT133:AW133"/>
     <mergeCell ref="AX133:BA133"/>
     <mergeCell ref="B84:E84"/>
@@ -29541,111 +29760,24 @@
     <mergeCell ref="AH108:AK108"/>
     <mergeCell ref="AL108:AO108"/>
     <mergeCell ref="AP108:AS108"/>
-    <mergeCell ref="BF9:BI9"/>
-    <mergeCell ref="BJ9:BM9"/>
-    <mergeCell ref="AX84:BA84"/>
-    <mergeCell ref="BB84:BE84"/>
-    <mergeCell ref="BF84:BI84"/>
-    <mergeCell ref="BJ84:BM84"/>
-    <mergeCell ref="Z84:AC84"/>
-    <mergeCell ref="AD84:AG84"/>
-    <mergeCell ref="BZ158:CC158"/>
-    <mergeCell ref="BR158:BU158"/>
-    <mergeCell ref="BV158:BY158"/>
-    <mergeCell ref="BR84:BU84"/>
-    <mergeCell ref="BV84:BY84"/>
-    <mergeCell ref="AH84:AK84"/>
-    <mergeCell ref="AL84:AO84"/>
-    <mergeCell ref="AP84:AS84"/>
-    <mergeCell ref="AL158:AO158"/>
-    <mergeCell ref="AP158:AS158"/>
-    <mergeCell ref="AT158:AW158"/>
-    <mergeCell ref="AX158:BA158"/>
-    <mergeCell ref="BJ108:BM108"/>
-    <mergeCell ref="BN108:BQ108"/>
-    <mergeCell ref="AL133:AO133"/>
-    <mergeCell ref="AP133:AS133"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="BB34:BE34"/>
-    <mergeCell ref="BF34:BI34"/>
-    <mergeCell ref="V34:Y34"/>
-    <mergeCell ref="Z34:AC34"/>
-    <mergeCell ref="AD34:AG34"/>
-    <mergeCell ref="AH34:AK34"/>
-    <mergeCell ref="AL34:AO34"/>
-    <mergeCell ref="AP34:AS34"/>
-    <mergeCell ref="AT34:AW34"/>
-    <mergeCell ref="AX34:BA34"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="AD9:AG9"/>
-    <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="AP9:AS9"/>
-    <mergeCell ref="AT9:AW9"/>
-    <mergeCell ref="AX9:BA9"/>
-    <mergeCell ref="BB9:BE9"/>
-    <mergeCell ref="AT108:AW108"/>
-    <mergeCell ref="AX108:BA108"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="R34:U34"/>
-    <mergeCell ref="AD59:AG59"/>
-    <mergeCell ref="AH59:AK59"/>
-    <mergeCell ref="AL59:AO59"/>
-    <mergeCell ref="AP59:AS59"/>
-    <mergeCell ref="AT59:AW59"/>
-    <mergeCell ref="AX59:BA59"/>
-    <mergeCell ref="AT84:AW84"/>
-    <mergeCell ref="B108:E108"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="J108:M108"/>
-    <mergeCell ref="N108:Q108"/>
-    <mergeCell ref="R108:U108"/>
-    <mergeCell ref="V158:Y158"/>
-    <mergeCell ref="Z158:AC158"/>
-    <mergeCell ref="AD158:AG158"/>
-    <mergeCell ref="AH158:AK158"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="F133:I133"/>
-    <mergeCell ref="J133:M133"/>
-    <mergeCell ref="N133:Q133"/>
-    <mergeCell ref="R133:U133"/>
-    <mergeCell ref="V133:Y133"/>
-    <mergeCell ref="Z133:AC133"/>
-    <mergeCell ref="AD133:AG133"/>
-    <mergeCell ref="AH133:AK133"/>
-    <mergeCell ref="B158:E158"/>
-    <mergeCell ref="F158:I158"/>
-    <mergeCell ref="J158:M158"/>
-    <mergeCell ref="N158:Q158"/>
-    <mergeCell ref="R158:U158"/>
-    <mergeCell ref="BJ34:BM34"/>
-    <mergeCell ref="BN34:BQ34"/>
-    <mergeCell ref="BF59:BI59"/>
-    <mergeCell ref="BJ59:BM59"/>
-    <mergeCell ref="BB59:BE59"/>
-    <mergeCell ref="BN59:BQ59"/>
-    <mergeCell ref="BZ108:CC108"/>
-    <mergeCell ref="BB158:BE158"/>
-    <mergeCell ref="BF158:BI158"/>
-    <mergeCell ref="BJ158:BM158"/>
-    <mergeCell ref="BN158:BQ158"/>
-    <mergeCell ref="BF133:BI133"/>
-    <mergeCell ref="BJ133:BM133"/>
-    <mergeCell ref="BN133:BQ133"/>
-    <mergeCell ref="BN84:BQ84"/>
-    <mergeCell ref="BB108:BE108"/>
-    <mergeCell ref="BF108:BI108"/>
-    <mergeCell ref="BB133:BE133"/>
-    <mergeCell ref="BR108:BU108"/>
-    <mergeCell ref="BV108:BY108"/>
+    <mergeCell ref="CD158:CG158"/>
+    <mergeCell ref="CD133:CG133"/>
+    <mergeCell ref="CD108:CG108"/>
+    <mergeCell ref="BN9:BQ9"/>
+    <mergeCell ref="BZ59:CC59"/>
+    <mergeCell ref="BZ84:CC84"/>
+    <mergeCell ref="CD9:CG9"/>
+    <mergeCell ref="BV9:BY9"/>
+    <mergeCell ref="BZ9:CC9"/>
+    <mergeCell ref="BR9:BU9"/>
+    <mergeCell ref="CD59:CG59"/>
+    <mergeCell ref="CD84:CG84"/>
+    <mergeCell ref="CD34:CG34"/>
+    <mergeCell ref="BZ34:CC34"/>
+    <mergeCell ref="BR59:BU59"/>
+    <mergeCell ref="BR34:BU34"/>
+    <mergeCell ref="BV34:BY34"/>
+    <mergeCell ref="BV59:BY59"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Q3 2024 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-05EOS_2018PSNA_Qrt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2024\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of November 2024\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CC2A88-56D7-439B-8BAE-7B3458D5F98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81861303-C04D-43AB-80BC-0D62B4EB43FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="975" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="975" windowWidth="12660" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EOS" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt" localSheetId="0">EOS!$A$37:$A$48</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EOS!$A$1:$CT$174</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EOS!$A$1:$CV$174</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="58">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -222,13 +222,13 @@
     <t>2023 - 2024</t>
   </si>
   <si>
-    <t>As of August 2024</t>
+    <t>As of November 2024</t>
   </si>
   <si>
-    <t>Q1 2000 to Q2 2024</t>
+    <t>Q1 2000 to Q3 2024</t>
   </si>
   <si>
-    <t>Q1 2001 to Q2 2024</t>
+    <t>Q1 2001 to Q3 2024</t>
   </si>
 </sst>
 </file>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -354,15 +354,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -707,19 +723,20 @@
   <dimension ref="A1:EU174"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="70" zoomScaleNormal="95" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CA3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CN3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="topRight" activeCell="P1" sqref="P1:AF1048576"/>
       <selection pane="bottomLeft" activeCell="P1" sqref="P1:AF1048576"/>
-      <selection pane="bottomRight" activeCell="CP1" sqref="CP1:CU1048576"/>
+      <selection pane="bottomRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.77734375" style="1" customWidth="1"/>
     <col min="2" max="73" width="8.77734375" style="1" customWidth="1"/>
-    <col min="74" max="99" width="10" style="1" customWidth="1"/>
-    <col min="100" max="16384" width="7.77734375" style="1"/>
+    <col min="74" max="93" width="10" style="1" customWidth="1"/>
+    <col min="94" max="100" width="10" style="23" customWidth="1"/>
+    <col min="101" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:151" x14ac:dyDescent="0.2">
@@ -754,132 +771,132 @@
     </row>
     <row r="9" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="25">
+      <c r="B9" s="35">
         <v>2000</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25">
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35">
         <v>2001</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25">
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35">
         <v>2002</v>
       </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25">
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35">
         <v>2003</v>
       </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25">
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35">
         <v>2004</v>
       </c>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25">
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35">
         <v>2005</v>
       </c>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25">
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35">
         <v>2006</v>
       </c>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="25"/>
-      <c r="AC9" s="25"/>
-      <c r="AD9" s="25">
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="35"/>
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35">
         <v>2007</v>
       </c>
-      <c r="AE9" s="25"/>
-      <c r="AF9" s="25"/>
-      <c r="AG9" s="25"/>
-      <c r="AH9" s="25">
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="35">
         <v>2008</v>
       </c>
-      <c r="AI9" s="25"/>
-      <c r="AJ9" s="25"/>
-      <c r="AK9" s="25"/>
-      <c r="AL9" s="25">
+      <c r="AI9" s="35"/>
+      <c r="AJ9" s="35"/>
+      <c r="AK9" s="35"/>
+      <c r="AL9" s="35">
         <v>2009</v>
       </c>
-      <c r="AM9" s="25"/>
-      <c r="AN9" s="25"/>
-      <c r="AO9" s="25"/>
-      <c r="AP9" s="25">
+      <c r="AM9" s="35"/>
+      <c r="AN9" s="35"/>
+      <c r="AO9" s="35"/>
+      <c r="AP9" s="35">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="25"/>
-      <c r="AR9" s="25"/>
-      <c r="AS9" s="25"/>
-      <c r="AT9" s="25">
+      <c r="AQ9" s="35"/>
+      <c r="AR9" s="35"/>
+      <c r="AS9" s="35"/>
+      <c r="AT9" s="35">
         <v>2011</v>
       </c>
-      <c r="AU9" s="25"/>
-      <c r="AV9" s="25"/>
-      <c r="AW9" s="25"/>
-      <c r="AX9" s="25">
+      <c r="AU9" s="35"/>
+      <c r="AV9" s="35"/>
+      <c r="AW9" s="35"/>
+      <c r="AX9" s="35">
         <v>2012</v>
       </c>
-      <c r="AY9" s="25"/>
-      <c r="AZ9" s="25"/>
-      <c r="BA9" s="25"/>
-      <c r="BB9" s="25">
+      <c r="AY9" s="35"/>
+      <c r="AZ9" s="35"/>
+      <c r="BA9" s="35"/>
+      <c r="BB9" s="35">
         <v>2013</v>
       </c>
-      <c r="BC9" s="25"/>
-      <c r="BD9" s="25"/>
-      <c r="BE9" s="25"/>
-      <c r="BF9" s="25">
+      <c r="BC9" s="35"/>
+      <c r="BD9" s="35"/>
+      <c r="BE9" s="35"/>
+      <c r="BF9" s="35">
         <v>2014</v>
       </c>
-      <c r="BG9" s="25"/>
-      <c r="BH9" s="25"/>
-      <c r="BI9" s="25"/>
-      <c r="BJ9" s="25">
+      <c r="BG9" s="35"/>
+      <c r="BH9" s="35"/>
+      <c r="BI9" s="35"/>
+      <c r="BJ9" s="35">
         <v>2015</v>
       </c>
-      <c r="BK9" s="25"/>
-      <c r="BL9" s="25"/>
-      <c r="BM9" s="25"/>
-      <c r="BN9" s="25">
+      <c r="BK9" s="35"/>
+      <c r="BL9" s="35"/>
+      <c r="BM9" s="35"/>
+      <c r="BN9" s="35">
         <v>2016</v>
       </c>
-      <c r="BO9" s="25"/>
-      <c r="BP9" s="25"/>
-      <c r="BQ9" s="25"/>
-      <c r="BR9" s="25">
+      <c r="BO9" s="35"/>
+      <c r="BP9" s="35"/>
+      <c r="BQ9" s="35"/>
+      <c r="BR9" s="35">
         <v>2017</v>
       </c>
-      <c r="BS9" s="25"/>
-      <c r="BT9" s="25"/>
-      <c r="BU9" s="25"/>
-      <c r="BV9" s="25">
+      <c r="BS9" s="35"/>
+      <c r="BT9" s="35"/>
+      <c r="BU9" s="35"/>
+      <c r="BV9" s="35">
         <v>2018</v>
       </c>
-      <c r="BW9" s="25"/>
-      <c r="BX9" s="25"/>
-      <c r="BY9" s="25"/>
-      <c r="BZ9" s="25">
+      <c r="BW9" s="35"/>
+      <c r="BX9" s="35"/>
+      <c r="BY9" s="35"/>
+      <c r="BZ9" s="35">
         <v>2019</v>
       </c>
-      <c r="CA9" s="25"/>
-      <c r="CB9" s="25"/>
-      <c r="CC9" s="25"/>
-      <c r="CD9" s="25">
+      <c r="CA9" s="35"/>
+      <c r="CB9" s="35"/>
+      <c r="CC9" s="35"/>
+      <c r="CD9" s="35">
         <v>2020</v>
       </c>
-      <c r="CE9" s="25"/>
-      <c r="CF9" s="25"/>
-      <c r="CG9" s="25"/>
+      <c r="CE9" s="35"/>
+      <c r="CF9" s="35"/>
+      <c r="CG9" s="35"/>
       <c r="CH9" s="21">
         <v>2021</v>
       </c>
@@ -892,16 +909,17 @@
       <c r="CM9" s="21"/>
       <c r="CN9" s="21"/>
       <c r="CO9" s="21"/>
-      <c r="CP9" s="21">
+      <c r="CP9" s="24">
         <v>2023</v>
       </c>
-      <c r="CQ9" s="21"/>
-      <c r="CR9" s="21"/>
-      <c r="CS9" s="21"/>
-      <c r="CT9" s="21">
+      <c r="CQ9" s="24"/>
+      <c r="CR9" s="24"/>
+      <c r="CS9" s="24"/>
+      <c r="CT9" s="24">
         <v>2024</v>
       </c>
-      <c r="CU9" s="21"/>
+      <c r="CU9" s="24"/>
+      <c r="CV9" s="24"/>
     </row>
     <row r="10" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -1181,23 +1199,26 @@
       <c r="CO10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CP10" s="5" t="s">
+      <c r="CP10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ10" s="5" t="s">
+      <c r="CQ10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CR10" s="5" t="s">
+      <c r="CR10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="CS10" s="5" t="s">
+      <c r="CS10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CT10" s="5" t="s">
+      <c r="CT10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CU10" s="5" t="s">
+      <c r="CU10" s="13" t="s">
         <v>8</v>
+      </c>
+      <c r="CV10" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1483,25 +1504,27 @@
       <c r="CO12" s="18">
         <v>54545.476736266144</v>
       </c>
-      <c r="CP12" s="18">
+      <c r="CP12" s="25">
         <v>91388.504694742951</v>
       </c>
-      <c r="CQ12" s="18">
+      <c r="CQ12" s="25">
         <v>34472.852940256031</v>
       </c>
-      <c r="CR12" s="18">
+      <c r="CR12" s="25">
         <v>51853.834593934924</v>
       </c>
-      <c r="CS12" s="18">
+      <c r="CS12" s="25">
         <v>61415.796931664518</v>
       </c>
-      <c r="CT12" s="18">
+      <c r="CT12" s="25">
         <v>102696.07234617718</v>
       </c>
-      <c r="CU12" s="18">
-        <v>38145.561898129105</v>
-      </c>
-      <c r="CV12" s="8"/>
+      <c r="CU12" s="25">
+        <v>38250.076815867869</v>
+      </c>
+      <c r="CV12" s="25">
+        <v>50573.182042746033</v>
+      </c>
       <c r="CW12" s="8"/>
       <c r="CX12" s="8"/>
       <c r="CY12" s="8"/>
@@ -1834,25 +1857,27 @@
       <c r="CO13" s="18">
         <v>1000.4370497140442</v>
       </c>
-      <c r="CP13" s="18">
+      <c r="CP13" s="25">
         <v>480.04158316722192</v>
       </c>
-      <c r="CQ13" s="18">
+      <c r="CQ13" s="25">
         <v>464.05012427240712</v>
       </c>
-      <c r="CR13" s="18">
+      <c r="CR13" s="25">
         <v>930.61252590324239</v>
       </c>
-      <c r="CS13" s="18">
+      <c r="CS13" s="25">
         <v>942.90067939335495</v>
       </c>
-      <c r="CT13" s="18">
+      <c r="CT13" s="25">
         <v>534.38963333813354</v>
       </c>
-      <c r="CU13" s="18">
-        <v>519.70697381865602</v>
-      </c>
-      <c r="CV13" s="8"/>
+      <c r="CU13" s="25">
+        <v>490.03761118240203</v>
+      </c>
+      <c r="CV13" s="25">
+        <v>1007.5205428879642</v>
+      </c>
       <c r="CW13" s="8"/>
       <c r="CX13" s="8"/>
       <c r="CY13" s="8"/>
@@ -2185,25 +2210,27 @@
       <c r="CO14" s="18">
         <v>64203.136054041541</v>
       </c>
-      <c r="CP14" s="18">
+      <c r="CP14" s="25">
         <v>128049.61270907105</v>
       </c>
-      <c r="CQ14" s="18">
+      <c r="CQ14" s="25">
         <v>132330.33872905793</v>
       </c>
-      <c r="CR14" s="18">
+      <c r="CR14" s="25">
         <v>174583.24150521151</v>
       </c>
-      <c r="CS14" s="18">
+      <c r="CS14" s="25">
         <v>107496.30220590543</v>
       </c>
-      <c r="CT14" s="18">
+      <c r="CT14" s="25">
         <v>151426.10425368711</v>
       </c>
-      <c r="CU14" s="18">
+      <c r="CU14" s="25">
         <v>167362.97894372992</v>
       </c>
-      <c r="CV14" s="8"/>
+      <c r="CV14" s="25">
+        <v>149127.23704708871</v>
+      </c>
       <c r="CW14" s="8"/>
       <c r="CX14" s="8"/>
       <c r="CY14" s="8"/>
@@ -2536,25 +2563,27 @@
       <c r="CO15" s="18">
         <v>4595.0686874499042</v>
       </c>
-      <c r="CP15" s="18">
+      <c r="CP15" s="25">
         <v>4570.1940500558103</v>
       </c>
-      <c r="CQ15" s="18">
+      <c r="CQ15" s="25">
         <v>5139.0553496337761</v>
       </c>
-      <c r="CR15" s="18">
+      <c r="CR15" s="25">
         <v>5303.5480278897912</v>
       </c>
-      <c r="CS15" s="18">
+      <c r="CS15" s="25">
         <v>5496.1059442223577</v>
       </c>
-      <c r="CT15" s="18">
+      <c r="CT15" s="25">
         <v>4977.9404636384443</v>
       </c>
-      <c r="CU15" s="18">
-        <v>5391.142877497583</v>
-      </c>
-      <c r="CV15" s="8"/>
+      <c r="CU15" s="25">
+        <v>5418.3606287574867</v>
+      </c>
+      <c r="CV15" s="25">
+        <v>5553.9493145297602</v>
+      </c>
       <c r="CW15" s="8"/>
       <c r="CX15" s="8"/>
       <c r="CY15" s="8"/>
@@ -2887,25 +2916,27 @@
       <c r="CO16" s="18">
         <v>88349.252531254111</v>
       </c>
-      <c r="CP16" s="18">
+      <c r="CP16" s="25">
         <v>136255.87042386705</v>
       </c>
-      <c r="CQ16" s="18">
+      <c r="CQ16" s="25">
         <v>132006.04495852461</v>
       </c>
-      <c r="CR16" s="18">
+      <c r="CR16" s="25">
         <v>90834.805619856139</v>
       </c>
-      <c r="CS16" s="18">
+      <c r="CS16" s="25">
         <v>100998.99676650774</v>
       </c>
-      <c r="CT16" s="18">
+      <c r="CT16" s="25">
         <v>144427.11597770988</v>
       </c>
-      <c r="CU16" s="18">
-        <v>142487.33049555379</v>
-      </c>
-      <c r="CV16" s="8"/>
+      <c r="CU16" s="25">
+        <v>142031.78516345526</v>
+      </c>
+      <c r="CV16" s="25">
+        <v>101431.26716389808</v>
+      </c>
       <c r="CW16" s="8"/>
       <c r="CX16" s="8"/>
       <c r="CY16" s="8"/>
@@ -3238,25 +3269,27 @@
       <c r="CO17" s="18">
         <v>330617.25478872925</v>
       </c>
-      <c r="CP17" s="18">
+      <c r="CP17" s="25">
         <v>438940.2579160161</v>
       </c>
-      <c r="CQ17" s="18">
+      <c r="CQ17" s="25">
         <v>442320.61266757833</v>
       </c>
-      <c r="CR17" s="18">
+      <c r="CR17" s="25">
         <v>334923.1459927574</v>
       </c>
-      <c r="CS17" s="18">
+      <c r="CS17" s="25">
         <v>354637.50058273773</v>
       </c>
-      <c r="CT17" s="18">
+      <c r="CT17" s="25">
         <v>489463.82320816326</v>
       </c>
-      <c r="CU17" s="18">
-        <v>472218.42256727559</v>
-      </c>
-      <c r="CV17" s="8"/>
+      <c r="CU17" s="25">
+        <v>469821.55779187358</v>
+      </c>
+      <c r="CV17" s="25">
+        <v>378125.3313893525</v>
+      </c>
       <c r="CW17" s="8"/>
       <c r="CX17" s="8"/>
       <c r="CY17" s="8"/>
@@ -3589,25 +3622,27 @@
       <c r="CO18" s="18">
         <v>66718.593327664843</v>
       </c>
-      <c r="CP18" s="18">
+      <c r="CP18" s="25">
         <v>68561.433407578908</v>
       </c>
-      <c r="CQ18" s="18">
+      <c r="CQ18" s="25">
         <v>79162.752002960682</v>
       </c>
-      <c r="CR18" s="18">
+      <c r="CR18" s="25">
         <v>65974.839012592245</v>
       </c>
-      <c r="CS18" s="18">
+      <c r="CS18" s="25">
         <v>72001.17877859922</v>
       </c>
-      <c r="CT18" s="18">
+      <c r="CT18" s="25">
         <v>74272.253945248944</v>
       </c>
-      <c r="CU18" s="18">
-        <v>83334.967220423583</v>
-      </c>
-      <c r="CV18" s="8"/>
+      <c r="CU18" s="25">
+        <v>85948.802711667129</v>
+      </c>
+      <c r="CV18" s="25">
+        <v>70845.972496813789</v>
+      </c>
       <c r="CW18" s="8"/>
       <c r="CX18" s="8"/>
       <c r="CY18" s="8"/>
@@ -3940,25 +3975,27 @@
       <c r="CO19" s="18">
         <v>11024.543795387575</v>
       </c>
-      <c r="CP19" s="18">
+      <c r="CP19" s="25">
         <v>8484.317640903666</v>
       </c>
-      <c r="CQ19" s="18">
+      <c r="CQ19" s="25">
         <v>11183.54873158895</v>
       </c>
-      <c r="CR19" s="18">
+      <c r="CR19" s="25">
         <v>9272.9031053682593</v>
       </c>
-      <c r="CS19" s="18">
+      <c r="CS19" s="25">
         <v>12603.042609203625</v>
       </c>
-      <c r="CT19" s="18">
+      <c r="CT19" s="25">
         <v>9152.9725122828659</v>
       </c>
-      <c r="CU19" s="18">
-        <v>14514.532929209307</v>
-      </c>
-      <c r="CV19" s="8"/>
+      <c r="CU19" s="25">
+        <v>15843.539534704643</v>
+      </c>
+      <c r="CV19" s="25">
+        <v>10065.050719549774</v>
+      </c>
       <c r="CW19" s="8"/>
       <c r="CX19" s="8"/>
       <c r="CY19" s="8"/>
@@ -4104,13 +4141,13 @@
       <c r="CM20" s="8"/>
       <c r="CN20" s="8"/>
       <c r="CO20" s="8"/>
-      <c r="CP20" s="8"/>
-      <c r="CQ20" s="8"/>
-      <c r="CR20" s="8"/>
-      <c r="CS20" s="8"/>
-      <c r="CT20" s="8"/>
-      <c r="CU20" s="8"/>
-      <c r="CV20" s="8"/>
+      <c r="CP20" s="26"/>
+      <c r="CQ20" s="26"/>
+      <c r="CR20" s="26"/>
+      <c r="CS20" s="26"/>
+      <c r="CT20" s="26"/>
+      <c r="CU20" s="26"/>
+      <c r="CV20" s="26"/>
       <c r="CW20" s="8"/>
       <c r="CX20" s="8"/>
       <c r="CY20" s="8"/>
@@ -4443,25 +4480,27 @@
       <c r="CO21" s="19">
         <v>621053.76297050749</v>
       </c>
-      <c r="CP21" s="19">
+      <c r="CP21" s="27">
         <v>876730.23242540262</v>
       </c>
-      <c r="CQ21" s="19">
+      <c r="CQ21" s="27">
         <v>837079.25550387276</v>
       </c>
-      <c r="CR21" s="19">
+      <c r="CR21" s="27">
         <v>733676.93038351345</v>
       </c>
-      <c r="CS21" s="19">
+      <c r="CS21" s="27">
         <v>715591.82449823397</v>
       </c>
-      <c r="CT21" s="19">
+      <c r="CT21" s="27">
         <v>976950.6723402458</v>
       </c>
-      <c r="CU21" s="19">
-        <v>923974.64390563755</v>
-      </c>
-      <c r="CV21" s="8"/>
+      <c r="CU21" s="27">
+        <v>925167.13920123829</v>
+      </c>
+      <c r="CV21" s="27">
+        <v>766729.51071686659</v>
+      </c>
       <c r="CW21" s="8"/>
       <c r="CX21" s="8"/>
       <c r="CY21" s="8"/>
@@ -4608,12 +4647,13 @@
       <c r="CM22" s="11"/>
       <c r="CN22" s="11"/>
       <c r="CO22" s="11"/>
-      <c r="CP22" s="11"/>
-      <c r="CQ22" s="11"/>
-      <c r="CR22" s="11"/>
-      <c r="CS22" s="11"/>
-      <c r="CT22" s="11"/>
-      <c r="CU22" s="11"/>
+      <c r="CP22" s="28"/>
+      <c r="CQ22" s="28"/>
+      <c r="CR22" s="28"/>
+      <c r="CS22" s="28"/>
+      <c r="CT22" s="28"/>
+      <c r="CU22" s="28"/>
+      <c r="CV22" s="28"/>
     </row>
     <row r="23" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
@@ -4713,13 +4753,13 @@
       <c r="CM24" s="8"/>
       <c r="CN24" s="8"/>
       <c r="CO24" s="8"/>
-      <c r="CP24" s="8"/>
-      <c r="CQ24" s="8"/>
-      <c r="CR24" s="8"/>
-      <c r="CS24" s="8"/>
-      <c r="CT24" s="8"/>
-      <c r="CU24" s="8"/>
-      <c r="CV24" s="8"/>
+      <c r="CP24" s="26"/>
+      <c r="CQ24" s="26"/>
+      <c r="CR24" s="26"/>
+      <c r="CS24" s="26"/>
+      <c r="CT24" s="26"/>
+      <c r="CU24" s="26"/>
+      <c r="CV24" s="26"/>
       <c r="CW24" s="8"/>
       <c r="CX24" s="8"/>
       <c r="CY24" s="8"/>
@@ -4865,13 +4905,13 @@
       <c r="CM25" s="8"/>
       <c r="CN25" s="8"/>
       <c r="CO25" s="8"/>
-      <c r="CP25" s="8"/>
-      <c r="CQ25" s="8"/>
-      <c r="CR25" s="8"/>
-      <c r="CS25" s="8"/>
-      <c r="CT25" s="8"/>
-      <c r="CU25" s="8"/>
-      <c r="CV25" s="8"/>
+      <c r="CP25" s="26"/>
+      <c r="CQ25" s="26"/>
+      <c r="CR25" s="26"/>
+      <c r="CS25" s="26"/>
+      <c r="CT25" s="26"/>
+      <c r="CU25" s="26"/>
+      <c r="CV25" s="26"/>
       <c r="CW25" s="8"/>
       <c r="CX25" s="8"/>
       <c r="CY25" s="8"/>
@@ -4956,132 +4996,132 @@
     </row>
     <row r="34" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-      <c r="B34" s="26">
+      <c r="B34" s="36">
         <v>2000</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26">
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36">
         <v>2001</v>
       </c>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26">
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36">
         <v>2002</v>
       </c>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26">
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="36">
         <v>2003</v>
       </c>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26">
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36">
         <v>2004</v>
       </c>
-      <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="26">
+      <c r="S34" s="36"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="36"/>
+      <c r="V34" s="36">
         <v>2005</v>
       </c>
-      <c r="W34" s="26"/>
-      <c r="X34" s="26"/>
-      <c r="Y34" s="26"/>
-      <c r="Z34" s="26">
+      <c r="W34" s="36"/>
+      <c r="X34" s="36"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36">
         <v>2006</v>
       </c>
-      <c r="AA34" s="26"/>
-      <c r="AB34" s="26"/>
-      <c r="AC34" s="26"/>
-      <c r="AD34" s="26">
+      <c r="AA34" s="36"/>
+      <c r="AB34" s="36"/>
+      <c r="AC34" s="36"/>
+      <c r="AD34" s="36">
         <v>2007</v>
       </c>
-      <c r="AE34" s="26"/>
-      <c r="AF34" s="26"/>
-      <c r="AG34" s="26"/>
-      <c r="AH34" s="26">
+      <c r="AE34" s="36"/>
+      <c r="AF34" s="36"/>
+      <c r="AG34" s="36"/>
+      <c r="AH34" s="36">
         <v>2008</v>
       </c>
-      <c r="AI34" s="26"/>
-      <c r="AJ34" s="26"/>
-      <c r="AK34" s="26"/>
-      <c r="AL34" s="26">
+      <c r="AI34" s="36"/>
+      <c r="AJ34" s="36"/>
+      <c r="AK34" s="36"/>
+      <c r="AL34" s="36">
         <v>2009</v>
       </c>
-      <c r="AM34" s="26"/>
-      <c r="AN34" s="26"/>
-      <c r="AO34" s="26"/>
-      <c r="AP34" s="26">
+      <c r="AM34" s="36"/>
+      <c r="AN34" s="36"/>
+      <c r="AO34" s="36"/>
+      <c r="AP34" s="36">
         <v>2010</v>
       </c>
-      <c r="AQ34" s="26"/>
-      <c r="AR34" s="26"/>
-      <c r="AS34" s="26"/>
-      <c r="AT34" s="26">
+      <c r="AQ34" s="36"/>
+      <c r="AR34" s="36"/>
+      <c r="AS34" s="36"/>
+      <c r="AT34" s="36">
         <v>2011</v>
       </c>
-      <c r="AU34" s="26"/>
-      <c r="AV34" s="26"/>
-      <c r="AW34" s="26"/>
-      <c r="AX34" s="26">
+      <c r="AU34" s="36"/>
+      <c r="AV34" s="36"/>
+      <c r="AW34" s="36"/>
+      <c r="AX34" s="36">
         <v>2012</v>
       </c>
-      <c r="AY34" s="26"/>
-      <c r="AZ34" s="26"/>
-      <c r="BA34" s="26"/>
-      <c r="BB34" s="26">
+      <c r="AY34" s="36"/>
+      <c r="AZ34" s="36"/>
+      <c r="BA34" s="36"/>
+      <c r="BB34" s="36">
         <v>2013</v>
       </c>
-      <c r="BC34" s="26"/>
-      <c r="BD34" s="26"/>
-      <c r="BE34" s="26"/>
-      <c r="BF34" s="26">
+      <c r="BC34" s="36"/>
+      <c r="BD34" s="36"/>
+      <c r="BE34" s="36"/>
+      <c r="BF34" s="36">
         <v>2014</v>
       </c>
-      <c r="BG34" s="26"/>
-      <c r="BH34" s="26"/>
-      <c r="BI34" s="26"/>
-      <c r="BJ34" s="26">
+      <c r="BG34" s="36"/>
+      <c r="BH34" s="36"/>
+      <c r="BI34" s="36"/>
+      <c r="BJ34" s="36">
         <v>2015</v>
       </c>
-      <c r="BK34" s="26"/>
-      <c r="BL34" s="26"/>
-      <c r="BM34" s="26"/>
-      <c r="BN34" s="26">
+      <c r="BK34" s="36"/>
+      <c r="BL34" s="36"/>
+      <c r="BM34" s="36"/>
+      <c r="BN34" s="36">
         <v>2016</v>
       </c>
-      <c r="BO34" s="26"/>
-      <c r="BP34" s="26"/>
-      <c r="BQ34" s="26"/>
-      <c r="BR34" s="26">
+      <c r="BO34" s="36"/>
+      <c r="BP34" s="36"/>
+      <c r="BQ34" s="36"/>
+      <c r="BR34" s="36">
         <v>2017</v>
       </c>
-      <c r="BS34" s="26"/>
-      <c r="BT34" s="26"/>
-      <c r="BU34" s="26"/>
-      <c r="BV34" s="26">
+      <c r="BS34" s="36"/>
+      <c r="BT34" s="36"/>
+      <c r="BU34" s="36"/>
+      <c r="BV34" s="36">
         <v>2018</v>
       </c>
-      <c r="BW34" s="26"/>
-      <c r="BX34" s="26"/>
-      <c r="BY34" s="26"/>
-      <c r="BZ34" s="26">
+      <c r="BW34" s="36"/>
+      <c r="BX34" s="36"/>
+      <c r="BY34" s="36"/>
+      <c r="BZ34" s="36">
         <v>2019</v>
       </c>
-      <c r="CA34" s="26"/>
-      <c r="CB34" s="26"/>
-      <c r="CC34" s="26"/>
-      <c r="CD34" s="25">
+      <c r="CA34" s="36"/>
+      <c r="CB34" s="36"/>
+      <c r="CC34" s="36"/>
+      <c r="CD34" s="35">
         <v>2020</v>
       </c>
-      <c r="CE34" s="25"/>
-      <c r="CF34" s="25"/>
-      <c r="CG34" s="25"/>
+      <c r="CE34" s="35"/>
+      <c r="CF34" s="35"/>
+      <c r="CG34" s="35"/>
       <c r="CH34" s="21">
         <v>2021</v>
       </c>
@@ -5094,16 +5134,17 @@
       <c r="CM34" s="21"/>
       <c r="CN34" s="21"/>
       <c r="CO34" s="21"/>
-      <c r="CP34" s="21">
+      <c r="CP34" s="24">
         <v>2023</v>
       </c>
-      <c r="CQ34" s="21"/>
-      <c r="CR34" s="21"/>
-      <c r="CS34" s="21"/>
-      <c r="CT34" s="21">
+      <c r="CQ34" s="24"/>
+      <c r="CR34" s="24"/>
+      <c r="CS34" s="24"/>
+      <c r="CT34" s="24">
         <v>2024</v>
       </c>
-      <c r="CU34" s="21"/>
+      <c r="CU34" s="24"/>
+      <c r="CV34" s="24"/>
     </row>
     <row r="35" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
@@ -5383,23 +5424,26 @@
       <c r="CO35" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP35" s="13" t="s">
+      <c r="CP35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CQ35" s="13" t="s">
+      <c r="CQ35" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="CR35" s="13" t="s">
+      <c r="CR35" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="CS35" s="13" t="s">
+      <c r="CS35" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="CT35" s="13" t="s">
+      <c r="CT35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CU35" s="13" t="s">
+      <c r="CU35" s="29" t="s">
         <v>8</v>
+      </c>
+      <c r="CV35" s="29" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -5685,25 +5729,27 @@
       <c r="CO37" s="18">
         <v>41001.743914789178</v>
       </c>
-      <c r="CP37" s="18">
+      <c r="CP37" s="25">
         <v>66840.507136195039</v>
       </c>
-      <c r="CQ37" s="18">
+      <c r="CQ37" s="25">
         <v>24335.490726229673</v>
       </c>
-      <c r="CR37" s="18">
+      <c r="CR37" s="25">
         <v>39801.249761229999</v>
       </c>
-      <c r="CS37" s="18">
+      <c r="CS37" s="25">
         <v>45097.200111910657</v>
       </c>
-      <c r="CT37" s="18">
+      <c r="CT37" s="25">
         <v>73763.569378939006</v>
       </c>
-      <c r="CU37" s="18">
-        <v>26958.75242415956</v>
-      </c>
-      <c r="CV37" s="8"/>
+      <c r="CU37" s="25">
+        <v>27032.616634089813</v>
+      </c>
+      <c r="CV37" s="25">
+        <v>38852.41629649551</v>
+      </c>
       <c r="CW37" s="8"/>
       <c r="CX37" s="8"/>
       <c r="CY37" s="8"/>
@@ -6036,25 +6082,27 @@
       <c r="CO38" s="18">
         <v>874.3698128567687</v>
       </c>
-      <c r="CP38" s="18">
+      <c r="CP38" s="25">
         <v>401.40117980165178</v>
       </c>
-      <c r="CQ38" s="18">
+      <c r="CQ38" s="25">
         <v>389.08013271399068</v>
       </c>
-      <c r="CR38" s="18">
+      <c r="CR38" s="25">
         <v>775.39169916792036</v>
       </c>
-      <c r="CS38" s="18">
+      <c r="CS38" s="25">
         <v>800.26199980740012</v>
       </c>
-      <c r="CT38" s="18">
+      <c r="CT38" s="25">
         <v>437.00790956349607</v>
       </c>
-      <c r="CU38" s="18">
-        <v>425.47272384273145</v>
-      </c>
-      <c r="CV38" s="8"/>
+      <c r="CU38" s="25">
+        <v>401.18306607121667</v>
+      </c>
+      <c r="CV38" s="25">
+        <v>816.81503332931379</v>
+      </c>
       <c r="CW38" s="8"/>
       <c r="CX38" s="8"/>
       <c r="CY38" s="8"/>
@@ -6387,25 +6435,27 @@
       <c r="CO39" s="18">
         <v>54857.258251901527</v>
       </c>
-      <c r="CP39" s="18">
+      <c r="CP39" s="25">
         <v>104952.98838100983</v>
       </c>
-      <c r="CQ39" s="18">
+      <c r="CQ39" s="25">
         <v>107908.32982931691</v>
       </c>
-      <c r="CR39" s="18">
+      <c r="CR39" s="25">
         <v>139971.22516500723</v>
       </c>
-      <c r="CS39" s="18">
+      <c r="CS39" s="25">
         <v>88041.043596806237</v>
       </c>
-      <c r="CT39" s="18">
+      <c r="CT39" s="25">
         <v>120172.09772732317</v>
       </c>
-      <c r="CU39" s="18">
+      <c r="CU39" s="25">
         <v>132251.56752630067</v>
       </c>
-      <c r="CV39" s="8"/>
+      <c r="CV39" s="25">
+        <v>118168.11838631412</v>
+      </c>
       <c r="CW39" s="8"/>
       <c r="CX39" s="8"/>
       <c r="CY39" s="8"/>
@@ -6738,25 +6788,27 @@
       <c r="CO40" s="18">
         <v>3977.1461621146914</v>
       </c>
-      <c r="CP40" s="18">
+      <c r="CP40" s="25">
         <v>3948.5227029077732</v>
       </c>
-      <c r="CQ40" s="18">
+      <c r="CQ40" s="25">
         <v>4411.1105877597493</v>
       </c>
-      <c r="CR40" s="18">
+      <c r="CR40" s="25">
         <v>4489.0256045275964</v>
       </c>
-      <c r="CS40" s="18">
+      <c r="CS40" s="25">
         <v>4564.4944289546966</v>
       </c>
-      <c r="CT40" s="18">
+      <c r="CT40" s="25">
         <v>4153.7012475273468</v>
       </c>
-      <c r="CU40" s="18">
-        <v>4540.1651977513411</v>
-      </c>
-      <c r="CV40" s="8"/>
+      <c r="CU40" s="25">
+        <v>4563.0866987835352</v>
+      </c>
+      <c r="CV40" s="25">
+        <v>4590.6186378588518</v>
+      </c>
       <c r="CW40" s="8"/>
       <c r="CX40" s="8"/>
       <c r="CY40" s="8"/>
@@ -7089,25 +7141,27 @@
       <c r="CO41" s="18">
         <v>85486.339096444455</v>
       </c>
-      <c r="CP41" s="18">
+      <c r="CP41" s="25">
         <v>132389.96761888449</v>
       </c>
-      <c r="CQ41" s="18">
+      <c r="CQ41" s="25">
         <v>127397.97452047073</v>
       </c>
-      <c r="CR41" s="18">
+      <c r="CR41" s="25">
         <v>88570.644729925349</v>
       </c>
-      <c r="CS41" s="18">
+      <c r="CS41" s="25">
         <v>97408.840224678061</v>
       </c>
-      <c r="CT41" s="18">
+      <c r="CT41" s="25">
         <v>139628.09619555547</v>
       </c>
-      <c r="CU41" s="18">
-        <v>136933.7534025386</v>
-      </c>
-      <c r="CV41" s="8"/>
+      <c r="CU41" s="25">
+        <v>136495.94832704976</v>
+      </c>
+      <c r="CV41" s="25">
+        <v>98232.123883433189</v>
+      </c>
       <c r="CW41" s="8"/>
       <c r="CX41" s="8"/>
       <c r="CY41" s="8"/>
@@ -7440,25 +7494,27 @@
       <c r="CO42" s="18">
         <v>282568.33591674821</v>
       </c>
-      <c r="CP42" s="18">
+      <c r="CP42" s="25">
         <v>370976.65010641125</v>
       </c>
-      <c r="CQ42" s="18">
+      <c r="CQ42" s="25">
         <v>372232.40369391814</v>
       </c>
-      <c r="CR42" s="18">
+      <c r="CR42" s="25">
         <v>279294.63152185868</v>
       </c>
-      <c r="CS42" s="18">
+      <c r="CS42" s="25">
         <v>294572.86033506453</v>
       </c>
-      <c r="CT42" s="18">
+      <c r="CT42" s="25">
         <v>405436.75997405779</v>
       </c>
-      <c r="CU42" s="18">
-        <v>388024.31549253245</v>
-      </c>
-      <c r="CV42" s="8"/>
+      <c r="CU42" s="25">
+        <v>386054.79933357524</v>
+      </c>
+      <c r="CV42" s="25">
+        <v>306808.35544004542</v>
+      </c>
       <c r="CW42" s="8"/>
       <c r="CX42" s="8"/>
       <c r="CY42" s="8"/>
@@ -7791,25 +7847,27 @@
       <c r="CO43" s="18">
         <v>56641.27780498279</v>
       </c>
-      <c r="CP43" s="18">
+      <c r="CP43" s="25">
         <v>56722.129138118144</v>
       </c>
-      <c r="CQ43" s="18">
+      <c r="CQ43" s="25">
         <v>66425.589510680875</v>
       </c>
-      <c r="CR43" s="18">
+      <c r="CR43" s="25">
         <v>54458.070986274273</v>
       </c>
-      <c r="CS43" s="18">
+      <c r="CS43" s="25">
         <v>60129.24129404522</v>
       </c>
-      <c r="CT43" s="18">
+      <c r="CT43" s="25">
         <v>60093.946607444414</v>
       </c>
-      <c r="CU43" s="18">
-        <v>68278.004479713622</v>
-      </c>
-      <c r="CV43" s="8"/>
+      <c r="CU43" s="25">
+        <v>70419.572147320781</v>
+      </c>
+      <c r="CV43" s="25">
+        <v>56900.572938345198</v>
+      </c>
       <c r="CW43" s="8"/>
       <c r="CX43" s="8"/>
       <c r="CY43" s="8"/>
@@ -8142,25 +8200,27 @@
       <c r="CO44" s="18">
         <v>9647.8221918255676</v>
       </c>
-      <c r="CP44" s="18">
+      <c r="CP44" s="25">
         <v>7111.5053813856466</v>
       </c>
-      <c r="CQ44" s="18">
+      <c r="CQ44" s="25">
         <v>9426.9331998502021</v>
       </c>
-      <c r="CR44" s="18">
+      <c r="CR44" s="25">
         <v>7972.0580263325928</v>
       </c>
-      <c r="CS44" s="18">
+      <c r="CS44" s="25">
         <v>10710.381145611891</v>
       </c>
-      <c r="CT44" s="18">
+      <c r="CT44" s="25">
         <v>7509.6085256193328</v>
       </c>
-      <c r="CU44" s="18">
-        <v>11946.285158690835</v>
-      </c>
-      <c r="CV44" s="8"/>
+      <c r="CU44" s="25">
+        <v>13040.133094719178</v>
+      </c>
+      <c r="CV44" s="25">
+        <v>8419.5378904147547</v>
+      </c>
       <c r="CW44" s="8"/>
       <c r="CX44" s="8"/>
       <c r="CY44" s="8"/>
@@ -8306,13 +8366,13 @@
       <c r="CM45" s="8"/>
       <c r="CN45" s="8"/>
       <c r="CO45" s="8"/>
-      <c r="CP45" s="8"/>
-      <c r="CQ45" s="8"/>
-      <c r="CR45" s="8"/>
-      <c r="CS45" s="8"/>
-      <c r="CT45" s="8"/>
-      <c r="CU45" s="8"/>
-      <c r="CV45" s="8"/>
+      <c r="CP45" s="26"/>
+      <c r="CQ45" s="26"/>
+      <c r="CR45" s="26"/>
+      <c r="CS45" s="26"/>
+      <c r="CT45" s="26"/>
+      <c r="CU45" s="26"/>
+      <c r="CV45" s="26"/>
       <c r="CW45" s="8"/>
       <c r="CX45" s="8"/>
       <c r="CY45" s="8"/>
@@ -8645,25 +8705,27 @@
       <c r="CO46" s="19">
         <v>535054.29315166315</v>
       </c>
-      <c r="CP46" s="19">
+      <c r="CP46" s="27">
         <v>743343.67164471385</v>
       </c>
-      <c r="CQ46" s="19">
+      <c r="CQ46" s="27">
         <v>712526.91220094031</v>
       </c>
-      <c r="CR46" s="19">
+      <c r="CR46" s="27">
         <v>615332.29749432369</v>
       </c>
-      <c r="CS46" s="19">
+      <c r="CS46" s="27">
         <v>601324.32313687867</v>
       </c>
-      <c r="CT46" s="19">
+      <c r="CT46" s="27">
         <v>811194.78756603005</v>
       </c>
-      <c r="CU46" s="19">
-        <v>769358.31640552985</v>
-      </c>
-      <c r="CV46" s="8"/>
+      <c r="CU46" s="27">
+        <v>770258.9068279101</v>
+      </c>
+      <c r="CV46" s="27">
+        <v>632788.55850623618</v>
+      </c>
       <c r="CW46" s="8"/>
       <c r="CX46" s="8"/>
       <c r="CY46" s="8"/>
@@ -8810,12 +8872,13 @@
       <c r="CM47" s="11"/>
       <c r="CN47" s="11"/>
       <c r="CO47" s="11"/>
-      <c r="CP47" s="11"/>
-      <c r="CQ47" s="11"/>
-      <c r="CR47" s="11"/>
-      <c r="CS47" s="11"/>
-      <c r="CT47" s="11"/>
-      <c r="CU47" s="11"/>
+      <c r="CP47" s="28"/>
+      <c r="CQ47" s="28"/>
+      <c r="CR47" s="28"/>
+      <c r="CS47" s="28"/>
+      <c r="CT47" s="28"/>
+      <c r="CU47" s="28"/>
+      <c r="CV47" s="28"/>
     </row>
     <row r="48" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
@@ -8915,13 +8978,13 @@
       <c r="CM49" s="8"/>
       <c r="CN49" s="8"/>
       <c r="CO49" s="8"/>
-      <c r="CP49" s="8"/>
-      <c r="CQ49" s="8"/>
-      <c r="CR49" s="8"/>
-      <c r="CS49" s="8"/>
-      <c r="CT49" s="8"/>
-      <c r="CU49" s="8"/>
-      <c r="CV49" s="8"/>
+      <c r="CP49" s="26"/>
+      <c r="CQ49" s="26"/>
+      <c r="CR49" s="26"/>
+      <c r="CS49" s="26"/>
+      <c r="CT49" s="26"/>
+      <c r="CU49" s="26"/>
+      <c r="CV49" s="26"/>
       <c r="CW49" s="8"/>
       <c r="CX49" s="8"/>
       <c r="CY49" s="8"/>
@@ -9067,13 +9130,13 @@
       <c r="CM50" s="8"/>
       <c r="CN50" s="8"/>
       <c r="CO50" s="8"/>
-      <c r="CP50" s="8"/>
-      <c r="CQ50" s="8"/>
-      <c r="CR50" s="8"/>
-      <c r="CS50" s="8"/>
-      <c r="CT50" s="8"/>
-      <c r="CU50" s="8"/>
-      <c r="CV50" s="8"/>
+      <c r="CP50" s="26"/>
+      <c r="CQ50" s="26"/>
+      <c r="CR50" s="26"/>
+      <c r="CS50" s="26"/>
+      <c r="CT50" s="26"/>
+      <c r="CU50" s="26"/>
+      <c r="CV50" s="26"/>
       <c r="CW50" s="8"/>
       <c r="CX50" s="8"/>
       <c r="CY50" s="8"/>
@@ -9145,165 +9208,162 @@
       <c r="A55" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="CP55" s="6"/>
-      <c r="CQ55" s="6"/>
-      <c r="CR55" s="6"/>
-      <c r="CS55" s="6"/>
-      <c r="CT55" s="6"/>
-      <c r="CU55" s="6"/>
+      <c r="CP55" s="30"/>
+      <c r="CQ55" s="30"/>
+      <c r="CR55" s="30"/>
+      <c r="CS55" s="30"/>
+      <c r="CT55" s="30"/>
+      <c r="CU55" s="30"/>
+      <c r="CV55" s="30"/>
     </row>
     <row r="56" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="CP56" s="6"/>
-      <c r="CQ56" s="6"/>
-      <c r="CR56" s="6"/>
-      <c r="CS56" s="6"/>
-      <c r="CT56" s="6"/>
-      <c r="CU56" s="6"/>
+      <c r="CS56" s="30"/>
+      <c r="CT56" s="30"/>
+      <c r="CU56" s="30"/>
+      <c r="CV56" s="30"/>
     </row>
     <row r="57" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="CR57" s="6"/>
-      <c r="CS57" s="6"/>
-      <c r="CU57" s="6"/>
+      <c r="CS57" s="30"/>
+      <c r="CV57" s="30"/>
     </row>
     <row r="58" spans="1:151" x14ac:dyDescent="0.2">
-      <c r="CR58" s="6"/>
-      <c r="CS58" s="6"/>
-      <c r="CU58" s="6"/>
+      <c r="CS58" s="30"/>
+      <c r="CV58" s="30"/>
     </row>
     <row r="59" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
-      <c r="B59" s="25" t="s">
+      <c r="B59" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25" t="s">
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
-      <c r="I59" s="25"/>
-      <c r="J59" s="25" t="s">
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="K59" s="25"/>
-      <c r="L59" s="25"/>
-      <c r="M59" s="25"/>
-      <c r="N59" s="25" t="s">
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="O59" s="25"/>
-      <c r="P59" s="25"/>
-      <c r="Q59" s="25"/>
-      <c r="R59" s="25" t="s">
+      <c r="O59" s="35"/>
+      <c r="P59" s="35"/>
+      <c r="Q59" s="35"/>
+      <c r="R59" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="S59" s="25"/>
-      <c r="T59" s="25"/>
-      <c r="U59" s="25"/>
-      <c r="V59" s="25" t="s">
+      <c r="S59" s="35"/>
+      <c r="T59" s="35"/>
+      <c r="U59" s="35"/>
+      <c r="V59" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="W59" s="25"/>
-      <c r="X59" s="25"/>
-      <c r="Y59" s="25"/>
-      <c r="Z59" s="25" t="s">
+      <c r="W59" s="35"/>
+      <c r="X59" s="35"/>
+      <c r="Y59" s="35"/>
+      <c r="Z59" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="AA59" s="25"/>
-      <c r="AB59" s="25"/>
-      <c r="AC59" s="25"/>
-      <c r="AD59" s="25" t="s">
+      <c r="AA59" s="35"/>
+      <c r="AB59" s="35"/>
+      <c r="AC59" s="35"/>
+      <c r="AD59" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="AE59" s="25"/>
-      <c r="AF59" s="25"/>
-      <c r="AG59" s="25"/>
-      <c r="AH59" s="25" t="s">
+      <c r="AE59" s="35"/>
+      <c r="AF59" s="35"/>
+      <c r="AG59" s="35"/>
+      <c r="AH59" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="AI59" s="25"/>
-      <c r="AJ59" s="25"/>
-      <c r="AK59" s="25"/>
-      <c r="AL59" s="25" t="s">
+      <c r="AI59" s="35"/>
+      <c r="AJ59" s="35"/>
+      <c r="AK59" s="35"/>
+      <c r="AL59" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="AM59" s="25"/>
-      <c r="AN59" s="25"/>
-      <c r="AO59" s="25"/>
-      <c r="AP59" s="25" t="s">
+      <c r="AM59" s="35"/>
+      <c r="AN59" s="35"/>
+      <c r="AO59" s="35"/>
+      <c r="AP59" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="AQ59" s="25"/>
-      <c r="AR59" s="25"/>
-      <c r="AS59" s="25"/>
-      <c r="AT59" s="25" t="s">
+      <c r="AQ59" s="35"/>
+      <c r="AR59" s="35"/>
+      <c r="AS59" s="35"/>
+      <c r="AT59" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AU59" s="25"/>
-      <c r="AV59" s="25"/>
-      <c r="AW59" s="25"/>
-      <c r="AX59" s="25" t="s">
+      <c r="AU59" s="35"/>
+      <c r="AV59" s="35"/>
+      <c r="AW59" s="35"/>
+      <c r="AX59" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="AY59" s="25"/>
-      <c r="AZ59" s="25"/>
-      <c r="BA59" s="25"/>
-      <c r="BB59" s="25" t="s">
+      <c r="AY59" s="35"/>
+      <c r="AZ59" s="35"/>
+      <c r="BA59" s="35"/>
+      <c r="BB59" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="BC59" s="25"/>
-      <c r="BD59" s="25"/>
-      <c r="BE59" s="25"/>
-      <c r="BF59" s="25" t="s">
+      <c r="BC59" s="35"/>
+      <c r="BD59" s="35"/>
+      <c r="BE59" s="35"/>
+      <c r="BF59" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="BG59" s="25"/>
-      <c r="BH59" s="25"/>
-      <c r="BI59" s="25"/>
-      <c r="BJ59" s="25" t="s">
+      <c r="BG59" s="35"/>
+      <c r="BH59" s="35"/>
+      <c r="BI59" s="35"/>
+      <c r="BJ59" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="BK59" s="25"/>
-      <c r="BL59" s="25"/>
-      <c r="BM59" s="25"/>
-      <c r="BN59" s="25" t="s">
+      <c r="BK59" s="35"/>
+      <c r="BL59" s="35"/>
+      <c r="BM59" s="35"/>
+      <c r="BN59" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="BO59" s="25"/>
-      <c r="BP59" s="25"/>
-      <c r="BQ59" s="25"/>
-      <c r="BR59" s="25" t="s">
+      <c r="BO59" s="35"/>
+      <c r="BP59" s="35"/>
+      <c r="BQ59" s="35"/>
+      <c r="BR59" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="BS59" s="25"/>
-      <c r="BT59" s="25"/>
-      <c r="BU59" s="25"/>
-      <c r="BV59" s="25" t="s">
+      <c r="BS59" s="35"/>
+      <c r="BT59" s="35"/>
+      <c r="BU59" s="35"/>
+      <c r="BV59" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="BW59" s="25"/>
-      <c r="BX59" s="25"/>
-      <c r="BY59" s="25"/>
-      <c r="BZ59" s="25" t="s">
+      <c r="BW59" s="35"/>
+      <c r="BX59" s="35"/>
+      <c r="BY59" s="35"/>
+      <c r="BZ59" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="CA59" s="25"/>
-      <c r="CB59" s="25"/>
-      <c r="CC59" s="25"/>
-      <c r="CD59" s="25" t="s">
+      <c r="CA59" s="35"/>
+      <c r="CB59" s="35"/>
+      <c r="CC59" s="35"/>
+      <c r="CD59" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="CE59" s="25"/>
-      <c r="CF59" s="25"/>
-      <c r="CG59" s="25"/>
+      <c r="CE59" s="35"/>
+      <c r="CF59" s="35"/>
+      <c r="CG59" s="35"/>
       <c r="CH59" s="21" t="s">
         <v>52</v>
       </c>
@@ -9316,14 +9376,15 @@
       <c r="CM59" s="21"/>
       <c r="CN59" s="21"/>
       <c r="CO59" s="21"/>
-      <c r="CP59" s="21" t="s">
+      <c r="CP59" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="CQ59" s="21"/>
-      <c r="CR59" s="22"/>
+      <c r="CQ59" s="24"/>
+      <c r="CR59" s="24"/>
       <c r="CS59" s="22"/>
-      <c r="CT59" s="21"/>
-      <c r="CU59" s="22"/>
+      <c r="CT59" s="24"/>
+      <c r="CU59" s="24"/>
+      <c r="CV59" s="22"/>
     </row>
     <row r="60" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
@@ -9603,22 +9664,24 @@
       <c r="CO60" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP60" s="13" t="s">
+      <c r="CP60" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CQ60" s="13" t="s">
+      <c r="CQ60" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="CR60" s="13"/>
-      <c r="CS60" s="13"/>
-      <c r="CT60" s="13"/>
-      <c r="CU60" s="13"/>
+      <c r="CR60" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS60" s="29"/>
+      <c r="CT60" s="29"/>
+      <c r="CU60" s="29"/>
+      <c r="CV60" s="29"/>
     </row>
     <row r="61" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
-      <c r="CR61" s="6"/>
-      <c r="CS61" s="6"/>
-      <c r="CU61" s="6"/>
+      <c r="CS61" s="30"/>
+      <c r="CV61" s="30"/>
     </row>
     <row r="62" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -9900,17 +9963,19 @@
       <c r="CO62" s="14">
         <v>12.595581900616963</v>
       </c>
-      <c r="CP62" s="14">
+      <c r="CP62" s="31">
         <v>12.373074369915457</v>
       </c>
-      <c r="CQ62" s="14">
-        <v>10.653916472298206</v>
-      </c>
-      <c r="CR62" s="23"/>
-      <c r="CS62" s="23"/>
-      <c r="CT62" s="14"/>
-      <c r="CU62" s="23"/>
-      <c r="CV62" s="8"/>
+      <c r="CQ62" s="31">
+        <v>10.957096826764072</v>
+      </c>
+      <c r="CR62" s="31">
+        <v>-2.4697354809294723</v>
+      </c>
+      <c r="CS62" s="32"/>
+      <c r="CT62" s="31"/>
+      <c r="CU62" s="31"/>
+      <c r="CV62" s="32"/>
       <c r="CW62" s="8"/>
       <c r="CX62" s="8"/>
       <c r="CY62" s="8"/>
@@ -10239,17 +10304,19 @@
       <c r="CO63" s="14">
         <v>-5.7511235051855465</v>
       </c>
-      <c r="CP63" s="14">
+      <c r="CP63" s="31">
         <v>11.321529650063567</v>
       </c>
-      <c r="CQ63" s="14">
-        <v>11.993715039622984</v>
-      </c>
-      <c r="CR63" s="23"/>
-      <c r="CS63" s="23"/>
-      <c r="CT63" s="14"/>
-      <c r="CU63" s="23"/>
-      <c r="CV63" s="8"/>
+      <c r="CQ63" s="31">
+        <v>5.600146525279186</v>
+      </c>
+      <c r="CR63" s="31">
+        <v>8.264236171770392</v>
+      </c>
+      <c r="CS63" s="32"/>
+      <c r="CT63" s="31"/>
+      <c r="CU63" s="31"/>
+      <c r="CV63" s="32"/>
       <c r="CW63" s="8"/>
       <c r="CX63" s="8"/>
       <c r="CY63" s="8"/>
@@ -10578,17 +10645,19 @@
       <c r="CO64" s="14">
         <v>67.431544333633241</v>
       </c>
-      <c r="CP64" s="14">
+      <c r="CP64" s="31">
         <v>18.255808080987705</v>
       </c>
-      <c r="CQ64" s="14">
+      <c r="CQ64" s="31">
         <v>26.473626948390262</v>
       </c>
-      <c r="CR64" s="23"/>
-      <c r="CS64" s="23"/>
-      <c r="CT64" s="14"/>
-      <c r="CU64" s="23"/>
-      <c r="CV64" s="8"/>
+      <c r="CR64" s="31">
+        <v>-14.581012609599711</v>
+      </c>
+      <c r="CS64" s="32"/>
+      <c r="CT64" s="31"/>
+      <c r="CU64" s="31"/>
+      <c r="CV64" s="32"/>
       <c r="CW64" s="8"/>
       <c r="CX64" s="8"/>
       <c r="CY64" s="8"/>
@@ -10917,17 +10986,19 @@
       <c r="CO65" s="14">
         <v>19.608787551606682</v>
       </c>
-      <c r="CP65" s="14">
+      <c r="CP65" s="31">
         <v>8.9218621598278673</v>
       </c>
-      <c r="CQ65" s="14">
-        <v>4.9053281335405643</v>
-      </c>
-      <c r="CR65" s="23"/>
-      <c r="CS65" s="23"/>
-      <c r="CT65" s="14"/>
-      <c r="CU65" s="23"/>
-      <c r="CV65" s="8"/>
+      <c r="CQ65" s="31">
+        <v>5.434953704937513</v>
+      </c>
+      <c r="CR65" s="31">
+        <v>4.7213918931851424</v>
+      </c>
+      <c r="CS65" s="32"/>
+      <c r="CT65" s="31"/>
+      <c r="CU65" s="31"/>
+      <c r="CV65" s="32"/>
       <c r="CW65" s="8"/>
       <c r="CX65" s="8"/>
       <c r="CY65" s="8"/>
@@ -11256,17 +11327,19 @@
       <c r="CO66" s="14">
         <v>14.317884840937054</v>
       </c>
-      <c r="CP66" s="14">
+      <c r="CP66" s="31">
         <v>5.9969860589665416</v>
       </c>
-      <c r="CQ66" s="14">
-        <v>7.9400042174752912</v>
-      </c>
-      <c r="CR66" s="23"/>
-      <c r="CS66" s="23"/>
-      <c r="CT66" s="14"/>
-      <c r="CU66" s="23"/>
-      <c r="CV66" s="8"/>
+      <c r="CQ66" s="31">
+        <v>7.5949099210423867</v>
+      </c>
+      <c r="CR66" s="31">
+        <v>11.665640138415839</v>
+      </c>
+      <c r="CS66" s="32"/>
+      <c r="CT66" s="31"/>
+      <c r="CU66" s="31"/>
+      <c r="CV66" s="32"/>
       <c r="CW66" s="8"/>
       <c r="CX66" s="8"/>
       <c r="CY66" s="8"/>
@@ -11595,17 +11668,19 @@
       <c r="CO67" s="14">
         <v>7.2652728936842408</v>
       </c>
-      <c r="CP67" s="14">
+      <c r="CP67" s="31">
         <v>11.510351210896232</v>
       </c>
-      <c r="CQ67" s="14">
-        <v>6.7593073990803703</v>
-      </c>
-      <c r="CR67" s="23"/>
-      <c r="CS67" s="23"/>
-      <c r="CT67" s="14"/>
-      <c r="CU67" s="23"/>
-      <c r="CV67" s="8"/>
+      <c r="CQ67" s="31">
+        <v>6.2174233659246738</v>
+      </c>
+      <c r="CR67" s="31">
+        <v>12.899133999394991</v>
+      </c>
+      <c r="CS67" s="32"/>
+      <c r="CT67" s="31"/>
+      <c r="CU67" s="31"/>
+      <c r="CV67" s="32"/>
       <c r="CW67" s="8"/>
       <c r="CX67" s="8"/>
       <c r="CY67" s="8"/>
@@ -11934,17 +12009,19 @@
       <c r="CO68" s="14">
         <v>7.917711071920877</v>
       </c>
-      <c r="CP68" s="14">
+      <c r="CP68" s="31">
         <v>8.3294940811998117</v>
       </c>
-      <c r="CQ68" s="14">
-        <v>5.2704272045858858</v>
-      </c>
-      <c r="CR68" s="23"/>
-      <c r="CS68" s="23"/>
-      <c r="CT68" s="14"/>
-      <c r="CU68" s="23"/>
-      <c r="CV68" s="8"/>
+      <c r="CQ68" s="31">
+        <v>8.5722774120493597</v>
+      </c>
+      <c r="CR68" s="31">
+        <v>7.383320000662394</v>
+      </c>
+      <c r="CS68" s="32"/>
+      <c r="CT68" s="31"/>
+      <c r="CU68" s="31"/>
+      <c r="CV68" s="32"/>
       <c r="CW68" s="8"/>
       <c r="CX68" s="8"/>
       <c r="CY68" s="8"/>
@@ -12273,17 +12350,19 @@
       <c r="CO69" s="14">
         <v>14.318042026160384</v>
       </c>
-      <c r="CP69" s="14">
+      <c r="CP69" s="31">
         <v>7.8810683390206293</v>
       </c>
-      <c r="CQ69" s="14">
-        <v>29.784679957728343</v>
-      </c>
-      <c r="CR69" s="23"/>
-      <c r="CS69" s="23"/>
-      <c r="CT69" s="14"/>
-      <c r="CU69" s="23"/>
-      <c r="CV69" s="8"/>
+      <c r="CQ69" s="31">
+        <v>41.668265726362222</v>
+      </c>
+      <c r="CR69" s="31">
+        <v>8.5426064003939075</v>
+      </c>
+      <c r="CS69" s="32"/>
+      <c r="CT69" s="31"/>
+      <c r="CU69" s="31"/>
+      <c r="CV69" s="32"/>
       <c r="CW69" s="8"/>
       <c r="CX69" s="8"/>
       <c r="CY69" s="8"/>
@@ -12425,13 +12504,13 @@
       <c r="CM70" s="8"/>
       <c r="CN70" s="8"/>
       <c r="CO70" s="8"/>
-      <c r="CP70" s="8"/>
-      <c r="CQ70" s="8"/>
-      <c r="CR70" s="24"/>
-      <c r="CS70" s="24"/>
-      <c r="CT70" s="8"/>
-      <c r="CU70" s="24"/>
-      <c r="CV70" s="8"/>
+      <c r="CP70" s="26"/>
+      <c r="CQ70" s="26"/>
+      <c r="CR70" s="26"/>
+      <c r="CS70" s="33"/>
+      <c r="CT70" s="26"/>
+      <c r="CU70" s="26"/>
+      <c r="CV70" s="33"/>
       <c r="CW70" s="8"/>
       <c r="CX70" s="8"/>
       <c r="CY70" s="8"/>
@@ -12760,17 +12839,19 @@
       <c r="CO71" s="14">
         <v>15.22220251521378</v>
       </c>
-      <c r="CP71" s="14">
+      <c r="CP71" s="31">
         <v>11.431160487940687</v>
       </c>
-      <c r="CQ71" s="14">
-        <v>10.380783878040177</v>
-      </c>
-      <c r="CR71" s="23"/>
-      <c r="CS71" s="23"/>
-      <c r="CT71" s="14"/>
-      <c r="CU71" s="23"/>
-      <c r="CV71" s="8"/>
+      <c r="CQ71" s="31">
+        <v>10.523242944820296</v>
+      </c>
+      <c r="CR71" s="31">
+        <v>4.5050592385500892</v>
+      </c>
+      <c r="CS71" s="32"/>
+      <c r="CT71" s="31"/>
+      <c r="CU71" s="31"/>
+      <c r="CV71" s="32"/>
       <c r="CW71" s="8"/>
       <c r="CX71" s="8"/>
       <c r="CY71" s="8"/>
@@ -12913,20 +12994,20 @@
       <c r="CM72" s="11"/>
       <c r="CN72" s="11"/>
       <c r="CO72" s="11"/>
-      <c r="CP72" s="11"/>
-      <c r="CQ72" s="11"/>
-      <c r="CR72" s="5"/>
-      <c r="CS72" s="5"/>
-      <c r="CT72" s="11"/>
-      <c r="CU72" s="5"/>
+      <c r="CP72" s="28"/>
+      <c r="CQ72" s="28"/>
+      <c r="CR72" s="28"/>
+      <c r="CS72" s="13"/>
+      <c r="CT72" s="28"/>
+      <c r="CU72" s="28"/>
+      <c r="CV72" s="13"/>
     </row>
     <row r="73" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="CR73" s="6"/>
-      <c r="CS73" s="6"/>
-      <c r="CU73" s="6"/>
+      <c r="CS73" s="30"/>
+      <c r="CV73" s="30"/>
     </row>
     <row r="74" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="8"/>
@@ -13021,13 +13102,13 @@
       <c r="CM74" s="8"/>
       <c r="CN74" s="8"/>
       <c r="CO74" s="8"/>
-      <c r="CP74" s="8"/>
-      <c r="CQ74" s="8"/>
-      <c r="CR74" s="24"/>
-      <c r="CS74" s="24"/>
-      <c r="CT74" s="8"/>
-      <c r="CU74" s="24"/>
-      <c r="CV74" s="8"/>
+      <c r="CP74" s="26"/>
+      <c r="CQ74" s="26"/>
+      <c r="CR74" s="26"/>
+      <c r="CS74" s="33"/>
+      <c r="CT74" s="26"/>
+      <c r="CU74" s="26"/>
+      <c r="CV74" s="33"/>
       <c r="CW74" s="8"/>
       <c r="CX74" s="8"/>
       <c r="CY74" s="8"/>
@@ -13169,13 +13250,13 @@
       <c r="CM75" s="8"/>
       <c r="CN75" s="8"/>
       <c r="CO75" s="8"/>
-      <c r="CP75" s="8"/>
-      <c r="CQ75" s="8"/>
-      <c r="CR75" s="24"/>
-      <c r="CS75" s="24"/>
-      <c r="CT75" s="8"/>
-      <c r="CU75" s="24"/>
-      <c r="CV75" s="8"/>
+      <c r="CP75" s="26"/>
+      <c r="CQ75" s="26"/>
+      <c r="CR75" s="26"/>
+      <c r="CS75" s="33"/>
+      <c r="CT75" s="26"/>
+      <c r="CU75" s="26"/>
+      <c r="CV75" s="33"/>
       <c r="CW75" s="8"/>
       <c r="CX75" s="8"/>
       <c r="CY75" s="8"/>
@@ -13228,188 +13309,180 @@
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="CR76" s="6"/>
-      <c r="CS76" s="6"/>
-      <c r="CU76" s="6"/>
+      <c r="CS76" s="30"/>
+      <c r="CV76" s="30"/>
     </row>
     <row r="77" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="CR77" s="6"/>
-      <c r="CS77" s="6"/>
-      <c r="CU77" s="6"/>
+      <c r="CS77" s="30"/>
+      <c r="CV77" s="30"/>
     </row>
     <row r="78" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="CR78" s="6"/>
-      <c r="CS78" s="6"/>
-      <c r="CU78" s="6"/>
+      <c r="CS78" s="30"/>
+      <c r="CV78" s="30"/>
     </row>
     <row r="79" spans="1:147" x14ac:dyDescent="0.2">
-      <c r="CR79" s="6"/>
-      <c r="CS79" s="6"/>
-      <c r="CU79" s="6"/>
+      <c r="CS79" s="30"/>
+      <c r="CV79" s="30"/>
     </row>
     <row r="80" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="CR80" s="6"/>
-      <c r="CS80" s="6"/>
-      <c r="CU80" s="6"/>
+      <c r="CS80" s="30"/>
+      <c r="CV80" s="30"/>
     </row>
     <row r="81" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="CR81" s="6"/>
-      <c r="CS81" s="6"/>
-      <c r="CU81" s="6"/>
+      <c r="CS81" s="30"/>
+      <c r="CV81" s="30"/>
     </row>
     <row r="82" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="CR82" s="6"/>
-      <c r="CS82" s="6"/>
-      <c r="CU82" s="6"/>
+      <c r="CS82" s="30"/>
+      <c r="CV82" s="30"/>
     </row>
     <row r="83" spans="1:147" x14ac:dyDescent="0.2">
-      <c r="CR83" s="6"/>
-      <c r="CS83" s="6"/>
-      <c r="CU83" s="6"/>
+      <c r="CS83" s="30"/>
+      <c r="CV83" s="30"/>
     </row>
     <row r="84" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
-      <c r="B84" s="25" t="s">
+      <c r="B84" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25" t="s">
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="35"/>
+      <c r="F84" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G84" s="25"/>
-      <c r="H84" s="25"/>
-      <c r="I84" s="25"/>
-      <c r="J84" s="25" t="s">
+      <c r="G84" s="35"/>
+      <c r="H84" s="35"/>
+      <c r="I84" s="35"/>
+      <c r="J84" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="K84" s="25"/>
-      <c r="L84" s="25"/>
-      <c r="M84" s="25"/>
-      <c r="N84" s="25" t="s">
+      <c r="K84" s="35"/>
+      <c r="L84" s="35"/>
+      <c r="M84" s="35"/>
+      <c r="N84" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="O84" s="25"/>
-      <c r="P84" s="25"/>
-      <c r="Q84" s="25"/>
-      <c r="R84" s="25" t="s">
+      <c r="O84" s="35"/>
+      <c r="P84" s="35"/>
+      <c r="Q84" s="35"/>
+      <c r="R84" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="S84" s="25"/>
-      <c r="T84" s="25"/>
-      <c r="U84" s="25"/>
-      <c r="V84" s="25" t="s">
+      <c r="S84" s="35"/>
+      <c r="T84" s="35"/>
+      <c r="U84" s="35"/>
+      <c r="V84" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="W84" s="25"/>
-      <c r="X84" s="25"/>
-      <c r="Y84" s="25"/>
-      <c r="Z84" s="25" t="s">
+      <c r="W84" s="35"/>
+      <c r="X84" s="35"/>
+      <c r="Y84" s="35"/>
+      <c r="Z84" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="AA84" s="25"/>
-      <c r="AB84" s="25"/>
-      <c r="AC84" s="25"/>
-      <c r="AD84" s="25" t="s">
+      <c r="AA84" s="35"/>
+      <c r="AB84" s="35"/>
+      <c r="AC84" s="35"/>
+      <c r="AD84" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="AE84" s="25"/>
-      <c r="AF84" s="25"/>
-      <c r="AG84" s="25"/>
-      <c r="AH84" s="25" t="s">
+      <c r="AE84" s="35"/>
+      <c r="AF84" s="35"/>
+      <c r="AG84" s="35"/>
+      <c r="AH84" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="AI84" s="25"/>
-      <c r="AJ84" s="25"/>
-      <c r="AK84" s="25"/>
-      <c r="AL84" s="25" t="s">
+      <c r="AI84" s="35"/>
+      <c r="AJ84" s="35"/>
+      <c r="AK84" s="35"/>
+      <c r="AL84" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="AM84" s="25"/>
-      <c r="AN84" s="25"/>
-      <c r="AO84" s="25"/>
-      <c r="AP84" s="25" t="s">
+      <c r="AM84" s="35"/>
+      <c r="AN84" s="35"/>
+      <c r="AO84" s="35"/>
+      <c r="AP84" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="AQ84" s="25"/>
-      <c r="AR84" s="25"/>
-      <c r="AS84" s="25"/>
-      <c r="AT84" s="25" t="s">
+      <c r="AQ84" s="35"/>
+      <c r="AR84" s="35"/>
+      <c r="AS84" s="35"/>
+      <c r="AT84" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AU84" s="25"/>
-      <c r="AV84" s="25"/>
-      <c r="AW84" s="25"/>
-      <c r="AX84" s="25" t="s">
+      <c r="AU84" s="35"/>
+      <c r="AV84" s="35"/>
+      <c r="AW84" s="35"/>
+      <c r="AX84" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="AY84" s="25"/>
-      <c r="AZ84" s="25"/>
-      <c r="BA84" s="25"/>
-      <c r="BB84" s="25" t="s">
+      <c r="AY84" s="35"/>
+      <c r="AZ84" s="35"/>
+      <c r="BA84" s="35"/>
+      <c r="BB84" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="BC84" s="25"/>
-      <c r="BD84" s="25"/>
-      <c r="BE84" s="25"/>
-      <c r="BF84" s="25" t="s">
+      <c r="BC84" s="35"/>
+      <c r="BD84" s="35"/>
+      <c r="BE84" s="35"/>
+      <c r="BF84" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="BG84" s="25"/>
-      <c r="BH84" s="25"/>
-      <c r="BI84" s="25"/>
-      <c r="BJ84" s="25" t="s">
+      <c r="BG84" s="35"/>
+      <c r="BH84" s="35"/>
+      <c r="BI84" s="35"/>
+      <c r="BJ84" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="BK84" s="25"/>
-      <c r="BL84" s="25"/>
-      <c r="BM84" s="25"/>
-      <c r="BN84" s="25" t="s">
+      <c r="BK84" s="35"/>
+      <c r="BL84" s="35"/>
+      <c r="BM84" s="35"/>
+      <c r="BN84" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="BO84" s="25"/>
-      <c r="BP84" s="25"/>
-      <c r="BQ84" s="25"/>
-      <c r="BR84" s="25" t="s">
+      <c r="BO84" s="35"/>
+      <c r="BP84" s="35"/>
+      <c r="BQ84" s="35"/>
+      <c r="BR84" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="BS84" s="25"/>
-      <c r="BT84" s="25"/>
-      <c r="BU84" s="25"/>
-      <c r="BV84" s="25" t="s">
+      <c r="BS84" s="35"/>
+      <c r="BT84" s="35"/>
+      <c r="BU84" s="35"/>
+      <c r="BV84" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="BW84" s="25"/>
-      <c r="BX84" s="25"/>
-      <c r="BY84" s="25"/>
-      <c r="BZ84" s="25" t="s">
+      <c r="BW84" s="35"/>
+      <c r="BX84" s="35"/>
+      <c r="BY84" s="35"/>
+      <c r="BZ84" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="CA84" s="25"/>
-      <c r="CB84" s="25"/>
-      <c r="CC84" s="25"/>
-      <c r="CD84" s="25" t="s">
+      <c r="CA84" s="35"/>
+      <c r="CB84" s="35"/>
+      <c r="CC84" s="35"/>
+      <c r="CD84" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="CE84" s="25"/>
-      <c r="CF84" s="25"/>
-      <c r="CG84" s="25"/>
+      <c r="CE84" s="35"/>
+      <c r="CF84" s="35"/>
+      <c r="CG84" s="35"/>
       <c r="CH84" s="21" t="s">
         <v>52</v>
       </c>
@@ -13422,14 +13495,15 @@
       <c r="CM84" s="21"/>
       <c r="CN84" s="21"/>
       <c r="CO84" s="21"/>
-      <c r="CP84" s="21" t="s">
+      <c r="CP84" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="CQ84" s="21"/>
-      <c r="CR84" s="22"/>
+      <c r="CQ84" s="24"/>
+      <c r="CR84" s="24"/>
       <c r="CS84" s="22"/>
-      <c r="CT84" s="21"/>
-      <c r="CU84" s="22"/>
+      <c r="CT84" s="24"/>
+      <c r="CU84" s="24"/>
+      <c r="CV84" s="22"/>
     </row>
     <row r="85" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
@@ -13709,22 +13783,24 @@
       <c r="CO85" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CP85" s="5" t="s">
+      <c r="CP85" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="CQ85" s="5" t="s">
+      <c r="CQ85" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="CR85" s="5"/>
-      <c r="CS85" s="5"/>
-      <c r="CT85" s="5"/>
-      <c r="CU85" s="5"/>
+      <c r="CR85" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CS85" s="13"/>
+      <c r="CT85" s="13"/>
+      <c r="CU85" s="13"/>
+      <c r="CV85" s="13"/>
     </row>
     <row r="86" spans="1:147" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
-      <c r="CR86" s="6"/>
-      <c r="CS86" s="6"/>
-      <c r="CU86" s="6"/>
+      <c r="CS86" s="30"/>
+      <c r="CV86" s="30"/>
     </row>
     <row r="87" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
@@ -14006,17 +14082,19 @@
       <c r="CO87" s="14">
         <v>9.9884926983417017</v>
       </c>
-      <c r="CP87" s="14">
+      <c r="CP87" s="31">
         <v>10.357584852905816</v>
       </c>
-      <c r="CQ87" s="14">
-        <v>10.779571809096254</v>
-      </c>
-      <c r="CR87" s="23"/>
-      <c r="CS87" s="23"/>
-      <c r="CT87" s="14"/>
-      <c r="CU87" s="23"/>
-      <c r="CV87" s="8"/>
+      <c r="CQ87" s="31">
+        <v>11.083096446265955</v>
+      </c>
+      <c r="CR87" s="31">
+        <v>-2.3839288224028081</v>
+      </c>
+      <c r="CS87" s="32"/>
+      <c r="CT87" s="31"/>
+      <c r="CU87" s="31"/>
+      <c r="CV87" s="32"/>
       <c r="CW87" s="8"/>
       <c r="CX87" s="8"/>
       <c r="CY87" s="8"/>
@@ -14345,17 +14423,19 @@
       <c r="CO88" s="14">
         <v>-8.4755685706075781</v>
       </c>
-      <c r="CP88" s="14">
+      <c r="CP88" s="31">
         <v>8.8706091445568234</v>
       </c>
-      <c r="CQ88" s="14">
-        <v>9.3534950949275526</v>
-      </c>
-      <c r="CR88" s="23"/>
-      <c r="CS88" s="23"/>
-      <c r="CT88" s="14"/>
-      <c r="CU88" s="23"/>
-      <c r="CV88" s="8"/>
+      <c r="CQ88" s="31">
+        <v>3.1106531379032845</v>
+      </c>
+      <c r="CR88" s="31">
+        <v>5.3422462744758832</v>
+      </c>
+      <c r="CS88" s="32"/>
+      <c r="CT88" s="31"/>
+      <c r="CU88" s="31"/>
+      <c r="CV88" s="32"/>
       <c r="CW88" s="8"/>
       <c r="CX88" s="8"/>
       <c r="CY88" s="8"/>
@@ -14684,17 +14764,19 @@
       <c r="CO89" s="14">
         <v>60.491148122143812</v>
       </c>
-      <c r="CP89" s="14">
+      <c r="CP89" s="31">
         <v>14.500882329394528</v>
       </c>
-      <c r="CQ89" s="14">
+      <c r="CQ89" s="31">
         <v>22.559183091322495</v>
       </c>
-      <c r="CR89" s="23"/>
-      <c r="CS89" s="23"/>
-      <c r="CT89" s="14"/>
-      <c r="CU89" s="23"/>
-      <c r="CV89" s="8"/>
+      <c r="CR89" s="31">
+        <v>-15.57684927955026</v>
+      </c>
+      <c r="CS89" s="32"/>
+      <c r="CT89" s="31"/>
+      <c r="CU89" s="31"/>
+      <c r="CV89" s="32"/>
       <c r="CW89" s="8"/>
       <c r="CX89" s="8"/>
       <c r="CY89" s="8"/>
@@ -15023,17 +15105,19 @@
       <c r="CO90" s="14">
         <v>14.768083517647383</v>
       </c>
-      <c r="CP90" s="14">
+      <c r="CP90" s="31">
         <v>5.1963369608708518</v>
       </c>
-      <c r="CQ90" s="14">
-        <v>2.9256716063682688</v>
-      </c>
-      <c r="CR90" s="23"/>
-      <c r="CS90" s="23"/>
-      <c r="CT90" s="14"/>
-      <c r="CU90" s="23"/>
-      <c r="CV90" s="8"/>
+      <c r="CQ90" s="31">
+        <v>3.445302673786955</v>
+      </c>
+      <c r="CR90" s="31">
+        <v>2.2631422112805382</v>
+      </c>
+      <c r="CS90" s="32"/>
+      <c r="CT90" s="31"/>
+      <c r="CU90" s="31"/>
+      <c r="CV90" s="32"/>
       <c r="CW90" s="8"/>
       <c r="CX90" s="8"/>
       <c r="CY90" s="8"/>
@@ -15362,17 +15446,19 @@
       <c r="CO91" s="14">
         <v>13.94667411688178</v>
       </c>
-      <c r="CP91" s="14">
+      <c r="CP91" s="31">
         <v>5.4672787574868522</v>
       </c>
-      <c r="CQ91" s="14">
-        <v>7.4850317816753176</v>
-      </c>
-      <c r="CR91" s="23"/>
-      <c r="CS91" s="23"/>
-      <c r="CT91" s="14"/>
-      <c r="CU91" s="23"/>
-      <c r="CV91" s="8"/>
+      <c r="CQ91" s="31">
+        <v>7.1413802619892692</v>
+      </c>
+      <c r="CR91" s="31">
+        <v>10.908218160732801</v>
+      </c>
+      <c r="CS91" s="32"/>
+      <c r="CT91" s="31"/>
+      <c r="CU91" s="31"/>
+      <c r="CV91" s="32"/>
       <c r="CW91" s="8"/>
       <c r="CX91" s="8"/>
       <c r="CY91" s="8"/>
@@ -15701,17 +15787,19 @@
       <c r="CO92" s="14">
         <v>4.2483615085071591</v>
       </c>
-      <c r="CP92" s="14">
+      <c r="CP92" s="31">
         <v>9.2890239473999259</v>
       </c>
-      <c r="CQ92" s="14">
-        <v>4.2424871241461943</v>
-      </c>
-      <c r="CR92" s="23"/>
-      <c r="CS92" s="23"/>
-      <c r="CT92" s="14"/>
-      <c r="CU92" s="23"/>
-      <c r="CV92" s="8"/>
+      <c r="CQ92" s="31">
+        <v>3.7133778527844328</v>
+      </c>
+      <c r="CR92" s="31">
+        <v>9.8511467149462248</v>
+      </c>
+      <c r="CS92" s="32"/>
+      <c r="CT92" s="31"/>
+      <c r="CU92" s="31"/>
+      <c r="CV92" s="32"/>
       <c r="CW92" s="8"/>
       <c r="CX92" s="8"/>
       <c r="CY92" s="8"/>
@@ -16040,17 +16128,19 @@
       <c r="CO93" s="14">
         <v>6.157988704053551</v>
       </c>
-      <c r="CP93" s="14">
+      <c r="CP93" s="31">
         <v>5.9444479968583579</v>
       </c>
-      <c r="CQ93" s="14">
-        <v>2.7887068563160966</v>
-      </c>
-      <c r="CR93" s="23"/>
-      <c r="CS93" s="23"/>
-      <c r="CT93" s="14"/>
-      <c r="CU93" s="23"/>
-      <c r="CV93" s="8"/>
+      <c r="CQ93" s="31">
+        <v>6.0127168852565376</v>
+      </c>
+      <c r="CR93" s="31">
+        <v>4.4851055276756711</v>
+      </c>
+      <c r="CS93" s="32"/>
+      <c r="CT93" s="31"/>
+      <c r="CU93" s="31"/>
+      <c r="CV93" s="32"/>
       <c r="CW93" s="8"/>
       <c r="CX93" s="8"/>
       <c r="CY93" s="8"/>
@@ -16379,17 +16469,19 @@
       <c r="CO94" s="14">
         <v>11.013459127455832</v>
       </c>
-      <c r="CP94" s="14">
+      <c r="CP94" s="31">
         <v>5.5980150879969699</v>
       </c>
-      <c r="CQ94" s="14">
-        <v>26.725043080613602</v>
-      </c>
-      <c r="CR94" s="23"/>
-      <c r="CS94" s="23"/>
-      <c r="CT94" s="14"/>
-      <c r="CU94" s="23"/>
-      <c r="CV94" s="8"/>
+      <c r="CQ94" s="31">
+        <v>38.328476698300904</v>
+      </c>
+      <c r="CR94" s="31">
+        <v>5.6131034496247594</v>
+      </c>
+      <c r="CS94" s="32"/>
+      <c r="CT94" s="31"/>
+      <c r="CU94" s="31"/>
+      <c r="CV94" s="32"/>
       <c r="CW94" s="8"/>
       <c r="CX94" s="8"/>
       <c r="CY94" s="8"/>
@@ -16531,13 +16623,13 @@
       <c r="CM95" s="8"/>
       <c r="CN95" s="8"/>
       <c r="CO95" s="8"/>
-      <c r="CP95" s="8"/>
-      <c r="CQ95" s="8"/>
-      <c r="CR95" s="24"/>
-      <c r="CS95" s="24"/>
-      <c r="CT95" s="8"/>
-      <c r="CU95" s="24"/>
-      <c r="CV95" s="8"/>
+      <c r="CP95" s="26"/>
+      <c r="CQ95" s="26"/>
+      <c r="CR95" s="26"/>
+      <c r="CS95" s="33"/>
+      <c r="CT95" s="26"/>
+      <c r="CU95" s="26"/>
+      <c r="CV95" s="33"/>
       <c r="CW95" s="8"/>
       <c r="CX95" s="8"/>
       <c r="CY95" s="8"/>
@@ -16866,17 +16958,19 @@
       <c r="CO96" s="14">
         <v>12.385664564031657</v>
       </c>
-      <c r="CP96" s="14">
+      <c r="CP96" s="31">
         <v>9.1278258643393713</v>
       </c>
-      <c r="CQ96" s="14">
-        <v>7.9760361652925837</v>
-      </c>
-      <c r="CR96" s="23"/>
-      <c r="CS96" s="23"/>
-      <c r="CT96" s="14"/>
-      <c r="CU96" s="23"/>
-      <c r="CV96" s="8"/>
+      <c r="CQ96" s="31">
+        <v>8.1024300469774886</v>
+      </c>
+      <c r="CR96" s="31">
+        <v>2.8368835965535482</v>
+      </c>
+      <c r="CS96" s="32"/>
+      <c r="CT96" s="31"/>
+      <c r="CU96" s="31"/>
+      <c r="CV96" s="32"/>
       <c r="CW96" s="8"/>
       <c r="CX96" s="8"/>
       <c r="CY96" s="8"/>
@@ -17019,20 +17113,20 @@
       <c r="CM97" s="11"/>
       <c r="CN97" s="11"/>
       <c r="CO97" s="11"/>
-      <c r="CP97" s="11"/>
-      <c r="CQ97" s="11"/>
-      <c r="CR97" s="5"/>
-      <c r="CS97" s="5"/>
-      <c r="CT97" s="11"/>
-      <c r="CU97" s="5"/>
+      <c r="CP97" s="28"/>
+      <c r="CQ97" s="28"/>
+      <c r="CR97" s="28"/>
+      <c r="CS97" s="13"/>
+      <c r="CT97" s="28"/>
+      <c r="CU97" s="28"/>
+      <c r="CV97" s="13"/>
     </row>
     <row r="98" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="CR98" s="6"/>
-      <c r="CS98" s="6"/>
-      <c r="CU98" s="6"/>
+      <c r="CS98" s="30"/>
+      <c r="CV98" s="30"/>
     </row>
     <row r="99" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="8"/>
@@ -17127,13 +17221,13 @@
       <c r="CM99" s="8"/>
       <c r="CN99" s="8"/>
       <c r="CO99" s="8"/>
-      <c r="CP99" s="8"/>
-      <c r="CQ99" s="8"/>
-      <c r="CR99" s="24"/>
-      <c r="CS99" s="24"/>
-      <c r="CT99" s="8"/>
-      <c r="CU99" s="24"/>
-      <c r="CV99" s="8"/>
+      <c r="CP99" s="26"/>
+      <c r="CQ99" s="26"/>
+      <c r="CR99" s="26"/>
+      <c r="CS99" s="33"/>
+      <c r="CT99" s="26"/>
+      <c r="CU99" s="26"/>
+      <c r="CV99" s="33"/>
       <c r="CW99" s="8"/>
       <c r="CX99" s="8"/>
       <c r="CY99" s="8"/>
@@ -17275,13 +17369,13 @@
       <c r="CM100" s="8"/>
       <c r="CN100" s="8"/>
       <c r="CO100" s="8"/>
-      <c r="CP100" s="8"/>
-      <c r="CQ100" s="8"/>
-      <c r="CR100" s="24"/>
-      <c r="CS100" s="24"/>
-      <c r="CT100" s="8"/>
-      <c r="CU100" s="24"/>
-      <c r="CV100" s="8"/>
+      <c r="CP100" s="26"/>
+      <c r="CQ100" s="26"/>
+      <c r="CR100" s="33"/>
+      <c r="CS100" s="33"/>
+      <c r="CT100" s="26"/>
+      <c r="CU100" s="26"/>
+      <c r="CV100" s="33"/>
       <c r="CW100" s="8"/>
       <c r="CX100" s="8"/>
       <c r="CY100" s="8"/>
@@ -17357,132 +17451,132 @@
     </row>
     <row r="108" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
-      <c r="B108" s="26">
+      <c r="B108" s="36">
         <v>2000</v>
       </c>
-      <c r="C108" s="26"/>
-      <c r="D108" s="26"/>
-      <c r="E108" s="26"/>
-      <c r="F108" s="26">
+      <c r="C108" s="36"/>
+      <c r="D108" s="36"/>
+      <c r="E108" s="36"/>
+      <c r="F108" s="36">
         <v>2001</v>
       </c>
-      <c r="G108" s="26"/>
-      <c r="H108" s="26"/>
-      <c r="I108" s="26"/>
-      <c r="J108" s="26">
+      <c r="G108" s="36"/>
+      <c r="H108" s="36"/>
+      <c r="I108" s="36"/>
+      <c r="J108" s="36">
         <v>2002</v>
       </c>
-      <c r="K108" s="26"/>
-      <c r="L108" s="26"/>
-      <c r="M108" s="26"/>
-      <c r="N108" s="26">
+      <c r="K108" s="36"/>
+      <c r="L108" s="36"/>
+      <c r="M108" s="36"/>
+      <c r="N108" s="36">
         <v>2003</v>
       </c>
-      <c r="O108" s="26"/>
-      <c r="P108" s="26"/>
-      <c r="Q108" s="26"/>
-      <c r="R108" s="26">
+      <c r="O108" s="36"/>
+      <c r="P108" s="36"/>
+      <c r="Q108" s="36"/>
+      <c r="R108" s="36">
         <v>2004</v>
       </c>
-      <c r="S108" s="26"/>
-      <c r="T108" s="26"/>
-      <c r="U108" s="26"/>
-      <c r="V108" s="26">
+      <c r="S108" s="36"/>
+      <c r="T108" s="36"/>
+      <c r="U108" s="36"/>
+      <c r="V108" s="36">
         <v>2005</v>
       </c>
-      <c r="W108" s="26"/>
-      <c r="X108" s="26"/>
-      <c r="Y108" s="26"/>
-      <c r="Z108" s="26">
+      <c r="W108" s="36"/>
+      <c r="X108" s="36"/>
+      <c r="Y108" s="36"/>
+      <c r="Z108" s="36">
         <v>2006</v>
       </c>
-      <c r="AA108" s="26"/>
-      <c r="AB108" s="26"/>
-      <c r="AC108" s="26"/>
-      <c r="AD108" s="26">
+      <c r="AA108" s="36"/>
+      <c r="AB108" s="36"/>
+      <c r="AC108" s="36"/>
+      <c r="AD108" s="36">
         <v>2007</v>
       </c>
-      <c r="AE108" s="26"/>
-      <c r="AF108" s="26"/>
-      <c r="AG108" s="26"/>
-      <c r="AH108" s="26">
+      <c r="AE108" s="36"/>
+      <c r="AF108" s="36"/>
+      <c r="AG108" s="36"/>
+      <c r="AH108" s="36">
         <v>2008</v>
       </c>
-      <c r="AI108" s="26"/>
-      <c r="AJ108" s="26"/>
-      <c r="AK108" s="26"/>
-      <c r="AL108" s="26">
+      <c r="AI108" s="36"/>
+      <c r="AJ108" s="36"/>
+      <c r="AK108" s="36"/>
+      <c r="AL108" s="36">
         <v>2009</v>
       </c>
-      <c r="AM108" s="26"/>
-      <c r="AN108" s="26"/>
-      <c r="AO108" s="26"/>
-      <c r="AP108" s="26">
+      <c r="AM108" s="36"/>
+      <c r="AN108" s="36"/>
+      <c r="AO108" s="36"/>
+      <c r="AP108" s="36">
         <v>2010</v>
       </c>
-      <c r="AQ108" s="26"/>
-      <c r="AR108" s="26"/>
-      <c r="AS108" s="26"/>
-      <c r="AT108" s="26">
+      <c r="AQ108" s="36"/>
+      <c r="AR108" s="36"/>
+      <c r="AS108" s="36"/>
+      <c r="AT108" s="36">
         <v>2011</v>
       </c>
-      <c r="AU108" s="26"/>
-      <c r="AV108" s="26"/>
-      <c r="AW108" s="26"/>
-      <c r="AX108" s="26">
+      <c r="AU108" s="36"/>
+      <c r="AV108" s="36"/>
+      <c r="AW108" s="36"/>
+      <c r="AX108" s="36">
         <v>2012</v>
       </c>
-      <c r="AY108" s="26"/>
-      <c r="AZ108" s="26"/>
-      <c r="BA108" s="26"/>
-      <c r="BB108" s="26">
+      <c r="AY108" s="36"/>
+      <c r="AZ108" s="36"/>
+      <c r="BA108" s="36"/>
+      <c r="BB108" s="36">
         <v>2013</v>
       </c>
-      <c r="BC108" s="26"/>
-      <c r="BD108" s="26"/>
-      <c r="BE108" s="26"/>
-      <c r="BF108" s="26">
+      <c r="BC108" s="36"/>
+      <c r="BD108" s="36"/>
+      <c r="BE108" s="36"/>
+      <c r="BF108" s="36">
         <v>2014</v>
       </c>
-      <c r="BG108" s="26"/>
-      <c r="BH108" s="26"/>
-      <c r="BI108" s="26"/>
-      <c r="BJ108" s="26">
+      <c r="BG108" s="36"/>
+      <c r="BH108" s="36"/>
+      <c r="BI108" s="36"/>
+      <c r="BJ108" s="36">
         <v>2015</v>
       </c>
-      <c r="BK108" s="26"/>
-      <c r="BL108" s="26"/>
-      <c r="BM108" s="26"/>
-      <c r="BN108" s="26">
+      <c r="BK108" s="36"/>
+      <c r="BL108" s="36"/>
+      <c r="BM108" s="36"/>
+      <c r="BN108" s="36">
         <v>2016</v>
       </c>
-      <c r="BO108" s="26"/>
-      <c r="BP108" s="26"/>
-      <c r="BQ108" s="26"/>
-      <c r="BR108" s="26">
+      <c r="BO108" s="36"/>
+      <c r="BP108" s="36"/>
+      <c r="BQ108" s="36"/>
+      <c r="BR108" s="36">
         <v>2017</v>
       </c>
-      <c r="BS108" s="26"/>
-      <c r="BT108" s="26"/>
-      <c r="BU108" s="26"/>
-      <c r="BV108" s="26">
+      <c r="BS108" s="36"/>
+      <c r="BT108" s="36"/>
+      <c r="BU108" s="36"/>
+      <c r="BV108" s="36">
         <v>2018</v>
       </c>
-      <c r="BW108" s="26"/>
-      <c r="BX108" s="26"/>
-      <c r="BY108" s="26"/>
-      <c r="BZ108" s="26">
+      <c r="BW108" s="36"/>
+      <c r="BX108" s="36"/>
+      <c r="BY108" s="36"/>
+      <c r="BZ108" s="36">
         <v>2019</v>
       </c>
-      <c r="CA108" s="26"/>
-      <c r="CB108" s="26"/>
-      <c r="CC108" s="26"/>
-      <c r="CD108" s="25">
+      <c r="CA108" s="36"/>
+      <c r="CB108" s="36"/>
+      <c r="CC108" s="36"/>
+      <c r="CD108" s="35">
         <v>2020</v>
       </c>
-      <c r="CE108" s="25"/>
-      <c r="CF108" s="25"/>
-      <c r="CG108" s="25"/>
+      <c r="CE108" s="35"/>
+      <c r="CF108" s="35"/>
+      <c r="CG108" s="35"/>
       <c r="CH108" s="21">
         <v>2021</v>
       </c>
@@ -17495,16 +17589,17 @@
       <c r="CM108" s="21"/>
       <c r="CN108" s="21"/>
       <c r="CO108" s="21"/>
-      <c r="CP108" s="21">
+      <c r="CP108" s="24">
         <v>2023</v>
       </c>
-      <c r="CQ108" s="21"/>
-      <c r="CR108" s="21"/>
-      <c r="CS108" s="21"/>
-      <c r="CT108" s="21">
+      <c r="CQ108" s="24"/>
+      <c r="CR108" s="24"/>
+      <c r="CS108" s="24"/>
+      <c r="CT108" s="24">
         <v>2024</v>
       </c>
-      <c r="CU108" s="21"/>
+      <c r="CU108" s="24"/>
+      <c r="CV108" s="24"/>
     </row>
     <row r="109" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
@@ -17784,23 +17879,26 @@
       <c r="CO109" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP109" s="13" t="s">
+      <c r="CP109" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CQ109" s="13" t="s">
+      <c r="CQ109" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="CR109" s="13" t="s">
+      <c r="CR109" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="CS109" s="13" t="s">
+      <c r="CS109" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="CT109" s="13" t="s">
+      <c r="CT109" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CU109" s="13" t="s">
+      <c r="CU109" s="29" t="s">
         <v>8</v>
+      </c>
+      <c r="CV109" s="29" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -18086,25 +18184,27 @@
       <c r="CO111" s="14">
         <v>133.0320896828776</v>
       </c>
-      <c r="CP111" s="14">
+      <c r="CP111" s="31">
         <v>136.72622876503405</v>
       </c>
-      <c r="CQ111" s="14">
+      <c r="CQ111" s="31">
         <v>141.65669937816352</v>
       </c>
-      <c r="CR111" s="14">
+      <c r="CR111" s="31">
         <v>130.28192558024955</v>
       </c>
-      <c r="CS111" s="14">
+      <c r="CS111" s="31">
         <v>136.18538796035799</v>
       </c>
-      <c r="CT111" s="14">
+      <c r="CT111" s="31">
         <v>139.22329574183948</v>
       </c>
-      <c r="CU111" s="14">
+      <c r="CU111" s="31">
         <v>141.49602065392421</v>
       </c>
-      <c r="CV111" s="8"/>
+      <c r="CV111" s="31">
+        <v>130.1674049222718</v>
+      </c>
       <c r="CW111" s="8"/>
       <c r="CX111" s="8"/>
       <c r="CY111" s="8"/>
@@ -18437,25 +18537,27 @@
       <c r="CO112" s="14">
         <v>114.41806830514707</v>
       </c>
-      <c r="CP112" s="14">
+      <c r="CP112" s="31">
         <v>119.59147290110843</v>
       </c>
-      <c r="CQ112" s="14">
+      <c r="CQ112" s="31">
         <v>119.26852215132922</v>
       </c>
-      <c r="CR112" s="14">
+      <c r="CR112" s="31">
         <v>120.01837611904935</v>
       </c>
-      <c r="CS112" s="14">
+      <c r="CS112" s="31">
         <v>117.82399759332367</v>
       </c>
-      <c r="CT112" s="14">
+      <c r="CT112" s="31">
         <v>122.28374398804517</v>
       </c>
-      <c r="CU112" s="14">
+      <c r="CU112" s="31">
         <v>122.14812952633753</v>
       </c>
-      <c r="CV112" s="8"/>
+      <c r="CV112" s="31">
+        <v>123.34745343524598</v>
+      </c>
       <c r="CW112" s="8"/>
       <c r="CX112" s="8"/>
       <c r="CY112" s="8"/>
@@ -18788,25 +18890,27 @@
       <c r="CO113" s="14">
         <v>117.03672057255258</v>
       </c>
-      <c r="CP113" s="14">
+      <c r="CP113" s="31">
         <v>122.00663809992125</v>
       </c>
-      <c r="CQ113" s="14">
+      <c r="CQ113" s="31">
         <v>122.63218135093956</v>
       </c>
-      <c r="CR113" s="14">
+      <c r="CR113" s="31">
         <v>124.72795126241223</v>
       </c>
-      <c r="CS113" s="14">
+      <c r="CS113" s="31">
         <v>122.09794183971367</v>
       </c>
-      <c r="CT113" s="14">
+      <c r="CT113" s="31">
         <v>126.00770654539204</v>
       </c>
-      <c r="CU113" s="14">
+      <c r="CU113" s="31">
         <v>126.54895671497179</v>
       </c>
-      <c r="CV113" s="8"/>
+      <c r="CV113" s="31">
+        <v>126.19921437655741</v>
+      </c>
       <c r="CW113" s="8"/>
       <c r="CX113" s="8"/>
       <c r="CY113" s="8"/>
@@ -19139,25 +19243,27 @@
       <c r="CO114" s="14">
         <v>115.53683219443604</v>
       </c>
-      <c r="CP114" s="14">
+      <c r="CP114" s="31">
         <v>115.7444035129955</v>
       </c>
-      <c r="CQ114" s="14">
+      <c r="CQ114" s="31">
         <v>116.50252804574835</v>
       </c>
-      <c r="CR114" s="14">
+      <c r="CR114" s="31">
         <v>118.14474888583113</v>
       </c>
-      <c r="CS114" s="14">
+      <c r="CS114" s="31">
         <v>120.40996061596701</v>
       </c>
-      <c r="CT114" s="14">
+      <c r="CT114" s="31">
         <v>119.8434881806138</v>
       </c>
-      <c r="CU114" s="14">
+      <c r="CU114" s="31">
         <v>118.7433197401653</v>
       </c>
-      <c r="CV114" s="8"/>
+      <c r="CV114" s="31">
+        <v>120.98476812528742</v>
+      </c>
       <c r="CW114" s="8"/>
       <c r="CX114" s="8"/>
       <c r="CY114" s="8"/>
@@ -19490,25 +19596,27 @@
       <c r="CO115" s="14">
         <v>103.34897185336216</v>
       </c>
-      <c r="CP115" s="14">
+      <c r="CP115" s="31">
         <v>102.92008743148232</v>
       </c>
-      <c r="CQ115" s="14">
+      <c r="CQ115" s="31">
         <v>103.61706726923939</v>
       </c>
-      <c r="CR115" s="14">
+      <c r="CR115" s="31">
         <v>102.55633330527829</v>
       </c>
-      <c r="CS115" s="14">
+      <c r="CS115" s="31">
         <v>103.68565782484302</v>
       </c>
-      <c r="CT115" s="14">
+      <c r="CT115" s="31">
         <v>103.43700151539213</v>
       </c>
-      <c r="CU115" s="14">
-        <v>104.05566703242958</v>
-      </c>
-      <c r="CV115" s="8"/>
+      <c r="CU115" s="31">
+        <v>104.05567850493365</v>
+      </c>
+      <c r="CV115" s="31">
+        <v>103.25671802053384</v>
+      </c>
       <c r="CW115" s="8"/>
       <c r="CX115" s="8"/>
       <c r="CY115" s="8"/>
@@ -19841,25 +19949,27 @@
       <c r="CO116" s="14">
         <v>117.00435355436905</v>
       </c>
-      <c r="CP116" s="14">
+      <c r="CP116" s="31">
         <v>118.32018478524459</v>
       </c>
-      <c r="CQ116" s="14">
+      <c r="CQ116" s="31">
         <v>118.82915304474481</v>
       </c>
-      <c r="CR116" s="14">
+      <c r="CR116" s="31">
         <v>119.9175022333163</v>
       </c>
-      <c r="CS116" s="14">
+      <c r="CS116" s="31">
         <v>120.3904189202468</v>
       </c>
-      <c r="CT116" s="14">
+      <c r="CT116" s="31">
         <v>120.72507269431662</v>
       </c>
-      <c r="CU116" s="14">
+      <c r="CU116" s="31">
         <v>121.69815233560111</v>
       </c>
-      <c r="CV116" s="8"/>
+      <c r="CV116" s="31">
+        <v>123.24479587494265</v>
+      </c>
       <c r="CW116" s="8"/>
       <c r="CX116" s="8"/>
       <c r="CY116" s="8"/>
@@ -20192,25 +20302,27 @@
       <c r="CO117" s="14">
         <v>117.79146924859019</v>
       </c>
-      <c r="CP117" s="14">
+      <c r="CP117" s="31">
         <v>120.87246097661833</v>
       </c>
-      <c r="CQ117" s="14">
+      <c r="CQ117" s="31">
         <v>119.17508385865622</v>
       </c>
-      <c r="CR117" s="14">
+      <c r="CR117" s="31">
         <v>121.14795441289259</v>
       </c>
-      <c r="CS117" s="14">
+      <c r="CS117" s="31">
         <v>119.74403340048416</v>
       </c>
-      <c r="CT117" s="14">
+      <c r="CT117" s="31">
         <v>123.59356996541166</v>
       </c>
-      <c r="CU117" s="14">
+      <c r="CU117" s="31">
         <v>122.05243526878937</v>
       </c>
-      <c r="CV117" s="8"/>
+      <c r="CV117" s="31">
+        <v>124.50836404332726</v>
+      </c>
       <c r="CW117" s="8"/>
       <c r="CX117" s="8"/>
       <c r="CY117" s="8"/>
@@ -20543,25 +20655,27 @@
       <c r="CO118" s="14">
         <v>114.26976550965544</v>
       </c>
-      <c r="CP118" s="14">
+      <c r="CP118" s="31">
         <v>119.3041020978674</v>
       </c>
-      <c r="CQ118" s="14">
+      <c r="CQ118" s="31">
         <v>118.63400847867109</v>
       </c>
-      <c r="CR118" s="14">
+      <c r="CR118" s="31">
         <v>116.31755657998011</v>
       </c>
-      <c r="CS118" s="14">
+      <c r="CS118" s="31">
         <v>117.67128020805468</v>
       </c>
-      <c r="CT118" s="14">
+      <c r="CT118" s="31">
         <v>121.88348408651571</v>
       </c>
-      <c r="CU118" s="14">
+      <c r="CU118" s="31">
         <v>121.49829621846997</v>
       </c>
-      <c r="CV118" s="8"/>
+      <c r="CV118" s="31">
+        <v>119.54398032947103</v>
+      </c>
       <c r="CW118" s="8"/>
       <c r="CX118" s="8"/>
       <c r="CY118" s="8"/>
@@ -20707,13 +20821,13 @@
       <c r="CM119" s="8"/>
       <c r="CN119" s="8"/>
       <c r="CO119" s="8"/>
-      <c r="CP119" s="8"/>
-      <c r="CQ119" s="8"/>
-      <c r="CR119" s="8"/>
-      <c r="CS119" s="8"/>
-      <c r="CT119" s="8"/>
-      <c r="CU119" s="8"/>
-      <c r="CV119" s="8"/>
+      <c r="CP119" s="26"/>
+      <c r="CQ119" s="26"/>
+      <c r="CR119" s="26"/>
+      <c r="CS119" s="26"/>
+      <c r="CT119" s="26"/>
+      <c r="CU119" s="26"/>
+      <c r="CV119" s="26"/>
       <c r="CW119" s="8"/>
       <c r="CX119" s="8"/>
       <c r="CY119" s="8"/>
@@ -21046,25 +21160,27 @@
       <c r="CO120" s="14">
         <v>116.07303612354485</v>
       </c>
-      <c r="CP120" s="14">
+      <c r="CP120" s="31">
         <v>117.94413080635491</v>
       </c>
-      <c r="CQ120" s="14">
+      <c r="CQ120" s="31">
         <v>117.48037037902188</v>
       </c>
-      <c r="CR120" s="14">
+      <c r="CR120" s="31">
         <v>119.232637937436</v>
       </c>
-      <c r="CS120" s="14">
+      <c r="CS120" s="31">
         <v>119.00264083203311</v>
       </c>
-      <c r="CT120" s="14">
+      <c r="CT120" s="31">
         <v>120.43354904579233</v>
       </c>
-      <c r="CU120" s="14">
-        <v>120.09679029954219</v>
-      </c>
-      <c r="CV120" s="8"/>
+      <c r="CU120" s="31">
+        <v>120.11119001677932</v>
+      </c>
+      <c r="CV120" s="31">
+        <v>121.16677844599657</v>
+      </c>
       <c r="CW120" s="8"/>
       <c r="CX120" s="8"/>
       <c r="CY120" s="8"/>
@@ -21211,12 +21327,13 @@
       <c r="CM121" s="11"/>
       <c r="CN121" s="11"/>
       <c r="CO121" s="11"/>
-      <c r="CP121" s="11"/>
-      <c r="CQ121" s="11"/>
-      <c r="CR121" s="11"/>
-      <c r="CS121" s="11"/>
-      <c r="CT121" s="11"/>
-      <c r="CU121" s="11"/>
+      <c r="CP121" s="28"/>
+      <c r="CQ121" s="28"/>
+      <c r="CR121" s="28"/>
+      <c r="CS121" s="28"/>
+      <c r="CT121" s="28"/>
+      <c r="CU121" s="28"/>
+      <c r="CV121" s="28"/>
     </row>
     <row r="122" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
@@ -21255,132 +21372,132 @@
     </row>
     <row r="133" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A133" s="3"/>
-      <c r="B133" s="26">
+      <c r="B133" s="36">
         <v>2000</v>
       </c>
-      <c r="C133" s="26"/>
-      <c r="D133" s="26"/>
-      <c r="E133" s="26"/>
-      <c r="F133" s="26">
+      <c r="C133" s="36"/>
+      <c r="D133" s="36"/>
+      <c r="E133" s="36"/>
+      <c r="F133" s="36">
         <v>2001</v>
       </c>
-      <c r="G133" s="26"/>
-      <c r="H133" s="26"/>
-      <c r="I133" s="26"/>
-      <c r="J133" s="26">
+      <c r="G133" s="36"/>
+      <c r="H133" s="36"/>
+      <c r="I133" s="36"/>
+      <c r="J133" s="36">
         <v>2002</v>
       </c>
-      <c r="K133" s="26"/>
-      <c r="L133" s="26"/>
-      <c r="M133" s="26"/>
-      <c r="N133" s="26">
+      <c r="K133" s="36"/>
+      <c r="L133" s="36"/>
+      <c r="M133" s="36"/>
+      <c r="N133" s="36">
         <v>2003</v>
       </c>
-      <c r="O133" s="26"/>
-      <c r="P133" s="26"/>
-      <c r="Q133" s="26"/>
-      <c r="R133" s="26">
+      <c r="O133" s="36"/>
+      <c r="P133" s="36"/>
+      <c r="Q133" s="36"/>
+      <c r="R133" s="36">
         <v>2004</v>
       </c>
-      <c r="S133" s="26"/>
-      <c r="T133" s="26"/>
-      <c r="U133" s="26"/>
-      <c r="V133" s="26">
+      <c r="S133" s="36"/>
+      <c r="T133" s="36"/>
+      <c r="U133" s="36"/>
+      <c r="V133" s="36">
         <v>2005</v>
       </c>
-      <c r="W133" s="26"/>
-      <c r="X133" s="26"/>
-      <c r="Y133" s="26"/>
-      <c r="Z133" s="26">
+      <c r="W133" s="36"/>
+      <c r="X133" s="36"/>
+      <c r="Y133" s="36"/>
+      <c r="Z133" s="36">
         <v>2006</v>
       </c>
-      <c r="AA133" s="26"/>
-      <c r="AB133" s="26"/>
-      <c r="AC133" s="26"/>
-      <c r="AD133" s="26">
+      <c r="AA133" s="36"/>
+      <c r="AB133" s="36"/>
+      <c r="AC133" s="36"/>
+      <c r="AD133" s="36">
         <v>2007</v>
       </c>
-      <c r="AE133" s="26"/>
-      <c r="AF133" s="26"/>
-      <c r="AG133" s="26"/>
-      <c r="AH133" s="26">
+      <c r="AE133" s="36"/>
+      <c r="AF133" s="36"/>
+      <c r="AG133" s="36"/>
+      <c r="AH133" s="36">
         <v>2008</v>
       </c>
-      <c r="AI133" s="26"/>
-      <c r="AJ133" s="26"/>
-      <c r="AK133" s="26"/>
-      <c r="AL133" s="26">
+      <c r="AI133" s="36"/>
+      <c r="AJ133" s="36"/>
+      <c r="AK133" s="36"/>
+      <c r="AL133" s="36">
         <v>2009</v>
       </c>
-      <c r="AM133" s="26"/>
-      <c r="AN133" s="26"/>
-      <c r="AO133" s="26"/>
-      <c r="AP133" s="26">
+      <c r="AM133" s="36"/>
+      <c r="AN133" s="36"/>
+      <c r="AO133" s="36"/>
+      <c r="AP133" s="36">
         <v>2010</v>
       </c>
-      <c r="AQ133" s="26"/>
-      <c r="AR133" s="26"/>
-      <c r="AS133" s="26"/>
-      <c r="AT133" s="26">
+      <c r="AQ133" s="36"/>
+      <c r="AR133" s="36"/>
+      <c r="AS133" s="36"/>
+      <c r="AT133" s="36">
         <v>2011</v>
       </c>
-      <c r="AU133" s="26"/>
-      <c r="AV133" s="26"/>
-      <c r="AW133" s="26"/>
-      <c r="AX133" s="26">
+      <c r="AU133" s="36"/>
+      <c r="AV133" s="36"/>
+      <c r="AW133" s="36"/>
+      <c r="AX133" s="36">
         <v>2012</v>
       </c>
-      <c r="AY133" s="26"/>
-      <c r="AZ133" s="26"/>
-      <c r="BA133" s="26"/>
-      <c r="BB133" s="26">
+      <c r="AY133" s="36"/>
+      <c r="AZ133" s="36"/>
+      <c r="BA133" s="36"/>
+      <c r="BB133" s="36">
         <v>2013</v>
       </c>
-      <c r="BC133" s="26"/>
-      <c r="BD133" s="26"/>
-      <c r="BE133" s="26"/>
-      <c r="BF133" s="26">
+      <c r="BC133" s="36"/>
+      <c r="BD133" s="36"/>
+      <c r="BE133" s="36"/>
+      <c r="BF133" s="36">
         <v>2014</v>
       </c>
-      <c r="BG133" s="26"/>
-      <c r="BH133" s="26"/>
-      <c r="BI133" s="26"/>
-      <c r="BJ133" s="26">
+      <c r="BG133" s="36"/>
+      <c r="BH133" s="36"/>
+      <c r="BI133" s="36"/>
+      <c r="BJ133" s="36">
         <v>2015</v>
       </c>
-      <c r="BK133" s="26"/>
-      <c r="BL133" s="26"/>
-      <c r="BM133" s="26"/>
-      <c r="BN133" s="26">
+      <c r="BK133" s="36"/>
+      <c r="BL133" s="36"/>
+      <c r="BM133" s="36"/>
+      <c r="BN133" s="36">
         <v>2016</v>
       </c>
-      <c r="BO133" s="26"/>
-      <c r="BP133" s="26"/>
-      <c r="BQ133" s="26"/>
-      <c r="BR133" s="26">
+      <c r="BO133" s="36"/>
+      <c r="BP133" s="36"/>
+      <c r="BQ133" s="36"/>
+      <c r="BR133" s="36">
         <v>2017</v>
       </c>
-      <c r="BS133" s="26"/>
-      <c r="BT133" s="26"/>
-      <c r="BU133" s="26"/>
-      <c r="BV133" s="26">
+      <c r="BS133" s="36"/>
+      <c r="BT133" s="36"/>
+      <c r="BU133" s="36"/>
+      <c r="BV133" s="36">
         <v>2018</v>
       </c>
-      <c r="BW133" s="26"/>
-      <c r="BX133" s="26"/>
-      <c r="BY133" s="26"/>
-      <c r="BZ133" s="26">
+      <c r="BW133" s="36"/>
+      <c r="BX133" s="36"/>
+      <c r="BY133" s="36"/>
+      <c r="BZ133" s="36">
         <v>2019</v>
       </c>
-      <c r="CA133" s="26"/>
-      <c r="CB133" s="26"/>
-      <c r="CC133" s="26"/>
-      <c r="CD133" s="25">
+      <c r="CA133" s="36"/>
+      <c r="CB133" s="36"/>
+      <c r="CC133" s="36"/>
+      <c r="CD133" s="35">
         <v>2020</v>
       </c>
-      <c r="CE133" s="25"/>
-      <c r="CF133" s="25"/>
-      <c r="CG133" s="25"/>
+      <c r="CE133" s="35"/>
+      <c r="CF133" s="35"/>
+      <c r="CG133" s="35"/>
       <c r="CH133" s="21">
         <v>2021</v>
       </c>
@@ -21393,16 +21510,17 @@
       <c r="CM133" s="21"/>
       <c r="CN133" s="21"/>
       <c r="CO133" s="21"/>
-      <c r="CP133" s="21">
+      <c r="CP133" s="24">
         <v>2023</v>
       </c>
-      <c r="CQ133" s="21"/>
-      <c r="CR133" s="21"/>
-      <c r="CS133" s="21"/>
-      <c r="CT133" s="21">
+      <c r="CQ133" s="24"/>
+      <c r="CR133" s="24"/>
+      <c r="CS133" s="24"/>
+      <c r="CT133" s="24">
         <v>2024</v>
       </c>
-      <c r="CU133" s="21"/>
+      <c r="CU133" s="24"/>
+      <c r="CV133" s="24"/>
     </row>
     <row r="134" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
@@ -21682,23 +21800,26 @@
       <c r="CO134" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP134" s="13" t="s">
+      <c r="CP134" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CQ134" s="13" t="s">
+      <c r="CQ134" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="CR134" s="13" t="s">
+      <c r="CR134" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="CS134" s="13" t="s">
+      <c r="CS134" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="CT134" s="13" t="s">
+      <c r="CT134" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CU134" s="13" t="s">
+      <c r="CU134" s="29" t="s">
         <v>8</v>
+      </c>
+      <c r="CV134" s="29" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -21984,25 +22105,27 @@
       <c r="CO136" s="20">
         <v>8.7827302543622761</v>
       </c>
-      <c r="CP136" s="20">
+      <c r="CP136" s="34">
         <v>10.423788448805297</v>
       </c>
-      <c r="CQ136" s="20">
+      <c r="CQ136" s="34">
         <v>4.1182304678552075</v>
       </c>
-      <c r="CR136" s="20">
+      <c r="CR136" s="34">
         <v>7.0676659503017865</v>
       </c>
-      <c r="CS136" s="20">
+      <c r="CS136" s="34">
         <v>8.5825179703148056</v>
       </c>
-      <c r="CT136" s="20">
+      <c r="CT136" s="34">
         <v>10.511899449352228</v>
       </c>
-      <c r="CU136" s="20">
-        <v>4.1284208554563735</v>
-      </c>
-      <c r="CV136" s="8"/>
+      <c r="CU136" s="34">
+        <v>4.1343963912176829</v>
+      </c>
+      <c r="CV136" s="34">
+        <v>6.5959613313255412</v>
+      </c>
       <c r="CW136" s="8"/>
       <c r="CX136" s="8"/>
       <c r="CY136" s="8"/>
@@ -22335,25 +22458,27 @@
       <c r="CO137" s="20">
         <v>0.16108702810670397</v>
       </c>
-      <c r="CP137" s="20">
+      <c r="CP137" s="34">
         <v>5.4753624936512799E-2</v>
       </c>
-      <c r="CQ137" s="20">
+      <c r="CQ137" s="34">
         <v>5.5436820494742294E-2</v>
       </c>
-      <c r="CR137" s="20">
+      <c r="CR137" s="34">
         <v>0.12684227721550209</v>
       </c>
-      <c r="CS137" s="20">
+      <c r="CS137" s="34">
         <v>0.13176515537394626</v>
       </c>
-      <c r="CT137" s="20">
+      <c r="CT137" s="34">
         <v>5.4699755931179699E-2</v>
       </c>
-      <c r="CU137" s="20">
-        <v>5.6246886994848304E-2</v>
-      </c>
-      <c r="CV137" s="8"/>
+      <c r="CU137" s="34">
+        <v>5.2967468300429033E-2</v>
+      </c>
+      <c r="CV137" s="34">
+        <v>0.13140495165576269</v>
+      </c>
       <c r="CW137" s="8"/>
       <c r="CX137" s="8"/>
       <c r="CY137" s="8"/>
@@ -22686,25 +22811,27 @@
       <c r="CO138" s="20">
         <v>10.337774260791397</v>
       </c>
-      <c r="CP138" s="20">
+      <c r="CP138" s="34">
         <v>14.605360688296587</v>
       </c>
-      <c r="CQ138" s="20">
+      <c r="CQ138" s="34">
         <v>15.808579397825692</v>
       </c>
-      <c r="CR138" s="20">
+      <c r="CR138" s="34">
         <v>23.795656408870862</v>
       </c>
-      <c r="CS138" s="20">
+      <c r="CS138" s="34">
         <v>15.022013741043057</v>
       </c>
-      <c r="CT138" s="20">
+      <c r="CT138" s="34">
         <v>15.499872055049821</v>
       </c>
-      <c r="CU138" s="20">
-        <v>18.113373570110884</v>
-      </c>
-      <c r="CV138" s="8"/>
+      <c r="CU138" s="34">
+        <v>18.090026315485666</v>
+      </c>
+      <c r="CV138" s="34">
+        <v>19.4497844367122</v>
+      </c>
       <c r="CW138" s="8"/>
       <c r="CX138" s="8"/>
       <c r="CY138" s="8"/>
@@ -23037,25 +23164,27 @@
       <c r="CO139" s="20">
         <v>0.73988259333163631</v>
       </c>
-      <c r="CP139" s="20">
+      <c r="CP139" s="34">
         <v>0.52127711364677609</v>
       </c>
-      <c r="CQ139" s="20">
+      <c r="CQ139" s="34">
         <v>0.6139269747570516</v>
       </c>
-      <c r="CR139" s="20">
+      <c r="CR139" s="34">
         <v>0.72287239904319722</v>
       </c>
-      <c r="CS139" s="20">
+      <c r="CS139" s="34">
         <v>0.7680504103126351</v>
       </c>
-      <c r="CT139" s="20">
+      <c r="CT139" s="34">
         <v>0.50953856776760176</v>
       </c>
-      <c r="CU139" s="20">
-        <v>0.58347303284311358</v>
-      </c>
-      <c r="CV139" s="8"/>
+      <c r="CU139" s="34">
+        <v>0.58566289259209281</v>
+      </c>
+      <c r="CV139" s="34">
+        <v>0.7243687945879379</v>
+      </c>
       <c r="CW139" s="8"/>
       <c r="CX139" s="8"/>
       <c r="CY139" s="8"/>
@@ -23388,25 +23517,27 @@
       <c r="CO140" s="20">
         <v>14.225701187072531</v>
       </c>
-      <c r="CP140" s="20">
+      <c r="CP140" s="34">
         <v>15.541367844351198</v>
       </c>
-      <c r="CQ140" s="20">
+      <c r="CQ140" s="34">
         <v>15.7698382907679</v>
       </c>
-      <c r="CR140" s="20">
+      <c r="CR140" s="34">
         <v>12.380763502046364</v>
       </c>
-      <c r="CS140" s="20">
+      <c r="CS140" s="34">
         <v>14.114051238263833</v>
       </c>
-      <c r="CT140" s="20">
+      <c r="CT140" s="34">
         <v>14.783460420958672</v>
       </c>
-      <c r="CU140" s="20">
-        <v>15.421129945001558</v>
-      </c>
-      <c r="CV140" s="8"/>
+      <c r="CU140" s="34">
+        <v>15.352013614110987</v>
+      </c>
+      <c r="CV140" s="34">
+        <v>13.229080887869207</v>
+      </c>
       <c r="CW140" s="8"/>
       <c r="CX140" s="8"/>
       <c r="CY140" s="8"/>
@@ -23739,25 +23870,27 @@
       <c r="CO141" s="20">
         <v>53.234884723567731</v>
       </c>
-      <c r="CP141" s="20">
+      <c r="CP141" s="34">
         <v>50.065600760877572</v>
       </c>
-      <c r="CQ141" s="20">
+      <c r="CQ141" s="34">
         <v>52.840947826538496</v>
       </c>
-      <c r="CR141" s="20">
+      <c r="CR141" s="34">
         <v>45.6499491973509</v>
       </c>
-      <c r="CS141" s="20">
+      <c r="CS141" s="34">
         <v>49.55862943674714</v>
       </c>
-      <c r="CT141" s="20">
+      <c r="CT141" s="34">
         <v>50.10118085447165</v>
       </c>
-      <c r="CU141" s="20">
-        <v>51.107292357202574</v>
-      </c>
-      <c r="CV141" s="8"/>
+      <c r="CU141" s="34">
+        <v>50.782343847351029</v>
+      </c>
+      <c r="CV141" s="34">
+        <v>49.316652887902791</v>
+      </c>
       <c r="CW141" s="8"/>
       <c r="CX141" s="8"/>
       <c r="CY141" s="8"/>
@@ -24090,25 +24223,27 @@
       <c r="CO142" s="20">
         <v>10.742804778856668</v>
       </c>
-      <c r="CP142" s="20">
+      <c r="CP142" s="34">
         <v>7.8201288003847322</v>
       </c>
-      <c r="CQ142" s="20">
+      <c r="CQ142" s="34">
         <v>9.4570199276183633</v>
       </c>
-      <c r="CR142" s="20">
+      <c r="CR142" s="34">
         <v>8.992355665061643</v>
       </c>
-      <c r="CS142" s="20">
+      <c r="CS142" s="34">
         <v>10.061766542551789</v>
       </c>
-      <c r="CT142" s="20">
+      <c r="CT142" s="34">
         <v>7.6024569149773722</v>
       </c>
-      <c r="CU142" s="20">
-        <v>9.0191833477341952</v>
-      </c>
-      <c r="CV142" s="8"/>
+      <c r="CU142" s="34">
+        <v>9.2900838205162337</v>
+      </c>
+      <c r="CV142" s="34">
+        <v>9.2400216121295724</v>
+      </c>
       <c r="CW142" s="8"/>
       <c r="CX142" s="8"/>
       <c r="CY142" s="8"/>
@@ -24441,25 +24576,27 @@
       <c r="CO143" s="20">
         <v>1.7751351739110399</v>
       </c>
-      <c r="CP143" s="20">
+      <c r="CP143" s="34">
         <v>0.96772271870133808</v>
       </c>
-      <c r="CQ143" s="20">
+      <c r="CQ143" s="34">
         <v>1.336020294142531</v>
       </c>
-      <c r="CR143" s="20">
+      <c r="CR143" s="34">
         <v>1.2638946001097586</v>
       </c>
-      <c r="CS143" s="20">
+      <c r="CS143" s="34">
         <v>1.7612055053927922</v>
       </c>
-      <c r="CT143" s="20">
+      <c r="CT143" s="34">
         <v>0.93689198149148001</v>
       </c>
-      <c r="CU143" s="20">
-        <v>1.5708800046564511</v>
-      </c>
-      <c r="CV143" s="8"/>
+      <c r="CU143" s="34">
+        <v>1.7125056504258769</v>
+      </c>
+      <c r="CV143" s="34">
+        <v>1.3127250978169975</v>
+      </c>
       <c r="CW143" s="8"/>
       <c r="CX143" s="8"/>
       <c r="CY143" s="8"/>
@@ -24605,13 +24742,13 @@
       <c r="CM144" s="8"/>
       <c r="CN144" s="8"/>
       <c r="CO144" s="8"/>
-      <c r="CP144" s="8"/>
-      <c r="CQ144" s="8"/>
-      <c r="CR144" s="8"/>
-      <c r="CS144" s="8"/>
-      <c r="CT144" s="8"/>
-      <c r="CU144" s="8"/>
-      <c r="CV144" s="8"/>
+      <c r="CP144" s="26"/>
+      <c r="CQ144" s="26"/>
+      <c r="CR144" s="26"/>
+      <c r="CS144" s="26"/>
+      <c r="CT144" s="26"/>
+      <c r="CU144" s="26"/>
+      <c r="CV144" s="26"/>
       <c r="CW144" s="8"/>
       <c r="CX144" s="8"/>
       <c r="CY144" s="8"/>
@@ -24944,25 +25081,27 @@
       <c r="CO145" s="14">
         <v>100</v>
       </c>
-      <c r="CP145" s="14">
+      <c r="CP145" s="31">
         <v>100</v>
       </c>
-      <c r="CQ145" s="14">
+      <c r="CQ145" s="31">
         <v>100</v>
       </c>
-      <c r="CR145" s="14">
+      <c r="CR145" s="31">
         <v>100</v>
       </c>
-      <c r="CS145" s="14">
+      <c r="CS145" s="31">
         <v>100</v>
       </c>
-      <c r="CT145" s="14">
+      <c r="CT145" s="31">
         <v>100</v>
       </c>
-      <c r="CU145" s="14">
+      <c r="CU145" s="31">
         <v>100</v>
       </c>
-      <c r="CV145" s="8"/>
+      <c r="CV145" s="31">
+        <v>100</v>
+      </c>
       <c r="CW145" s="8"/>
       <c r="CX145" s="8"/>
       <c r="CY145" s="8"/>
@@ -25109,12 +25248,13 @@
       <c r="CM146" s="11"/>
       <c r="CN146" s="11"/>
       <c r="CO146" s="11"/>
-      <c r="CP146" s="11"/>
-      <c r="CQ146" s="11"/>
-      <c r="CR146" s="11"/>
-      <c r="CS146" s="11"/>
-      <c r="CT146" s="11"/>
-      <c r="CU146" s="11"/>
+      <c r="CP146" s="28"/>
+      <c r="CQ146" s="28"/>
+      <c r="CR146" s="28"/>
+      <c r="CS146" s="28"/>
+      <c r="CT146" s="28"/>
+      <c r="CU146" s="28"/>
+      <c r="CV146" s="28"/>
     </row>
     <row r="147" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="s">
@@ -25214,13 +25354,13 @@
       <c r="CM148" s="8"/>
       <c r="CN148" s="8"/>
       <c r="CO148" s="8"/>
-      <c r="CP148" s="8"/>
-      <c r="CQ148" s="8"/>
-      <c r="CR148" s="8"/>
-      <c r="CS148" s="8"/>
-      <c r="CT148" s="8"/>
-      <c r="CU148" s="8"/>
-      <c r="CV148" s="8"/>
+      <c r="CP148" s="26"/>
+      <c r="CQ148" s="26"/>
+      <c r="CR148" s="26"/>
+      <c r="CS148" s="26"/>
+      <c r="CT148" s="26"/>
+      <c r="CU148" s="26"/>
+      <c r="CV148" s="26"/>
       <c r="CW148" s="8"/>
       <c r="CX148" s="8"/>
       <c r="CY148" s="8"/>
@@ -25366,13 +25506,13 @@
       <c r="CM149" s="8"/>
       <c r="CN149" s="8"/>
       <c r="CO149" s="8"/>
-      <c r="CP149" s="8"/>
-      <c r="CQ149" s="8"/>
-      <c r="CR149" s="8"/>
-      <c r="CS149" s="8"/>
-      <c r="CT149" s="8"/>
-      <c r="CU149" s="8"/>
-      <c r="CV149" s="8"/>
+      <c r="CP149" s="26"/>
+      <c r="CQ149" s="26"/>
+      <c r="CR149" s="26"/>
+      <c r="CS149" s="26"/>
+      <c r="CT149" s="26"/>
+      <c r="CU149" s="26"/>
+      <c r="CV149" s="26"/>
       <c r="CW149" s="8"/>
       <c r="CX149" s="8"/>
       <c r="CY149" s="8"/>
@@ -25457,132 +25597,132 @@
     </row>
     <row r="158" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
-      <c r="B158" s="26">
+      <c r="B158" s="36">
         <v>2000</v>
       </c>
-      <c r="C158" s="26"/>
-      <c r="D158" s="26"/>
-      <c r="E158" s="26"/>
-      <c r="F158" s="26">
+      <c r="C158" s="36"/>
+      <c r="D158" s="36"/>
+      <c r="E158" s="36"/>
+      <c r="F158" s="36">
         <v>2001</v>
       </c>
-      <c r="G158" s="26"/>
-      <c r="H158" s="26"/>
-      <c r="I158" s="26"/>
-      <c r="J158" s="26">
+      <c r="G158" s="36"/>
+      <c r="H158" s="36"/>
+      <c r="I158" s="36"/>
+      <c r="J158" s="36">
         <v>2002</v>
       </c>
-      <c r="K158" s="26"/>
-      <c r="L158" s="26"/>
-      <c r="M158" s="26"/>
-      <c r="N158" s="26">
+      <c r="K158" s="36"/>
+      <c r="L158" s="36"/>
+      <c r="M158" s="36"/>
+      <c r="N158" s="36">
         <v>2003</v>
       </c>
-      <c r="O158" s="26"/>
-      <c r="P158" s="26"/>
-      <c r="Q158" s="26"/>
-      <c r="R158" s="26">
+      <c r="O158" s="36"/>
+      <c r="P158" s="36"/>
+      <c r="Q158" s="36"/>
+      <c r="R158" s="36">
         <v>2004</v>
       </c>
-      <c r="S158" s="26"/>
-      <c r="T158" s="26"/>
-      <c r="U158" s="26"/>
-      <c r="V158" s="26">
+      <c r="S158" s="36"/>
+      <c r="T158" s="36"/>
+      <c r="U158" s="36"/>
+      <c r="V158" s="36">
         <v>2005</v>
       </c>
-      <c r="W158" s="26"/>
-      <c r="X158" s="26"/>
-      <c r="Y158" s="26"/>
-      <c r="Z158" s="26">
+      <c r="W158" s="36"/>
+      <c r="X158" s="36"/>
+      <c r="Y158" s="36"/>
+      <c r="Z158" s="36">
         <v>2006</v>
       </c>
-      <c r="AA158" s="26"/>
-      <c r="AB158" s="26"/>
-      <c r="AC158" s="26"/>
-      <c r="AD158" s="26">
+      <c r="AA158" s="36"/>
+      <c r="AB158" s="36"/>
+      <c r="AC158" s="36"/>
+      <c r="AD158" s="36">
         <v>2007</v>
       </c>
-      <c r="AE158" s="26"/>
-      <c r="AF158" s="26"/>
-      <c r="AG158" s="26"/>
-      <c r="AH158" s="26">
+      <c r="AE158" s="36"/>
+      <c r="AF158" s="36"/>
+      <c r="AG158" s="36"/>
+      <c r="AH158" s="36">
         <v>2008</v>
       </c>
-      <c r="AI158" s="26"/>
-      <c r="AJ158" s="26"/>
-      <c r="AK158" s="26"/>
-      <c r="AL158" s="26">
+      <c r="AI158" s="36"/>
+      <c r="AJ158" s="36"/>
+      <c r="AK158" s="36"/>
+      <c r="AL158" s="36">
         <v>2009</v>
       </c>
-      <c r="AM158" s="26"/>
-      <c r="AN158" s="26"/>
-      <c r="AO158" s="26"/>
-      <c r="AP158" s="26">
+      <c r="AM158" s="36"/>
+      <c r="AN158" s="36"/>
+      <c r="AO158" s="36"/>
+      <c r="AP158" s="36">
         <v>2010</v>
       </c>
-      <c r="AQ158" s="26"/>
-      <c r="AR158" s="26"/>
-      <c r="AS158" s="26"/>
-      <c r="AT158" s="26">
+      <c r="AQ158" s="36"/>
+      <c r="AR158" s="36"/>
+      <c r="AS158" s="36"/>
+      <c r="AT158" s="36">
         <v>2011</v>
       </c>
-      <c r="AU158" s="26"/>
-      <c r="AV158" s="26"/>
-      <c r="AW158" s="26"/>
-      <c r="AX158" s="26">
+      <c r="AU158" s="36"/>
+      <c r="AV158" s="36"/>
+      <c r="AW158" s="36"/>
+      <c r="AX158" s="36">
         <v>2012</v>
       </c>
-      <c r="AY158" s="26"/>
-      <c r="AZ158" s="26"/>
-      <c r="BA158" s="26"/>
-      <c r="BB158" s="26">
+      <c r="AY158" s="36"/>
+      <c r="AZ158" s="36"/>
+      <c r="BA158" s="36"/>
+      <c r="BB158" s="36">
         <v>2013</v>
       </c>
-      <c r="BC158" s="26"/>
-      <c r="BD158" s="26"/>
-      <c r="BE158" s="26"/>
-      <c r="BF158" s="26">
+      <c r="BC158" s="36"/>
+      <c r="BD158" s="36"/>
+      <c r="BE158" s="36"/>
+      <c r="BF158" s="36">
         <v>2014</v>
       </c>
-      <c r="BG158" s="26"/>
-      <c r="BH158" s="26"/>
-      <c r="BI158" s="26"/>
-      <c r="BJ158" s="26">
+      <c r="BG158" s="36"/>
+      <c r="BH158" s="36"/>
+      <c r="BI158" s="36"/>
+      <c r="BJ158" s="36">
         <v>2015</v>
       </c>
-      <c r="BK158" s="26"/>
-      <c r="BL158" s="26"/>
-      <c r="BM158" s="26"/>
-      <c r="BN158" s="26">
+      <c r="BK158" s="36"/>
+      <c r="BL158" s="36"/>
+      <c r="BM158" s="36"/>
+      <c r="BN158" s="36">
         <v>2016</v>
       </c>
-      <c r="BO158" s="26"/>
-      <c r="BP158" s="26"/>
-      <c r="BQ158" s="26"/>
-      <c r="BR158" s="26">
+      <c r="BO158" s="36"/>
+      <c r="BP158" s="36"/>
+      <c r="BQ158" s="36"/>
+      <c r="BR158" s="36">
         <v>2017</v>
       </c>
-      <c r="BS158" s="26"/>
-      <c r="BT158" s="26"/>
-      <c r="BU158" s="26"/>
-      <c r="BV158" s="26">
+      <c r="BS158" s="36"/>
+      <c r="BT158" s="36"/>
+      <c r="BU158" s="36"/>
+      <c r="BV158" s="36">
         <v>2018</v>
       </c>
-      <c r="BW158" s="26"/>
-      <c r="BX158" s="26"/>
-      <c r="BY158" s="26"/>
-      <c r="BZ158" s="26">
+      <c r="BW158" s="36"/>
+      <c r="BX158" s="36"/>
+      <c r="BY158" s="36"/>
+      <c r="BZ158" s="36">
         <v>2019</v>
       </c>
-      <c r="CA158" s="26"/>
-      <c r="CB158" s="26"/>
-      <c r="CC158" s="26"/>
-      <c r="CD158" s="25">
+      <c r="CA158" s="36"/>
+      <c r="CB158" s="36"/>
+      <c r="CC158" s="36"/>
+      <c r="CD158" s="35">
         <v>2020</v>
       </c>
-      <c r="CE158" s="25"/>
-      <c r="CF158" s="25"/>
-      <c r="CG158" s="25"/>
+      <c r="CE158" s="35"/>
+      <c r="CF158" s="35"/>
+      <c r="CG158" s="35"/>
       <c r="CH158" s="21">
         <v>2021</v>
       </c>
@@ -25595,16 +25735,17 @@
       <c r="CM158" s="21"/>
       <c r="CN158" s="21"/>
       <c r="CO158" s="21"/>
-      <c r="CP158" s="21">
+      <c r="CP158" s="24">
         <v>2023</v>
       </c>
-      <c r="CQ158" s="21"/>
-      <c r="CR158" s="21"/>
-      <c r="CS158" s="21"/>
-      <c r="CT158" s="21">
+      <c r="CQ158" s="24"/>
+      <c r="CR158" s="24"/>
+      <c r="CS158" s="24"/>
+      <c r="CT158" s="24">
         <v>2024</v>
       </c>
-      <c r="CU158" s="21"/>
+      <c r="CU158" s="24"/>
+      <c r="CV158" s="24"/>
     </row>
     <row r="159" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A159" s="4"/>
@@ -25884,23 +26025,26 @@
       <c r="CO159" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="CP159" s="13" t="s">
+      <c r="CP159" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CQ159" s="13" t="s">
+      <c r="CQ159" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="CR159" s="13" t="s">
+      <c r="CR159" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="CS159" s="13" t="s">
+      <c r="CS159" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="CT159" s="13" t="s">
+      <c r="CT159" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="CU159" s="13" t="s">
+      <c r="CU159" s="29" t="s">
         <v>8</v>
+      </c>
+      <c r="CV159" s="29" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -26186,25 +26330,27 @@
       <c r="CO161" s="20">
         <v>7.6630996965324938</v>
       </c>
-      <c r="CP161" s="20">
+      <c r="CP161" s="34">
         <v>8.9918714163940461</v>
       </c>
-      <c r="CQ161" s="20">
+      <c r="CQ161" s="34">
         <v>3.4153784663458158</v>
       </c>
-      <c r="CR161" s="20">
+      <c r="CR161" s="34">
         <v>6.4682529948945442</v>
       </c>
-      <c r="CS161" s="20">
+      <c r="CS161" s="34">
         <v>7.4996467591159188</v>
       </c>
-      <c r="CT161" s="20">
+      <c r="CT161" s="34">
         <v>9.0932006109487933</v>
       </c>
-      <c r="CU161" s="20">
-        <v>3.5040568028317205</v>
-      </c>
-      <c r="CV161" s="8"/>
+      <c r="CU161" s="34">
+        <v>3.5095493728746185</v>
+      </c>
+      <c r="CV161" s="34">
+        <v>6.1398733864927513</v>
+      </c>
       <c r="CW161" s="8"/>
       <c r="CX161" s="8"/>
       <c r="CY161" s="8"/>
@@ -26537,25 +26683,27 @@
       <c r="CO162" s="20">
         <v>0.16341702590711205</v>
       </c>
-      <c r="CP162" s="20">
+      <c r="CP162" s="34">
         <v>5.3999407691669186E-2</v>
       </c>
-      <c r="CQ162" s="20">
+      <c r="CQ162" s="34">
         <v>5.4605675385951721E-2</v>
       </c>
-      <c r="CR162" s="20">
+      <c r="CR162" s="34">
         <v>0.12601186421147886</v>
       </c>
-      <c r="CS162" s="20">
+      <c r="CS162" s="34">
         <v>0.13308325790527478</v>
       </c>
-      <c r="CT162" s="20">
+      <c r="CT162" s="34">
         <v>5.3872129883221702E-2</v>
       </c>
-      <c r="CU162" s="20">
-        <v>5.5302284354389719E-2</v>
-      </c>
-      <c r="CV162" s="8"/>
+      <c r="CU162" s="34">
+        <v>5.2084183969176523E-2</v>
+      </c>
+      <c r="CV162" s="34">
+        <v>0.12908182715210453</v>
+      </c>
       <c r="CW162" s="8"/>
       <c r="CX162" s="8"/>
       <c r="CY162" s="8"/>
@@ -26888,25 +27036,27 @@
       <c r="CO163" s="20">
         <v>10.252652666100939</v>
       </c>
-      <c r="CP163" s="20">
+      <c r="CP163" s="34">
         <v>14.119039736867878</v>
       </c>
-      <c r="CQ163" s="20">
+      <c r="CQ163" s="34">
         <v>15.144456718974508</v>
       </c>
-      <c r="CR163" s="20">
+      <c r="CR163" s="34">
         <v>22.747257983203529</v>
       </c>
-      <c r="CS163" s="20">
+      <c r="CS163" s="34">
         <v>14.64119115247656</v>
       </c>
-      <c r="CT163" s="20">
+      <c r="CT163" s="34">
         <v>14.814209801310064</v>
       </c>
-      <c r="CU163" s="20">
-        <v>17.189853505995075</v>
-      </c>
-      <c r="CV163" s="8"/>
+      <c r="CU163" s="34">
+        <v>17.169755046512964</v>
+      </c>
+      <c r="CV163" s="34">
+        <v>18.674186945677775</v>
+      </c>
       <c r="CW163" s="8"/>
       <c r="CX163" s="8"/>
       <c r="CY163" s="8"/>
@@ -27239,25 +27389,27 @@
       <c r="CO164" s="20">
         <v>0.74331637237930814</v>
       </c>
-      <c r="CP164" s="20">
+      <c r="CP164" s="34">
         <v>0.53118400728041659</v>
       </c>
-      <c r="CQ164" s="20">
+      <c r="CQ164" s="34">
         <v>0.61907985680627431</v>
       </c>
-      <c r="CR164" s="20">
+      <c r="CR164" s="34">
         <v>0.72952868276331728</v>
       </c>
-      <c r="CS164" s="20">
+      <c r="CS164" s="34">
         <v>0.75907364018529599</v>
       </c>
-      <c r="CT164" s="20">
+      <c r="CT164" s="34">
         <v>0.51204732959273869</v>
       </c>
-      <c r="CU164" s="20">
-        <v>0.59012362652595463</v>
-      </c>
-      <c r="CV164" s="8"/>
+      <c r="CU164" s="34">
+        <v>0.59240946885967161</v>
+      </c>
+      <c r="CV164" s="34">
+        <v>0.72545854000513044</v>
+      </c>
       <c r="CW164" s="8"/>
       <c r="CX164" s="8"/>
       <c r="CY164" s="8"/>
@@ -27590,25 +27742,27 @@
       <c r="CO165" s="20">
         <v>15.977133571417401</v>
       </c>
-      <c r="CP165" s="20">
+      <c r="CP165" s="34">
         <v>17.810061842049443</v>
       </c>
-      <c r="CQ165" s="20">
+      <c r="CQ165" s="34">
         <v>17.879742131696933</v>
       </c>
-      <c r="CR165" s="20">
+      <c r="CR165" s="34">
         <v>14.393953493192416</v>
       </c>
-      <c r="CS165" s="20">
+      <c r="CS165" s="34">
         <v>16.199052071689611</v>
       </c>
-      <c r="CT165" s="20">
+      <c r="CT165" s="34">
         <v>17.212647114573571</v>
       </c>
-      <c r="CU165" s="20">
-        <v>17.79843675990897</v>
-      </c>
-      <c r="CV165" s="8"/>
+      <c r="CU165" s="34">
+        <v>17.720788051535695</v>
+      </c>
+      <c r="CV165" s="34">
+        <v>15.523688373146383</v>
+      </c>
       <c r="CW165" s="8"/>
       <c r="CX165" s="8"/>
       <c r="CY165" s="8"/>
@@ -27941,25 +28095,27 @@
       <c r="CO166" s="20">
         <v>52.81115197717947</v>
       </c>
-      <c r="CP166" s="20">
+      <c r="CP166" s="34">
         <v>49.906478558644686</v>
       </c>
-      <c r="CQ166" s="20">
+      <c r="CQ166" s="34">
         <v>52.241171150170473</v>
       </c>
-      <c r="CR166" s="20">
+      <c r="CR166" s="34">
         <v>45.389236459579003</v>
       </c>
-      <c r="CS166" s="20">
+      <c r="CS166" s="34">
         <v>48.987351583982289</v>
       </c>
-      <c r="CT166" s="20">
+      <c r="CT166" s="34">
         <v>49.980197874614156</v>
       </c>
-      <c r="CU166" s="20">
-        <v>50.434798353177776</v>
-      </c>
-      <c r="CV166" s="8"/>
+      <c r="CU166" s="34">
+        <v>50.12013440044867</v>
+      </c>
+      <c r="CV166" s="34">
+        <v>48.485130035267822</v>
+      </c>
       <c r="CW166" s="8"/>
       <c r="CX166" s="8"/>
       <c r="CY166" s="8"/>
@@ -28292,25 +28448,27 @@
       <c r="CO167" s="20">
         <v>10.586080427716073</v>
       </c>
-      <c r="CP167" s="20">
+      <c r="CP167" s="34">
         <v>7.6306735769493264</v>
       </c>
-      <c r="CQ167" s="20">
+      <c r="CQ167" s="34">
         <v>9.3225376295608804</v>
       </c>
-      <c r="CR167" s="20">
+      <c r="CR167" s="34">
         <v>8.850188947993038</v>
       </c>
-      <c r="CS167" s="20">
+      <c r="CS167" s="34">
         <v>9.9994693346801604</v>
       </c>
-      <c r="CT167" s="20">
+      <c r="CT167" s="34">
         <v>7.4080784946553733</v>
       </c>
-      <c r="CU167" s="20">
-        <v>8.874669061707289</v>
-      </c>
-      <c r="CV167" s="8"/>
+      <c r="CU167" s="34">
+        <v>9.1423249407557705</v>
+      </c>
+      <c r="CV167" s="34">
+        <v>8.9920356766034111</v>
+      </c>
       <c r="CW167" s="8"/>
       <c r="CX167" s="8"/>
       <c r="CY167" s="8"/>
@@ -28643,25 +28801,27 @@
       <c r="CO168" s="20">
         <v>1.8031482627672057</v>
       </c>
-      <c r="CP168" s="20">
+      <c r="CP168" s="34">
         <v>0.95669145412253398</v>
       </c>
-      <c r="CQ168" s="20">
+      <c r="CQ168" s="34">
         <v>1.3230283710591559</v>
       </c>
-      <c r="CR168" s="20">
+      <c r="CR168" s="34">
         <v>1.2955695741626716</v>
       </c>
-      <c r="CS168" s="20">
+      <c r="CS168" s="34">
         <v>1.7811321999648935</v>
       </c>
-      <c r="CT168" s="20">
+      <c r="CT168" s="34">
         <v>0.92574664442207877</v>
       </c>
-      <c r="CU168" s="20">
-        <v>1.5527596054988155</v>
-      </c>
-      <c r="CV168" s="8"/>
+      <c r="CU168" s="34">
+        <v>1.6929545350434463</v>
+      </c>
+      <c r="CV168" s="34">
+        <v>1.3305452156546504</v>
+      </c>
       <c r="CW168" s="8"/>
       <c r="CX168" s="8"/>
       <c r="CY168" s="8"/>
@@ -28807,13 +28967,13 @@
       <c r="CM169" s="8"/>
       <c r="CN169" s="8"/>
       <c r="CO169" s="8"/>
-      <c r="CP169" s="8"/>
-      <c r="CQ169" s="8"/>
-      <c r="CR169" s="8"/>
-      <c r="CS169" s="8"/>
-      <c r="CT169" s="8"/>
-      <c r="CU169" s="8"/>
-      <c r="CV169" s="8"/>
+      <c r="CP169" s="26"/>
+      <c r="CQ169" s="26"/>
+      <c r="CR169" s="26"/>
+      <c r="CS169" s="26"/>
+      <c r="CT169" s="26"/>
+      <c r="CU169" s="26"/>
+      <c r="CV169" s="26"/>
       <c r="CW169" s="8"/>
       <c r="CX169" s="8"/>
       <c r="CY169" s="8"/>
@@ -29146,25 +29306,27 @@
       <c r="CO170" s="14">
         <v>100</v>
       </c>
-      <c r="CP170" s="14">
+      <c r="CP170" s="31">
         <v>100</v>
       </c>
-      <c r="CQ170" s="14">
+      <c r="CQ170" s="31">
         <v>100</v>
       </c>
-      <c r="CR170" s="14">
+      <c r="CR170" s="31">
         <v>100</v>
       </c>
-      <c r="CS170" s="14">
+      <c r="CS170" s="31">
         <v>100</v>
       </c>
-      <c r="CT170" s="14">
+      <c r="CT170" s="31">
         <v>100</v>
       </c>
-      <c r="CU170" s="14">
+      <c r="CU170" s="31">
         <v>100</v>
       </c>
-      <c r="CV170" s="8"/>
+      <c r="CV170" s="31">
+        <v>100</v>
+      </c>
       <c r="CW170" s="8"/>
       <c r="CX170" s="8"/>
       <c r="CY170" s="8"/>
@@ -29311,12 +29473,13 @@
       <c r="CM171" s="11"/>
       <c r="CN171" s="11"/>
       <c r="CO171" s="11"/>
-      <c r="CP171" s="11"/>
-      <c r="CQ171" s="11"/>
-      <c r="CR171" s="11"/>
-      <c r="CS171" s="11"/>
-      <c r="CT171" s="11"/>
-      <c r="CU171" s="11"/>
+      <c r="CP171" s="28"/>
+      <c r="CQ171" s="28"/>
+      <c r="CR171" s="28"/>
+      <c r="CS171" s="28"/>
+      <c r="CT171" s="28"/>
+      <c r="CU171" s="28"/>
+      <c r="CV171" s="28"/>
     </row>
     <row r="172" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A172" s="12" t="s">
@@ -29417,13 +29580,13 @@
       <c r="CM173" s="1"/>
       <c r="CN173" s="1"/>
       <c r="CO173" s="1"/>
-      <c r="CP173" s="1"/>
-      <c r="CQ173" s="1"/>
-      <c r="CR173" s="1"/>
-      <c r="CS173" s="1"/>
-      <c r="CT173" s="1"/>
-      <c r="CU173" s="1"/>
-      <c r="CV173" s="16"/>
+      <c r="CP173" s="23"/>
+      <c r="CQ173" s="23"/>
+      <c r="CR173" s="23"/>
+      <c r="CS173" s="23"/>
+      <c r="CT173" s="23"/>
+      <c r="CU173" s="23"/>
+      <c r="CV173" s="23"/>
       <c r="CW173" s="16"/>
       <c r="CX173" s="16"/>
       <c r="CY173" s="16"/>
@@ -29570,13 +29733,13 @@
       <c r="CM174" s="1"/>
       <c r="CN174" s="1"/>
       <c r="CO174" s="1"/>
-      <c r="CP174" s="1"/>
-      <c r="CQ174" s="1"/>
-      <c r="CR174" s="1"/>
-      <c r="CS174" s="1"/>
-      <c r="CT174" s="1"/>
-      <c r="CU174" s="1"/>
-      <c r="CV174" s="16"/>
+      <c r="CP174" s="23"/>
+      <c r="CQ174" s="23"/>
+      <c r="CR174" s="23"/>
+      <c r="CS174" s="23"/>
+      <c r="CT174" s="23"/>
+      <c r="CU174" s="23"/>
+      <c r="CV174" s="23"/>
       <c r="CW174" s="16"/>
       <c r="CX174" s="16"/>
       <c r="CY174" s="16"/>
@@ -29783,9 +29946,9 @@
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="50" max="97" man="1"/>
-    <brk id="100" max="97" man="1"/>
-    <brk id="124" max="97" man="1"/>
+    <brk id="50" max="99" man="1"/>
+    <brk id="100" max="99" man="1"/>
+    <brk id="124" max="99" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>